<commit_message>
Added more card designs
</commit_message>
<xml_diff>
--- a/ShipCardGameCalcs.xlsx
+++ b/ShipCardGameCalcs.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26322"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{B3CB0283-09D9-4255-AD72-C8700D867087}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{2BF1CDC4-7C6D-4D8A-9522-8189B67BAC22}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-15" yWindow="-15" windowWidth="14415" windowHeight="12495" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-15" yWindow="-15" windowWidth="14415" windowHeight="12495" firstSheet="4" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Values" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="319" uniqueCount="146">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="323" uniqueCount="150">
   <si>
     <t>Ship Parameters</t>
   </si>
@@ -349,7 +349,7 @@
     <t>When only 1 player remains in the game they win</t>
   </si>
   <si>
-    <t>If player wants to draw from crew/leader deck and there are no cards left in players crew/leader deck then shuffle are crew/leader deck cards from junkyard back to that deck spot</t>
+    <t>If player wants to draw from crew/leader deck and there are no cards left in players crew/leader deck then shuffle are crew/leader deck cards from stasis back to that deck spot</t>
   </si>
   <si>
     <t>If there are no cards left in the main deck during the draw phase that player loses and is out of the game</t>
@@ -358,7 +358,7 @@
     <t>A player can only have 1 admiral card in play on their side of the battlefield</t>
   </si>
   <si>
-    <t>Both the main deck and crew/leader deck have its own assigned junkyard where certain cards go once played</t>
+    <t>Both the main deck and crew/leader deck have its own assigned stasis where certain cards go once played</t>
   </si>
   <si>
     <t>Controlled deck is the battlefield conditions which affects the battlefield</t>
@@ -442,7 +442,7 @@
     <t>Admiral cards can only be played on your turn</t>
   </si>
   <si>
-    <t>Research Project</t>
+    <t>Event</t>
   </si>
   <si>
     <t>Research project cards are ways for the player to potentially change the tide of battle with either basic card drawing to removing a ships upgrade.</t>
@@ -494,6 +494,18 @@
   </si>
   <si>
     <t>On Going Event cards can only be played on your turn</t>
+  </si>
+  <si>
+    <t>Crew Attachment</t>
+  </si>
+  <si>
+    <t>Attach to crew member to add extract abilities</t>
+  </si>
+  <si>
+    <t>You can play a many Crew Attachment cards as long as you can pay their cost</t>
+  </si>
+  <si>
+    <t>Crew Attachment cards can only be played on your turn</t>
   </si>
   <si>
     <t>Player A</t>
@@ -864,7 +876,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="51">
+  <cellXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -904,42 +916,27 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -947,25 +944,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -974,13 +961,37 @@
     <xf numFmtId="0" fontId="1" fillId="5" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="22" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -3076,21 +3087,21 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17">
-      <c r="A1" s="19" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="19"/>
-      <c r="C1" s="19"/>
-      <c r="D1" s="19"/>
-      <c r="E1" s="19"/>
-      <c r="F1" s="19"/>
-      <c r="G1" s="19"/>
-      <c r="H1" s="19"/>
-      <c r="N1" s="19" t="s">
+      <c r="A1" s="42" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="42"/>
+      <c r="C1" s="42"/>
+      <c r="D1" s="42"/>
+      <c r="E1" s="42"/>
+      <c r="F1" s="42"/>
+      <c r="G1" s="42"/>
+      <c r="H1" s="42"/>
+      <c r="N1" s="42" t="s">
         <v>1</v>
       </c>
-      <c r="O1" s="19"/>
-      <c r="P1" s="19"/>
+      <c r="O1" s="42"/>
+      <c r="P1" s="42"/>
     </row>
     <row r="2" spans="1:17">
       <c r="A2" s="9" t="s">
@@ -3357,25 +3368,25 @@
       </c>
     </row>
     <row r="8" spans="1:17">
-      <c r="A8" s="19" t="s">
+      <c r="A8" s="42" t="s">
         <v>18</v>
       </c>
-      <c r="B8" s="19"/>
-      <c r="C8" s="19"/>
-      <c r="D8" s="19"/>
-      <c r="E8" s="19"/>
-      <c r="F8" s="19"/>
-      <c r="G8" s="19"/>
-      <c r="J8" s="19" t="s">
+      <c r="B8" s="42"/>
+      <c r="C8" s="42"/>
+      <c r="D8" s="42"/>
+      <c r="E8" s="42"/>
+      <c r="F8" s="42"/>
+      <c r="G8" s="42"/>
+      <c r="J8" s="42" t="s">
         <v>19</v>
       </c>
-      <c r="K8" s="19"/>
-      <c r="L8" s="19"/>
-      <c r="M8" s="19"/>
-      <c r="N8" s="19"/>
-      <c r="O8" s="19"/>
-      <c r="P8" s="19"/>
-      <c r="Q8" s="19"/>
+      <c r="K8" s="42"/>
+      <c r="L8" s="42"/>
+      <c r="M8" s="42"/>
+      <c r="N8" s="42"/>
+      <c r="O8" s="42"/>
+      <c r="P8" s="42"/>
+      <c r="Q8" s="42"/>
     </row>
     <row r="9" spans="1:17">
       <c r="A9" s="8" t="s">
@@ -3715,15 +3726,15 @@
       <c r="Q15" s="1"/>
     </row>
     <row r="16" spans="1:17">
-      <c r="A16" s="19" t="s">
+      <c r="A16" s="42" t="s">
         <v>35</v>
       </c>
-      <c r="B16" s="19"/>
-      <c r="C16" s="19"/>
-      <c r="D16" s="19"/>
-      <c r="E16" s="19"/>
-      <c r="F16" s="19"/>
-      <c r="G16" s="19"/>
+      <c r="B16" s="42"/>
+      <c r="C16" s="42"/>
+      <c r="D16" s="42"/>
+      <c r="E16" s="42"/>
+      <c r="F16" s="42"/>
+      <c r="G16" s="42"/>
       <c r="K16" s="1"/>
       <c r="L16" s="1"/>
       <c r="M16" s="1"/>
@@ -3883,30 +3894,30 @@
       <c r="Q20" s="1"/>
     </row>
     <row r="21" spans="1:18">
-      <c r="A21" s="40" t="s">
+      <c r="A21" t="s">
         <v>33</v>
       </c>
-      <c r="B21" s="41">
+      <c r="B21" s="1">
         <f>SUBTOTAL(109,TblFltCrewSizes[A])</f>
         <v>15</v>
       </c>
-      <c r="C21" s="41">
+      <c r="C21" s="1">
         <f>SUBTOTAL(109,TblFltCrewSizes[B])</f>
         <v>15</v>
       </c>
-      <c r="D21" s="41">
+      <c r="D21" s="1">
         <f>SUBTOTAL(109,TblFltCrewSizes[C])</f>
         <v>16</v>
       </c>
-      <c r="E21" s="41">
+      <c r="E21" s="1">
         <f>SUBTOTAL(109,TblFltCrewSizes[D])</f>
         <v>14</v>
       </c>
-      <c r="F21" s="41">
+      <c r="F21" s="1">
         <f>SUBTOTAL(109,TblFltCrewSizes[E])</f>
         <v>16</v>
       </c>
-      <c r="G21" s="41">
+      <c r="G21" s="1">
         <f>SUBTOTAL(109,TblFltCrewSizes[F])</f>
         <v>17</v>
       </c>
@@ -3940,27 +3951,27 @@
       <c r="R22" s="4"/>
     </row>
     <row r="23" spans="1:18">
-      <c r="A23" s="19" t="s">
+      <c r="A23" s="42" t="s">
         <v>40</v>
       </c>
-      <c r="B23" s="19"/>
-      <c r="C23" s="19"/>
-      <c r="D23" s="19"/>
-      <c r="E23" s="19"/>
-      <c r="F23" s="19"/>
-      <c r="G23" s="19"/>
-      <c r="H23" s="19"/>
+      <c r="B23" s="42"/>
+      <c r="C23" s="42"/>
+      <c r="D23" s="42"/>
+      <c r="E23" s="42"/>
+      <c r="F23" s="42"/>
+      <c r="G23" s="42"/>
+      <c r="H23" s="42"/>
       <c r="I23" s="4"/>
-      <c r="J23" s="19" t="s">
+      <c r="J23" s="42" t="s">
         <v>41</v>
       </c>
-      <c r="K23" s="19"/>
-      <c r="L23" s="19"/>
-      <c r="M23" s="19"/>
-      <c r="N23" s="19"/>
-      <c r="O23" s="19"/>
-      <c r="P23" s="19"/>
-      <c r="Q23" s="19"/>
+      <c r="K23" s="42"/>
+      <c r="L23" s="42"/>
+      <c r="M23" s="42"/>
+      <c r="N23" s="42"/>
+      <c r="O23" s="42"/>
+      <c r="P23" s="42"/>
+      <c r="Q23" s="42"/>
     </row>
     <row r="24" spans="1:18">
       <c r="A24" s="8" t="s">
@@ -4388,25 +4399,25 @@
       <c r="Q30" s="1"/>
     </row>
     <row r="31" spans="1:18">
-      <c r="A31" s="19" t="s">
+      <c r="A31" s="42" t="s">
         <v>47</v>
       </c>
-      <c r="B31" s="19"/>
-      <c r="C31" s="19"/>
-      <c r="D31" s="19"/>
-      <c r="E31" s="19"/>
-      <c r="F31" s="19"/>
-      <c r="G31" s="19"/>
+      <c r="B31" s="42"/>
+      <c r="C31" s="42"/>
+      <c r="D31" s="42"/>
+      <c r="E31" s="42"/>
+      <c r="F31" s="42"/>
+      <c r="G31" s="42"/>
       <c r="I31" s="4"/>
-      <c r="J31" s="19" t="s">
+      <c r="J31" s="42" t="s">
         <v>48</v>
       </c>
-      <c r="K31" s="19"/>
-      <c r="L31" s="19"/>
-      <c r="M31" s="19"/>
-      <c r="N31" s="19"/>
-      <c r="O31" s="19"/>
-      <c r="P31" s="19"/>
+      <c r="K31" s="42"/>
+      <c r="L31" s="42"/>
+      <c r="M31" s="42"/>
+      <c r="N31" s="42"/>
+      <c r="O31" s="42"/>
+      <c r="P31" s="42"/>
     </row>
     <row r="32" spans="1:18">
       <c r="A32" t="s">
@@ -5150,22 +5161,22 @@
       </c>
     </row>
     <row r="2" spans="2:22">
-      <c r="B2" s="22" t="s">
+      <c r="B2" s="21" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="25" t="s">
+      <c r="C2" s="24" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="25" t="s">
+      <c r="D2" s="24" t="s">
         <v>50</v>
       </c>
-      <c r="E2" s="25" t="s">
+      <c r="E2" s="24" t="s">
         <v>51</v>
       </c>
-      <c r="F2" s="25" t="s">
+      <c r="F2" s="24" t="s">
         <v>52</v>
       </c>
-      <c r="G2" s="25" t="s">
+      <c r="G2" s="24" t="s">
         <v>53</v>
       </c>
       <c r="L2" t="s">
@@ -5188,22 +5199,22 @@
       </c>
     </row>
     <row r="3" spans="2:22">
-      <c r="B3" s="26" t="s">
+      <c r="B3" s="25" t="s">
         <v>13</v>
       </c>
-      <c r="C3" s="26">
+      <c r="C3" s="25">
         <v>2000</v>
       </c>
-      <c r="D3" s="26">
+      <c r="D3" s="25">
         <v>2000</v>
       </c>
-      <c r="E3" s="26">
+      <c r="E3" s="25">
         <v>2000</v>
       </c>
-      <c r="F3" s="26">
+      <c r="F3" s="25">
         <v>100</v>
       </c>
-      <c r="G3" s="43">
+      <c r="G3" s="34">
         <v>10</v>
       </c>
       <c r="L3">
@@ -5246,22 +5257,22 @@
       </c>
     </row>
     <row r="4" spans="2:22">
-      <c r="B4" s="27" t="s">
+      <c r="B4" s="26" t="s">
         <v>14</v>
       </c>
-      <c r="C4" s="27">
+      <c r="C4" s="26">
         <v>1500</v>
       </c>
-      <c r="D4" s="27">
+      <c r="D4" s="26">
         <v>1500</v>
       </c>
-      <c r="E4" s="27">
+      <c r="E4" s="26">
         <v>1500</v>
       </c>
-      <c r="F4" s="27">
+      <c r="F4" s="26">
         <v>100</v>
       </c>
-      <c r="G4" s="44">
+      <c r="G4" s="35">
         <v>7</v>
       </c>
       <c r="L4">
@@ -5304,22 +5315,22 @@
       </c>
     </row>
     <row r="5" spans="2:22">
-      <c r="B5" s="28" t="s">
+      <c r="B5" s="27" t="s">
         <v>15</v>
       </c>
-      <c r="C5" s="28">
+      <c r="C5" s="27">
         <v>1000</v>
       </c>
-      <c r="D5" s="28">
+      <c r="D5" s="27">
         <v>1000</v>
       </c>
-      <c r="E5" s="28">
+      <c r="E5" s="27">
         <v>1000</v>
       </c>
-      <c r="F5" s="28">
+      <c r="F5" s="27">
         <v>100</v>
       </c>
-      <c r="G5" s="43">
+      <c r="G5" s="34">
         <v>5</v>
       </c>
       <c r="L5">
@@ -5355,22 +5366,22 @@
       </c>
     </row>
     <row r="6" spans="2:22">
-      <c r="B6" s="27" t="s">
+      <c r="B6" s="26" t="s">
         <v>16</v>
       </c>
-      <c r="C6" s="27">
+      <c r="C6" s="26">
         <v>500</v>
       </c>
-      <c r="D6" s="27">
+      <c r="D6" s="26">
         <v>500</v>
       </c>
-      <c r="E6" s="27">
+      <c r="E6" s="26">
         <v>500</v>
       </c>
-      <c r="F6" s="27">
+      <c r="F6" s="26">
         <v>100</v>
       </c>
-      <c r="G6" s="44">
+      <c r="G6" s="35">
         <v>3</v>
       </c>
       <c r="L6">
@@ -5406,22 +5417,22 @@
       </c>
     </row>
     <row r="7" spans="2:22">
-      <c r="B7" s="28" t="s">
+      <c r="B7" s="27" t="s">
         <v>17</v>
       </c>
-      <c r="C7" s="28">
+      <c r="C7" s="27">
         <v>100</v>
       </c>
-      <c r="D7" s="28">
+      <c r="D7" s="27">
         <v>100</v>
       </c>
-      <c r="E7" s="28">
+      <c r="E7" s="27">
         <v>100</v>
       </c>
-      <c r="F7" s="28">
+      <c r="F7" s="27">
         <v>100</v>
       </c>
-      <c r="G7" s="43">
+      <c r="G7" s="34">
         <v>1</v>
       </c>
       <c r="L7">
@@ -5517,19 +5528,19 @@
       </c>
     </row>
     <row r="11" spans="2:22">
-      <c r="B11" s="20" t="s">
+      <c r="B11" s="19" t="s">
         <v>56</v>
       </c>
-      <c r="C11" s="20" t="s">
+      <c r="C11" s="19" t="s">
         <v>57</v>
       </c>
-      <c r="D11" s="20" t="s">
+      <c r="D11" s="19" t="s">
         <v>58</v>
       </c>
-      <c r="E11" s="20" t="s">
+      <c r="E11" s="19" t="s">
         <v>59</v>
       </c>
-      <c r="F11" s="20" t="s">
+      <c r="F11" s="19" t="s">
         <v>60</v>
       </c>
       <c r="L11">
@@ -5551,19 +5562,19 @@
       </c>
     </row>
     <row r="12" spans="2:22" ht="76.5">
-      <c r="B12" s="21" t="s">
+      <c r="B12" s="20" t="s">
         <v>61</v>
       </c>
-      <c r="C12" s="21" t="s">
+      <c r="C12" s="20" t="s">
         <v>62</v>
       </c>
-      <c r="D12" s="21" t="s">
+      <c r="D12" s="20" t="s">
         <v>63</v>
       </c>
-      <c r="E12" s="21" t="s">
+      <c r="E12" s="20" t="s">
         <v>64</v>
       </c>
-      <c r="F12" s="21" t="s">
+      <c r="F12" s="20" t="s">
         <v>65</v>
       </c>
       <c r="L12">
@@ -5602,16 +5613,16 @@
       </c>
     </row>
     <row r="15" spans="2:22">
-      <c r="B15" s="22" t="s">
+      <c r="B15" s="21" t="s">
         <v>2</v>
       </c>
-      <c r="C15" s="42" t="s">
+      <c r="C15" s="33" t="s">
         <v>4</v>
       </c>
-      <c r="D15" s="42" t="s">
+      <c r="D15" s="33" t="s">
         <v>5</v>
       </c>
-      <c r="E15" s="42" t="s">
+      <c r="E15" s="33" t="s">
         <v>6</v>
       </c>
       <c r="L15">
@@ -5619,16 +5630,16 @@
       </c>
     </row>
     <row r="16" spans="2:22">
-      <c r="B16" s="23" t="s">
+      <c r="B16" s="22" t="s">
         <v>13</v>
       </c>
-      <c r="C16" s="43">
+      <c r="C16" s="34">
         <v>11</v>
       </c>
-      <c r="D16" s="43">
+      <c r="D16" s="34">
         <v>3</v>
       </c>
-      <c r="E16" s="43">
+      <c r="E16" s="34">
         <v>1</v>
       </c>
       <c r="L16">
@@ -5636,16 +5647,16 @@
       </c>
     </row>
     <row r="17" spans="2:12">
-      <c r="B17" s="24" t="s">
+      <c r="B17" s="23" t="s">
         <v>14</v>
       </c>
-      <c r="C17" s="44">
+      <c r="C17" s="35">
         <v>8</v>
       </c>
-      <c r="D17" s="44">
+      <c r="D17" s="35">
         <v>2</v>
       </c>
-      <c r="E17" s="44">
+      <c r="E17" s="35">
         <v>1</v>
       </c>
       <c r="L17">
@@ -5653,16 +5664,16 @@
       </c>
     </row>
     <row r="18" spans="2:12">
-      <c r="B18" s="23" t="s">
+      <c r="B18" s="22" t="s">
         <v>15</v>
       </c>
-      <c r="C18" s="43">
+      <c r="C18" s="34">
         <v>5</v>
       </c>
-      <c r="D18" s="43">
+      <c r="D18" s="34">
         <v>1</v>
       </c>
-      <c r="E18" s="43">
+      <c r="E18" s="34">
         <v>1</v>
       </c>
       <c r="L18">
@@ -5670,16 +5681,16 @@
       </c>
     </row>
     <row r="19" spans="2:12">
-      <c r="B19" s="24" t="s">
+      <c r="B19" s="23" t="s">
         <v>16</v>
       </c>
-      <c r="C19" s="44">
+      <c r="C19" s="35">
         <v>3</v>
       </c>
-      <c r="D19" s="44">
+      <c r="D19" s="35">
         <v>1</v>
       </c>
-      <c r="E19" s="44">
+      <c r="E19" s="35">
         <v>0</v>
       </c>
       <c r="L19">
@@ -5687,16 +5698,16 @@
       </c>
     </row>
     <row r="20" spans="2:12">
-      <c r="B20" s="23" t="s">
+      <c r="B20" s="22" t="s">
         <v>17</v>
       </c>
-      <c r="C20" s="43">
+      <c r="C20" s="34">
         <v>1</v>
       </c>
-      <c r="D20" s="43">
-        <v>0</v>
-      </c>
-      <c r="E20" s="43">
+      <c r="D20" s="34">
+        <v>0</v>
+      </c>
+      <c r="E20" s="34">
         <v>0</v>
       </c>
       <c r="L20">
@@ -5714,25 +5725,25 @@
       </c>
     </row>
     <row r="23" spans="2:12">
-      <c r="B23" s="45" t="s">
+      <c r="B23" s="36" t="s">
         <v>20</v>
       </c>
-      <c r="C23" s="46" t="s">
+      <c r="C23" s="37" t="s">
         <v>21</v>
       </c>
-      <c r="D23" s="46" t="s">
+      <c r="D23" s="37" t="s">
         <v>22</v>
       </c>
-      <c r="E23" s="46" t="s">
+      <c r="E23" s="37" t="s">
         <v>23</v>
       </c>
-      <c r="F23" s="46" t="s">
+      <c r="F23" s="37" t="s">
         <v>24</v>
       </c>
-      <c r="G23" s="46" t="s">
+      <c r="G23" s="37" t="s">
         <v>25</v>
       </c>
-      <c r="H23" s="46" t="s">
+      <c r="H23" s="37" t="s">
         <v>26</v>
       </c>
       <c r="L23">
@@ -5740,53 +5751,53 @@
       </c>
     </row>
     <row r="24" spans="2:12">
-      <c r="B24" s="47" t="s">
+      <c r="B24" s="38" t="s">
         <v>13</v>
       </c>
-      <c r="C24" s="48">
+      <c r="C24" s="39">
         <v>1</v>
       </c>
-      <c r="D24" s="48"/>
-      <c r="E24" s="48"/>
-      <c r="F24" s="48"/>
-      <c r="G24" s="48"/>
-      <c r="H24" s="48"/>
+      <c r="D24" s="39"/>
+      <c r="E24" s="39"/>
+      <c r="F24" s="39"/>
+      <c r="G24" s="39"/>
+      <c r="H24" s="39"/>
       <c r="L24">
         <v>22</v>
       </c>
     </row>
     <row r="25" spans="2:12">
-      <c r="B25" s="49" t="s">
+      <c r="B25" s="40" t="s">
         <v>14</v>
       </c>
-      <c r="C25" s="50"/>
-      <c r="D25" s="50">
+      <c r="C25" s="41"/>
+      <c r="D25" s="41">
         <v>1</v>
       </c>
-      <c r="E25" s="50">
+      <c r="E25" s="41">
         <v>1</v>
       </c>
-      <c r="F25" s="50"/>
-      <c r="G25" s="50"/>
-      <c r="H25" s="50"/>
+      <c r="F25" s="41"/>
+      <c r="G25" s="41"/>
+      <c r="H25" s="41"/>
       <c r="L25">
         <v>23</v>
       </c>
     </row>
     <row r="26" spans="2:12">
-      <c r="B26" s="47" t="s">
+      <c r="B26" s="38" t="s">
         <v>15</v>
       </c>
-      <c r="C26" s="48"/>
-      <c r="D26" s="48"/>
-      <c r="E26" s="48"/>
-      <c r="F26" s="48">
+      <c r="C26" s="39"/>
+      <c r="D26" s="39"/>
+      <c r="E26" s="39"/>
+      <c r="F26" s="39">
         <v>2</v>
       </c>
-      <c r="G26" s="48">
+      <c r="G26" s="39">
         <v>1</v>
       </c>
-      <c r="H26" s="48">
+      <c r="H26" s="39">
         <v>1</v>
       </c>
       <c r="L26">
@@ -5794,37 +5805,37 @@
       </c>
     </row>
     <row r="27" spans="2:12">
-      <c r="B27" s="49" t="s">
+      <c r="B27" s="40" t="s">
         <v>16</v>
       </c>
-      <c r="C27" s="50"/>
-      <c r="D27" s="50">
+      <c r="C27" s="41"/>
+      <c r="D27" s="41">
         <v>1</v>
       </c>
-      <c r="E27" s="50"/>
-      <c r="F27" s="50"/>
-      <c r="G27" s="50">
+      <c r="E27" s="41"/>
+      <c r="F27" s="41"/>
+      <c r="G27" s="41">
         <v>1</v>
       </c>
-      <c r="H27" s="50"/>
+      <c r="H27" s="41"/>
       <c r="L27">
         <v>25</v>
       </c>
     </row>
     <row r="28" spans="2:12">
-      <c r="B28" s="47" t="s">
+      <c r="B28" s="38" t="s">
         <v>17</v>
       </c>
-      <c r="C28" s="48"/>
-      <c r="D28" s="48"/>
-      <c r="E28" s="48">
+      <c r="C28" s="39"/>
+      <c r="D28" s="39"/>
+      <c r="E28" s="39">
         <v>5</v>
       </c>
-      <c r="F28" s="48"/>
-      <c r="G28" s="48">
+      <c r="F28" s="39"/>
+      <c r="G28" s="39">
         <v>5</v>
       </c>
-      <c r="H28" s="48">
+      <c r="H28" s="39">
         <v>10</v>
       </c>
       <c r="L28">
@@ -5867,7 +5878,7 @@
   <dimension ref="B2:B30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="L17" sqref="L17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -5876,7 +5887,7 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:2">
-      <c r="B2" s="22" t="s">
+      <c r="B2" s="21" t="s">
         <v>66</v>
       </c>
     </row>
@@ -6027,7 +6038,7 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6016CF9E-E144-48D8-959F-618B8D85D284}">
-  <dimension ref="B2:M15"/>
+  <dimension ref="B2:B11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="I20" sqref="I20"/>
@@ -6035,108 +6046,55 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="2" spans="2:13">
+    <row r="2" spans="2:2">
       <c r="B2" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="3" spans="2:13">
+    <row r="3" spans="2:2">
       <c r="B3" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="4" spans="2:13">
+    <row r="4" spans="2:2">
       <c r="B4" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="5" spans="2:13">
+    <row r="5" spans="2:2">
       <c r="B5" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="6" spans="2:13">
+    <row r="6" spans="2:2">
       <c r="B6" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="7" spans="2:13">
+    <row r="7" spans="2:2">
       <c r="B7" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="8" spans="2:13">
+    <row r="8" spans="2:2">
       <c r="B8" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="9" spans="2:13">
+    <row r="9" spans="2:2">
       <c r="B9" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="10" spans="2:13">
+    <row r="10" spans="2:2">
       <c r="B10" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="11" spans="2:13">
+    <row r="11" spans="2:2">
       <c r="B11" t="s">
         <v>104</v>
       </c>
-      <c r="E11" s="40"/>
-      <c r="F11" s="40"/>
-      <c r="G11" s="40"/>
-      <c r="H11" s="40"/>
-      <c r="I11" s="40"/>
-      <c r="J11" s="40"/>
-      <c r="K11" s="40"/>
-      <c r="L11" s="40"/>
-      <c r="M11" s="40"/>
-    </row>
-    <row r="12" spans="2:13">
-      <c r="E12" s="40"/>
-      <c r="F12" s="40"/>
-      <c r="G12" s="40"/>
-      <c r="H12" s="40"/>
-      <c r="I12" s="40"/>
-      <c r="J12" s="40"/>
-      <c r="K12" s="40"/>
-      <c r="L12" s="40"/>
-      <c r="M12" s="40"/>
-    </row>
-    <row r="13" spans="2:13">
-      <c r="E13" s="40"/>
-      <c r="F13" s="40"/>
-      <c r="G13" s="40"/>
-      <c r="H13" s="40"/>
-      <c r="I13" s="40"/>
-      <c r="J13" s="40"/>
-      <c r="K13" s="40"/>
-      <c r="L13" s="40"/>
-      <c r="M13" s="40"/>
-    </row>
-    <row r="14" spans="2:13">
-      <c r="E14" s="40"/>
-      <c r="F14" s="40"/>
-      <c r="G14" s="40"/>
-      <c r="H14" s="40"/>
-      <c r="I14" s="40"/>
-      <c r="J14" s="40"/>
-      <c r="K14" s="40"/>
-      <c r="L14" s="40"/>
-      <c r="M14" s="40"/>
-    </row>
-    <row r="15" spans="2:13">
-      <c r="E15" s="40"/>
-      <c r="F15" s="40"/>
-      <c r="G15" s="40"/>
-      <c r="H15" s="40"/>
-      <c r="I15" s="40"/>
-      <c r="J15" s="40"/>
-      <c r="K15" s="40"/>
-      <c r="L15" s="40"/>
-      <c r="M15" s="40"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -6145,10 +6103,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1CADF2F4-A124-44BC-8A72-4CE3F16F5D04}">
-  <dimension ref="B2:D20"/>
+  <dimension ref="B2:D22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="D22" sqref="B21:D22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -6159,178 +6117,192 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:4">
-      <c r="B2" s="39" t="s">
+      <c r="B2" s="32" t="s">
         <v>105</v>
       </c>
-      <c r="C2" s="39" t="s">
+      <c r="C2" s="32" t="s">
         <v>106</v>
       </c>
-      <c r="D2" s="39" t="s">
+      <c r="D2" s="32" t="s">
         <v>107</v>
       </c>
     </row>
     <row r="3" spans="2:4" ht="106.5" customHeight="1">
-      <c r="B3" s="29" t="s">
+      <c r="B3" s="45" t="s">
         <v>108</v>
       </c>
-      <c r="C3" s="30" t="s">
+      <c r="C3" s="43" t="s">
         <v>109</v>
       </c>
-      <c r="D3" s="31" t="s">
+      <c r="D3" s="28" t="s">
         <v>110</v>
       </c>
     </row>
     <row r="4" spans="2:4" ht="106.5">
-      <c r="B4" s="32"/>
-      <c r="C4" s="33"/>
-      <c r="D4" s="34" t="s">
+      <c r="B4" s="48"/>
+      <c r="C4" s="47"/>
+      <c r="D4" s="29" t="s">
         <v>111</v>
       </c>
     </row>
     <row r="5" spans="2:4" ht="60.75">
-      <c r="B5" s="32"/>
-      <c r="C5" s="33"/>
-      <c r="D5" s="35" t="s">
+      <c r="B5" s="48"/>
+      <c r="C5" s="47"/>
+      <c r="D5" s="30" t="s">
         <v>112</v>
       </c>
     </row>
     <row r="6" spans="2:4" ht="76.5">
-      <c r="B6" s="32"/>
-      <c r="C6" s="33"/>
-      <c r="D6" s="35" t="s">
+      <c r="B6" s="48"/>
+      <c r="C6" s="47"/>
+      <c r="D6" s="30" t="s">
         <v>113</v>
       </c>
     </row>
     <row r="7" spans="2:4" ht="91.5">
-      <c r="B7" s="29" t="s">
+      <c r="B7" s="45" t="s">
         <v>114</v>
       </c>
-      <c r="C7" s="30" t="s">
+      <c r="C7" s="43" t="s">
         <v>115</v>
       </c>
-      <c r="D7" s="31" t="s">
+      <c r="D7" s="28" t="s">
         <v>116</v>
       </c>
     </row>
     <row r="8" spans="2:4" ht="91.5">
-      <c r="B8" s="32"/>
-      <c r="C8" s="33"/>
-      <c r="D8" s="35" t="s">
+      <c r="B8" s="48"/>
+      <c r="C8" s="47"/>
+      <c r="D8" s="30" t="s">
         <v>117</v>
       </c>
     </row>
     <row r="9" spans="2:4" ht="76.5">
-      <c r="B9" s="29" t="s">
+      <c r="B9" s="45" t="s">
         <v>118</v>
       </c>
-      <c r="C9" s="30" t="s">
+      <c r="C9" s="43" t="s">
         <v>119</v>
       </c>
-      <c r="D9" s="31" t="s">
+      <c r="D9" s="28" t="s">
         <v>120</v>
       </c>
     </row>
     <row r="10" spans="2:4" ht="30.75">
-      <c r="B10" s="36"/>
-      <c r="C10" s="37"/>
-      <c r="D10" s="38" t="s">
+      <c r="B10" s="46"/>
+      <c r="C10" s="44"/>
+      <c r="D10" s="31" t="s">
         <v>121</v>
       </c>
     </row>
     <row r="11" spans="2:4" ht="76.5" customHeight="1">
-      <c r="B11" s="29" t="s">
+      <c r="B11" s="45" t="s">
         <v>122</v>
       </c>
-      <c r="C11" s="30" t="s">
+      <c r="C11" s="43" t="s">
         <v>123</v>
       </c>
-      <c r="D11" s="31" t="s">
+      <c r="D11" s="28" t="s">
         <v>124</v>
       </c>
     </row>
     <row r="12" spans="2:4" ht="30.75">
-      <c r="B12" s="32"/>
-      <c r="C12" s="33"/>
-      <c r="D12" s="35" t="s">
+      <c r="B12" s="48"/>
+      <c r="C12" s="47"/>
+      <c r="D12" s="30" t="s">
         <v>125</v>
       </c>
     </row>
     <row r="13" spans="2:4" ht="45.75">
-      <c r="B13" s="29" t="s">
+      <c r="B13" s="45" t="s">
         <v>126</v>
       </c>
-      <c r="C13" s="30" t="s">
+      <c r="C13" s="43" t="s">
         <v>127</v>
       </c>
-      <c r="D13" s="31" t="s">
+      <c r="D13" s="28" t="s">
         <v>128</v>
       </c>
     </row>
     <row r="14" spans="2:4" ht="30.75">
-      <c r="B14" s="32"/>
-      <c r="C14" s="33"/>
-      <c r="D14" s="35" t="s">
+      <c r="B14" s="48"/>
+      <c r="C14" s="47"/>
+      <c r="D14" s="30" t="s">
         <v>129</v>
       </c>
     </row>
     <row r="15" spans="2:4" ht="45.75">
-      <c r="B15" s="32"/>
-      <c r="C15" s="33"/>
-      <c r="D15" s="35" t="s">
+      <c r="B15" s="48"/>
+      <c r="C15" s="47"/>
+      <c r="D15" s="30" t="s">
         <v>130</v>
       </c>
     </row>
     <row r="16" spans="2:4" ht="60.75">
-      <c r="B16" s="32"/>
-      <c r="C16" s="33"/>
-      <c r="D16" s="35" t="s">
+      <c r="B16" s="48"/>
+      <c r="C16" s="47"/>
+      <c r="D16" s="30" t="s">
         <v>131</v>
       </c>
     </row>
     <row r="17" spans="2:4" ht="45.75">
-      <c r="B17" s="29" t="s">
+      <c r="B17" s="45" t="s">
         <v>132</v>
       </c>
-      <c r="C17" s="30" t="s">
+      <c r="C17" s="43" t="s">
         <v>133</v>
       </c>
-      <c r="D17" s="31" t="s">
+      <c r="D17" s="28" t="s">
         <v>134</v>
       </c>
     </row>
     <row r="18" spans="2:4" ht="45.75">
-      <c r="B18" s="32"/>
-      <c r="C18" s="33"/>
-      <c r="D18" s="35" t="s">
+      <c r="B18" s="48"/>
+      <c r="C18" s="47"/>
+      <c r="D18" s="30" t="s">
         <v>135</v>
       </c>
     </row>
     <row r="19" spans="2:4" ht="60.75" customHeight="1">
-      <c r="B19" s="29" t="s">
+      <c r="B19" s="45" t="s">
         <v>136</v>
       </c>
-      <c r="C19" s="30" t="s">
+      <c r="C19" s="43" t="s">
         <v>137</v>
       </c>
-      <c r="D19" s="31" t="s">
+      <c r="D19" s="28" t="s">
         <v>138</v>
       </c>
     </row>
     <row r="20" spans="2:4" ht="30.75">
-      <c r="B20" s="36"/>
-      <c r="C20" s="37"/>
-      <c r="D20" s="38" t="s">
+      <c r="B20" s="48"/>
+      <c r="C20" s="49"/>
+      <c r="D20" s="30" t="s">
         <v>139</v>
       </c>
     </row>
+    <row r="21" spans="2:4" ht="45.75">
+      <c r="B21" s="45" t="s">
+        <v>140</v>
+      </c>
+      <c r="C21" s="43" t="s">
+        <v>141</v>
+      </c>
+      <c r="D21" s="28" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="22" spans="2:4" ht="30.75">
+      <c r="B22" s="46"/>
+      <c r="C22" s="44"/>
+      <c r="D22" s="31" t="s">
+        <v>143</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="14">
-    <mergeCell ref="C9:C10"/>
-    <mergeCell ref="B9:B10"/>
-    <mergeCell ref="C13:C16"/>
-    <mergeCell ref="B13:B16"/>
-    <mergeCell ref="C17:C18"/>
-    <mergeCell ref="B17:B18"/>
+  <mergeCells count="16">
+    <mergeCell ref="C21:C22"/>
+    <mergeCell ref="B21:B22"/>
     <mergeCell ref="C19:C20"/>
     <mergeCell ref="B19:B20"/>
     <mergeCell ref="B3:B6"/>
@@ -6339,6 +6311,12 @@
     <mergeCell ref="C7:C8"/>
     <mergeCell ref="B11:B12"/>
     <mergeCell ref="C11:C12"/>
+    <mergeCell ref="C9:C10"/>
+    <mergeCell ref="B9:B10"/>
+    <mergeCell ref="C13:C16"/>
+    <mergeCell ref="B13:B16"/>
+    <mergeCell ref="C17:C18"/>
+    <mergeCell ref="B17:B18"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -6363,26 +6341,26 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:19">
-      <c r="A2" s="19" t="s">
-        <v>140</v>
-      </c>
-      <c r="B2" s="19"/>
-      <c r="C2" s="19"/>
-      <c r="F2" s="19" t="s">
-        <v>141</v>
-      </c>
-      <c r="G2" s="19"/>
-      <c r="H2" s="19"/>
+      <c r="A2" s="42" t="s">
+        <v>144</v>
+      </c>
+      <c r="B2" s="42"/>
+      <c r="C2" s="42"/>
+      <c r="F2" s="42" t="s">
+        <v>145</v>
+      </c>
+      <c r="G2" s="42"/>
+      <c r="H2" s="42"/>
     </row>
     <row r="3" spans="1:19">
       <c r="A3" t="s">
-        <v>142</v>
+        <v>146</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>21</v>
       </c>
       <c r="F3" t="s">
-        <v>142</v>
+        <v>146</v>
       </c>
       <c r="G3" s="1" t="s">
         <v>26</v>
@@ -6406,14 +6384,14 @@
     </row>
     <row r="5" spans="1:19">
       <c r="A5" t="s">
-        <v>143</v>
+        <v>147</v>
       </c>
       <c r="B5">
         <f>SUM(C10:C14)</f>
         <v>5000</v>
       </c>
       <c r="F5" t="s">
-        <v>143</v>
+        <v>147</v>
       </c>
       <c r="G5">
         <f>SUM(H10:H14)</f>
@@ -6422,14 +6400,14 @@
     </row>
     <row r="6" spans="1:19">
       <c r="A6" t="s">
-        <v>144</v>
+        <v>148</v>
       </c>
       <c r="B6">
         <f>SUM(C17:C19)</f>
         <v>2000</v>
       </c>
       <c r="F6" t="s">
-        <v>144</v>
+        <v>148</v>
       </c>
       <c r="G6">
         <f>SUM(H17:H19)</f>
@@ -6451,7 +6429,7 @@
         <v>2</v>
       </c>
       <c r="B9" s="17" t="s">
-        <v>145</v>
+        <v>149</v>
       </c>
       <c r="C9" s="17" t="s">
         <v>3</v>
@@ -6460,7 +6438,7 @@
         <v>2</v>
       </c>
       <c r="G9" s="17" t="s">
-        <v>145</v>
+        <v>149</v>
       </c>
       <c r="H9" s="17" t="s">
         <v>3</v>
@@ -6650,7 +6628,7 @@
         <v>108</v>
       </c>
       <c r="B16" s="17" t="s">
-        <v>145</v>
+        <v>149</v>
       </c>
       <c r="C16" t="s">
         <v>3</v>
@@ -6659,7 +6637,7 @@
         <v>108</v>
       </c>
       <c r="G16" s="17" t="s">
-        <v>145</v>
+        <v>149</v>
       </c>
       <c r="H16" t="s">
         <v>3</v>

</xml_diff>

<commit_message>
Added pivot tables to keep track of card count and reached 100 card designs.Need to add more higher costing cards since a lot of cards allow crew members to increase their output
</commit_message>
<xml_diff>
--- a/ShipCardGameCalcs.xlsx
+++ b/ShipCardGameCalcs.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26322"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26324"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{2BF1CDC4-7C6D-4D8A-9522-8189B67BAC22}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{4287F3BC-8CF1-471C-BCF0-1A757F5C6452}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-15" yWindow="-15" windowWidth="14415" windowHeight="12495" firstSheet="4" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-15" yWindow="-15" windowWidth="14415" windowHeight="12495" firstSheet="4" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Values" sheetId="1" r:id="rId1"/>
@@ -286,10 +286,10 @@
     <t>Players can't see what ships the other player has picked until both have locked them in</t>
   </si>
   <si>
-    <t>Once players have picked their ships, they then start off by drawing two cards from their crew/leaders deck and 5 from their main deck</t>
-  </si>
-  <si>
-    <t>A player gets 1 free mulligan but if they choose to mulligan anymore times than that they reduce the amount of cards drawn from main deck by 1 each time. Down to a minimum of 1 card from their main deck and 2 from their leader deck</t>
+    <t>Once players have picked their ships, they then start off by drawing two cards from their crew/leaders deck and 5 from their strategy deck</t>
+  </si>
+  <si>
+    <t>A player gets 1 free mulligan but if they choose to mulligan anymore times than that they reduce the amount of cards drawn from strategy deck by 1 each time. Down to a minimum of 1 card from their strategy deck and 2 from their leader deck</t>
   </si>
   <si>
     <t>Any crew card placed cant be used to tap on first turn placed (unless card in play says otherwise)</t>
@@ -301,13 +301,13 @@
     <t>A crew /leader deck can only contain cards of Type Captain, Leuitenant and Crew Rank 1</t>
   </si>
   <si>
-    <t>The main deck has every other card</t>
+    <t>The strategy deck has every other card</t>
   </si>
   <si>
     <t>A player can only play 1 crew member and 1 Captain/Leuitenant per turn</t>
   </si>
   <si>
-    <t>On start of turn player can choose to either draw 2 cards from main deck, 2 cards from crew/leader deck or 1 from each.</t>
+    <t>On start of turn player can choose to either draw 2 cards from strategy deck, 2 cards from crew/leader deck or 1 from each.</t>
   </si>
   <si>
     <t>On end of turn if player has more than Max player hand size they must discard cards down to max hand size</t>
@@ -352,13 +352,13 @@
     <t>If player wants to draw from crew/leader deck and there are no cards left in players crew/leader deck then shuffle are crew/leader deck cards from stasis back to that deck spot</t>
   </si>
   <si>
-    <t>If there are no cards left in the main deck during the draw phase that player loses and is out of the game</t>
+    <t>If there are no cards left in the strategy deck during the draw phase that player loses and is out of the game</t>
   </si>
   <si>
     <t>A player can only have 1 admiral card in play on their side of the battlefield</t>
   </si>
   <si>
-    <t>Both the main deck and crew/leader deck have its own assigned stasis where certain cards go once played</t>
+    <t>Both the strategy deck and crew/leader deck have its own assigned stasis where certain cards go once played</t>
   </si>
   <si>
     <t>Controlled deck is the battlefield conditions which affects the battlefield</t>
@@ -876,7 +876,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="50">
+  <cellXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -989,9 +989,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -5141,8 +5138,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{91273792-62E9-442E-9CC7-E8C6E6BD4008}">
   <dimension ref="B1:V29"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J15" sqref="J15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H7" sqref="H3:H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -5878,7 +5875,7 @@
   <dimension ref="B2:B30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="L17" sqref="L17"/>
+      <selection activeCell="M13" sqref="M13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -6105,7 +6102,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1CADF2F4-A124-44BC-8A72-4CE3F16F5D04}">
   <dimension ref="B2:D22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D22" sqref="B21:D22"/>
     </sheetView>
   </sheetViews>
@@ -6276,7 +6273,7 @@
     </row>
     <row r="20" spans="2:4" ht="30.75">
       <c r="B20" s="48"/>
-      <c r="C20" s="49"/>
+      <c r="C20" s="47"/>
       <c r="D20" s="30" t="s">
         <v>139</v>
       </c>

</xml_diff>

<commit_message>
Been play testing etc
</commit_message>
<xml_diff>
--- a/ShipCardGameCalcs.xlsx
+++ b/ShipCardGameCalcs.xlsx
@@ -3,17 +3,18 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26324"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{4287F3BC-8CF1-471C-BCF0-1A757F5C6452}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{CC049761-E7FC-4643-98CB-6C747A6B0A47}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-15" yWindow="-15" windowWidth="14415" windowHeight="12495" firstSheet="4" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-15" yWindow="-15" windowWidth="14415" windowHeight="12495" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Values" sheetId="1" r:id="rId1"/>
     <sheet name="Ships and Crew Details" sheetId="3" r:id="rId2"/>
-    <sheet name="Game Rules and Turn Example" sheetId="4" r:id="rId3"/>
-    <sheet name="Ideas" sheetId="6" r:id="rId4"/>
-    <sheet name="Card Details" sheetId="5" r:id="rId5"/>
-    <sheet name="Comparison" sheetId="2" r:id="rId6"/>
+    <sheet name="Game Setup" sheetId="7" r:id="rId3"/>
+    <sheet name="Game Rules and Turn Example" sheetId="4" r:id="rId4"/>
+    <sheet name="Ideas" sheetId="6" r:id="rId5"/>
+    <sheet name="Card Details" sheetId="5" r:id="rId6"/>
+    <sheet name="Comparison" sheetId="2" r:id="rId7"/>
   </sheets>
   <calcPr calcId="191028"/>
   <extLst>
@@ -33,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="323" uniqueCount="150">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="367" uniqueCount="159">
   <si>
     <t>Ship Parameters</t>
   </si>
@@ -238,6 +239,9 @@
     <t>Guns</t>
   </si>
   <si>
+    <t>Escape Pods</t>
+  </si>
+  <si>
     <t>Turn</t>
   </si>
   <si>
@@ -247,7 +251,7 @@
     <t>Research</t>
   </si>
   <si>
-    <t xml:space="preserve">Maneuverability </t>
+    <t>Handling</t>
   </si>
   <si>
     <t xml:space="preserve">Medical </t>
@@ -274,6 +278,27 @@
     <t>Points towards cards based around enemy crew</t>
   </si>
   <si>
+    <t>Assault</t>
+  </si>
+  <si>
+    <t>Player 1</t>
+  </si>
+  <si>
+    <t>Junkyard</t>
+  </si>
+  <si>
+    <t>Strategy Deck</t>
+  </si>
+  <si>
+    <t>Stasis</t>
+  </si>
+  <si>
+    <t>Crew Deck</t>
+  </si>
+  <si>
+    <t>Player 2</t>
+  </si>
+  <si>
     <t>Game Rules</t>
   </si>
   <si>
@@ -286,16 +311,19 @@
     <t>Players can't see what ships the other player has picked until both have locked them in</t>
   </si>
   <si>
-    <t>Once players have picked their ships, they then start off by drawing two cards from their crew/leaders deck and 5 from their strategy deck</t>
+    <t>Once players have picked their ships, they then start off by drawing two cards from their crew/leaders deck and 4 from their strategy deck</t>
   </si>
   <si>
     <t>A player gets 1 free mulligan but if they choose to mulligan anymore times than that they reduce the amount of cards drawn from strategy deck by 1 each time. Down to a minimum of 1 card from their strategy deck and 2 from their leader deck</t>
   </si>
   <si>
-    <t>Any crew card placed cant be used to tap on first turn placed (unless card in play says otherwise)</t>
-  </si>
-  <si>
-    <t>Max player hand size is 6 (unless card in play says otherwise)</t>
+    <t>A crew member first placed on to a ship can't be used in a gun slot</t>
+  </si>
+  <si>
+    <t>Any crew card placed can be used to tap on first turn placed</t>
+  </si>
+  <si>
+    <t>Max player hand size is 8 (unless card in play says otherwise)</t>
   </si>
   <si>
     <t>A crew /leader deck can only contain cards of Type Captain, Leuitenant and Crew Rank 1</t>
@@ -530,7 +558,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
-  <fonts count="6">
+  <fonts count="8">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -573,8 +601,22 @@
       <name val="Calibri"/>
       <charset val="1"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF444444"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
   </fonts>
-  <fills count="7">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -609,6 +651,18 @@
       <patternFill patternType="solid">
         <fgColor theme="0" tint="-0.14999847407452621"/>
         <bgColor theme="0" tint="-0.14999847407452621"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF0070C0"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -876,7 +930,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="49">
+  <cellXfs count="55">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -990,6 +1044,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -3062,7 +3122,7 @@
   <dimension ref="A1:R51"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I14" sqref="I14"/>
+      <selection activeCell="I10" sqref="I10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -5139,7 +5199,7 @@
   <dimension ref="B1:V29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H7" sqref="H3:H7"/>
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -5149,6 +5209,7 @@
     <col min="4" max="4" width="15.7109375" customWidth="1"/>
     <col min="5" max="5" width="17.140625" customWidth="1"/>
     <col min="6" max="6" width="17.7109375" customWidth="1"/>
+    <col min="8" max="8" width="12" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="34" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -5176,8 +5237,11 @@
       <c r="G2" s="24" t="s">
         <v>53</v>
       </c>
+      <c r="H2" s="24" t="s">
+        <v>54</v>
+      </c>
       <c r="L2" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="M2" t="s">
         <v>13</v>
@@ -5214,6 +5278,9 @@
       <c r="G3" s="34">
         <v>10</v>
       </c>
+      <c r="H3">
+        <v>5</v>
+      </c>
       <c r="L3">
         <v>1</v>
       </c>
@@ -5272,6 +5339,9 @@
       <c r="G4" s="35">
         <v>7</v>
       </c>
+      <c r="H4">
+        <v>4</v>
+      </c>
       <c r="L4">
         <v>2</v>
       </c>
@@ -5330,6 +5400,9 @@
       <c r="G5" s="34">
         <v>5</v>
       </c>
+      <c r="H5">
+        <v>3</v>
+      </c>
       <c r="L5">
         <v>3</v>
       </c>
@@ -5381,6 +5454,9 @@
       <c r="G6" s="35">
         <v>3</v>
       </c>
+      <c r="H6">
+        <v>2</v>
+      </c>
       <c r="L6">
         <v>4</v>
       </c>
@@ -5432,6 +5508,9 @@
       <c r="G7" s="34">
         <v>1</v>
       </c>
+      <c r="H7">
+        <v>1</v>
+      </c>
       <c r="L7">
         <v>5</v>
       </c>
@@ -5504,7 +5583,7 @@
     </row>
     <row r="10" spans="2:22">
       <c r="B10" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="L10">
         <v>8</v>
@@ -5526,19 +5605,19 @@
     </row>
     <row r="11" spans="2:22">
       <c r="B11" s="19" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="C11" s="19" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="D11" s="19" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="E11" s="19" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="F11" s="19" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="L11">
         <v>9</v>
@@ -5560,19 +5639,19 @@
     </row>
     <row r="12" spans="2:22" ht="76.5">
       <c r="B12" s="20" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="C12" s="20" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="D12" s="20" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="E12" s="20" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="F12" s="20" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="L12">
         <v>10</v>
@@ -5871,11 +5950,335 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F5EC53A5-8F19-4711-93EA-0F4CBD261EC8}">
-  <dimension ref="B2:B30"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{478582BA-383F-47D3-8480-5088EC096D30}">
+  <dimension ref="B1:S25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="M13" sqref="M13"/>
+      <selection activeCell="P25" sqref="P24:Q25"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="2:19">
+      <c r="D1">
+        <v>38</v>
+      </c>
+      <c r="E1">
+        <v>44</v>
+      </c>
+      <c r="F1">
+        <v>119</v>
+      </c>
+      <c r="G1">
+        <v>35</v>
+      </c>
+      <c r="H1">
+        <v>54</v>
+      </c>
+      <c r="J1">
+        <v>2</v>
+      </c>
+      <c r="K1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="2:19">
+      <c r="J2" t="s">
+        <v>58</v>
+      </c>
+      <c r="K2" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="3" spans="2:19">
+      <c r="B3" s="50"/>
+      <c r="C3" s="50"/>
+      <c r="D3" s="50"/>
+      <c r="E3" s="50"/>
+      <c r="F3" s="50"/>
+      <c r="G3" s="50" t="s">
+        <v>68</v>
+      </c>
+      <c r="H3" s="50"/>
+      <c r="I3" s="50"/>
+      <c r="J3" s="50"/>
+      <c r="K3" s="50"/>
+      <c r="L3" s="50"/>
+      <c r="N3" s="21" t="s">
+        <v>2</v>
+      </c>
+      <c r="O3" s="24" t="s">
+        <v>3</v>
+      </c>
+      <c r="P3" s="24" t="s">
+        <v>50</v>
+      </c>
+      <c r="Q3" s="24" t="s">
+        <v>51</v>
+      </c>
+      <c r="R3" s="24" t="s">
+        <v>52</v>
+      </c>
+      <c r="S3" s="24" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="4" spans="2:19">
+      <c r="B4" s="53" t="s">
+        <v>69</v>
+      </c>
+      <c r="N4" s="25" t="s">
+        <v>13</v>
+      </c>
+      <c r="O4" s="25">
+        <v>2000</v>
+      </c>
+      <c r="P4" s="25">
+        <v>2000</v>
+      </c>
+      <c r="Q4" s="25">
+        <v>2000</v>
+      </c>
+      <c r="R4" s="25">
+        <v>100</v>
+      </c>
+      <c r="S4" s="34">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="2:19">
+      <c r="B5" s="51" t="s">
+        <v>70</v>
+      </c>
+      <c r="N5" s="26" t="s">
+        <v>14</v>
+      </c>
+      <c r="O5" s="26">
+        <v>1500</v>
+      </c>
+      <c r="P5" s="26">
+        <v>1500</v>
+      </c>
+      <c r="Q5" s="26">
+        <v>1500</v>
+      </c>
+      <c r="R5" s="26">
+        <v>100</v>
+      </c>
+      <c r="S5" s="35">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6" spans="2:19">
+      <c r="B6" s="53" t="s">
+        <v>71</v>
+      </c>
+      <c r="N6" s="27" t="s">
+        <v>15</v>
+      </c>
+      <c r="O6" s="27">
+        <v>1000</v>
+      </c>
+      <c r="P6" s="27">
+        <v>1000</v>
+      </c>
+      <c r="Q6" s="27">
+        <v>1000</v>
+      </c>
+      <c r="R6" s="27">
+        <v>100</v>
+      </c>
+      <c r="S6" s="34">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="2:19">
+      <c r="B7" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="N7" s="26" t="s">
+        <v>16</v>
+      </c>
+      <c r="O7" s="26">
+        <v>500</v>
+      </c>
+      <c r="P7" s="26">
+        <v>500</v>
+      </c>
+      <c r="Q7" s="26">
+        <v>500</v>
+      </c>
+      <c r="R7" s="26">
+        <v>100</v>
+      </c>
+      <c r="S7" s="35">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="2:19">
+      <c r="G8" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="N8" s="27" t="s">
+        <v>17</v>
+      </c>
+      <c r="O8" s="27">
+        <v>100</v>
+      </c>
+      <c r="P8" s="27">
+        <v>100</v>
+      </c>
+      <c r="Q8" s="27">
+        <v>100</v>
+      </c>
+      <c r="R8" s="27">
+        <v>100</v>
+      </c>
+      <c r="S8" s="34">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="2:19">
+      <c r="N10" s="19" t="s">
+        <v>57</v>
+      </c>
+      <c r="O10" s="19" t="s">
+        <v>58</v>
+      </c>
+      <c r="P10" s="19" t="s">
+        <v>59</v>
+      </c>
+      <c r="Q10" s="19" t="s">
+        <v>60</v>
+      </c>
+      <c r="R10" s="19" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="15" spans="2:19">
+      <c r="C15" s="52" t="s">
+        <v>17</v>
+      </c>
+      <c r="E15" s="52" t="s">
+        <v>17</v>
+      </c>
+      <c r="G15" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="I15" s="52" t="s">
+        <v>17</v>
+      </c>
+      <c r="K15" s="52" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="16" spans="2:19">
+      <c r="P16">
+        <f ca="1">RANDBETWEEN(0,123)</f>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="17" spans="2:16">
+      <c r="P17" s="54">
+        <f ca="1">RANDBETWEEN(0,6)</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="18" spans="2:16">
+      <c r="C18" s="52" t="s">
+        <v>17</v>
+      </c>
+      <c r="E18" s="52" t="s">
+        <v>17</v>
+      </c>
+      <c r="I18" s="52" t="s">
+        <v>17</v>
+      </c>
+      <c r="K18" s="52" t="s">
+        <v>17</v>
+      </c>
+      <c r="L18" s="6" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="19" spans="2:16">
+      <c r="L19" s="53" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="20" spans="2:16">
+      <c r="E20" s="52" t="s">
+        <v>17</v>
+      </c>
+      <c r="I20" s="52" t="s">
+        <v>17</v>
+      </c>
+      <c r="L20" s="51" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="21" spans="2:16">
+      <c r="L21" s="53" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="22" spans="2:16">
+      <c r="B22" s="2"/>
+      <c r="C22" s="2"/>
+      <c r="D22" s="2"/>
+      <c r="E22" s="2"/>
+      <c r="F22" s="2"/>
+      <c r="G22" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="H22" s="2"/>
+      <c r="I22" s="2"/>
+      <c r="J22" s="2"/>
+      <c r="K22" s="2"/>
+      <c r="L22" s="2"/>
+    </row>
+    <row r="24" spans="2:16">
+      <c r="E24">
+        <v>64</v>
+      </c>
+      <c r="F24">
+        <v>114</v>
+      </c>
+      <c r="G24">
+        <v>118</v>
+      </c>
+      <c r="H24">
+        <v>73</v>
+      </c>
+      <c r="I24">
+        <v>80</v>
+      </c>
+      <c r="K24">
+        <v>2</v>
+      </c>
+      <c r="L24">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="25" spans="2:16">
+      <c r="K25" t="s">
+        <v>58</v>
+      </c>
+      <c r="L25" t="s">
+        <v>67</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F5EC53A5-8F19-4711-93EA-0F4CBD261EC8}">
+  <dimension ref="B2:B31"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -5885,147 +6288,152 @@
   <sheetData>
     <row r="2" spans="2:2">
       <c r="B2" s="21" t="s">
-        <v>66</v>
+        <v>74</v>
       </c>
     </row>
     <row r="3" spans="2:2">
       <c r="B3" t="s">
-        <v>67</v>
+        <v>75</v>
       </c>
     </row>
     <row r="4" spans="2:2">
       <c r="B4" t="s">
-        <v>68</v>
+        <v>76</v>
       </c>
     </row>
     <row r="5" spans="2:2">
       <c r="B5" t="s">
-        <v>69</v>
+        <v>77</v>
       </c>
     </row>
     <row r="6" spans="2:2">
       <c r="B6" t="s">
-        <v>70</v>
+        <v>78</v>
       </c>
     </row>
     <row r="7" spans="2:2">
       <c r="B7" t="s">
-        <v>71</v>
+        <v>79</v>
       </c>
     </row>
     <row r="8" spans="2:2">
       <c r="B8" t="s">
-        <v>72</v>
+        <v>80</v>
       </c>
     </row>
     <row r="9" spans="2:2">
-      <c r="B9" t="s">
-        <v>73</v>
+      <c r="B9" s="49" t="s">
+        <v>81</v>
       </c>
     </row>
     <row r="10" spans="2:2">
       <c r="B10" t="s">
-        <v>74</v>
+        <v>82</v>
       </c>
     </row>
     <row r="11" spans="2:2">
       <c r="B11" t="s">
-        <v>75</v>
+        <v>83</v>
       </c>
     </row>
     <row r="12" spans="2:2">
       <c r="B12" t="s">
-        <v>76</v>
+        <v>84</v>
       </c>
     </row>
     <row r="13" spans="2:2">
       <c r="B13" t="s">
-        <v>77</v>
+        <v>85</v>
       </c>
     </row>
     <row r="14" spans="2:2">
       <c r="B14" t="s">
-        <v>78</v>
+        <v>86</v>
       </c>
     </row>
     <row r="15" spans="2:2">
       <c r="B15" t="s">
-        <v>79</v>
+        <v>87</v>
       </c>
     </row>
     <row r="16" spans="2:2">
       <c r="B16" t="s">
-        <v>80</v>
+        <v>88</v>
       </c>
     </row>
     <row r="17" spans="2:2">
       <c r="B17" t="s">
-        <v>81</v>
+        <v>89</v>
       </c>
     </row>
     <row r="18" spans="2:2">
       <c r="B18" t="s">
-        <v>82</v>
+        <v>90</v>
       </c>
     </row>
     <row r="19" spans="2:2">
       <c r="B19" t="s">
-        <v>83</v>
+        <v>91</v>
       </c>
     </row>
     <row r="20" spans="2:2">
       <c r="B20" t="s">
-        <v>84</v>
+        <v>92</v>
       </c>
     </row>
     <row r="21" spans="2:2">
       <c r="B21" t="s">
-        <v>85</v>
+        <v>93</v>
       </c>
     </row>
     <row r="22" spans="2:2">
       <c r="B22" t="s">
-        <v>86</v>
+        <v>94</v>
       </c>
     </row>
     <row r="23" spans="2:2">
       <c r="B23" t="s">
-        <v>87</v>
+        <v>95</v>
       </c>
     </row>
     <row r="24" spans="2:2">
       <c r="B24" t="s">
-        <v>88</v>
+        <v>96</v>
       </c>
     </row>
     <row r="25" spans="2:2">
       <c r="B25" t="s">
-        <v>89</v>
+        <v>97</v>
       </c>
     </row>
     <row r="26" spans="2:2">
       <c r="B26" t="s">
-        <v>90</v>
+        <v>98</v>
       </c>
     </row>
     <row r="27" spans="2:2">
       <c r="B27" t="s">
-        <v>91</v>
+        <v>99</v>
       </c>
     </row>
     <row r="28" spans="2:2">
       <c r="B28" t="s">
-        <v>92</v>
+        <v>100</v>
       </c>
     </row>
     <row r="29" spans="2:2">
       <c r="B29" t="s">
-        <v>93</v>
+        <v>101</v>
       </c>
     </row>
     <row r="30" spans="2:2">
       <c r="B30" t="s">
-        <v>94</v>
+        <v>102</v>
+      </c>
+    </row>
+    <row r="31" spans="2:2">
+      <c r="B31" t="s">
+        <v>103</v>
       </c>
     </row>
   </sheetData>
@@ -6033,64 +6441,64 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6016CF9E-E144-48D8-959F-618B8D85D284}">
   <dimension ref="B2:B11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I20" sqref="I20"/>
+      <selection activeCell="J14" sqref="J14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="2" spans="2:2">
       <c r="B2" t="s">
-        <v>95</v>
+        <v>104</v>
       </c>
     </row>
     <row r="3" spans="2:2">
       <c r="B3" t="s">
-        <v>96</v>
+        <v>105</v>
       </c>
     </row>
     <row r="4" spans="2:2">
       <c r="B4" t="s">
-        <v>97</v>
+        <v>106</v>
       </c>
     </row>
     <row r="5" spans="2:2">
       <c r="B5" t="s">
-        <v>98</v>
+        <v>107</v>
       </c>
     </row>
     <row r="6" spans="2:2">
       <c r="B6" t="s">
-        <v>99</v>
+        <v>108</v>
       </c>
     </row>
     <row r="7" spans="2:2">
       <c r="B7" t="s">
-        <v>100</v>
+        <v>109</v>
       </c>
     </row>
     <row r="8" spans="2:2">
       <c r="B8" t="s">
-        <v>101</v>
+        <v>110</v>
       </c>
     </row>
     <row r="9" spans="2:2">
       <c r="B9" t="s">
-        <v>102</v>
+        <v>111</v>
       </c>
     </row>
     <row r="10" spans="2:2">
       <c r="B10" t="s">
-        <v>103</v>
+        <v>112</v>
       </c>
     </row>
     <row r="11" spans="2:2">
       <c r="B11" t="s">
-        <v>104</v>
+        <v>113</v>
       </c>
     </row>
   </sheetData>
@@ -6098,12 +6506,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1CADF2F4-A124-44BC-8A72-4CE3F16F5D04}">
   <dimension ref="B2:D22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D22" sqref="B21:D22"/>
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -6115,185 +6523,185 @@
   <sheetData>
     <row r="2" spans="2:4">
       <c r="B2" s="32" t="s">
-        <v>105</v>
+        <v>114</v>
       </c>
       <c r="C2" s="32" t="s">
-        <v>106</v>
+        <v>115</v>
       </c>
       <c r="D2" s="32" t="s">
-        <v>107</v>
+        <v>116</v>
       </c>
     </row>
     <row r="3" spans="2:4" ht="106.5" customHeight="1">
       <c r="B3" s="45" t="s">
-        <v>108</v>
+        <v>117</v>
       </c>
       <c r="C3" s="43" t="s">
-        <v>109</v>
+        <v>118</v>
       </c>
       <c r="D3" s="28" t="s">
-        <v>110</v>
+        <v>119</v>
       </c>
     </row>
     <row r="4" spans="2:4" ht="106.5">
       <c r="B4" s="48"/>
       <c r="C4" s="47"/>
       <c r="D4" s="29" t="s">
-        <v>111</v>
+        <v>120</v>
       </c>
     </row>
     <row r="5" spans="2:4" ht="60.75">
       <c r="B5" s="48"/>
       <c r="C5" s="47"/>
       <c r="D5" s="30" t="s">
-        <v>112</v>
+        <v>121</v>
       </c>
     </row>
     <row r="6" spans="2:4" ht="76.5">
       <c r="B6" s="48"/>
       <c r="C6" s="47"/>
       <c r="D6" s="30" t="s">
-        <v>113</v>
+        <v>122</v>
       </c>
     </row>
     <row r="7" spans="2:4" ht="91.5">
       <c r="B7" s="45" t="s">
-        <v>114</v>
+        <v>123</v>
       </c>
       <c r="C7" s="43" t="s">
-        <v>115</v>
+        <v>124</v>
       </c>
       <c r="D7" s="28" t="s">
-        <v>116</v>
+        <v>125</v>
       </c>
     </row>
     <row r="8" spans="2:4" ht="91.5">
       <c r="B8" s="48"/>
       <c r="C8" s="47"/>
       <c r="D8" s="30" t="s">
-        <v>117</v>
+        <v>126</v>
       </c>
     </row>
     <row r="9" spans="2:4" ht="76.5">
       <c r="B9" s="45" t="s">
-        <v>118</v>
+        <v>127</v>
       </c>
       <c r="C9" s="43" t="s">
-        <v>119</v>
+        <v>128</v>
       </c>
       <c r="D9" s="28" t="s">
-        <v>120</v>
+        <v>129</v>
       </c>
     </row>
     <row r="10" spans="2:4" ht="30.75">
       <c r="B10" s="46"/>
       <c r="C10" s="44"/>
       <c r="D10" s="31" t="s">
-        <v>121</v>
+        <v>130</v>
       </c>
     </row>
     <row r="11" spans="2:4" ht="76.5" customHeight="1">
       <c r="B11" s="45" t="s">
-        <v>122</v>
+        <v>131</v>
       </c>
       <c r="C11" s="43" t="s">
-        <v>123</v>
+        <v>132</v>
       </c>
       <c r="D11" s="28" t="s">
-        <v>124</v>
+        <v>133</v>
       </c>
     </row>
     <row r="12" spans="2:4" ht="30.75">
       <c r="B12" s="48"/>
       <c r="C12" s="47"/>
       <c r="D12" s="30" t="s">
-        <v>125</v>
+        <v>134</v>
       </c>
     </row>
     <row r="13" spans="2:4" ht="45.75">
       <c r="B13" s="45" t="s">
-        <v>126</v>
+        <v>135</v>
       </c>
       <c r="C13" s="43" t="s">
-        <v>127</v>
+        <v>136</v>
       </c>
       <c r="D13" s="28" t="s">
-        <v>128</v>
+        <v>137</v>
       </c>
     </row>
     <row r="14" spans="2:4" ht="30.75">
       <c r="B14" s="48"/>
       <c r="C14" s="47"/>
       <c r="D14" s="30" t="s">
-        <v>129</v>
+        <v>138</v>
       </c>
     </row>
     <row r="15" spans="2:4" ht="45.75">
       <c r="B15" s="48"/>
       <c r="C15" s="47"/>
       <c r="D15" s="30" t="s">
-        <v>130</v>
+        <v>139</v>
       </c>
     </row>
     <row r="16" spans="2:4" ht="60.75">
       <c r="B16" s="48"/>
       <c r="C16" s="47"/>
       <c r="D16" s="30" t="s">
-        <v>131</v>
+        <v>140</v>
       </c>
     </row>
     <row r="17" spans="2:4" ht="45.75">
       <c r="B17" s="45" t="s">
-        <v>132</v>
+        <v>141</v>
       </c>
       <c r="C17" s="43" t="s">
-        <v>133</v>
+        <v>142</v>
       </c>
       <c r="D17" s="28" t="s">
-        <v>134</v>
+        <v>143</v>
       </c>
     </row>
     <row r="18" spans="2:4" ht="45.75">
       <c r="B18" s="48"/>
       <c r="C18" s="47"/>
       <c r="D18" s="30" t="s">
-        <v>135</v>
+        <v>144</v>
       </c>
     </row>
     <row r="19" spans="2:4" ht="60.75" customHeight="1">
       <c r="B19" s="45" t="s">
-        <v>136</v>
+        <v>145</v>
       </c>
       <c r="C19" s="43" t="s">
-        <v>137</v>
+        <v>146</v>
       </c>
       <c r="D19" s="28" t="s">
-        <v>138</v>
+        <v>147</v>
       </c>
     </row>
     <row r="20" spans="2:4" ht="30.75">
       <c r="B20" s="48"/>
       <c r="C20" s="47"/>
       <c r="D20" s="30" t="s">
-        <v>139</v>
+        <v>148</v>
       </c>
     </row>
     <row r="21" spans="2:4" ht="45.75">
       <c r="B21" s="45" t="s">
-        <v>140</v>
+        <v>149</v>
       </c>
       <c r="C21" s="43" t="s">
-        <v>141</v>
+        <v>150</v>
       </c>
       <c r="D21" s="28" t="s">
-        <v>142</v>
+        <v>151</v>
       </c>
     </row>
     <row r="22" spans="2:4" ht="30.75">
       <c r="B22" s="46"/>
       <c r="C22" s="44"/>
       <c r="D22" s="31" t="s">
-        <v>143</v>
+        <v>152</v>
       </c>
     </row>
   </sheetData>
@@ -6319,7 +6727,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A2:S19"/>
   <sheetViews>
@@ -6339,25 +6747,25 @@
   <sheetData>
     <row r="2" spans="1:19">
       <c r="A2" s="42" t="s">
-        <v>144</v>
+        <v>153</v>
       </c>
       <c r="B2" s="42"/>
       <c r="C2" s="42"/>
       <c r="F2" s="42" t="s">
-        <v>145</v>
+        <v>154</v>
       </c>
       <c r="G2" s="42"/>
       <c r="H2" s="42"/>
     </row>
     <row r="3" spans="1:19">
       <c r="A3" t="s">
-        <v>146</v>
+        <v>155</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>21</v>
       </c>
       <c r="F3" t="s">
-        <v>146</v>
+        <v>155</v>
       </c>
       <c r="G3" s="1" t="s">
         <v>26</v>
@@ -6381,14 +6789,14 @@
     </row>
     <row r="5" spans="1:19">
       <c r="A5" t="s">
-        <v>147</v>
+        <v>156</v>
       </c>
       <c r="B5">
         <f>SUM(C10:C14)</f>
         <v>5000</v>
       </c>
       <c r="F5" t="s">
-        <v>147</v>
+        <v>156</v>
       </c>
       <c r="G5">
         <f>SUM(H10:H14)</f>
@@ -6397,14 +6805,14 @@
     </row>
     <row r="6" spans="1:19">
       <c r="A6" t="s">
-        <v>148</v>
+        <v>157</v>
       </c>
       <c r="B6">
         <f>SUM(C17:C19)</f>
         <v>2000</v>
       </c>
       <c r="F6" t="s">
-        <v>148</v>
+        <v>157</v>
       </c>
       <c r="G6">
         <f>SUM(H17:H19)</f>
@@ -6426,7 +6834,7 @@
         <v>2</v>
       </c>
       <c r="B9" s="17" t="s">
-        <v>149</v>
+        <v>158</v>
       </c>
       <c r="C9" s="17" t="s">
         <v>3</v>
@@ -6435,7 +6843,7 @@
         <v>2</v>
       </c>
       <c r="G9" s="17" t="s">
-        <v>149</v>
+        <v>158</v>
       </c>
       <c r="H9" s="17" t="s">
         <v>3</v>
@@ -6622,19 +7030,19 @@
     </row>
     <row r="16" spans="1:19">
       <c r="A16" s="17" t="s">
-        <v>108</v>
+        <v>117</v>
       </c>
       <c r="B16" s="17" t="s">
-        <v>149</v>
+        <v>158</v>
       </c>
       <c r="C16" t="s">
         <v>3</v>
       </c>
       <c r="F16" s="17" t="s">
-        <v>108</v>
+        <v>117</v>
       </c>
       <c r="G16" s="17" t="s">
-        <v>149</v>
+        <v>158</v>
       </c>
       <c r="H16" t="s">
         <v>3</v>

</xml_diff>

<commit_message>
Updated rules, need to add rules for strategy cards
</commit_message>
<xml_diff>
--- a/ShipCardGameCalcs.xlsx
+++ b/ShipCardGameCalcs.xlsx
@@ -1,11 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26324"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26130"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{CC049761-E7FC-4643-98CB-6C747A6B0A47}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MultiplayerGame\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67DAF753-3355-4F68-B221-8E532364658F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-15" yWindow="-15" windowWidth="14415" windowHeight="12495" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="1" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Values" sheetId="1" r:id="rId1"/>
@@ -34,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="367" uniqueCount="159">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="398" uniqueCount="190">
   <si>
     <t>Ship Parameters</t>
   </si>
@@ -317,57 +322,24 @@
     <t>A player gets 1 free mulligan but if they choose to mulligan anymore times than that they reduce the amount of cards drawn from strategy deck by 1 each time. Down to a minimum of 1 card from their strategy deck and 2 from their leader deck</t>
   </si>
   <si>
-    <t>A crew member first placed on to a ship can't be used in a gun slot</t>
-  </si>
-  <si>
-    <t>Any crew card placed can be used to tap on first turn placed</t>
-  </si>
-  <si>
     <t>Max player hand size is 8 (unless card in play says otherwise)</t>
   </si>
   <si>
-    <t>A crew /leader deck can only contain cards of Type Captain, Leuitenant and Crew Rank 1</t>
-  </si>
-  <si>
     <t>The strategy deck has every other card</t>
   </si>
   <si>
-    <t>A player can only play 1 crew member and 1 Captain/Leuitenant per turn</t>
-  </si>
-  <si>
-    <t>On start of turn player can choose to either draw 2 cards from strategy deck, 2 cards from crew/leader deck or 1 from each.</t>
-  </si>
-  <si>
-    <t>On end of turn if player has more than Max player hand size they must discard cards down to max hand size</t>
-  </si>
-  <si>
-    <t>A ship can only hold x amount of crew members where x is equal to the ships service slots</t>
-  </si>
-  <si>
     <t>A ship can only hold x amount of Captains where x is equal to ships Captains slots</t>
   </si>
   <si>
     <t>A ship can only hold x amount of Leuitenant where x is equal to ships Leuitenant slots</t>
   </si>
   <si>
-    <t>Ship Upgrade cards can only be used on ships where at least one crew member used is on targeted ship</t>
-  </si>
-  <si>
-    <t>Cards with Target Owned Ship can only be used on ships where at least one crew member used is on targeted ship</t>
-  </si>
-  <si>
-    <t>At the start of players turn all their cards are untapped (unless card in play says otherwise)</t>
-  </si>
-  <si>
     <t>A crew type card has a 1 to 1 relationship when being tapped to a gun slot. Meaning you can't tap more than 1 crew card type to the same gun slot on the same turn.</t>
   </si>
   <si>
     <t>When crew type card is being used to a gun slot, it will deal damage to the players ship shield, if the players ship shield is at 0 or deactivated then it will deal damage to the players ship hull</t>
   </si>
   <si>
-    <t>Once a players ship hull reaches 0 it is destroyed and all cards part of that ship are sent to cards deck junkyard e.g crew types and ship upgrades etc</t>
-  </si>
-  <si>
     <t>Once a players ship is destroyed remove the ship card from play</t>
   </si>
   <si>
@@ -377,18 +349,12 @@
     <t>When only 1 player remains in the game they win</t>
   </si>
   <si>
-    <t>If player wants to draw from crew/leader deck and there are no cards left in players crew/leader deck then shuffle are crew/leader deck cards from stasis back to that deck spot</t>
-  </si>
-  <si>
     <t>If there are no cards left in the strategy deck during the draw phase that player loses and is out of the game</t>
   </si>
   <si>
     <t>A player can only have 1 admiral card in play on their side of the battlefield</t>
   </si>
   <si>
-    <t>Both the strategy deck and crew/leader deck have its own assigned stasis where certain cards go once played</t>
-  </si>
-  <si>
     <t>Controlled deck is the battlefield conditions which affects the battlefield</t>
   </si>
   <si>
@@ -552,13 +518,145 @@
   </si>
   <si>
     <t>No. of</t>
+  </si>
+  <si>
+    <t>Pre Game Rules:</t>
+  </si>
+  <si>
+    <t>Pick a random Player to go first, since they started they don't draw a card from either the crew or strategy decks at the start of turn.</t>
+  </si>
+  <si>
+    <t>A crew member first placed on to a ship can't be used in a gun slot, however they can be used to tap for anything else</t>
+  </si>
+  <si>
+    <t>A crew /leader deck can only contain cards of Type Captain, Leuitenant and Crew</t>
+  </si>
+  <si>
+    <t>First Turn Rules:</t>
+  </si>
+  <si>
+    <t>After the first player, Players can draw either 1 card from the strategy deck, or they can choose the see the top 3 cards of the crew deck and then get to pick 1. The rest get sent to the bottom of the crew deck.</t>
+  </si>
+  <si>
+    <t>In Game Rules</t>
+  </si>
+  <si>
+    <t>A player can only place Crew cards to their ship with an available crew slot unless stated otherwise</t>
+  </si>
+  <si>
+    <t>A player can only play 1 crew member and 1 Captain/Leuitenant per their turn</t>
+  </si>
+  <si>
+    <t>Each players turn consist of the following phases</t>
+  </si>
+  <si>
+    <t>Untap Phase</t>
+  </si>
+  <si>
+    <t>This is where the player untaps all their cards unless stated otherwise</t>
+  </si>
+  <si>
+    <t>Draw Phase</t>
+  </si>
+  <si>
+    <t>This is where the player chooses to draw from their Strategy or Crew Deck</t>
+  </si>
+  <si>
+    <t>Strategy Phase</t>
+  </si>
+  <si>
+    <t>This is where the player can play their cards, tap to gain department resourse or tap cards to use gun slots</t>
+  </si>
+  <si>
+    <t>End Phase</t>
+  </si>
+  <si>
+    <t>At this phase if the player has cards greater than their max hand size then they must discard back down to that size</t>
+  </si>
+  <si>
+    <t>In Game Rules Continued</t>
+  </si>
+  <si>
+    <t>Any department resource not used does NOT get transferred to later turns</t>
+  </si>
+  <si>
+    <t>During the phases players can activate certain types of cards on other players turns</t>
+  </si>
+  <si>
+    <t>Players can draw either 1 card from the strategy deck, or they can choose the see the top 3 cards of the crew deck and then get to pick 1. The rest get sent to the bottom of the crew deck.</t>
+  </si>
+  <si>
+    <t>A ship can only hold x amount of crew members where x is equal to the ships crew slots</t>
+  </si>
+  <si>
+    <t>Some cards might allow a crew card to tap more than one gun slot</t>
+  </si>
+  <si>
+    <t>Gun Slots/Attacking Player Ships</t>
+  </si>
+  <si>
+    <t>Ship Destroyed</t>
+  </si>
+  <si>
+    <t>Once a players ship hull reaches 0 it is destroyed</t>
+  </si>
+  <si>
+    <t>Crew Cards</t>
+  </si>
+  <si>
+    <t>A Crew Card can have various tap abilities, the standard abilities they get are as follows unless stated otherwise:</t>
+  </si>
+  <si>
+    <t>Crew can tap to provide department resource</t>
+  </si>
+  <si>
+    <t>Crew can tap to move from one ship to another ship the player owns</t>
+  </si>
+  <si>
+    <t>Crew can tap to use a gun slot on assigned ship</t>
+  </si>
+  <si>
+    <t>All ship upgrades attached to destroyed ship are sent to the junkyard</t>
+  </si>
+  <si>
+    <t>Each ship will have had assigned amount of escape pods. The player owning the destroyed ship may pick to move that amount of crew with their attachments from the destroyed ship to another ship they own</t>
+  </si>
+  <si>
+    <t>The rest of the crew and crew attachment cards are sent to stasis and the junkyard</t>
+  </si>
+  <si>
+    <t>If player wants to draw from crew/leader deck and there are no cards left in players crew/leader deck then shuffle the crew/leader cards from stasis back to that deck spot and draw</t>
+  </si>
+  <si>
+    <t>If there are less than 3 cards in the crew/eader deck then they draw the rest of the deck, shuffle the stasis pile back to the deck position and draw up to the 3 cards. Then continue process of picking 1 card and putting rest to the stasis pile</t>
+  </si>
+  <si>
+    <t>When a strategy card has been played and doesn’t stay on the field, then that card gets sent to the junkyard</t>
+  </si>
+  <si>
+    <t>Cards in the Junkyard can't be played unless stated otherwise</t>
+  </si>
+  <si>
+    <t>When a crew card is destroyed send it to the stasis pile</t>
+  </si>
+  <si>
+    <t>Crew cards in the stasis pile can't be played unless stated otherwise</t>
+  </si>
+  <si>
+    <t>A rank 1 crew card can be played for free</t>
+  </si>
+  <si>
+    <t>Captain and Leuitenant cards cost department resource to play</t>
+  </si>
+  <si>
+    <t>Crew cards higher than Rank 1 will require at least a sacrifice of a crew card currently in play that you own with a Rank lower than the crew card trying to play</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
-  <fonts count="8">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1023,6 +1121,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1045,11 +1148,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1058,14 +1156,6 @@
     <dxf>
       <fill>
         <patternFill patternType="none">
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
           <fgColor indexed="64"/>
           <bgColor indexed="65"/>
         </patternFill>
@@ -1160,15 +1250,23 @@
     <dxf>
       <fill>
         <patternFill patternType="none">
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
           <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1280,13 +1378,6 @@
     </dxf>
     <dxf>
       <border outline="0">
-        <bottom style="thin">
-          <color theme="4" tint="0.39997558519241921"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
         <left style="thin">
           <color theme="4" tint="0.39997558519241921"/>
         </left>
@@ -1305,6 +1396,13 @@
           <bgColor indexed="65"/>
         </patternFill>
       </fill>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </bottom>
+      </border>
     </dxf>
     <dxf>
       <font>
@@ -1620,13 +1718,6 @@
     </dxf>
     <dxf>
       <border outline="0">
-        <bottom style="thin">
-          <color theme="4" tint="0.39997558519241921"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
         <left style="thin">
           <color theme="4" tint="0.39997558519241921"/>
         </left>
@@ -1663,6 +1754,13 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
       <font>
         <b/>
         <i val="0"/>
@@ -1713,9 +1811,6 @@
       </border>
     </dxf>
     <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0" outline="0">
         <left/>
@@ -1737,7 +1832,6 @@
       </border>
     </dxf>
     <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -1748,6 +1842,10 @@
         <top/>
         <bottom/>
       </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <border diagonalUp="0" diagonalDown="0" outline="0">
@@ -1792,6 +1890,9 @@
       </border>
     </dxf>
     <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
@@ -1835,9 +1936,6 @@
     </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -1910,6 +2008,9 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -1924,9 +2025,6 @@
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -1963,6 +2061,15 @@
       </border>
     </dxf>
     <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
       <fill>
         <patternFill patternType="none">
@@ -2093,7 +2200,6 @@
           <bgColor indexed="65"/>
         </patternFill>
       </fill>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -2121,14 +2227,6 @@
     <dxf>
       <fill>
         <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
           <bgColor auto="1"/>
         </patternFill>
       </fill>
@@ -2233,14 +2331,6 @@
     <dxf>
       <fill>
         <patternFill patternType="none">
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
           <fgColor indexed="64"/>
           <bgColor indexed="65"/>
         </patternFill>
@@ -2333,6 +2423,23 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
       <fill>
         <patternFill patternType="none">
@@ -2348,20 +2455,11 @@
           <bgColor indexed="65"/>
         </patternFill>
       </fill>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <fill>
         <patternFill patternType="none">
           <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
         </patternFill>
       </fill>
     </dxf>
@@ -2405,6 +2503,9 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <fill>
         <patternFill patternType="none">
           <fgColor indexed="64"/>
@@ -2472,9 +2573,6 @@
         </patternFill>
       </fill>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <fill>
@@ -2610,12 +2708,12 @@
   <autoFilter ref="A9:G14" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="7">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Option" totalsRowLabel="Total" dataDxfId="129"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="A" totalsRowFunction="sum" dataDxfId="127" totalsRowDxfId="128"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="B" totalsRowFunction="sum" dataDxfId="125" totalsRowDxfId="126"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="C" totalsRowFunction="sum" dataDxfId="123" totalsRowDxfId="124"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="D" totalsRowFunction="sum" dataDxfId="121" totalsRowDxfId="122"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="E" totalsRowFunction="sum" dataDxfId="119" totalsRowDxfId="120"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="F" totalsRowFunction="sum" dataDxfId="117" totalsRowDxfId="118"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="A" totalsRowFunction="sum" dataDxfId="128" totalsRowDxfId="127"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="B" totalsRowFunction="sum" dataDxfId="126" totalsRowDxfId="125"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="C" totalsRowFunction="sum" dataDxfId="124" totalsRowDxfId="123"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="D" totalsRowFunction="sum" dataDxfId="122" totalsRowDxfId="121"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="E" totalsRowFunction="sum" dataDxfId="120" totalsRowDxfId="119"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="F" totalsRowFunction="sum" dataDxfId="118" totalsRowDxfId="117"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium15" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2625,23 +2723,23 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="14" xr:uid="{00000000-000C-0000-FFFF-FFFF09000000}" name="TblFltCrewSizes" displayName="TblFltCrewSizes" ref="A17:G21" totalsRowCount="1" headerRowDxfId="15" dataDxfId="14">
   <autoFilter ref="A17:G20" xr:uid="{00000000-0009-0000-0100-00000E000000}"/>
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0900-000001000000}" name="Option" totalsRowLabel="Total" dataDxfId="12" totalsRowDxfId="13"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0900-000002000000}" name="A" totalsRowFunction="custom" dataDxfId="10" totalsRowDxfId="11">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0900-000001000000}" name="Option" totalsRowLabel="Total" dataDxfId="13" totalsRowDxfId="12"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0900-000002000000}" name="A" totalsRowFunction="custom" dataDxfId="11" totalsRowDxfId="10">
       <totalsRowFormula>SUBTOTAL(109,TblFltCrewSizes[A])</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0900-000003000000}" name="B" totalsRowFunction="custom" dataDxfId="8" totalsRowDxfId="9">
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0900-000003000000}" name="B" totalsRowFunction="custom" dataDxfId="9" totalsRowDxfId="8">
       <totalsRowFormula>SUBTOTAL(109,TblFltCrewSizes[B])</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0900-000004000000}" name="C" totalsRowFunction="custom" dataDxfId="6" totalsRowDxfId="7">
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0900-000004000000}" name="C" totalsRowFunction="custom" dataDxfId="7" totalsRowDxfId="6">
       <totalsRowFormula>SUBTOTAL(109,TblFltCrewSizes[C])</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0900-000005000000}" name="D" totalsRowFunction="custom" dataDxfId="4" totalsRowDxfId="5">
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0900-000005000000}" name="D" totalsRowFunction="custom" dataDxfId="5" totalsRowDxfId="4">
       <totalsRowFormula>SUBTOTAL(109,TblFltCrewSizes[D])</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0900-000006000000}" name="E" totalsRowFunction="custom" dataDxfId="2" totalsRowDxfId="3">
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0900-000006000000}" name="E" totalsRowFunction="custom" dataDxfId="3" totalsRowDxfId="2">
       <totalsRowFormula>SUBTOTAL(109,TblFltCrewSizes[E])</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0900-000007000000}" name="F" totalsRowFunction="sum" dataDxfId="0" totalsRowDxfId="1"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0900-000007000000}" name="F" totalsRowFunction="sum" dataDxfId="1" totalsRowDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium13" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2651,26 +2749,26 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="TblFleetShipValues" displayName="TblFleetShipValues" ref="J9:Q15" totalsRowCount="1" headerRowDxfId="116" dataDxfId="115" totalsRowDxfId="114">
   <autoFilter ref="J9:Q14" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
   <tableColumns count="8">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="Option" totalsRowLabel="Total " dataDxfId="112" totalsRowDxfId="113"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="A" totalsRowFunction="sum" dataDxfId="110" totalsRowDxfId="111">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="Option" totalsRowLabel="Total " dataDxfId="113" totalsRowDxfId="112"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="A" totalsRowFunction="sum" dataDxfId="111" totalsRowDxfId="110">
       <calculatedColumnFormula>(INDEX(TblBattlefieldFlt[[A]:[F]],MATCH(TblFleetShipValues[[#This Row],[Option]],TblBattlefieldFlt[Option],0),MATCH(TblFleetShipValues[[#Headers],[A]],TblBattlefieldFlt[[#Headers],[A]:[F]],0)))*(INDEX(TblShipPoints[Points],MATCH(TblFleetShipValues[[#This Row],[Option]],TblShipPoints[Ships],0)))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0100-000003000000}" name="B" totalsRowFunction="sum" dataDxfId="108" totalsRowDxfId="109">
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0100-000003000000}" name="B" totalsRowFunction="sum" dataDxfId="109" totalsRowDxfId="108">
       <calculatedColumnFormula>C10*#REF!</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0100-000004000000}" name="C" totalsRowFunction="sum" dataDxfId="106" totalsRowDxfId="107">
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0100-000004000000}" name="C" totalsRowFunction="sum" dataDxfId="107" totalsRowDxfId="106">
       <calculatedColumnFormula>D10*#REF!</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0100-000005000000}" name="D" totalsRowFunction="sum" dataDxfId="104" totalsRowDxfId="105">
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0100-000005000000}" name="D" totalsRowFunction="sum" dataDxfId="105" totalsRowDxfId="104">
       <calculatedColumnFormula>E10*#REF!</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0100-000006000000}" name="E" totalsRowFunction="sum" dataDxfId="102" totalsRowDxfId="103">
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0100-000006000000}" name="E" totalsRowFunction="sum" dataDxfId="103" totalsRowDxfId="102">
       <calculatedColumnFormula>F10*#REF!</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0100-000007000000}" name="F" totalsRowFunction="sum" dataDxfId="100" totalsRowDxfId="101">
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0100-000007000000}" name="F" totalsRowFunction="sum" dataDxfId="101" totalsRowDxfId="100">
       <calculatedColumnFormula>G10*#REF!</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0100-000008000000}" name="Name" dataDxfId="98" totalsRowDxfId="99"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0100-000008000000}" name="Name" dataDxfId="99" totalsRowDxfId="98"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium13" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2693,26 +2791,26 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{00000000-000C-0000-FFFF-FFFF03000000}" name="TblAdjFleetRolesValues" displayName="TblAdjFleetRolesValues" ref="A24:H30" totalsRowCount="1" headerRowDxfId="91" dataDxfId="90" totalsRowDxfId="89">
   <autoFilter ref="A24:H29" xr:uid="{00000000-0009-0000-0100-000006000000}"/>
   <tableColumns count="8">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0300-000001000000}" name="Option" totalsRowLabel="Total" dataDxfId="87" totalsRowDxfId="88"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0300-000002000000}" name="A" totalsRowFunction="sum" dataDxfId="85" totalsRowDxfId="86">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0300-000001000000}" name="Option" totalsRowLabel="Total" dataDxfId="88" totalsRowDxfId="87"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0300-000002000000}" name="A" totalsRowFunction="sum" dataDxfId="86" totalsRowDxfId="85">
       <calculatedColumnFormula>(INDEX(TblBattlefieldFlt[[A]:[F]],MATCH($A25,TblBattlefieldFlt[Option],0),MATCH(B$24,TblBattlefieldFlt[[#Headers],[A]:[F]],0)))*(INDEX(TblShipCrew[Adjusted],MATCH($A25,TblShipCrew[Ships],0)))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0300-000003000000}" name="B" totalsRowFunction="sum" dataDxfId="83" totalsRowDxfId="84">
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0300-000003000000}" name="B" totalsRowFunction="sum" dataDxfId="84" totalsRowDxfId="83">
       <calculatedColumnFormula>(INDEX(TblBattlefieldFlt[[A]:[F]],MATCH($A25,TblBattlefieldFlt[Option],0),MATCH(C$24,TblBattlefieldFlt[[#Headers],[A]:[F]],0)))*(INDEX(TblShipCrew[Adjusted],MATCH($A25,TblShipCrew[Ships],0)))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0300-000004000000}" name="C" totalsRowFunction="sum" dataDxfId="81" totalsRowDxfId="82">
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0300-000004000000}" name="C" totalsRowFunction="sum" dataDxfId="82" totalsRowDxfId="81">
       <calculatedColumnFormula>(INDEX(TblBattlefieldFlt[[A]:[F]],MATCH($A25,TblBattlefieldFlt[Option],0),MATCH(D$24,TblBattlefieldFlt[[#Headers],[A]:[F]],0)))*(INDEX(TblShipCrew[Adjusted],MATCH($A25,TblShipCrew[Ships],0)))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0300-000005000000}" name="D" totalsRowFunction="sum" dataDxfId="79" totalsRowDxfId="80">
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0300-000005000000}" name="D" totalsRowFunction="sum" dataDxfId="80" totalsRowDxfId="79">
       <calculatedColumnFormula>(INDEX(TblBattlefieldFlt[[A]:[F]],MATCH($A25,TblBattlefieldFlt[Option],0),MATCH(E$24,TblBattlefieldFlt[[#Headers],[A]:[F]],0)))*(INDEX(TblShipCrew[Adjusted],MATCH($A25,TblShipCrew[Ships],0)))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0300-000006000000}" name="E" totalsRowFunction="sum" dataDxfId="77" totalsRowDxfId="78">
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0300-000006000000}" name="E" totalsRowFunction="sum" dataDxfId="78" totalsRowDxfId="77">
       <calculatedColumnFormula>(INDEX(TblBattlefieldFlt[[A]:[F]],MATCH($A25,TblBattlefieldFlt[Option],0),MATCH(F$24,TblBattlefieldFlt[[#Headers],[A]:[F]],0)))*(INDEX(TblShipCrew[Adjusted],MATCH($A25,TblShipCrew[Ships],0)))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0300-000007000000}" name="F" totalsRowFunction="sum" dataDxfId="75" totalsRowDxfId="76">
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0300-000007000000}" name="F" totalsRowFunction="sum" dataDxfId="76" totalsRowDxfId="75">
       <calculatedColumnFormula>(INDEX(TblBattlefieldFlt[[A]:[F]],MATCH($A25,TblBattlefieldFlt[Option],0),MATCH(G$24,TblBattlefieldFlt[[#Headers],[A]:[F]],0)))*(INDEX(TblShipCrew[Adjusted],MATCH($A25,TblShipCrew[Ships],0)))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0300-000008000000}" name="Name" dataDxfId="73" totalsRowDxfId="74"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0300-000008000000}" name="Name" dataDxfId="74" totalsRowDxfId="73"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium13" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2723,11 +2821,11 @@
   <autoFilter ref="A32:G42" xr:uid="{00000000-0009-0000-0100-000008000000}"/>
   <tableColumns count="7">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0400-000001000000}" name="Option" totalsRowLabel="Total"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0400-000002000000}" name="A" totalsRowFunction="sum" dataDxfId="70" totalsRowDxfId="71">
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0400-000002000000}" name="A" totalsRowFunction="sum" dataDxfId="71" totalsRowDxfId="70">
       <calculatedColumnFormula>K10</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0400-000003000000}" name="B" totalsRowFunction="sum" dataDxfId="68" totalsRowDxfId="69"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0400-000004000000}" name="C" totalsRowFunction="sum" dataDxfId="66" totalsRowDxfId="67"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0400-000003000000}" name="B" totalsRowFunction="sum" dataDxfId="69" totalsRowDxfId="68"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0400-000004000000}" name="C" totalsRowFunction="sum" dataDxfId="67" totalsRowDxfId="66"/>
     <tableColumn id="5" xr3:uid="{00000000-0010-0000-0400-000005000000}" name="D" totalsRowFunction="sum" totalsRowDxfId="65"/>
     <tableColumn id="6" xr3:uid="{00000000-0010-0000-0400-000006000000}" name="E" totalsRowFunction="sum" totalsRowDxfId="64"/>
     <tableColumn id="7" xr3:uid="{00000000-0010-0000-0400-000007000000}" name="F" totalsRowFunction="sum" totalsRowDxfId="63"/>
@@ -2741,25 +2839,25 @@
   <autoFilter ref="J24:Q29" xr:uid="{00000000-0009-0000-0100-000009000000}"/>
   <tableColumns count="8">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0500-000001000000}" name="Option" totalsRowLabel="Total" dataDxfId="60"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0500-000002000000}" name="A" totalsRowFunction="sum" dataDxfId="58" totalsRowDxfId="59">
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0500-000002000000}" name="A" totalsRowFunction="sum" dataDxfId="59" totalsRowDxfId="58">
       <calculatedColumnFormula>(INDEX(TblBattlefieldFlt[[A]:[F]],MATCH($J25,TblBattlefieldFlt[Option],0),MATCH(K$24,TblBattlefieldFlt[[#Headers],[A]:[F]],0)))*(INDEX(TblShipCrew[Generic (500)],MATCH($J25,TblShipCrew[Ships],0)))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0500-000003000000}" name="B" totalsRowFunction="sum" dataDxfId="56" totalsRowDxfId="57">
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0500-000003000000}" name="B" totalsRowFunction="sum" dataDxfId="57" totalsRowDxfId="56">
       <calculatedColumnFormula>(INDEX(TblBattlefieldFlt[[A]:[F]],MATCH($J25,TblBattlefieldFlt[Option],0),MATCH(L$24,TblBattlefieldFlt[[#Headers],[A]:[F]],0)))*(INDEX(TblShipCrew[Generic (500)],MATCH($J25,TblShipCrew[Ships],0)))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0500-000004000000}" name="C" totalsRowFunction="sum" dataDxfId="54" totalsRowDxfId="55">
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0500-000004000000}" name="C" totalsRowFunction="sum" dataDxfId="55" totalsRowDxfId="54">
       <calculatedColumnFormula>(INDEX(TblBattlefieldFlt[[A]:[F]],MATCH($J25,TblBattlefieldFlt[Option],0),MATCH(M$24,TblBattlefieldFlt[[#Headers],[A]:[F]],0)))*(INDEX(TblShipCrew[Generic (500)],MATCH($J25,TblShipCrew[Ships],0)))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0500-000005000000}" name="D" totalsRowFunction="sum" dataDxfId="52" totalsRowDxfId="53">
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0500-000005000000}" name="D" totalsRowFunction="sum" dataDxfId="53" totalsRowDxfId="52">
       <calculatedColumnFormula>(INDEX(TblBattlefieldFlt[[A]:[F]],MATCH($J25,TblBattlefieldFlt[Option],0),MATCH(N$24,TblBattlefieldFlt[[#Headers],[A]:[F]],0)))*(INDEX(TblShipCrew[Generic (500)],MATCH($J25,TblShipCrew[Ships],0)))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0500-000006000000}" name="E" totalsRowFunction="sum" dataDxfId="50" totalsRowDxfId="51">
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0500-000006000000}" name="E" totalsRowFunction="sum" dataDxfId="51" totalsRowDxfId="50">
       <calculatedColumnFormula>(INDEX(TblBattlefieldFlt[[A]:[F]],MATCH($J25,TblBattlefieldFlt[Option],0),MATCH(O$24,TblBattlefieldFlt[[#Headers],[A]:[F]],0)))*(INDEX(TblShipCrew[Generic (500)],MATCH($J25,TblShipCrew[Ships],0)))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0500-000007000000}" name="F" totalsRowFunction="sum" dataDxfId="48" totalsRowDxfId="49">
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0500-000007000000}" name="F" totalsRowFunction="sum" dataDxfId="49" totalsRowDxfId="48">
       <calculatedColumnFormula>(INDEX(TblBattlefieldFlt[[A]:[F]],MATCH($J25,TblBattlefieldFlt[Option],0),MATCH(P$24,TblBattlefieldFlt[[#Headers],[A]:[F]],0)))*(INDEX(TblShipCrew[Generic (500)],MATCH($J25,TblShipCrew[Ships],0)))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0500-000008000000}" name="Name" dataDxfId="46" totalsRowDxfId="47"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0500-000008000000}" name="Name" dataDxfId="47" totalsRowDxfId="46"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium10" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2770,11 +2868,11 @@
   <autoFilter ref="J32:P42" xr:uid="{00000000-0009-0000-0100-00000A000000}"/>
   <tableColumns count="7">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0600-000001000000}" name="Option" totalsRowLabel="Total" totalsRowDxfId="44"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0600-000002000000}" name="A" totalsRowFunction="sum" dataDxfId="42" totalsRowDxfId="43">
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0600-000002000000}" name="A" totalsRowFunction="sum" dataDxfId="43" totalsRowDxfId="42">
       <calculatedColumnFormula>T10</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0600-000003000000}" name="B" totalsRowFunction="sum" dataDxfId="40" totalsRowDxfId="41"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0600-000004000000}" name="C" totalsRowFunction="sum" dataDxfId="38" totalsRowDxfId="39"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0600-000003000000}" name="B" totalsRowFunction="sum" dataDxfId="41" totalsRowDxfId="40"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0600-000004000000}" name="C" totalsRowFunction="sum" dataDxfId="39" totalsRowDxfId="38"/>
     <tableColumn id="5" xr3:uid="{00000000-0010-0000-0600-000005000000}" name="D" totalsRowFunction="sum" totalsRowDxfId="37"/>
     <tableColumn id="6" xr3:uid="{00000000-0010-0000-0600-000006000000}" name="E" totalsRowFunction="sum" totalsRowDxfId="36"/>
     <tableColumn id="7" xr3:uid="{00000000-0010-0000-0600-000007000000}" name="F" totalsRowFunction="sum" totalsRowDxfId="35"/>
@@ -2784,7 +2882,7 @@
 </file>
 
 <file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="13" xr:uid="{00000000-000C-0000-FFFF-FFFF07000000}" name="TblShipCrew" displayName="TblShipCrew" ref="D2:L7" totalsRowShown="0" headerRowDxfId="34" dataDxfId="33" headerRowBorderDxfId="31" tableBorderDxfId="32">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="13" xr:uid="{00000000-000C-0000-FFFF-FFFF07000000}" name="TblShipCrew" displayName="TblShipCrew" ref="D2:L7" totalsRowShown="0" headerRowDxfId="34" dataDxfId="32" headerRowBorderDxfId="33" tableBorderDxfId="31">
   <autoFilter ref="D2:L7" xr:uid="{00000000-0009-0000-0100-00000D000000}"/>
   <tableColumns count="9">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0700-000001000000}" name="Ships" dataDxfId="30"/>
@@ -2812,7 +2910,7 @@
 </file>
 
 <file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="12" xr:uid="{00000000-000C-0000-FFFF-FFFF08000000}" name="TblShipPoints" displayName="TblShipPoints" ref="A2:B7" totalsRowShown="0" headerRowDxfId="21" dataDxfId="20" headerRowBorderDxfId="18" tableBorderDxfId="19">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="12" xr:uid="{00000000-000C-0000-FFFF-FFFF08000000}" name="TblShipPoints" displayName="TblShipPoints" ref="A2:B7" totalsRowShown="0" headerRowDxfId="21" dataDxfId="19" headerRowBorderDxfId="20" tableBorderDxfId="18">
   <autoFilter ref="A2:B7" xr:uid="{00000000-0009-0000-0100-00000C000000}"/>
   <tableColumns count="2">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0800-000001000000}" name="Ships" dataDxfId="17"/>
@@ -3125,7 +3223,7 @@
       <selection activeCell="I10" sqref="I10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="14.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="7" width="15.42578125" customWidth="1"/>
@@ -3143,24 +3241,24 @@
     <col min="24" max="24" width="10" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17">
-      <c r="A1" s="42" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="42"/>
-      <c r="C1" s="42"/>
-      <c r="D1" s="42"/>
-      <c r="E1" s="42"/>
-      <c r="F1" s="42"/>
-      <c r="G1" s="42"/>
-      <c r="H1" s="42"/>
-      <c r="N1" s="42" t="s">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A1" s="47" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="47"/>
+      <c r="C1" s="47"/>
+      <c r="D1" s="47"/>
+      <c r="E1" s="47"/>
+      <c r="F1" s="47"/>
+      <c r="G1" s="47"/>
+      <c r="H1" s="47"/>
+      <c r="N1" s="47" t="s">
         <v>1</v>
       </c>
-      <c r="O1" s="42"/>
-      <c r="P1" s="42"/>
-    </row>
-    <row r="2" spans="1:17">
+      <c r="O1" s="47"/>
+      <c r="P1" s="47"/>
+    </row>
+    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2" s="9" t="s">
         <v>2</v>
       </c>
@@ -3207,7 +3305,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:17">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A3" s="15" t="s">
         <v>13</v>
       </c>
@@ -3260,7 +3358,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="4" spans="1:17">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A4" s="10" t="s">
         <v>14</v>
       </c>
@@ -3301,7 +3399,7 @@
         <v>5500</v>
       </c>
     </row>
-    <row r="5" spans="1:17">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A5" s="10" t="s">
         <v>15</v>
       </c>
@@ -3342,7 +3440,7 @@
         <v>3500</v>
       </c>
     </row>
-    <row r="6" spans="1:17">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A6" s="10" t="s">
         <v>16</v>
       </c>
@@ -3383,7 +3481,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="7" spans="1:17">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>17</v>
       </c>
@@ -3424,28 +3522,28 @@
         <v>500</v>
       </c>
     </row>
-    <row r="8" spans="1:17">
-      <c r="A8" s="42" t="s">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A8" s="47" t="s">
         <v>18</v>
       </c>
-      <c r="B8" s="42"/>
-      <c r="C8" s="42"/>
-      <c r="D8" s="42"/>
-      <c r="E8" s="42"/>
-      <c r="F8" s="42"/>
-      <c r="G8" s="42"/>
-      <c r="J8" s="42" t="s">
+      <c r="B8" s="47"/>
+      <c r="C8" s="47"/>
+      <c r="D8" s="47"/>
+      <c r="E8" s="47"/>
+      <c r="F8" s="47"/>
+      <c r="G8" s="47"/>
+      <c r="J8" s="47" t="s">
         <v>19</v>
       </c>
-      <c r="K8" s="42"/>
-      <c r="L8" s="42"/>
-      <c r="M8" s="42"/>
-      <c r="N8" s="42"/>
-      <c r="O8" s="42"/>
-      <c r="P8" s="42"/>
-      <c r="Q8" s="42"/>
-    </row>
-    <row r="9" spans="1:17">
+      <c r="K8" s="47"/>
+      <c r="L8" s="47"/>
+      <c r="M8" s="47"/>
+      <c r="N8" s="47"/>
+      <c r="O8" s="47"/>
+      <c r="P8" s="47"/>
+      <c r="Q8" s="47"/>
+    </row>
+    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A9" s="8" t="s">
         <v>20</v>
       </c>
@@ -3493,7 +3591,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="10" spans="1:17">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>13</v>
       </c>
@@ -3537,7 +3635,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="11" spans="1:17">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>14</v>
       </c>
@@ -3583,7 +3681,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="12" spans="1:17">
+    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>15</v>
       </c>
@@ -3631,7 +3729,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="13" spans="1:17">
+    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>16</v>
       </c>
@@ -3677,7 +3775,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="14" spans="1:17">
+    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>17</v>
       </c>
@@ -3725,7 +3823,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="15" spans="1:17">
+    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>33</v>
       </c>
@@ -3782,16 +3880,16 @@
       </c>
       <c r="Q15" s="1"/>
     </row>
-    <row r="16" spans="1:17">
-      <c r="A16" s="42" t="s">
+    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A16" s="47" t="s">
         <v>35</v>
       </c>
-      <c r="B16" s="42"/>
-      <c r="C16" s="42"/>
-      <c r="D16" s="42"/>
-      <c r="E16" s="42"/>
-      <c r="F16" s="42"/>
-      <c r="G16" s="42"/>
+      <c r="B16" s="47"/>
+      <c r="C16" s="47"/>
+      <c r="D16" s="47"/>
+      <c r="E16" s="47"/>
+      <c r="F16" s="47"/>
+      <c r="G16" s="47"/>
       <c r="K16" s="1"/>
       <c r="L16" s="1"/>
       <c r="M16" s="1"/>
@@ -3800,7 +3898,7 @@
       <c r="P16" s="1"/>
       <c r="Q16" s="1"/>
     </row>
-    <row r="17" spans="1:18">
+    <row r="17" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>20</v>
       </c>
@@ -3833,7 +3931,7 @@
       <c r="P17" s="1"/>
       <c r="Q17" s="1"/>
     </row>
-    <row r="18" spans="1:18">
+    <row r="18" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>4</v>
       </c>
@@ -3872,7 +3970,7 @@
       <c r="P18" s="1"/>
       <c r="Q18" s="1"/>
     </row>
-    <row r="19" spans="1:18">
+    <row r="19" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>5</v>
       </c>
@@ -3911,7 +4009,7 @@
       <c r="P19" s="1"/>
       <c r="Q19" s="1"/>
     </row>
-    <row r="20" spans="1:18">
+    <row r="20" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>6</v>
       </c>
@@ -3950,7 +4048,7 @@
       <c r="P20" s="1"/>
       <c r="Q20" s="1"/>
     </row>
-    <row r="21" spans="1:18">
+    <row r="21" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>33</v>
       </c>
@@ -3987,7 +4085,7 @@
       <c r="P21" s="1"/>
       <c r="Q21" s="1"/>
     </row>
-    <row r="22" spans="1:18">
+    <row r="22" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A22" s="4"/>
       <c r="B22" s="5"/>
       <c r="C22" s="5"/>
@@ -4007,30 +4105,30 @@
       <c r="Q22" s="4"/>
       <c r="R22" s="4"/>
     </row>
-    <row r="23" spans="1:18">
-      <c r="A23" s="42" t="s">
+    <row r="23" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A23" s="47" t="s">
         <v>40</v>
       </c>
-      <c r="B23" s="42"/>
-      <c r="C23" s="42"/>
-      <c r="D23" s="42"/>
-      <c r="E23" s="42"/>
-      <c r="F23" s="42"/>
-      <c r="G23" s="42"/>
-      <c r="H23" s="42"/>
+      <c r="B23" s="47"/>
+      <c r="C23" s="47"/>
+      <c r="D23" s="47"/>
+      <c r="E23" s="47"/>
+      <c r="F23" s="47"/>
+      <c r="G23" s="47"/>
+      <c r="H23" s="47"/>
       <c r="I23" s="4"/>
-      <c r="J23" s="42" t="s">
+      <c r="J23" s="47" t="s">
         <v>41</v>
       </c>
-      <c r="K23" s="42"/>
-      <c r="L23" s="42"/>
-      <c r="M23" s="42"/>
-      <c r="N23" s="42"/>
-      <c r="O23" s="42"/>
-      <c r="P23" s="42"/>
-      <c r="Q23" s="42"/>
-    </row>
-    <row r="24" spans="1:18">
+      <c r="K23" s="47"/>
+      <c r="L23" s="47"/>
+      <c r="M23" s="47"/>
+      <c r="N23" s="47"/>
+      <c r="O23" s="47"/>
+      <c r="P23" s="47"/>
+      <c r="Q23" s="47"/>
+    </row>
+    <row r="24" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A24" s="8" t="s">
         <v>20</v>
       </c>
@@ -4081,7 +4179,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="25" spans="1:18">
+    <row r="25" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>13</v>
       </c>
@@ -4144,7 +4242,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="26" spans="1:18">
+    <row r="26" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>14</v>
       </c>
@@ -4207,7 +4305,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="27" spans="1:18">
+    <row r="27" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>15</v>
       </c>
@@ -4270,7 +4368,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="28" spans="1:18">
+    <row r="28" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>16</v>
       </c>
@@ -4333,7 +4431,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="29" spans="1:18">
+    <row r="29" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>17</v>
       </c>
@@ -4396,7 +4494,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="30" spans="1:18">
+    <row r="30" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>33</v>
       </c>
@@ -4455,28 +4553,28 @@
       </c>
       <c r="Q30" s="1"/>
     </row>
-    <row r="31" spans="1:18">
-      <c r="A31" s="42" t="s">
+    <row r="31" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A31" s="47" t="s">
         <v>47</v>
       </c>
-      <c r="B31" s="42"/>
-      <c r="C31" s="42"/>
-      <c r="D31" s="42"/>
-      <c r="E31" s="42"/>
-      <c r="F31" s="42"/>
-      <c r="G31" s="42"/>
+      <c r="B31" s="47"/>
+      <c r="C31" s="47"/>
+      <c r="D31" s="47"/>
+      <c r="E31" s="47"/>
+      <c r="F31" s="47"/>
+      <c r="G31" s="47"/>
       <c r="I31" s="4"/>
-      <c r="J31" s="42" t="s">
+      <c r="J31" s="47" t="s">
         <v>48</v>
       </c>
-      <c r="K31" s="42"/>
-      <c r="L31" s="42"/>
-      <c r="M31" s="42"/>
-      <c r="N31" s="42"/>
-      <c r="O31" s="42"/>
-      <c r="P31" s="42"/>
-    </row>
-    <row r="32" spans="1:18">
+      <c r="K31" s="47"/>
+      <c r="L31" s="47"/>
+      <c r="M31" s="47"/>
+      <c r="N31" s="47"/>
+      <c r="O31" s="47"/>
+      <c r="P31" s="47"/>
+    </row>
+    <row r="32" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>20</v>
       </c>
@@ -4521,7 +4619,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="33" spans="1:16">
+    <row r="33" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>28</v>
       </c>
@@ -4578,7 +4676,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:16">
+    <row r="34" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>42</v>
       </c>
@@ -4635,7 +4733,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:16">
+    <row r="35" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>29</v>
       </c>
@@ -4692,7 +4790,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:16">
+    <row r="36" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>43</v>
       </c>
@@ -4749,7 +4847,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:16">
+    <row r="37" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>30</v>
       </c>
@@ -4806,7 +4904,7 @@
         <v>2500</v>
       </c>
     </row>
-    <row r="38" spans="1:16">
+    <row r="38" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>44</v>
       </c>
@@ -4863,7 +4961,7 @@
         <v>3500</v>
       </c>
     </row>
-    <row r="39" spans="1:16">
+    <row r="39" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>31</v>
       </c>
@@ -4920,7 +5018,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:16">
+    <row r="40" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>45</v>
       </c>
@@ -4977,7 +5075,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:16">
+    <row r="41" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>32</v>
       </c>
@@ -5034,7 +5132,7 @@
         <v>5000</v>
       </c>
     </row>
-    <row r="42" spans="1:16">
+    <row r="42" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>46</v>
       </c>
@@ -5091,7 +5189,7 @@
         <v>5000</v>
       </c>
     </row>
-    <row r="43" spans="1:16">
+    <row r="43" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>33</v>
       </c>
@@ -5148,17 +5246,17 @@
         <v>16000</v>
       </c>
     </row>
-    <row r="45" spans="1:16">
+    <row r="45" spans="1:16" x14ac:dyDescent="0.25">
       <c r="C45" s="1"/>
       <c r="D45" s="1"/>
       <c r="E45" s="1"/>
       <c r="F45" s="1"/>
       <c r="G45" s="1"/>
     </row>
-    <row r="50" spans="2:2">
+    <row r="50" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B50" s="1"/>
     </row>
-    <row r="51" spans="2:2">
+    <row r="51" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B51" s="1"/>
     </row>
   </sheetData>
@@ -5198,11 +5296,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{91273792-62E9-442E-9CC7-E8C6E6BD4008}">
   <dimension ref="B1:V29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="16.5703125" customWidth="1"/>
     <col min="3" max="3" width="18" customWidth="1"/>
@@ -5213,12 +5311,12 @@
     <col min="13" max="13" width="34" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:22">
+    <row r="1" spans="2:22" x14ac:dyDescent="0.25">
       <c r="M1" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="2" spans="2:22">
+    <row r="2" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B2" s="21" t="s">
         <v>2</v>
       </c>
@@ -5259,7 +5357,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="3" spans="2:22">
+    <row r="3" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B3" s="25" t="s">
         <v>13</v>
       </c>
@@ -5320,7 +5418,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="2:22">
+    <row r="4" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B4" s="26" t="s">
         <v>14</v>
       </c>
@@ -5349,7 +5447,7 @@
         <v>1</v>
       </c>
       <c r="N4">
-        <f t="shared" ref="N4:O14" si="0">M4*100</f>
+        <f t="shared" ref="N4:N14" si="0">M4*100</f>
         <v>100</v>
       </c>
       <c r="O4">
@@ -5381,7 +5479,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="5" spans="2:22">
+    <row r="5" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B5" s="27" t="s">
         <v>15</v>
       </c>
@@ -5435,7 +5533,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="6" spans="2:22">
+    <row r="6" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B6" s="26" t="s">
         <v>16</v>
       </c>
@@ -5489,7 +5587,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="7" spans="2:22">
+    <row r="7" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B7" s="27" t="s">
         <v>17</v>
       </c>
@@ -5536,7 +5634,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="8" spans="2:22">
+    <row r="8" spans="2:22" x14ac:dyDescent="0.25">
       <c r="L8">
         <v>6</v>
       </c>
@@ -5562,7 +5660,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="9" spans="2:22">
+    <row r="9" spans="2:22" x14ac:dyDescent="0.25">
       <c r="L9">
         <v>7</v>
       </c>
@@ -5581,7 +5679,7 @@
         <v>600</v>
       </c>
     </row>
-    <row r="10" spans="2:22">
+    <row r="10" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
         <v>56</v>
       </c>
@@ -5603,7 +5701,7 @@
         <v>700</v>
       </c>
     </row>
-    <row r="11" spans="2:22">
+    <row r="11" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B11" s="19" t="s">
         <v>57</v>
       </c>
@@ -5637,7 +5735,7 @@
         <v>800</v>
       </c>
     </row>
-    <row r="12" spans="2:22" ht="76.5">
+    <row r="12" spans="2:22" ht="75" x14ac:dyDescent="0.25">
       <c r="B12" s="20" t="s">
         <v>62</v>
       </c>
@@ -5664,7 +5762,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="13" spans="2:22">
+    <row r="13" spans="2:22" x14ac:dyDescent="0.25">
       <c r="L13">
         <v>11</v>
       </c>
@@ -5676,7 +5774,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="14" spans="2:22">
+    <row r="14" spans="2:22" x14ac:dyDescent="0.25">
       <c r="L14">
         <v>12</v>
       </c>
@@ -5688,7 +5786,7 @@
         <v>1100</v>
       </c>
     </row>
-    <row r="15" spans="2:22">
+    <row r="15" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B15" s="21" t="s">
         <v>2</v>
       </c>
@@ -5705,7 +5803,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="16" spans="2:22">
+    <row r="16" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B16" s="22" t="s">
         <v>13</v>
       </c>
@@ -5722,7 +5820,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="17" spans="2:12">
+    <row r="17" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B17" s="23" t="s">
         <v>14</v>
       </c>
@@ -5739,7 +5837,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="18" spans="2:12">
+    <row r="18" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B18" s="22" t="s">
         <v>15</v>
       </c>
@@ -5756,7 +5854,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="19" spans="2:12">
+    <row r="19" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B19" s="23" t="s">
         <v>16</v>
       </c>
@@ -5773,7 +5871,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="20" spans="2:12">
+    <row r="20" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B20" s="22" t="s">
         <v>17</v>
       </c>
@@ -5790,17 +5888,17 @@
         <v>18</v>
       </c>
     </row>
-    <row r="21" spans="2:12">
+    <row r="21" spans="2:12" x14ac:dyDescent="0.25">
       <c r="L21">
         <v>19</v>
       </c>
     </row>
-    <row r="22" spans="2:12">
+    <row r="22" spans="2:12" x14ac:dyDescent="0.25">
       <c r="L22">
         <v>20</v>
       </c>
     </row>
-    <row r="23" spans="2:12">
+    <row r="23" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B23" s="36" t="s">
         <v>20</v>
       </c>
@@ -5826,7 +5924,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="24" spans="2:12">
+    <row r="24" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B24" s="38" t="s">
         <v>13</v>
       </c>
@@ -5842,7 +5940,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="25" spans="2:12">
+    <row r="25" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B25" s="40" t="s">
         <v>14</v>
       </c>
@@ -5860,7 +5958,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="26" spans="2:12">
+    <row r="26" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B26" s="38" t="s">
         <v>15</v>
       </c>
@@ -5880,7 +5978,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="27" spans="2:12">
+    <row r="27" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B27" s="40" t="s">
         <v>16</v>
       </c>
@@ -5898,7 +5996,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="28" spans="2:12">
+    <row r="28" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B28" s="38" t="s">
         <v>17</v>
       </c>
@@ -5918,7 +6016,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="29" spans="2:12">
+    <row r="29" spans="2:12" x14ac:dyDescent="0.25">
       <c r="C29">
         <f>C24*G3*F3</f>
         <v>1000</v>
@@ -5957,9 +6055,9 @@
       <selection activeCell="P25" sqref="P24:Q25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="2:19">
+    <row r="1" spans="2:19" x14ac:dyDescent="0.25">
       <c r="D1">
         <v>38</v>
       </c>
@@ -5982,7 +6080,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="2:19">
+    <row r="2" spans="2:19" x14ac:dyDescent="0.25">
       <c r="J2" t="s">
         <v>58</v>
       </c>
@@ -5990,20 +6088,20 @@
         <v>67</v>
       </c>
     </row>
-    <row r="3" spans="2:19">
-      <c r="B3" s="50"/>
-      <c r="C3" s="50"/>
-      <c r="D3" s="50"/>
-      <c r="E3" s="50"/>
-      <c r="F3" s="50"/>
-      <c r="G3" s="50" t="s">
+    <row r="3" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B3" s="42"/>
+      <c r="C3" s="42"/>
+      <c r="D3" s="42"/>
+      <c r="E3" s="42"/>
+      <c r="F3" s="42"/>
+      <c r="G3" s="42" t="s">
         <v>68</v>
       </c>
-      <c r="H3" s="50"/>
-      <c r="I3" s="50"/>
-      <c r="J3" s="50"/>
-      <c r="K3" s="50"/>
-      <c r="L3" s="50"/>
+      <c r="H3" s="42"/>
+      <c r="I3" s="42"/>
+      <c r="J3" s="42"/>
+      <c r="K3" s="42"/>
+      <c r="L3" s="42"/>
       <c r="N3" s="21" t="s">
         <v>2</v>
       </c>
@@ -6023,8 +6121,8 @@
         <v>53</v>
       </c>
     </row>
-    <row r="4" spans="2:19">
-      <c r="B4" s="53" t="s">
+    <row r="4" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B4" s="45" t="s">
         <v>69</v>
       </c>
       <c r="N4" s="25" t="s">
@@ -6046,8 +6144,8 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="2:19">
-      <c r="B5" s="51" t="s">
+    <row r="5" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B5" s="43" t="s">
         <v>70</v>
       </c>
       <c r="N5" s="26" t="s">
@@ -6069,8 +6167,8 @@
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="2:19">
-      <c r="B6" s="53" t="s">
+    <row r="6" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B6" s="45" t="s">
         <v>71</v>
       </c>
       <c r="N6" s="27" t="s">
@@ -6092,7 +6190,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="2:19">
+    <row r="7" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B7" s="6" t="s">
         <v>72</v>
       </c>
@@ -6115,7 +6213,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="2:19">
+    <row r="8" spans="2:19" x14ac:dyDescent="0.25">
       <c r="G8" s="6" t="s">
         <v>13</v>
       </c>
@@ -6138,7 +6236,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="2:19">
+    <row r="10" spans="2:19" x14ac:dyDescent="0.25">
       <c r="N10" s="19" t="s">
         <v>57</v>
       </c>
@@ -6155,74 +6253,74 @@
         <v>61</v>
       </c>
     </row>
-    <row r="15" spans="2:19">
-      <c r="C15" s="52" t="s">
+    <row r="15" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="C15" s="44" t="s">
         <v>17</v>
       </c>
-      <c r="E15" s="52" t="s">
+      <c r="E15" s="44" t="s">
         <v>17</v>
       </c>
       <c r="G15" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="I15" s="52" t="s">
+      <c r="I15" s="44" t="s">
         <v>17</v>
       </c>
-      <c r="K15" s="52" t="s">
+      <c r="K15" s="44" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="16" spans="2:19">
+    <row r="16" spans="2:19" x14ac:dyDescent="0.25">
       <c r="P16">
         <f ca="1">RANDBETWEEN(0,123)</f>
-        <v>16</v>
-      </c>
-    </row>
-    <row r="17" spans="2:16">
-      <c r="P17" s="54">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="17" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="P17" s="46">
         <f ca="1">RANDBETWEEN(0,6)</f>
-        <v>3</v>
-      </c>
-    </row>
-    <row r="18" spans="2:16">
-      <c r="C18" s="52" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="18" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="C18" s="44" t="s">
         <v>17</v>
       </c>
-      <c r="E18" s="52" t="s">
+      <c r="E18" s="44" t="s">
         <v>17</v>
       </c>
-      <c r="I18" s="52" t="s">
+      <c r="I18" s="44" t="s">
         <v>17</v>
       </c>
-      <c r="K18" s="52" t="s">
+      <c r="K18" s="44" t="s">
         <v>17</v>
       </c>
       <c r="L18" s="6" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="19" spans="2:16">
-      <c r="L19" s="53" t="s">
+    <row r="19" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="L19" s="45" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="20" spans="2:16">
-      <c r="E20" s="52" t="s">
+    <row r="20" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="E20" s="44" t="s">
         <v>17</v>
       </c>
-      <c r="I20" s="52" t="s">
+      <c r="I20" s="44" t="s">
         <v>17</v>
       </c>
-      <c r="L20" s="51" t="s">
+      <c r="L20" s="43" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="21" spans="2:16">
-      <c r="L21" s="53" t="s">
+    <row r="21" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="L21" s="45" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="22" spans="2:16">
+    <row r="22" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B22" s="2"/>
       <c r="C22" s="2"/>
       <c r="D22" s="2"/>
@@ -6237,7 +6335,7 @@
       <c r="K22" s="2"/>
       <c r="L22" s="2"/>
     </row>
-    <row r="24" spans="2:16">
+    <row r="24" spans="2:16" x14ac:dyDescent="0.25">
       <c r="E24">
         <v>64</v>
       </c>
@@ -6260,7 +6358,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="25" spans="2:16">
+    <row r="25" spans="2:16" x14ac:dyDescent="0.25">
       <c r="K25" t="s">
         <v>58</v>
       </c>
@@ -6275,169 +6373,331 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F5EC53A5-8F19-4711-93EA-0F4CBD261EC8}">
-  <dimension ref="B2:B31"/>
+  <dimension ref="B2:B72"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
+      <selection activeCell="I53" sqref="I53"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="11.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:2">
+    <row r="2" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B2" s="21" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="3" spans="2:2">
-      <c r="B3" t="s">
+    <row r="3" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B3" s="3" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="4" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="4" spans="2:2">
-      <c r="B4" t="s">
+    <row r="5" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="5" spans="2:2">
-      <c r="B5" t="s">
+    <row r="6" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="6" spans="2:2">
-      <c r="B6" t="s">
+    <row r="7" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B7" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="7" spans="2:2">
-      <c r="B7" t="s">
+    <row r="8" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B8" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="8" spans="2:2">
-      <c r="B8" t="s">
+    <row r="9" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B9" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="10" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B10" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="12" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B12" s="3" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="13" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B13" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="14" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B14" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="16" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B16" s="3" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="17" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B17" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="9" spans="2:2">
-      <c r="B9" s="49" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="10" spans="2:2">
-      <c r="B10" t="s">
+    <row r="18" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B18" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="19" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B19" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="20" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B20" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="21" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B21" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="23" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B23" s="3" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="24" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B24" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="26" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B26" s="3" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="27" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B27" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="28" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B28" s="54" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="29" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B29" s="54"/>
+    </row>
+    <row r="30" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B30" s="3" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="31" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B31" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="33" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B33" s="3" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="34" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B34" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="35" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B35" s="54" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="36" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B36" s="54"/>
+    </row>
+    <row r="37" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B37" s="3" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="38" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B38" s="54" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="39" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B39" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="40" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B40" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="11" spans="2:2">
-      <c r="B11" t="s">
+    <row r="41" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B41" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="12" spans="2:2">
-      <c r="B12" t="s">
+    <row r="42" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B42" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="43" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B43" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="44" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B44" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="45" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B45" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="46" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B46" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="47" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B47" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="48" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B48" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="50" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B50" s="3" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="51" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B51" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="52" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B52" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="53" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B53" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="54" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B54" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="55" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B55" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="56" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B56" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="57" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B57" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="58" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B58" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="60" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B60" s="3" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="61" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B61" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="13" spans="2:2">
-      <c r="B13" t="s">
+    <row r="62" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B62" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="63" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B63" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="14" spans="2:2">
-      <c r="B14" t="s">
+    <row r="65" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B65" s="3" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="66" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B66" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="67" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B67" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="15" spans="2:2">
-      <c r="B15" t="s">
+    <row r="68" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B68" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="69" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B69" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="70" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B70" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="71" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B71" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="16" spans="2:2">
-      <c r="B16" t="s">
+    <row r="72" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B72" t="s">
         <v>88</v>
-      </c>
-    </row>
-    <row r="17" spans="2:2">
-      <c r="B17" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="18" spans="2:2">
-      <c r="B18" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="19" spans="2:2">
-      <c r="B19" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="20" spans="2:2">
-      <c r="B20" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="21" spans="2:2">
-      <c r="B21" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="22" spans="2:2">
-      <c r="B22" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="23" spans="2:2">
-      <c r="B23" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="24" spans="2:2">
-      <c r="B24" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="25" spans="2:2">
-      <c r="B25" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="26" spans="2:2">
-      <c r="B26" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="27" spans="2:2">
-      <c r="B27" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="28" spans="2:2">
-      <c r="B28" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="29" spans="2:2">
-      <c r="B29" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="30" spans="2:2">
-      <c r="B30" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="31" spans="2:2">
-      <c r="B31" t="s">
-        <v>103</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -6449,56 +6709,56 @@
       <selection activeCell="J14" sqref="J14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="2" spans="2:2">
+    <row r="2" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="3" spans="2:2">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="3" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="4" spans="2:2">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="4" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="5" spans="2:2">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="5" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="6" spans="2:2">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="6" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="7" spans="2:2">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="7" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="8" spans="2:2">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="8" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="9" spans="2:2">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="9" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="10" spans="2:2">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="10" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="11" spans="2:2">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="11" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
-        <v>113</v>
+        <v>100</v>
       </c>
     </row>
   </sheetData>
@@ -6514,194 +6774,194 @@
       <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="18.28515625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="29.42578125" customWidth="1"/>
     <col min="4" max="4" width="27.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:4">
+    <row r="2" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B2" s="32" t="s">
+        <v>101</v>
+      </c>
+      <c r="C2" s="32" t="s">
+        <v>102</v>
+      </c>
+      <c r="D2" s="32" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="3" spans="2:4" ht="106.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B3" s="50" t="s">
+        <v>104</v>
+      </c>
+      <c r="C3" s="48" t="s">
+        <v>105</v>
+      </c>
+      <c r="D3" s="28" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="4" spans="2:4" ht="120" x14ac:dyDescent="0.25">
+      <c r="B4" s="53"/>
+      <c r="C4" s="52"/>
+      <c r="D4" s="29" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="5" spans="2:4" ht="60" x14ac:dyDescent="0.25">
+      <c r="B5" s="53"/>
+      <c r="C5" s="52"/>
+      <c r="D5" s="30" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="6" spans="2:4" ht="75" x14ac:dyDescent="0.25">
+      <c r="B6" s="53"/>
+      <c r="C6" s="52"/>
+      <c r="D6" s="30" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="7" spans="2:4" ht="90" x14ac:dyDescent="0.25">
+      <c r="B7" s="50" t="s">
+        <v>110</v>
+      </c>
+      <c r="C7" s="48" t="s">
+        <v>111</v>
+      </c>
+      <c r="D7" s="28" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="8" spans="2:4" ht="90" x14ac:dyDescent="0.25">
+      <c r="B8" s="53"/>
+      <c r="C8" s="52"/>
+      <c r="D8" s="30" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="9" spans="2:4" ht="75" x14ac:dyDescent="0.25">
+      <c r="B9" s="50" t="s">
         <v>114</v>
       </c>
-      <c r="C2" s="32" t="s">
+      <c r="C9" s="48" t="s">
         <v>115</v>
       </c>
-      <c r="D2" s="32" t="s">
+      <c r="D9" s="28" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="3" spans="2:4" ht="106.5" customHeight="1">
-      <c r="B3" s="45" t="s">
+    <row r="10" spans="2:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="B10" s="51"/>
+      <c r="C10" s="49"/>
+      <c r="D10" s="31" t="s">
         <v>117</v>
       </c>
-      <c r="C3" s="43" t="s">
+    </row>
+    <row r="11" spans="2:4" ht="76.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B11" s="50" t="s">
         <v>118</v>
       </c>
-      <c r="D3" s="28" t="s">
+      <c r="C11" s="48" t="s">
         <v>119</v>
       </c>
-    </row>
-    <row r="4" spans="2:4" ht="106.5">
-      <c r="B4" s="48"/>
-      <c r="C4" s="47"/>
-      <c r="D4" s="29" t="s">
+      <c r="D11" s="28" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="5" spans="2:4" ht="60.75">
-      <c r="B5" s="48"/>
-      <c r="C5" s="47"/>
-      <c r="D5" s="30" t="s">
+    <row r="12" spans="2:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="B12" s="53"/>
+      <c r="C12" s="52"/>
+      <c r="D12" s="30" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="6" spans="2:4" ht="76.5">
-      <c r="B6" s="48"/>
-      <c r="C6" s="47"/>
-      <c r="D6" s="30" t="s">
+    <row r="13" spans="2:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="B13" s="50" t="s">
         <v>122</v>
       </c>
-    </row>
-    <row r="7" spans="2:4" ht="91.5">
-      <c r="B7" s="45" t="s">
+      <c r="C13" s="48" t="s">
         <v>123</v>
       </c>
-      <c r="C7" s="43" t="s">
+      <c r="D13" s="28" t="s">
         <v>124</v>
       </c>
-      <c r="D7" s="28" t="s">
+    </row>
+    <row r="14" spans="2:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="B14" s="53"/>
+      <c r="C14" s="52"/>
+      <c r="D14" s="30" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="8" spans="2:4" ht="91.5">
-      <c r="B8" s="48"/>
-      <c r="C8" s="47"/>
-      <c r="D8" s="30" t="s">
+    <row r="15" spans="2:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="B15" s="53"/>
+      <c r="C15" s="52"/>
+      <c r="D15" s="30" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="9" spans="2:4" ht="76.5">
-      <c r="B9" s="45" t="s">
+    <row r="16" spans="2:4" ht="60" x14ac:dyDescent="0.25">
+      <c r="B16" s="53"/>
+      <c r="C16" s="52"/>
+      <c r="D16" s="30" t="s">
         <v>127</v>
       </c>
-      <c r="C9" s="43" t="s">
+    </row>
+    <row r="17" spans="2:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="B17" s="50" t="s">
         <v>128</v>
       </c>
-      <c r="D9" s="28" t="s">
+      <c r="C17" s="48" t="s">
         <v>129</v>
       </c>
-    </row>
-    <row r="10" spans="2:4" ht="30.75">
-      <c r="B10" s="46"/>
-      <c r="C10" s="44"/>
-      <c r="D10" s="31" t="s">
+      <c r="D17" s="28" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="11" spans="2:4" ht="76.5" customHeight="1">
-      <c r="B11" s="45" t="s">
+    <row r="18" spans="2:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="B18" s="53"/>
+      <c r="C18" s="52"/>
+      <c r="D18" s="30" t="s">
         <v>131</v>
       </c>
-      <c r="C11" s="43" t="s">
+    </row>
+    <row r="19" spans="2:4" ht="60.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B19" s="50" t="s">
         <v>132</v>
       </c>
-      <c r="D11" s="28" t="s">
+      <c r="C19" s="48" t="s">
         <v>133</v>
       </c>
-    </row>
-    <row r="12" spans="2:4" ht="30.75">
-      <c r="B12" s="48"/>
-      <c r="C12" s="47"/>
-      <c r="D12" s="30" t="s">
+      <c r="D19" s="28" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="13" spans="2:4" ht="45.75">
-      <c r="B13" s="45" t="s">
+    <row r="20" spans="2:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="B20" s="53"/>
+      <c r="C20" s="52"/>
+      <c r="D20" s="30" t="s">
         <v>135</v>
       </c>
-      <c r="C13" s="43" t="s">
+    </row>
+    <row r="21" spans="2:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="B21" s="50" t="s">
         <v>136</v>
       </c>
-      <c r="D13" s="28" t="s">
+      <c r="C21" s="48" t="s">
         <v>137</v>
       </c>
-    </row>
-    <row r="14" spans="2:4" ht="30.75">
-      <c r="B14" s="48"/>
-      <c r="C14" s="47"/>
-      <c r="D14" s="30" t="s">
+      <c r="D21" s="28" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="15" spans="2:4" ht="45.75">
-      <c r="B15" s="48"/>
-      <c r="C15" s="47"/>
-      <c r="D15" s="30" t="s">
+    <row r="22" spans="2:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="B22" s="51"/>
+      <c r="C22" s="49"/>
+      <c r="D22" s="31" t="s">
         <v>139</v>
-      </c>
-    </row>
-    <row r="16" spans="2:4" ht="60.75">
-      <c r="B16" s="48"/>
-      <c r="C16" s="47"/>
-      <c r="D16" s="30" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="17" spans="2:4" ht="45.75">
-      <c r="B17" s="45" t="s">
-        <v>141</v>
-      </c>
-      <c r="C17" s="43" t="s">
-        <v>142</v>
-      </c>
-      <c r="D17" s="28" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="18" spans="2:4" ht="45.75">
-      <c r="B18" s="48"/>
-      <c r="C18" s="47"/>
-      <c r="D18" s="30" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="19" spans="2:4" ht="60.75" customHeight="1">
-      <c r="B19" s="45" t="s">
-        <v>145</v>
-      </c>
-      <c r="C19" s="43" t="s">
-        <v>146</v>
-      </c>
-      <c r="D19" s="28" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="20" spans="2:4" ht="30.75">
-      <c r="B20" s="48"/>
-      <c r="C20" s="47"/>
-      <c r="D20" s="30" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="21" spans="2:4" ht="45.75">
-      <c r="B21" s="45" t="s">
-        <v>149</v>
-      </c>
-      <c r="C21" s="43" t="s">
-        <v>150</v>
-      </c>
-      <c r="D21" s="28" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="22" spans="2:4" ht="30.75">
-      <c r="B22" s="46"/>
-      <c r="C22" s="44"/>
-      <c r="D22" s="31" t="s">
-        <v>152</v>
       </c>
     </row>
   </sheetData>
@@ -6735,7 +6995,7 @@
       <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12.140625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="10.5703125" bestFit="1" customWidth="1"/>
@@ -6745,33 +7005,33 @@
     <col min="11" max="11" width="9.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:19">
-      <c r="A2" s="42" t="s">
-        <v>153</v>
-      </c>
-      <c r="B2" s="42"/>
-      <c r="C2" s="42"/>
-      <c r="F2" s="42" t="s">
-        <v>154</v>
-      </c>
-      <c r="G2" s="42"/>
-      <c r="H2" s="42"/>
-    </row>
-    <row r="3" spans="1:19">
+    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A2" s="47" t="s">
+        <v>140</v>
+      </c>
+      <c r="B2" s="47"/>
+      <c r="C2" s="47"/>
+      <c r="F2" s="47" t="s">
+        <v>141</v>
+      </c>
+      <c r="G2" s="47"/>
+      <c r="H2" s="47"/>
+    </row>
+    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>155</v>
+        <v>142</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>21</v>
       </c>
       <c r="F3" t="s">
-        <v>155</v>
+        <v>142</v>
       </c>
       <c r="G3" s="1" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="4" spans="1:19">
+    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -6787,54 +7047,54 @@
         <v>9500</v>
       </c>
     </row>
-    <row r="5" spans="1:19">
+    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>156</v>
+        <v>143</v>
       </c>
       <c r="B5">
         <f>SUM(C10:C14)</f>
         <v>5000</v>
       </c>
       <c r="F5" t="s">
-        <v>156</v>
+        <v>143</v>
       </c>
       <c r="G5">
         <f>SUM(H10:H14)</f>
         <v>7500</v>
       </c>
     </row>
-    <row r="6" spans="1:19">
+    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>157</v>
+        <v>144</v>
       </c>
       <c r="B6">
         <f>SUM(C17:C19)</f>
         <v>2000</v>
       </c>
       <c r="F6" t="s">
-        <v>157</v>
+        <v>144</v>
       </c>
       <c r="G6">
         <f>SUM(H17:H19)</f>
         <v>2000</v>
       </c>
     </row>
-    <row r="7" spans="1:19">
+    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
       <c r="C7" s="17"/>
       <c r="H7" s="17"/>
     </row>
-    <row r="8" spans="1:19">
+    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
       <c r="C8" s="17"/>
       <c r="H8" s="17"/>
       <c r="Q8" s="3"/>
       <c r="S8" s="3"/>
     </row>
-    <row r="9" spans="1:19">
+    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A9" s="17" t="s">
         <v>2</v>
       </c>
       <c r="B9" s="17" t="s">
-        <v>158</v>
+        <v>145</v>
       </c>
       <c r="C9" s="17" t="s">
         <v>3</v>
@@ -6843,7 +7103,7 @@
         <v>2</v>
       </c>
       <c r="G9" s="17" t="s">
-        <v>158</v>
+        <v>145</v>
       </c>
       <c r="H9" s="17" t="s">
         <v>3</v>
@@ -6860,7 +7120,7 @@
       <c r="R9" s="1"/>
       <c r="S9" s="7"/>
     </row>
-    <row r="10" spans="1:19">
+    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A10" s="17" t="s">
         <v>13</v>
       </c>
@@ -6895,7 +7155,7 @@
       <c r="R10" s="1"/>
       <c r="S10" s="7"/>
     </row>
-    <row r="11" spans="1:19">
+    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A11" s="17" t="s">
         <v>14</v>
       </c>
@@ -6932,7 +7192,7 @@
       <c r="R11" s="1"/>
       <c r="S11" s="7"/>
     </row>
-    <row r="12" spans="1:19">
+    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A12" s="17" t="s">
         <v>15</v>
       </c>
@@ -6969,7 +7229,7 @@
       <c r="R12" s="1"/>
       <c r="S12" s="7"/>
     </row>
-    <row r="13" spans="1:19">
+    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A13" s="17" t="s">
         <v>16</v>
       </c>
@@ -7004,7 +7264,7 @@
       <c r="R13" s="1"/>
       <c r="S13" s="7"/>
     </row>
-    <row r="14" spans="1:19">
+    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A14" s="17" t="s">
         <v>17</v>
       </c>
@@ -7028,27 +7288,27 @@
         <v>5000</v>
       </c>
     </row>
-    <row r="16" spans="1:19">
+    <row r="16" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A16" s="17" t="s">
-        <v>117</v>
+        <v>104</v>
       </c>
       <c r="B16" s="17" t="s">
-        <v>158</v>
+        <v>145</v>
       </c>
       <c r="C16" t="s">
         <v>3</v>
       </c>
       <c r="F16" s="17" t="s">
-        <v>117</v>
+        <v>104</v>
       </c>
       <c r="G16" s="17" t="s">
-        <v>158</v>
+        <v>145</v>
       </c>
       <c r="H16" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="17" spans="1:8">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="17" t="s">
         <v>4</v>
       </c>
@@ -7072,7 +7332,7 @@
         <v>1500</v>
       </c>
     </row>
-    <row r="18" spans="1:8">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" s="17" t="s">
         <v>5</v>
       </c>
@@ -7096,7 +7356,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="19" spans="1:8">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" s="17" t="s">
         <v>6</v>
       </c>

</xml_diff>

<commit_message>
Added some cards and put together a potential deck for research and medic
</commit_message>
<xml_diff>
--- a/ShipCardGameCalcs.xlsx
+++ b/ShipCardGameCalcs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MultiplayerGame\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67DAF753-3355-4F68-B221-8E532364658F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83C7D053-EF0D-456D-AAFD-1BF2AD9DFFB5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="1" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Values" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="398" uniqueCount="190">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="399" uniqueCount="191">
   <si>
     <t>Ship Parameters</t>
   </si>
@@ -650,6 +650,9 @@
   </si>
   <si>
     <t>Crew cards higher than Rank 1 will require at least a sacrifice of a crew card currently in play that you own with a Rank lower than the crew card trying to play</t>
+  </si>
+  <si>
+    <t>You Strategy and card decks can only contain 4 duplicates of any card</t>
   </si>
 </sst>
 </file>
@@ -697,7 +700,7 @@
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
-      <charset val="1"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
@@ -1028,7 +1031,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="55">
+  <cellXfs count="54">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1147,7 +1150,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -3220,7 +3222,7 @@
   <dimension ref="A1:R51"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I10" sqref="I10"/>
+      <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5297,7 +5299,7 @@
   <dimension ref="B1:V29"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+      <selection activeCell="F26" sqref="F26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6273,13 +6275,13 @@
     <row r="16" spans="2:19" x14ac:dyDescent="0.25">
       <c r="P16">
         <f ca="1">RANDBETWEEN(0,123)</f>
-        <v>103</v>
+        <v>65</v>
       </c>
     </row>
     <row r="17" spans="2:16" x14ac:dyDescent="0.25">
       <c r="P17" s="46">
         <f ca="1">RANDBETWEEN(0,6)</f>
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="18" spans="2:16" x14ac:dyDescent="0.25">
@@ -6373,10 +6375,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F5EC53A5-8F19-4711-93EA-0F4CBD261EC8}">
-  <dimension ref="B2:B72"/>
+  <dimension ref="B2:B73"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
-      <selection activeCell="I53" sqref="I53"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="N21" sqref="N21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6429,269 +6431,268 @@
         <v>81</v>
       </c>
     </row>
-    <row r="12" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B12" s="3" t="s">
+    <row r="11" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B11" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="13" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B13" s="3" t="s">
         <v>150</v>
-      </c>
-    </row>
-    <row r="13" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B13" t="s">
-        <v>147</v>
       </c>
     </row>
     <row r="14" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="15" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B15" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="16" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B16" s="3" t="s">
+    <row r="17" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B17" s="3" t="s">
         <v>152</v>
-      </c>
-    </row>
-    <row r="17" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B17" t="s">
-        <v>80</v>
       </c>
     </row>
     <row r="18" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
-        <v>153</v>
+        <v>80</v>
       </c>
     </row>
     <row r="19" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
-        <v>148</v>
+        <v>153</v>
       </c>
     </row>
     <row r="20" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
-        <v>154</v>
+        <v>148</v>
       </c>
     </row>
     <row r="21" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="22" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B22" t="s">
         <v>155</v>
       </c>
     </row>
-    <row r="23" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B23" s="3" t="s">
+    <row r="24" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B24" s="3" t="s">
         <v>156</v>
       </c>
     </row>
-    <row r="24" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B24" t="s">
+    <row r="25" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B25" t="s">
         <v>157</v>
       </c>
     </row>
-    <row r="26" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B26" s="3" t="s">
+    <row r="27" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B27" s="3" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="27" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B27" t="s">
+    <row r="28" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B28" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="28" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B28" s="54" t="s">
+    <row r="29" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B29" t="s">
         <v>167</v>
       </c>
     </row>
-    <row r="29" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B29" s="54"/>
-    </row>
-    <row r="30" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B30" s="3" t="s">
+    <row r="31" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B31" s="3" t="s">
         <v>160</v>
       </c>
     </row>
-    <row r="31" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B31" t="s">
+    <row r="32" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B32" t="s">
         <v>161</v>
       </c>
     </row>
-    <row r="33" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B33" s="3" t="s">
+    <row r="34" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B34" s="3" t="s">
         <v>162</v>
       </c>
     </row>
-    <row r="34" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B34" t="s">
+    <row r="35" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B35" t="s">
         <v>163</v>
       </c>
     </row>
-    <row r="35" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B35" s="54" t="s">
+    <row r="36" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B36" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="36" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B36" s="54"/>
-    </row>
-    <row r="37" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B37" s="3" t="s">
+    <row r="38" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B38" s="3" t="s">
         <v>164</v>
-      </c>
-    </row>
-    <row r="38" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B38" s="54" t="s">
-        <v>166</v>
       </c>
     </row>
     <row r="39" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B39" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
     </row>
     <row r="40" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B40" t="s">
-        <v>82</v>
+        <v>168</v>
       </c>
     </row>
     <row r="41" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B41" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="42" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B42" t="s">
-        <v>181</v>
+        <v>83</v>
       </c>
     </row>
     <row r="43" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B43" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="44" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B44" t="s">
-        <v>89</v>
+        <v>182</v>
       </c>
     </row>
     <row r="45" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B45" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="46" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B46" t="s">
-        <v>183</v>
+        <v>90</v>
       </c>
     </row>
     <row r="47" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B47" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="48" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B48" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="49" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B49" t="s">
         <v>186</v>
       </c>
     </row>
-    <row r="50" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B50" s="3" t="s">
+    <row r="51" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B51" s="3" t="s">
         <v>173</v>
-      </c>
-    </row>
-    <row r="51" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B51" t="s">
-        <v>174</v>
       </c>
     </row>
     <row r="52" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B52" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="53" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B53" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
     </row>
     <row r="54" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B54" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
     </row>
     <row r="55" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B55" t="s">
-        <v>185</v>
+        <v>176</v>
       </c>
     </row>
     <row r="56" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B56" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
     </row>
     <row r="57" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B57" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
     </row>
     <row r="58" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B58" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="59" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B59" t="s">
         <v>188</v>
       </c>
     </row>
-    <row r="60" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B60" s="3" t="s">
+    <row r="61" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B61" s="3" t="s">
         <v>170</v>
-      </c>
-    </row>
-    <row r="61" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B61" t="s">
-        <v>84</v>
       </c>
     </row>
     <row r="62" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B62" t="s">
-        <v>169</v>
+        <v>84</v>
       </c>
     </row>
     <row r="63" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B63" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="64" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B64" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="65" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B65" s="3" t="s">
+    <row r="66" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B66" s="3" t="s">
         <v>171</v>
-      </c>
-    </row>
-    <row r="66" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B66" t="s">
-        <v>172</v>
       </c>
     </row>
     <row r="67" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B67" t="s">
-        <v>86</v>
+        <v>172</v>
       </c>
     </row>
     <row r="68" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B68" t="s">
-        <v>178</v>
+        <v>86</v>
       </c>
     </row>
     <row r="69" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B69" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="70" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B70" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="71" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B71" t="s">
-        <v>87</v>
+        <v>180</v>
       </c>
     </row>
     <row r="72" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B72" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="73" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B73" t="s">
         <v>88</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Added assault engineer deck list and tweaked card designs
</commit_message>
<xml_diff>
--- a/ShipCardGameCalcs.xlsx
+++ b/ShipCardGameCalcs.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26324"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MultiplayerGame\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83C7D053-EF0D-456D-AAFD-1BF2AD9DFFB5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{4CAF5471-AA79-41FB-8CC4-B0B4A5BB074C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="3" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Values" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="399" uniqueCount="191">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="402" uniqueCount="194">
   <si>
     <t>Ship Parameters</t>
   </si>
@@ -307,6 +307,9 @@
     <t>Game Rules</t>
   </si>
   <si>
+    <t>Pre Game Rules:</t>
+  </si>
+  <si>
     <t>When picking ships at start of turn player must have at least 1 ship that can have a Captain and players picked ships must equal the ship total game points</t>
   </si>
   <si>
@@ -322,10 +325,82 @@
     <t>A player gets 1 free mulligan but if they choose to mulligan anymore times than that they reduce the amount of cards drawn from strategy deck by 1 each time. Down to a minimum of 1 card from their strategy deck and 2 from their leader deck</t>
   </si>
   <si>
+    <t>A crew /leader deck can only contain cards of Type Captain, Leuitenant and Crew</t>
+  </si>
+  <si>
+    <t>The strategy deck has every other card</t>
+  </si>
+  <si>
+    <t>You Strategy and card decks can only contain 4 duplicates of any card</t>
+  </si>
+  <si>
+    <t>First Turn Rules:</t>
+  </si>
+  <si>
+    <t>Pick a random Player to go first, since they started they don't draw a card from either the crew or strategy decks at the start of turn.</t>
+  </si>
+  <si>
+    <t>After the first player, Players can draw either 1 card from the strategy deck, or they can choose the see the top 3 cards of the crew deck and then get to pick 1. The rest get sent to the bottom of the crew deck.</t>
+  </si>
+  <si>
+    <t>In Game Rules</t>
+  </si>
+  <si>
     <t>Max player hand size is 8 (unless card in play says otherwise)</t>
   </si>
   <si>
-    <t>The strategy deck has every other card</t>
+    <t>A player can only place Crew cards to their ship with an available crew slot unless stated otherwise</t>
+  </si>
+  <si>
+    <t>A crew member first placed on to a ship can't be used in a gun slot, however they can be used to tap for anything else</t>
+  </si>
+  <si>
+    <t>A player can only play 1 crew member and 1 Captain/Leuitenant per their turn</t>
+  </si>
+  <si>
+    <t>Each players turn consist of the following phases</t>
+  </si>
+  <si>
+    <t>Untap Phase</t>
+  </si>
+  <si>
+    <t>This is where the player untaps all their cards unless stated otherwise</t>
+  </si>
+  <si>
+    <t>Any of your ships shield damaged, restore 100 shield</t>
+  </si>
+  <si>
+    <t>Draw Phase</t>
+  </si>
+  <si>
+    <t>This is where the player chooses to draw from their Strategy or Crew Deck</t>
+  </si>
+  <si>
+    <t>Players can draw either 1 card from the strategy deck, or they can choose the see the top 3 cards of the crew deck and then get to pick 1. The rest get sent to the bottom of the crew deck.</t>
+  </si>
+  <si>
+    <t>Strategy Phase</t>
+  </si>
+  <si>
+    <t>This is where the player can play their cards, tap to gain department resourse or tap cards to use gun slots</t>
+  </si>
+  <si>
+    <t>End Phase</t>
+  </si>
+  <si>
+    <t>At this phase if the player has cards greater than their max hand size then they must discard back down to that size</t>
+  </si>
+  <si>
+    <t>Any department resource not used does NOT get transferred to later turns</t>
+  </si>
+  <si>
+    <t>In Game Rules Continued</t>
+  </si>
+  <si>
+    <t>During the phases players can activate certain types of cards on other players turns</t>
+  </si>
+  <si>
+    <t>A ship can only hold x amount of crew members where x is equal to the ships crew slots</t>
   </si>
   <si>
     <t>A ship can only hold x amount of Captains where x is equal to ships Captains slots</t>
@@ -334,27 +409,96 @@
     <t>A ship can only hold x amount of Leuitenant where x is equal to ships Leuitenant slots</t>
   </si>
   <si>
+    <t>If player wants to draw from crew/leader deck and there are no cards left in players crew/leader deck then shuffle the crew/leader cards from stasis back to that deck spot and draw</t>
+  </si>
+  <si>
+    <t>If there are less than 3 cards in the crew/eader deck then they draw the rest of the deck, shuffle the stasis pile back to the deck position and draw up to the 3 cards. Then continue process of picking 1 card and putting rest to the stasis pile</t>
+  </si>
+  <si>
+    <t>If there are no cards left in the strategy deck during the draw phase that player loses and is out of the game</t>
+  </si>
+  <si>
+    <t>A player can only have 1 admiral card in play on their side of the battlefield</t>
+  </si>
+  <si>
+    <t>When a strategy card has been played and doesn’t stay on the field, then that card gets sent to the junkyard</t>
+  </si>
+  <si>
+    <t>Cards in the Junkyard can't be played unless stated otherwise</t>
+  </si>
+  <si>
+    <t>Crew cards in the stasis pile can't be played unless stated otherwise</t>
+  </si>
+  <si>
+    <t>Crew Cards</t>
+  </si>
+  <si>
+    <t>A Crew Card can have various tap abilities, the standard abilities they get are as follows unless stated otherwise:</t>
+  </si>
+  <si>
+    <t>Crew can tap to provide department resource</t>
+  </si>
+  <si>
+    <t>Crew can tap to use a gun slot on assigned ship</t>
+  </si>
+  <si>
+    <t>Crew can tap to move from one ship to another ship the player owns</t>
+  </si>
+  <si>
+    <t>When a crew card is destroyed send it to the stasis pile</t>
+  </si>
+  <si>
+    <t>A rank 1 crew card can be played for free</t>
+  </si>
+  <si>
+    <t>Crew cards higher than Rank 1 will require at least a sacrifice of a crew card currently in play that you own with a Rank lower than the crew card trying to play</t>
+  </si>
+  <si>
+    <t>Captain and Leuitenant cards cost department resource to play</t>
+  </si>
+  <si>
+    <t>Gun Slots/Attacking Player Ships</t>
+  </si>
+  <si>
     <t>A crew type card has a 1 to 1 relationship when being tapped to a gun slot. Meaning you can't tap more than 1 crew card type to the same gun slot on the same turn.</t>
   </si>
   <si>
+    <t>Some cards might allow a crew card to tap more than one gun slot</t>
+  </si>
+  <si>
     <t>When crew type card is being used to a gun slot, it will deal damage to the players ship shield, if the players ship shield is at 0 or deactivated then it will deal damage to the players ship hull</t>
   </si>
   <si>
+    <t>Taking Damage</t>
+  </si>
+  <si>
+    <t>When a ship takes hull damage, sacrifice 1 crew member from ship. Only do this once per strategy phase</t>
+  </si>
+  <si>
+    <t>Ship Destroyed</t>
+  </si>
+  <si>
+    <t>Once a players ship hull reaches 0 it is destroyed</t>
+  </si>
+  <si>
     <t>Once a players ship is destroyed remove the ship card from play</t>
   </si>
   <si>
+    <t>All ship upgrades attached to destroyed ship are sent to the junkyard</t>
+  </si>
+  <si>
+    <t>Each ship will have had assigned amount of escape pods. The player owning the destroyed ship may pick to move that amount of crew with their attachments from the destroyed ship to another ship they own</t>
+  </si>
+  <si>
+    <t>The rest of the crew and crew attachment cards are sent to stasis and the junkyard</t>
+  </si>
+  <si>
     <t>Once all of a players ship is destroyed they lose and are out of the game</t>
   </si>
   <si>
     <t>When only 1 player remains in the game they win</t>
   </si>
   <si>
-    <t>If there are no cards left in the strategy deck during the draw phase that player loses and is out of the game</t>
-  </si>
-  <si>
-    <t>A player can only have 1 admiral card in play on their side of the battlefield</t>
-  </si>
-  <si>
     <t>Controlled deck is the battlefield conditions which affects the battlefield</t>
   </si>
   <si>
@@ -518,148 +662,13 @@
   </si>
   <si>
     <t>No. of</t>
-  </si>
-  <si>
-    <t>Pre Game Rules:</t>
-  </si>
-  <si>
-    <t>Pick a random Player to go first, since they started they don't draw a card from either the crew or strategy decks at the start of turn.</t>
-  </si>
-  <si>
-    <t>A crew member first placed on to a ship can't be used in a gun slot, however they can be used to tap for anything else</t>
-  </si>
-  <si>
-    <t>A crew /leader deck can only contain cards of Type Captain, Leuitenant and Crew</t>
-  </si>
-  <si>
-    <t>First Turn Rules:</t>
-  </si>
-  <si>
-    <t>After the first player, Players can draw either 1 card from the strategy deck, or they can choose the see the top 3 cards of the crew deck and then get to pick 1. The rest get sent to the bottom of the crew deck.</t>
-  </si>
-  <si>
-    <t>In Game Rules</t>
-  </si>
-  <si>
-    <t>A player can only place Crew cards to their ship with an available crew slot unless stated otherwise</t>
-  </si>
-  <si>
-    <t>A player can only play 1 crew member and 1 Captain/Leuitenant per their turn</t>
-  </si>
-  <si>
-    <t>Each players turn consist of the following phases</t>
-  </si>
-  <si>
-    <t>Untap Phase</t>
-  </si>
-  <si>
-    <t>This is where the player untaps all their cards unless stated otherwise</t>
-  </si>
-  <si>
-    <t>Draw Phase</t>
-  </si>
-  <si>
-    <t>This is where the player chooses to draw from their Strategy or Crew Deck</t>
-  </si>
-  <si>
-    <t>Strategy Phase</t>
-  </si>
-  <si>
-    <t>This is where the player can play their cards, tap to gain department resourse or tap cards to use gun slots</t>
-  </si>
-  <si>
-    <t>End Phase</t>
-  </si>
-  <si>
-    <t>At this phase if the player has cards greater than their max hand size then they must discard back down to that size</t>
-  </si>
-  <si>
-    <t>In Game Rules Continued</t>
-  </si>
-  <si>
-    <t>Any department resource not used does NOT get transferred to later turns</t>
-  </si>
-  <si>
-    <t>During the phases players can activate certain types of cards on other players turns</t>
-  </si>
-  <si>
-    <t>Players can draw either 1 card from the strategy deck, or they can choose the see the top 3 cards of the crew deck and then get to pick 1. The rest get sent to the bottom of the crew deck.</t>
-  </si>
-  <si>
-    <t>A ship can only hold x amount of crew members where x is equal to the ships crew slots</t>
-  </si>
-  <si>
-    <t>Some cards might allow a crew card to tap more than one gun slot</t>
-  </si>
-  <si>
-    <t>Gun Slots/Attacking Player Ships</t>
-  </si>
-  <si>
-    <t>Ship Destroyed</t>
-  </si>
-  <si>
-    <t>Once a players ship hull reaches 0 it is destroyed</t>
-  </si>
-  <si>
-    <t>Crew Cards</t>
-  </si>
-  <si>
-    <t>A Crew Card can have various tap abilities, the standard abilities they get are as follows unless stated otherwise:</t>
-  </si>
-  <si>
-    <t>Crew can tap to provide department resource</t>
-  </si>
-  <si>
-    <t>Crew can tap to move from one ship to another ship the player owns</t>
-  </si>
-  <si>
-    <t>Crew can tap to use a gun slot on assigned ship</t>
-  </si>
-  <si>
-    <t>All ship upgrades attached to destroyed ship are sent to the junkyard</t>
-  </si>
-  <si>
-    <t>Each ship will have had assigned amount of escape pods. The player owning the destroyed ship may pick to move that amount of crew with their attachments from the destroyed ship to another ship they own</t>
-  </si>
-  <si>
-    <t>The rest of the crew and crew attachment cards are sent to stasis and the junkyard</t>
-  </si>
-  <si>
-    <t>If player wants to draw from crew/leader deck and there are no cards left in players crew/leader deck then shuffle the crew/leader cards from stasis back to that deck spot and draw</t>
-  </si>
-  <si>
-    <t>If there are less than 3 cards in the crew/eader deck then they draw the rest of the deck, shuffle the stasis pile back to the deck position and draw up to the 3 cards. Then continue process of picking 1 card and putting rest to the stasis pile</t>
-  </si>
-  <si>
-    <t>When a strategy card has been played and doesn’t stay on the field, then that card gets sent to the junkyard</t>
-  </si>
-  <si>
-    <t>Cards in the Junkyard can't be played unless stated otherwise</t>
-  </si>
-  <si>
-    <t>When a crew card is destroyed send it to the stasis pile</t>
-  </si>
-  <si>
-    <t>Crew cards in the stasis pile can't be played unless stated otherwise</t>
-  </si>
-  <si>
-    <t>A rank 1 crew card can be played for free</t>
-  </si>
-  <si>
-    <t>Captain and Leuitenant cards cost department resource to play</t>
-  </si>
-  <si>
-    <t>Crew cards higher than Rank 1 will require at least a sacrifice of a crew card currently in play that you own with a Rank lower than the crew card trying to play</t>
-  </si>
-  <si>
-    <t>You Strategy and card decks can only contain 4 duplicates of any card</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="8">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1031,7 +1040,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="54">
+  <cellXfs count="55">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1150,6 +1159,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1158,6 +1168,14 @@
     <dxf>
       <fill>
         <patternFill patternType="none">
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
           <fgColor indexed="64"/>
           <bgColor indexed="65"/>
         </patternFill>
@@ -1252,23 +1270,15 @@
     <dxf>
       <fill>
         <patternFill patternType="none">
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
     </dxf>
     <dxf>
       <fill>
         <patternFill patternType="none">
           <fgColor indexed="64"/>
           <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <bgColor auto="1"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1380,6 +1390,13 @@
     </dxf>
     <dxf>
       <border outline="0">
+        <bottom style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
         <left style="thin">
           <color theme="4" tint="0.39997558519241921"/>
         </left>
@@ -1398,13 +1415,6 @@
           <bgColor indexed="65"/>
         </patternFill>
       </fill>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <bottom style="thin">
-          <color theme="4" tint="0.39997558519241921"/>
-        </bottom>
-      </border>
     </dxf>
     <dxf>
       <font>
@@ -1720,6 +1730,13 @@
     </dxf>
     <dxf>
       <border outline="0">
+        <bottom style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
         <left style="thin">
           <color theme="4" tint="0.39997558519241921"/>
         </left>
@@ -1756,13 +1773,6 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <border outline="0">
-        <bottom style="thin">
-          <color theme="4" tint="0.39997558519241921"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
       <font>
         <b/>
         <i val="0"/>
@@ -1813,6 +1823,9 @@
       </border>
     </dxf>
     <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0" outline="0">
         <left/>
@@ -1834,6 +1847,7 @@
       </border>
     </dxf>
     <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -1844,10 +1858,6 @@
         <top/>
         <bottom/>
       </border>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <border diagonalUp="0" diagonalDown="0" outline="0">
@@ -1892,9 +1902,6 @@
       </border>
     </dxf>
     <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
@@ -1938,6 +1945,9 @@
     </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -2010,9 +2020,6 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -2027,6 +2034,9 @@
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -2063,6 +2073,7 @@
       </border>
     </dxf>
     <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
       <fill>
         <patternFill patternType="none">
           <fgColor indexed="64"/>
@@ -2072,6 +2083,15 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
       <fill>
         <patternFill patternType="none">
@@ -2184,24 +2204,6 @@
         </patternFill>
       </fill>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
     </dxf>
     <dxf>
       <font>
@@ -2229,6 +2231,14 @@
     <dxf>
       <fill>
         <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
           <bgColor auto="1"/>
         </patternFill>
       </fill>
@@ -2333,6 +2343,14 @@
     <dxf>
       <fill>
         <patternFill patternType="none">
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
           <fgColor indexed="64"/>
           <bgColor indexed="65"/>
         </patternFill>
@@ -2425,6 +2443,7 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
       <fill>
         <patternFill patternType="none">
           <bgColor indexed="65"/>
@@ -2442,26 +2461,17 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill patternType="none">
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
     </dxf>
     <dxf>
       <fill>
         <patternFill patternType="none">
           <fgColor indexed="64"/>
           <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <bgColor auto="1"/>
         </patternFill>
       </fill>
     </dxf>
@@ -2505,6 +2515,15 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -2566,15 +2585,6 @@
     </dxf>
     <dxf>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <fill>
@@ -2710,12 +2720,12 @@
   <autoFilter ref="A9:G14" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="7">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Option" totalsRowLabel="Total" dataDxfId="129"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="A" totalsRowFunction="sum" dataDxfId="128" totalsRowDxfId="127"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="B" totalsRowFunction="sum" dataDxfId="126" totalsRowDxfId="125"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="C" totalsRowFunction="sum" dataDxfId="124" totalsRowDxfId="123"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="D" totalsRowFunction="sum" dataDxfId="122" totalsRowDxfId="121"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="E" totalsRowFunction="sum" dataDxfId="120" totalsRowDxfId="119"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="F" totalsRowFunction="sum" dataDxfId="118" totalsRowDxfId="117"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="A" totalsRowFunction="sum" dataDxfId="127" totalsRowDxfId="128"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="B" totalsRowFunction="sum" dataDxfId="125" totalsRowDxfId="126"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="C" totalsRowFunction="sum" dataDxfId="123" totalsRowDxfId="124"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="D" totalsRowFunction="sum" dataDxfId="121" totalsRowDxfId="122"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="E" totalsRowFunction="sum" dataDxfId="119" totalsRowDxfId="120"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="F" totalsRowFunction="sum" dataDxfId="117" totalsRowDxfId="118"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium15" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2725,23 +2735,23 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="14" xr:uid="{00000000-000C-0000-FFFF-FFFF09000000}" name="TblFltCrewSizes" displayName="TblFltCrewSizes" ref="A17:G21" totalsRowCount="1" headerRowDxfId="15" dataDxfId="14">
   <autoFilter ref="A17:G20" xr:uid="{00000000-0009-0000-0100-00000E000000}"/>
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0900-000001000000}" name="Option" totalsRowLabel="Total" dataDxfId="13" totalsRowDxfId="12"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0900-000002000000}" name="A" totalsRowFunction="custom" dataDxfId="11" totalsRowDxfId="10">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0900-000001000000}" name="Option" totalsRowLabel="Total" dataDxfId="12" totalsRowDxfId="13"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0900-000002000000}" name="A" totalsRowFunction="custom" dataDxfId="10" totalsRowDxfId="11">
       <totalsRowFormula>SUBTOTAL(109,TblFltCrewSizes[A])</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0900-000003000000}" name="B" totalsRowFunction="custom" dataDxfId="9" totalsRowDxfId="8">
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0900-000003000000}" name="B" totalsRowFunction="custom" dataDxfId="8" totalsRowDxfId="9">
       <totalsRowFormula>SUBTOTAL(109,TblFltCrewSizes[B])</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0900-000004000000}" name="C" totalsRowFunction="custom" dataDxfId="7" totalsRowDxfId="6">
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0900-000004000000}" name="C" totalsRowFunction="custom" dataDxfId="6" totalsRowDxfId="7">
       <totalsRowFormula>SUBTOTAL(109,TblFltCrewSizes[C])</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0900-000005000000}" name="D" totalsRowFunction="custom" dataDxfId="5" totalsRowDxfId="4">
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0900-000005000000}" name="D" totalsRowFunction="custom" dataDxfId="4" totalsRowDxfId="5">
       <totalsRowFormula>SUBTOTAL(109,TblFltCrewSizes[D])</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0900-000006000000}" name="E" totalsRowFunction="custom" dataDxfId="3" totalsRowDxfId="2">
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0900-000006000000}" name="E" totalsRowFunction="custom" dataDxfId="2" totalsRowDxfId="3">
       <totalsRowFormula>SUBTOTAL(109,TblFltCrewSizes[E])</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0900-000007000000}" name="F" totalsRowFunction="sum" dataDxfId="1" totalsRowDxfId="0"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0900-000007000000}" name="F" totalsRowFunction="sum" dataDxfId="0" totalsRowDxfId="1"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium13" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2751,26 +2761,26 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="TblFleetShipValues" displayName="TblFleetShipValues" ref="J9:Q15" totalsRowCount="1" headerRowDxfId="116" dataDxfId="115" totalsRowDxfId="114">
   <autoFilter ref="J9:Q14" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
   <tableColumns count="8">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="Option" totalsRowLabel="Total " dataDxfId="113" totalsRowDxfId="112"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="A" totalsRowFunction="sum" dataDxfId="111" totalsRowDxfId="110">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="Option" totalsRowLabel="Total " dataDxfId="112" totalsRowDxfId="113"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="A" totalsRowFunction="sum" dataDxfId="110" totalsRowDxfId="111">
       <calculatedColumnFormula>(INDEX(TblBattlefieldFlt[[A]:[F]],MATCH(TblFleetShipValues[[#This Row],[Option]],TblBattlefieldFlt[Option],0),MATCH(TblFleetShipValues[[#Headers],[A]],TblBattlefieldFlt[[#Headers],[A]:[F]],0)))*(INDEX(TblShipPoints[Points],MATCH(TblFleetShipValues[[#This Row],[Option]],TblShipPoints[Ships],0)))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0100-000003000000}" name="B" totalsRowFunction="sum" dataDxfId="109" totalsRowDxfId="108">
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0100-000003000000}" name="B" totalsRowFunction="sum" dataDxfId="108" totalsRowDxfId="109">
       <calculatedColumnFormula>C10*#REF!</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0100-000004000000}" name="C" totalsRowFunction="sum" dataDxfId="107" totalsRowDxfId="106">
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0100-000004000000}" name="C" totalsRowFunction="sum" dataDxfId="106" totalsRowDxfId="107">
       <calculatedColumnFormula>D10*#REF!</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0100-000005000000}" name="D" totalsRowFunction="sum" dataDxfId="105" totalsRowDxfId="104">
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0100-000005000000}" name="D" totalsRowFunction="sum" dataDxfId="104" totalsRowDxfId="105">
       <calculatedColumnFormula>E10*#REF!</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0100-000006000000}" name="E" totalsRowFunction="sum" dataDxfId="103" totalsRowDxfId="102">
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0100-000006000000}" name="E" totalsRowFunction="sum" dataDxfId="102" totalsRowDxfId="103">
       <calculatedColumnFormula>F10*#REF!</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0100-000007000000}" name="F" totalsRowFunction="sum" dataDxfId="101" totalsRowDxfId="100">
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0100-000007000000}" name="F" totalsRowFunction="sum" dataDxfId="100" totalsRowDxfId="101">
       <calculatedColumnFormula>G10*#REF!</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0100-000008000000}" name="Name" dataDxfId="99" totalsRowDxfId="98"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0100-000008000000}" name="Name" dataDxfId="98" totalsRowDxfId="99"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium13" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2793,26 +2803,26 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{00000000-000C-0000-FFFF-FFFF03000000}" name="TblAdjFleetRolesValues" displayName="TblAdjFleetRolesValues" ref="A24:H30" totalsRowCount="1" headerRowDxfId="91" dataDxfId="90" totalsRowDxfId="89">
   <autoFilter ref="A24:H29" xr:uid="{00000000-0009-0000-0100-000006000000}"/>
   <tableColumns count="8">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0300-000001000000}" name="Option" totalsRowLabel="Total" dataDxfId="88" totalsRowDxfId="87"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0300-000002000000}" name="A" totalsRowFunction="sum" dataDxfId="86" totalsRowDxfId="85">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0300-000001000000}" name="Option" totalsRowLabel="Total" dataDxfId="87" totalsRowDxfId="88"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0300-000002000000}" name="A" totalsRowFunction="sum" dataDxfId="85" totalsRowDxfId="86">
       <calculatedColumnFormula>(INDEX(TblBattlefieldFlt[[A]:[F]],MATCH($A25,TblBattlefieldFlt[Option],0),MATCH(B$24,TblBattlefieldFlt[[#Headers],[A]:[F]],0)))*(INDEX(TblShipCrew[Adjusted],MATCH($A25,TblShipCrew[Ships],0)))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0300-000003000000}" name="B" totalsRowFunction="sum" dataDxfId="84" totalsRowDxfId="83">
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0300-000003000000}" name="B" totalsRowFunction="sum" dataDxfId="83" totalsRowDxfId="84">
       <calculatedColumnFormula>(INDEX(TblBattlefieldFlt[[A]:[F]],MATCH($A25,TblBattlefieldFlt[Option],0),MATCH(C$24,TblBattlefieldFlt[[#Headers],[A]:[F]],0)))*(INDEX(TblShipCrew[Adjusted],MATCH($A25,TblShipCrew[Ships],0)))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0300-000004000000}" name="C" totalsRowFunction="sum" dataDxfId="82" totalsRowDxfId="81">
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0300-000004000000}" name="C" totalsRowFunction="sum" dataDxfId="81" totalsRowDxfId="82">
       <calculatedColumnFormula>(INDEX(TblBattlefieldFlt[[A]:[F]],MATCH($A25,TblBattlefieldFlt[Option],0),MATCH(D$24,TblBattlefieldFlt[[#Headers],[A]:[F]],0)))*(INDEX(TblShipCrew[Adjusted],MATCH($A25,TblShipCrew[Ships],0)))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0300-000005000000}" name="D" totalsRowFunction="sum" dataDxfId="80" totalsRowDxfId="79">
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0300-000005000000}" name="D" totalsRowFunction="sum" dataDxfId="79" totalsRowDxfId="80">
       <calculatedColumnFormula>(INDEX(TblBattlefieldFlt[[A]:[F]],MATCH($A25,TblBattlefieldFlt[Option],0),MATCH(E$24,TblBattlefieldFlt[[#Headers],[A]:[F]],0)))*(INDEX(TblShipCrew[Adjusted],MATCH($A25,TblShipCrew[Ships],0)))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0300-000006000000}" name="E" totalsRowFunction="sum" dataDxfId="78" totalsRowDxfId="77">
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0300-000006000000}" name="E" totalsRowFunction="sum" dataDxfId="77" totalsRowDxfId="78">
       <calculatedColumnFormula>(INDEX(TblBattlefieldFlt[[A]:[F]],MATCH($A25,TblBattlefieldFlt[Option],0),MATCH(F$24,TblBattlefieldFlt[[#Headers],[A]:[F]],0)))*(INDEX(TblShipCrew[Adjusted],MATCH($A25,TblShipCrew[Ships],0)))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0300-000007000000}" name="F" totalsRowFunction="sum" dataDxfId="76" totalsRowDxfId="75">
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0300-000007000000}" name="F" totalsRowFunction="sum" dataDxfId="75" totalsRowDxfId="76">
       <calculatedColumnFormula>(INDEX(TblBattlefieldFlt[[A]:[F]],MATCH($A25,TblBattlefieldFlt[Option],0),MATCH(G$24,TblBattlefieldFlt[[#Headers],[A]:[F]],0)))*(INDEX(TblShipCrew[Adjusted],MATCH($A25,TblShipCrew[Ships],0)))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0300-000008000000}" name="Name" dataDxfId="74" totalsRowDxfId="73"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0300-000008000000}" name="Name" dataDxfId="73" totalsRowDxfId="74"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium13" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2823,11 +2833,11 @@
   <autoFilter ref="A32:G42" xr:uid="{00000000-0009-0000-0100-000008000000}"/>
   <tableColumns count="7">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0400-000001000000}" name="Option" totalsRowLabel="Total"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0400-000002000000}" name="A" totalsRowFunction="sum" dataDxfId="71" totalsRowDxfId="70">
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0400-000002000000}" name="A" totalsRowFunction="sum" dataDxfId="70" totalsRowDxfId="71">
       <calculatedColumnFormula>K10</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0400-000003000000}" name="B" totalsRowFunction="sum" dataDxfId="69" totalsRowDxfId="68"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0400-000004000000}" name="C" totalsRowFunction="sum" dataDxfId="67" totalsRowDxfId="66"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0400-000003000000}" name="B" totalsRowFunction="sum" dataDxfId="68" totalsRowDxfId="69"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0400-000004000000}" name="C" totalsRowFunction="sum" dataDxfId="66" totalsRowDxfId="67"/>
     <tableColumn id="5" xr3:uid="{00000000-0010-0000-0400-000005000000}" name="D" totalsRowFunction="sum" totalsRowDxfId="65"/>
     <tableColumn id="6" xr3:uid="{00000000-0010-0000-0400-000006000000}" name="E" totalsRowFunction="sum" totalsRowDxfId="64"/>
     <tableColumn id="7" xr3:uid="{00000000-0010-0000-0400-000007000000}" name="F" totalsRowFunction="sum" totalsRowDxfId="63"/>
@@ -2841,25 +2851,25 @@
   <autoFilter ref="J24:Q29" xr:uid="{00000000-0009-0000-0100-000009000000}"/>
   <tableColumns count="8">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0500-000001000000}" name="Option" totalsRowLabel="Total" dataDxfId="60"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0500-000002000000}" name="A" totalsRowFunction="sum" dataDxfId="59" totalsRowDxfId="58">
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0500-000002000000}" name="A" totalsRowFunction="sum" dataDxfId="58" totalsRowDxfId="59">
       <calculatedColumnFormula>(INDEX(TblBattlefieldFlt[[A]:[F]],MATCH($J25,TblBattlefieldFlt[Option],0),MATCH(K$24,TblBattlefieldFlt[[#Headers],[A]:[F]],0)))*(INDEX(TblShipCrew[Generic (500)],MATCH($J25,TblShipCrew[Ships],0)))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0500-000003000000}" name="B" totalsRowFunction="sum" dataDxfId="57" totalsRowDxfId="56">
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0500-000003000000}" name="B" totalsRowFunction="sum" dataDxfId="56" totalsRowDxfId="57">
       <calculatedColumnFormula>(INDEX(TblBattlefieldFlt[[A]:[F]],MATCH($J25,TblBattlefieldFlt[Option],0),MATCH(L$24,TblBattlefieldFlt[[#Headers],[A]:[F]],0)))*(INDEX(TblShipCrew[Generic (500)],MATCH($J25,TblShipCrew[Ships],0)))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0500-000004000000}" name="C" totalsRowFunction="sum" dataDxfId="55" totalsRowDxfId="54">
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0500-000004000000}" name="C" totalsRowFunction="sum" dataDxfId="54" totalsRowDxfId="55">
       <calculatedColumnFormula>(INDEX(TblBattlefieldFlt[[A]:[F]],MATCH($J25,TblBattlefieldFlt[Option],0),MATCH(M$24,TblBattlefieldFlt[[#Headers],[A]:[F]],0)))*(INDEX(TblShipCrew[Generic (500)],MATCH($J25,TblShipCrew[Ships],0)))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0500-000005000000}" name="D" totalsRowFunction="sum" dataDxfId="53" totalsRowDxfId="52">
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0500-000005000000}" name="D" totalsRowFunction="sum" dataDxfId="52" totalsRowDxfId="53">
       <calculatedColumnFormula>(INDEX(TblBattlefieldFlt[[A]:[F]],MATCH($J25,TblBattlefieldFlt[Option],0),MATCH(N$24,TblBattlefieldFlt[[#Headers],[A]:[F]],0)))*(INDEX(TblShipCrew[Generic (500)],MATCH($J25,TblShipCrew[Ships],0)))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0500-000006000000}" name="E" totalsRowFunction="sum" dataDxfId="51" totalsRowDxfId="50">
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0500-000006000000}" name="E" totalsRowFunction="sum" dataDxfId="50" totalsRowDxfId="51">
       <calculatedColumnFormula>(INDEX(TblBattlefieldFlt[[A]:[F]],MATCH($J25,TblBattlefieldFlt[Option],0),MATCH(O$24,TblBattlefieldFlt[[#Headers],[A]:[F]],0)))*(INDEX(TblShipCrew[Generic (500)],MATCH($J25,TblShipCrew[Ships],0)))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0500-000007000000}" name="F" totalsRowFunction="sum" dataDxfId="49" totalsRowDxfId="48">
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0500-000007000000}" name="F" totalsRowFunction="sum" dataDxfId="48" totalsRowDxfId="49">
       <calculatedColumnFormula>(INDEX(TblBattlefieldFlt[[A]:[F]],MATCH($J25,TblBattlefieldFlt[Option],0),MATCH(P$24,TblBattlefieldFlt[[#Headers],[A]:[F]],0)))*(INDEX(TblShipCrew[Generic (500)],MATCH($J25,TblShipCrew[Ships],0)))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0500-000008000000}" name="Name" dataDxfId="47" totalsRowDxfId="46"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0500-000008000000}" name="Name" dataDxfId="46" totalsRowDxfId="47"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium10" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2870,11 +2880,11 @@
   <autoFilter ref="J32:P42" xr:uid="{00000000-0009-0000-0100-00000A000000}"/>
   <tableColumns count="7">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0600-000001000000}" name="Option" totalsRowLabel="Total" totalsRowDxfId="44"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0600-000002000000}" name="A" totalsRowFunction="sum" dataDxfId="43" totalsRowDxfId="42">
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0600-000002000000}" name="A" totalsRowFunction="sum" dataDxfId="42" totalsRowDxfId="43">
       <calculatedColumnFormula>T10</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0600-000003000000}" name="B" totalsRowFunction="sum" dataDxfId="41" totalsRowDxfId="40"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0600-000004000000}" name="C" totalsRowFunction="sum" dataDxfId="39" totalsRowDxfId="38"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0600-000003000000}" name="B" totalsRowFunction="sum" dataDxfId="40" totalsRowDxfId="41"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0600-000004000000}" name="C" totalsRowFunction="sum" dataDxfId="38" totalsRowDxfId="39"/>
     <tableColumn id="5" xr3:uid="{00000000-0010-0000-0600-000005000000}" name="D" totalsRowFunction="sum" totalsRowDxfId="37"/>
     <tableColumn id="6" xr3:uid="{00000000-0010-0000-0600-000006000000}" name="E" totalsRowFunction="sum" totalsRowDxfId="36"/>
     <tableColumn id="7" xr3:uid="{00000000-0010-0000-0600-000007000000}" name="F" totalsRowFunction="sum" totalsRowDxfId="35"/>
@@ -2884,7 +2894,7 @@
 </file>
 
 <file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="13" xr:uid="{00000000-000C-0000-FFFF-FFFF07000000}" name="TblShipCrew" displayName="TblShipCrew" ref="D2:L7" totalsRowShown="0" headerRowDxfId="34" dataDxfId="32" headerRowBorderDxfId="33" tableBorderDxfId="31">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="13" xr:uid="{00000000-000C-0000-FFFF-FFFF07000000}" name="TblShipCrew" displayName="TblShipCrew" ref="D2:L7" totalsRowShown="0" headerRowDxfId="34" dataDxfId="33" headerRowBorderDxfId="31" tableBorderDxfId="32">
   <autoFilter ref="D2:L7" xr:uid="{00000000-0009-0000-0100-00000D000000}"/>
   <tableColumns count="9">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0700-000001000000}" name="Ships" dataDxfId="30"/>
@@ -2912,7 +2922,7 @@
 </file>
 
 <file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="12" xr:uid="{00000000-000C-0000-FFFF-FFFF08000000}" name="TblShipPoints" displayName="TblShipPoints" ref="A2:B7" totalsRowShown="0" headerRowDxfId="21" dataDxfId="19" headerRowBorderDxfId="20" tableBorderDxfId="18">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="12" xr:uid="{00000000-000C-0000-FFFF-FFFF08000000}" name="TblShipPoints" displayName="TblShipPoints" ref="A2:B7" totalsRowShown="0" headerRowDxfId="21" dataDxfId="20" headerRowBorderDxfId="18" tableBorderDxfId="19">
   <autoFilter ref="A2:B7" xr:uid="{00000000-0009-0000-0100-00000C000000}"/>
   <tableColumns count="2">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0800-000001000000}" name="Ships" dataDxfId="17"/>
@@ -3225,7 +3235,7 @@
       <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="14.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="7" width="15.42578125" customWidth="1"/>
@@ -3243,7 +3253,7 @@
     <col min="24" max="24" width="10" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:17">
       <c r="A1" s="47" t="s">
         <v>0</v>
       </c>
@@ -3260,7 +3270,7 @@
       <c r="O1" s="47"/>
       <c r="P1" s="47"/>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:17">
       <c r="A2" s="9" t="s">
         <v>2</v>
       </c>
@@ -3307,7 +3317,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:17">
       <c r="A3" s="15" t="s">
         <v>13</v>
       </c>
@@ -3360,7 +3370,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:17">
       <c r="A4" s="10" t="s">
         <v>14</v>
       </c>
@@ -3401,7 +3411,7 @@
         <v>5500</v>
       </c>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:17">
       <c r="A5" s="10" t="s">
         <v>15</v>
       </c>
@@ -3442,7 +3452,7 @@
         <v>3500</v>
       </c>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:17">
       <c r="A6" s="10" t="s">
         <v>16</v>
       </c>
@@ -3483,7 +3493,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:17">
       <c r="A7" t="s">
         <v>17</v>
       </c>
@@ -3524,7 +3534,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:17">
       <c r="A8" s="47" t="s">
         <v>18</v>
       </c>
@@ -3545,7 +3555,7 @@
       <c r="P8" s="47"/>
       <c r="Q8" s="47"/>
     </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:17">
       <c r="A9" s="8" t="s">
         <v>20</v>
       </c>
@@ -3593,7 +3603,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:17">
       <c r="A10" t="s">
         <v>13</v>
       </c>
@@ -3637,7 +3647,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:17">
       <c r="A11" t="s">
         <v>14</v>
       </c>
@@ -3683,7 +3693,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:17">
       <c r="A12" t="s">
         <v>15</v>
       </c>
@@ -3731,7 +3741,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:17">
       <c r="A13" t="s">
         <v>16</v>
       </c>
@@ -3777,7 +3787,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:17">
       <c r="A14" t="s">
         <v>17</v>
       </c>
@@ -3825,7 +3835,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:17">
       <c r="A15" t="s">
         <v>33</v>
       </c>
@@ -3882,7 +3892,7 @@
       </c>
       <c r="Q15" s="1"/>
     </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:17">
       <c r="A16" s="47" t="s">
         <v>35</v>
       </c>
@@ -3900,7 +3910,7 @@
       <c r="P16" s="1"/>
       <c r="Q16" s="1"/>
     </row>
-    <row r="17" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:18">
       <c r="A17" t="s">
         <v>20</v>
       </c>
@@ -3933,7 +3943,7 @@
       <c r="P17" s="1"/>
       <c r="Q17" s="1"/>
     </row>
-    <row r="18" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:18">
       <c r="A18" t="s">
         <v>4</v>
       </c>
@@ -3972,7 +3982,7 @@
       <c r="P18" s="1"/>
       <c r="Q18" s="1"/>
     </row>
-    <row r="19" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:18">
       <c r="A19" t="s">
         <v>5</v>
       </c>
@@ -4011,7 +4021,7 @@
       <c r="P19" s="1"/>
       <c r="Q19" s="1"/>
     </row>
-    <row r="20" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:18">
       <c r="A20" t="s">
         <v>6</v>
       </c>
@@ -4050,7 +4060,7 @@
       <c r="P20" s="1"/>
       <c r="Q20" s="1"/>
     </row>
-    <row r="21" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:18">
       <c r="A21" t="s">
         <v>33</v>
       </c>
@@ -4087,7 +4097,7 @@
       <c r="P21" s="1"/>
       <c r="Q21" s="1"/>
     </row>
-    <row r="22" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:18">
       <c r="A22" s="4"/>
       <c r="B22" s="5"/>
       <c r="C22" s="5"/>
@@ -4107,7 +4117,7 @@
       <c r="Q22" s="4"/>
       <c r="R22" s="4"/>
     </row>
-    <row r="23" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:18">
       <c r="A23" s="47" t="s">
         <v>40</v>
       </c>
@@ -4130,7 +4140,7 @@
       <c r="P23" s="47"/>
       <c r="Q23" s="47"/>
     </row>
-    <row r="24" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:18">
       <c r="A24" s="8" t="s">
         <v>20</v>
       </c>
@@ -4181,7 +4191,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="25" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:18">
       <c r="A25" t="s">
         <v>13</v>
       </c>
@@ -4244,7 +4254,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="26" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:18">
       <c r="A26" t="s">
         <v>14</v>
       </c>
@@ -4307,7 +4317,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="27" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:18">
       <c r="A27" t="s">
         <v>15</v>
       </c>
@@ -4370,7 +4380,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="28" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:18">
       <c r="A28" t="s">
         <v>16</v>
       </c>
@@ -4433,7 +4443,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="29" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:18">
       <c r="A29" t="s">
         <v>17</v>
       </c>
@@ -4496,7 +4506,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="30" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:18">
       <c r="A30" t="s">
         <v>33</v>
       </c>
@@ -4555,7 +4565,7 @@
       </c>
       <c r="Q30" s="1"/>
     </row>
-    <row r="31" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:18">
       <c r="A31" s="47" t="s">
         <v>47</v>
       </c>
@@ -4576,7 +4586,7 @@
       <c r="O31" s="47"/>
       <c r="P31" s="47"/>
     </row>
-    <row r="32" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:18">
       <c r="A32" t="s">
         <v>20</v>
       </c>
@@ -4621,7 +4631,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="33" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:16">
       <c r="A33" t="s">
         <v>28</v>
       </c>
@@ -4678,7 +4688,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:16">
       <c r="A34" t="s">
         <v>42</v>
       </c>
@@ -4735,7 +4745,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:16">
       <c r="A35" t="s">
         <v>29</v>
       </c>
@@ -4792,7 +4802,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:16">
       <c r="A36" t="s">
         <v>43</v>
       </c>
@@ -4849,7 +4859,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:16">
       <c r="A37" t="s">
         <v>30</v>
       </c>
@@ -4906,7 +4916,7 @@
         <v>2500</v>
       </c>
     </row>
-    <row r="38" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:16">
       <c r="A38" t="s">
         <v>44</v>
       </c>
@@ -4963,7 +4973,7 @@
         <v>3500</v>
       </c>
     </row>
-    <row r="39" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:16">
       <c r="A39" t="s">
         <v>31</v>
       </c>
@@ -5020,7 +5030,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:16">
       <c r="A40" t="s">
         <v>45</v>
       </c>
@@ -5077,7 +5087,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:16">
       <c r="A41" t="s">
         <v>32</v>
       </c>
@@ -5134,7 +5144,7 @@
         <v>5000</v>
       </c>
     </row>
-    <row r="42" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:16">
       <c r="A42" t="s">
         <v>46</v>
       </c>
@@ -5191,7 +5201,7 @@
         <v>5000</v>
       </c>
     </row>
-    <row r="43" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:16">
       <c r="A43" t="s">
         <v>33</v>
       </c>
@@ -5248,17 +5258,17 @@
         <v>16000</v>
       </c>
     </row>
-    <row r="45" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:16">
       <c r="C45" s="1"/>
       <c r="D45" s="1"/>
       <c r="E45" s="1"/>
       <c r="F45" s="1"/>
       <c r="G45" s="1"/>
     </row>
-    <row r="50" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="50" spans="2:2">
       <c r="B50" s="1"/>
     </row>
-    <row r="51" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="51" spans="2:2">
       <c r="B51" s="1"/>
     </row>
   </sheetData>
@@ -5302,7 +5312,7 @@
       <selection activeCell="F26" sqref="F26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="2" max="2" width="16.5703125" customWidth="1"/>
     <col min="3" max="3" width="18" customWidth="1"/>
@@ -5313,12 +5323,12 @@
     <col min="13" max="13" width="34" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:22" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:22">
       <c r="M1" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="2" spans="2:22" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:22">
       <c r="B2" s="21" t="s">
         <v>2</v>
       </c>
@@ -5359,7 +5369,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="3" spans="2:22" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:22">
       <c r="B3" s="25" t="s">
         <v>13</v>
       </c>
@@ -5420,7 +5430,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="2:22" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:22">
       <c r="B4" s="26" t="s">
         <v>14</v>
       </c>
@@ -5481,7 +5491,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="5" spans="2:22" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:22">
       <c r="B5" s="27" t="s">
         <v>15</v>
       </c>
@@ -5535,7 +5545,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="6" spans="2:22" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:22">
       <c r="B6" s="26" t="s">
         <v>16</v>
       </c>
@@ -5589,7 +5599,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="7" spans="2:22" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:22">
       <c r="B7" s="27" t="s">
         <v>17</v>
       </c>
@@ -5636,7 +5646,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="8" spans="2:22" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:22">
       <c r="L8">
         <v>6</v>
       </c>
@@ -5662,7 +5672,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="9" spans="2:22" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:22">
       <c r="L9">
         <v>7</v>
       </c>
@@ -5681,7 +5691,7 @@
         <v>600</v>
       </c>
     </row>
-    <row r="10" spans="2:22" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:22">
       <c r="B10" t="s">
         <v>56</v>
       </c>
@@ -5703,7 +5713,7 @@
         <v>700</v>
       </c>
     </row>
-    <row r="11" spans="2:22" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:22">
       <c r="B11" s="19" t="s">
         <v>57</v>
       </c>
@@ -5737,7 +5747,7 @@
         <v>800</v>
       </c>
     </row>
-    <row r="12" spans="2:22" ht="75" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:22" ht="75">
       <c r="B12" s="20" t="s">
         <v>62</v>
       </c>
@@ -5764,7 +5774,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="13" spans="2:22" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:22">
       <c r="L13">
         <v>11</v>
       </c>
@@ -5776,7 +5786,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="14" spans="2:22" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:22">
       <c r="L14">
         <v>12</v>
       </c>
@@ -5788,7 +5798,7 @@
         <v>1100</v>
       </c>
     </row>
-    <row r="15" spans="2:22" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:22">
       <c r="B15" s="21" t="s">
         <v>2</v>
       </c>
@@ -5805,7 +5815,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="16" spans="2:22" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:22">
       <c r="B16" s="22" t="s">
         <v>13</v>
       </c>
@@ -5822,7 +5832,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="17" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:12">
       <c r="B17" s="23" t="s">
         <v>14</v>
       </c>
@@ -5839,7 +5849,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="18" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:12">
       <c r="B18" s="22" t="s">
         <v>15</v>
       </c>
@@ -5856,7 +5866,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="19" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:12">
       <c r="B19" s="23" t="s">
         <v>16</v>
       </c>
@@ -5873,7 +5883,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="20" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:12">
       <c r="B20" s="22" t="s">
         <v>17</v>
       </c>
@@ -5890,17 +5900,17 @@
         <v>18</v>
       </c>
     </row>
-    <row r="21" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:12">
       <c r="L21">
         <v>19</v>
       </c>
     </row>
-    <row r="22" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:12">
       <c r="L22">
         <v>20</v>
       </c>
     </row>
-    <row r="23" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:12">
       <c r="B23" s="36" t="s">
         <v>20</v>
       </c>
@@ -5926,7 +5936,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="24" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:12">
       <c r="B24" s="38" t="s">
         <v>13</v>
       </c>
@@ -5942,7 +5952,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="25" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:12">
       <c r="B25" s="40" t="s">
         <v>14</v>
       </c>
@@ -5960,7 +5970,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="26" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:12">
       <c r="B26" s="38" t="s">
         <v>15</v>
       </c>
@@ -5980,7 +5990,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="27" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:12">
       <c r="B27" s="40" t="s">
         <v>16</v>
       </c>
@@ -5998,7 +6008,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="28" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:12">
       <c r="B28" s="38" t="s">
         <v>17</v>
       </c>
@@ -6018,7 +6028,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="29" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:12">
       <c r="C29">
         <f>C24*G3*F3</f>
         <v>1000</v>
@@ -6057,9 +6067,9 @@
       <selection activeCell="P25" sqref="P24:Q25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:19">
       <c r="D1">
         <v>38</v>
       </c>
@@ -6082,7 +6092,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:19">
       <c r="J2" t="s">
         <v>58</v>
       </c>
@@ -6090,7 +6100,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="3" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:19">
       <c r="B3" s="42"/>
       <c r="C3" s="42"/>
       <c r="D3" s="42"/>
@@ -6123,7 +6133,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="4" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:19">
       <c r="B4" s="45" t="s">
         <v>69</v>
       </c>
@@ -6146,7 +6156,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:19">
       <c r="B5" s="43" t="s">
         <v>70</v>
       </c>
@@ -6169,7 +6179,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:19">
       <c r="B6" s="45" t="s">
         <v>71</v>
       </c>
@@ -6192,7 +6202,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:19">
       <c r="B7" s="6" t="s">
         <v>72</v>
       </c>
@@ -6215,7 +6225,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:19">
       <c r="G8" s="6" t="s">
         <v>13</v>
       </c>
@@ -6238,7 +6248,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:19">
       <c r="N10" s="19" t="s">
         <v>57</v>
       </c>
@@ -6255,7 +6265,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="15" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:19">
       <c r="C15" s="44" t="s">
         <v>17</v>
       </c>
@@ -6272,19 +6282,19 @@
         <v>17</v>
       </c>
     </row>
-    <row r="16" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:19">
       <c r="P16">
         <f ca="1">RANDBETWEEN(0,123)</f>
-        <v>65</v>
-      </c>
-    </row>
-    <row r="17" spans="2:16" x14ac:dyDescent="0.25">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="17" spans="2:16">
       <c r="P17" s="46">
         <f ca="1">RANDBETWEEN(0,6)</f>
-        <v>6</v>
-      </c>
-    </row>
-    <row r="18" spans="2:16" x14ac:dyDescent="0.25">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="18" spans="2:16">
       <c r="C18" s="44" t="s">
         <v>17</v>
       </c>
@@ -6301,12 +6311,12 @@
         <v>72</v>
       </c>
     </row>
-    <row r="19" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:16">
       <c r="L19" s="45" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="20" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:16">
       <c r="E20" s="44" t="s">
         <v>17</v>
       </c>
@@ -6317,12 +6327,12 @@
         <v>70</v>
       </c>
     </row>
-    <row r="21" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:16">
       <c r="L21" s="45" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="22" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:16">
       <c r="B22" s="2"/>
       <c r="C22" s="2"/>
       <c r="D22" s="2"/>
@@ -6337,7 +6347,7 @@
       <c r="K22" s="2"/>
       <c r="L22" s="2"/>
     </row>
-    <row r="24" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:16">
       <c r="E24">
         <v>64</v>
       </c>
@@ -6360,7 +6370,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="25" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:16">
       <c r="K25" t="s">
         <v>58</v>
       </c>
@@ -6375,325 +6385,340 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F5EC53A5-8F19-4711-93EA-0F4CBD261EC8}">
-  <dimension ref="B2:B73"/>
+  <dimension ref="B2:B77"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N21" sqref="N21"/>
+    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
+      <selection activeCell="A69" sqref="A69:XFD69"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="2" max="2" width="11.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:2">
       <c r="B2" s="21" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="3" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:2">
       <c r="B3" s="3" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="4" spans="2:2" x14ac:dyDescent="0.25">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="4" spans="2:2">
       <c r="B4" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="5" spans="2:2" x14ac:dyDescent="0.25">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="5" spans="2:2">
       <c r="B5" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="6" spans="2:2" x14ac:dyDescent="0.25">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="6" spans="2:2">
       <c r="B6" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="7" spans="2:2" x14ac:dyDescent="0.25">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="7" spans="2:2">
       <c r="B7" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="8" spans="2:2" x14ac:dyDescent="0.25">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="8" spans="2:2">
       <c r="B8" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="9" spans="2:2" x14ac:dyDescent="0.25">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="9" spans="2:2">
       <c r="B9" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="10" spans="2:2" x14ac:dyDescent="0.25">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="10" spans="2:2">
       <c r="B10" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="11" spans="2:2" x14ac:dyDescent="0.25">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="11" spans="2:2">
       <c r="B11" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="13" spans="2:2" x14ac:dyDescent="0.25">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="13" spans="2:2">
       <c r="B13" s="3" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="14" spans="2:2" x14ac:dyDescent="0.25">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="14" spans="2:2">
       <c r="B14" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="15" spans="2:2" x14ac:dyDescent="0.25">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="15" spans="2:2">
       <c r="B15" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="17" spans="2:2" x14ac:dyDescent="0.25">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="17" spans="2:2">
       <c r="B17" s="3" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="18" spans="2:2" x14ac:dyDescent="0.25">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="18" spans="2:2">
       <c r="B18" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="19" spans="2:2" x14ac:dyDescent="0.25">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="19" spans="2:2">
       <c r="B19" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="20" spans="2:2" x14ac:dyDescent="0.25">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="20" spans="2:2">
       <c r="B20" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="21" spans="2:2" x14ac:dyDescent="0.25">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="21" spans="2:2">
       <c r="B21" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="22" spans="2:2" x14ac:dyDescent="0.25">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="22" spans="2:2">
       <c r="B22" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="24" spans="2:2" x14ac:dyDescent="0.25">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="24" spans="2:2">
       <c r="B24" s="3" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="25" spans="2:2" x14ac:dyDescent="0.25">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="25" spans="2:2">
       <c r="B25" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="27" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B27" s="3" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="28" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B28" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="29" spans="2:2" x14ac:dyDescent="0.25">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="26" spans="2:2">
+      <c r="B26" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="28" spans="2:2">
+      <c r="B28" s="3" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="29" spans="2:2">
       <c r="B29" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="31" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B31" s="3" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="32" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B32" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="34" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B34" s="3" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="35" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B35" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="36" spans="2:2" x14ac:dyDescent="0.25">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="30" spans="2:2">
+      <c r="B30" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="32" spans="2:2">
+      <c r="B32" s="3" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="33" spans="2:2">
+      <c r="B33" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="35" spans="2:2">
+      <c r="B35" s="3" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="36" spans="2:2">
       <c r="B36" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="38" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B38" s="3" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="39" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B39" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="40" spans="2:2" x14ac:dyDescent="0.25">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="37" spans="2:2">
+      <c r="B37" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="39" spans="2:2">
+      <c r="B39" s="3" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="40" spans="2:2">
       <c r="B40" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="41" spans="2:2" x14ac:dyDescent="0.25">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="41" spans="2:2">
       <c r="B41" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="42" spans="2:2" x14ac:dyDescent="0.25">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="42" spans="2:2">
       <c r="B42" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="43" spans="2:2" x14ac:dyDescent="0.25">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="43" spans="2:2">
       <c r="B43" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="44" spans="2:2" x14ac:dyDescent="0.25">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="44" spans="2:2">
       <c r="B44" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="45" spans="2:2" x14ac:dyDescent="0.25">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="45" spans="2:2">
       <c r="B45" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="46" spans="2:2" x14ac:dyDescent="0.25">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="46" spans="2:2">
       <c r="B46" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="47" spans="2:2" x14ac:dyDescent="0.25">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="47" spans="2:2">
       <c r="B47" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="48" spans="2:2" x14ac:dyDescent="0.25">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="48" spans="2:2">
       <c r="B48" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="49" spans="2:2" x14ac:dyDescent="0.25">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="49" spans="2:2">
       <c r="B49" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="51" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B51" s="3" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="52" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B52" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="53" spans="2:2" x14ac:dyDescent="0.25">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="50" spans="2:2">
+      <c r="B50" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="52" spans="2:2">
+      <c r="B52" s="3" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="53" spans="2:2">
       <c r="B53" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="54" spans="2:2" x14ac:dyDescent="0.25">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="54" spans="2:2">
       <c r="B54" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="55" spans="2:2" x14ac:dyDescent="0.25">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="55" spans="2:2">
       <c r="B55" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="56" spans="2:2" x14ac:dyDescent="0.25">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="56" spans="2:2">
       <c r="B56" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="57" spans="2:2" x14ac:dyDescent="0.25">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="57" spans="2:2">
       <c r="B57" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="58" spans="2:2" x14ac:dyDescent="0.25">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="58" spans="2:2">
       <c r="B58" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="59" spans="2:2" x14ac:dyDescent="0.25">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="59" spans="2:2">
       <c r="B59" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="61" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B61" s="3" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="62" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B62" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="63" spans="2:2" x14ac:dyDescent="0.25">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="60" spans="2:2">
+      <c r="B60" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="62" spans="2:2">
+      <c r="B62" s="3" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="63" spans="2:2">
       <c r="B63" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="64" spans="2:2" x14ac:dyDescent="0.25">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="64" spans="2:2">
       <c r="B64" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="66" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B66" s="3" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="67" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B67" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="68" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B68" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="69" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B69" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="70" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B70" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="71" spans="2:2" x14ac:dyDescent="0.25">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="65" spans="2:2">
+      <c r="B65" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="67" spans="2:2">
+      <c r="B67" s="3" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="68" spans="2:2">
+      <c r="B68" s="54" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="70" spans="2:2">
+      <c r="B70" s="3" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="71" spans="2:2">
       <c r="B71" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="72" spans="2:2" x14ac:dyDescent="0.25">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="72" spans="2:2">
       <c r="B72" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="73" spans="2:2" x14ac:dyDescent="0.25">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="73" spans="2:2">
       <c r="B73" t="s">
-        <v>88</v>
+        <v>134</v>
+      </c>
+    </row>
+    <row r="74" spans="2:2">
+      <c r="B74" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="75" spans="2:2">
+      <c r="B75" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="76" spans="2:2">
+      <c r="B76" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="77" spans="2:2">
+      <c r="B77" t="s">
+        <v>138</v>
       </c>
     </row>
   </sheetData>
@@ -6710,56 +6735,56 @@
       <selection activeCell="J14" sqref="J14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="2" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:2">
       <c r="B2" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="3" spans="2:2" x14ac:dyDescent="0.25">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="3" spans="2:2">
       <c r="B3" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="4" spans="2:2" x14ac:dyDescent="0.25">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="4" spans="2:2">
       <c r="B4" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="5" spans="2:2" x14ac:dyDescent="0.25">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="5" spans="2:2">
       <c r="B5" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="6" spans="2:2" x14ac:dyDescent="0.25">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="6" spans="2:2">
       <c r="B6" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="7" spans="2:2" x14ac:dyDescent="0.25">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="7" spans="2:2">
       <c r="B7" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="8" spans="2:2" x14ac:dyDescent="0.25">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="8" spans="2:2">
       <c r="B8" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="9" spans="2:2" x14ac:dyDescent="0.25">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="9" spans="2:2">
       <c r="B9" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="10" spans="2:2" x14ac:dyDescent="0.25">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="10" spans="2:2">
       <c r="B10" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="11" spans="2:2" x14ac:dyDescent="0.25">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="11" spans="2:2">
       <c r="B11" t="s">
-        <v>100</v>
+        <v>148</v>
       </c>
     </row>
   </sheetData>
@@ -6775,194 +6800,194 @@
       <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="2" max="2" width="18.28515625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="29.42578125" customWidth="1"/>
     <col min="4" max="4" width="27.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:4">
       <c r="B2" s="32" t="s">
-        <v>101</v>
+        <v>149</v>
       </c>
       <c r="C2" s="32" t="s">
-        <v>102</v>
+        <v>150</v>
       </c>
       <c r="D2" s="32" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="3" spans="2:4" ht="106.5" customHeight="1" x14ac:dyDescent="0.25">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="3" spans="2:4" ht="106.5" customHeight="1">
       <c r="B3" s="50" t="s">
-        <v>104</v>
+        <v>152</v>
       </c>
       <c r="C3" s="48" t="s">
-        <v>105</v>
+        <v>153</v>
       </c>
       <c r="D3" s="28" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="4" spans="2:4" ht="120" x14ac:dyDescent="0.25">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="4" spans="2:4" ht="120">
       <c r="B4" s="53"/>
       <c r="C4" s="52"/>
       <c r="D4" s="29" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="5" spans="2:4" ht="60" x14ac:dyDescent="0.25">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="5" spans="2:4" ht="60">
       <c r="B5" s="53"/>
       <c r="C5" s="52"/>
       <c r="D5" s="30" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="6" spans="2:4" ht="75" x14ac:dyDescent="0.25">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="6" spans="2:4" ht="75">
       <c r="B6" s="53"/>
       <c r="C6" s="52"/>
       <c r="D6" s="30" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="7" spans="2:4" ht="90" x14ac:dyDescent="0.25">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="7" spans="2:4" ht="90">
       <c r="B7" s="50" t="s">
-        <v>110</v>
+        <v>158</v>
       </c>
       <c r="C7" s="48" t="s">
-        <v>111</v>
+        <v>159</v>
       </c>
       <c r="D7" s="28" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="8" spans="2:4" ht="90" x14ac:dyDescent="0.25">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="8" spans="2:4" ht="90">
       <c r="B8" s="53"/>
       <c r="C8" s="52"/>
       <c r="D8" s="30" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="9" spans="2:4" ht="75" x14ac:dyDescent="0.25">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="9" spans="2:4" ht="75">
       <c r="B9" s="50" t="s">
-        <v>114</v>
+        <v>162</v>
       </c>
       <c r="C9" s="48" t="s">
-        <v>115</v>
+        <v>163</v>
       </c>
       <c r="D9" s="28" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="10" spans="2:4" ht="30" x14ac:dyDescent="0.25">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="10" spans="2:4" ht="30">
       <c r="B10" s="51"/>
       <c r="C10" s="49"/>
       <c r="D10" s="31" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="11" spans="2:4" ht="76.5" customHeight="1" x14ac:dyDescent="0.25">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="11" spans="2:4" ht="76.5" customHeight="1">
       <c r="B11" s="50" t="s">
-        <v>118</v>
+        <v>166</v>
       </c>
       <c r="C11" s="48" t="s">
-        <v>119</v>
+        <v>167</v>
       </c>
       <c r="D11" s="28" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="12" spans="2:4" ht="30" x14ac:dyDescent="0.25">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="12" spans="2:4" ht="30">
       <c r="B12" s="53"/>
       <c r="C12" s="52"/>
       <c r="D12" s="30" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="13" spans="2:4" ht="45" x14ac:dyDescent="0.25">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="13" spans="2:4" ht="45">
       <c r="B13" s="50" t="s">
-        <v>122</v>
+        <v>170</v>
       </c>
       <c r="C13" s="48" t="s">
-        <v>123</v>
+        <v>171</v>
       </c>
       <c r="D13" s="28" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="14" spans="2:4" ht="30" x14ac:dyDescent="0.25">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="14" spans="2:4" ht="30">
       <c r="B14" s="53"/>
       <c r="C14" s="52"/>
       <c r="D14" s="30" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="15" spans="2:4" ht="45" x14ac:dyDescent="0.25">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="15" spans="2:4" ht="45">
       <c r="B15" s="53"/>
       <c r="C15" s="52"/>
       <c r="D15" s="30" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="16" spans="2:4" ht="60" x14ac:dyDescent="0.25">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="16" spans="2:4" ht="60">
       <c r="B16" s="53"/>
       <c r="C16" s="52"/>
       <c r="D16" s="30" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="17" spans="2:4" ht="45" x14ac:dyDescent="0.25">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="17" spans="2:4" ht="45">
       <c r="B17" s="50" t="s">
-        <v>128</v>
+        <v>176</v>
       </c>
       <c r="C17" s="48" t="s">
-        <v>129</v>
+        <v>177</v>
       </c>
       <c r="D17" s="28" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="18" spans="2:4" ht="45" x14ac:dyDescent="0.25">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="18" spans="2:4" ht="45">
       <c r="B18" s="53"/>
       <c r="C18" s="52"/>
       <c r="D18" s="30" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="19" spans="2:4" ht="60.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="19" spans="2:4" ht="60.75" customHeight="1">
       <c r="B19" s="50" t="s">
-        <v>132</v>
+        <v>180</v>
       </c>
       <c r="C19" s="48" t="s">
-        <v>133</v>
+        <v>181</v>
       </c>
       <c r="D19" s="28" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="20" spans="2:4" ht="30" x14ac:dyDescent="0.25">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="20" spans="2:4" ht="30">
       <c r="B20" s="53"/>
       <c r="C20" s="52"/>
       <c r="D20" s="30" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="21" spans="2:4" ht="45" x14ac:dyDescent="0.25">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="21" spans="2:4" ht="45">
       <c r="B21" s="50" t="s">
-        <v>136</v>
+        <v>184</v>
       </c>
       <c r="C21" s="48" t="s">
-        <v>137</v>
+        <v>185</v>
       </c>
       <c r="D21" s="28" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="22" spans="2:4" ht="30" x14ac:dyDescent="0.25">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="22" spans="2:4" ht="30">
       <c r="B22" s="51"/>
       <c r="C22" s="49"/>
       <c r="D22" s="31" t="s">
-        <v>139</v>
+        <v>187</v>
       </c>
     </row>
   </sheetData>
@@ -6996,7 +7021,7 @@
       <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="12.140625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="10.5703125" bestFit="1" customWidth="1"/>
@@ -7006,33 +7031,33 @@
     <col min="11" max="11" width="9.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:19">
       <c r="A2" s="47" t="s">
-        <v>140</v>
+        <v>188</v>
       </c>
       <c r="B2" s="47"/>
       <c r="C2" s="47"/>
       <c r="F2" s="47" t="s">
-        <v>141</v>
+        <v>189</v>
       </c>
       <c r="G2" s="47"/>
       <c r="H2" s="47"/>
     </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:19">
       <c r="A3" t="s">
-        <v>142</v>
+        <v>190</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>21</v>
       </c>
       <c r="F3" t="s">
-        <v>142</v>
+        <v>190</v>
       </c>
       <c r="G3" s="1" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:19">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -7048,54 +7073,54 @@
         <v>9500</v>
       </c>
     </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:19">
       <c r="A5" t="s">
-        <v>143</v>
+        <v>191</v>
       </c>
       <c r="B5">
         <f>SUM(C10:C14)</f>
         <v>5000</v>
       </c>
       <c r="F5" t="s">
-        <v>143</v>
+        <v>191</v>
       </c>
       <c r="G5">
         <f>SUM(H10:H14)</f>
         <v>7500</v>
       </c>
     </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:19">
       <c r="A6" t="s">
-        <v>144</v>
+        <v>192</v>
       </c>
       <c r="B6">
         <f>SUM(C17:C19)</f>
         <v>2000</v>
       </c>
       <c r="F6" t="s">
-        <v>144</v>
+        <v>192</v>
       </c>
       <c r="G6">
         <f>SUM(H17:H19)</f>
         <v>2000</v>
       </c>
     </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:19">
       <c r="C7" s="17"/>
       <c r="H7" s="17"/>
     </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:19">
       <c r="C8" s="17"/>
       <c r="H8" s="17"/>
       <c r="Q8" s="3"/>
       <c r="S8" s="3"/>
     </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:19">
       <c r="A9" s="17" t="s">
         <v>2</v>
       </c>
       <c r="B9" s="17" t="s">
-        <v>145</v>
+        <v>193</v>
       </c>
       <c r="C9" s="17" t="s">
         <v>3</v>
@@ -7104,7 +7129,7 @@
         <v>2</v>
       </c>
       <c r="G9" s="17" t="s">
-        <v>145</v>
+        <v>193</v>
       </c>
       <c r="H9" s="17" t="s">
         <v>3</v>
@@ -7121,7 +7146,7 @@
       <c r="R9" s="1"/>
       <c r="S9" s="7"/>
     </row>
-    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:19">
       <c r="A10" s="17" t="s">
         <v>13</v>
       </c>
@@ -7156,7 +7181,7 @@
       <c r="R10" s="1"/>
       <c r="S10" s="7"/>
     </row>
-    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:19">
       <c r="A11" s="17" t="s">
         <v>14</v>
       </c>
@@ -7193,7 +7218,7 @@
       <c r="R11" s="1"/>
       <c r="S11" s="7"/>
     </row>
-    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:19">
       <c r="A12" s="17" t="s">
         <v>15</v>
       </c>
@@ -7230,7 +7255,7 @@
       <c r="R12" s="1"/>
       <c r="S12" s="7"/>
     </row>
-    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:19">
       <c r="A13" s="17" t="s">
         <v>16</v>
       </c>
@@ -7265,7 +7290,7 @@
       <c r="R13" s="1"/>
       <c r="S13" s="7"/>
     </row>
-    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:19">
       <c r="A14" s="17" t="s">
         <v>17</v>
       </c>
@@ -7289,27 +7314,27 @@
         <v>5000</v>
       </c>
     </row>
-    <row r="16" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:19">
       <c r="A16" s="17" t="s">
-        <v>104</v>
+        <v>152</v>
       </c>
       <c r="B16" s="17" t="s">
-        <v>145</v>
+        <v>193</v>
       </c>
       <c r="C16" t="s">
         <v>3</v>
       </c>
       <c r="F16" s="17" t="s">
-        <v>104</v>
+        <v>152</v>
       </c>
       <c r="G16" s="17" t="s">
-        <v>145</v>
+        <v>193</v>
       </c>
       <c r="H16" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8">
       <c r="A17" s="17" t="s">
         <v>4</v>
       </c>
@@ -7333,7 +7358,7 @@
         <v>1500</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:8">
       <c r="A18" s="17" t="s">
         <v>5</v>
       </c>
@@ -7357,7 +7382,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:8">
       <c r="A19" s="17" t="s">
         <v>6</v>
       </c>

</xml_diff>

<commit_message>
Added neutral cards and updated rules
</commit_message>
<xml_diff>
--- a/ShipCardGameCalcs.xlsx
+++ b/ShipCardGameCalcs.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26324"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26330"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MultiplayerGame\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{0467AE46-17F3-4346-8506-05E8CC4D416A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{57862236-6CE4-4D3E-9525-D568A7EBB5BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="3" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -487,7 +487,7 @@
     <t>All ship upgrades attached to destroyed ship are sent to the junkyard</t>
   </si>
   <si>
-    <t>Each ship will have had assigned amount of escape pods. The player owning the destroyed ship may pick to move that amount of crew with their attachments from the destroyed ship to another ship they own</t>
+    <t>Each ship will have had assigned amount of escape pods. The player owning the destroyed ship may pick to move that amount of crew with their attachments from the destroyed ship to another ship they own as long as there is space left on the ship</t>
   </si>
   <si>
     <t>The rest of the crew and crew attachment cards are sent to stasis and the junkyard</t>
@@ -6284,13 +6284,13 @@
     <row r="16" spans="2:19">
       <c r="P16">
         <f ca="1">RANDBETWEEN(0,123)</f>
-        <v>104</v>
+        <v>44</v>
       </c>
     </row>
     <row r="17" spans="2:16">
       <c r="P17" s="46">
         <f ca="1">RANDBETWEEN(0,6)</f>
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="18" spans="2:16">
@@ -6386,8 +6386,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F5EC53A5-8F19-4711-93EA-0F4CBD261EC8}">
   <dimension ref="B2:B77"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="D27" sqref="D27"/>
+    <sheetView tabSelected="1" topLeftCell="A51" workbookViewId="0">
+      <selection activeCell="B75" sqref="B75"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>

</xml_diff>

<commit_message>
Have nerfed and buffed various cards and added a few more new ones
</commit_message>
<xml_diff>
--- a/ShipCardGameCalcs.xlsx
+++ b/ShipCardGameCalcs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MultiplayerGame\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53BB1DCC-95A0-442C-A428-8C62AA11E512}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2FDE9412-D2BF-4730-BF55-A39F428F72A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Values" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="402" uniqueCount="194">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="406" uniqueCount="198">
   <si>
     <t>Ship Parameters</t>
   </si>
@@ -364,27 +364,18 @@
     <t>Untap Phase</t>
   </si>
   <si>
-    <t>This is where the player untaps all their cards unless stated otherwise</t>
-  </si>
-  <si>
     <t>All player ships shield damaged, restore 100 shield</t>
   </si>
   <si>
     <t>Draw Phase</t>
   </si>
   <si>
-    <t>This is where the player chooses to draw from their Strategy or Crew Deck</t>
-  </si>
-  <si>
     <t>Players can draw either 1 card from the strategy deck, or they can choose the see the top 3 cards of the crew deck and then get to pick 1. The rest get sent to the bottom of the crew deck.</t>
   </si>
   <si>
     <t>Strategy Phase</t>
   </si>
   <si>
-    <t>This is where the player can play their cards, tap to gain department resourse or tap cards to use gun slots</t>
-  </si>
-  <si>
     <t>End Phase</t>
   </si>
   <si>
@@ -472,9 +463,6 @@
     <t>Taking Damage</t>
   </si>
   <si>
-    <t>When a ship takes hull damage, sacrifice 1 crew member from ship. Only do this once per strategy phase</t>
-  </si>
-  <si>
     <t>Ship Destroyed</t>
   </si>
   <si>
@@ -662,6 +650,30 @@
   </si>
   <si>
     <t>No. of</t>
+  </si>
+  <si>
+    <t>Battle Phase</t>
+  </si>
+  <si>
+    <t>Reaction Phase</t>
+  </si>
+  <si>
+    <t>This is where any player can play cards to react to the battle phase, such as playing a tactic card to change the ships target</t>
+  </si>
+  <si>
+    <t>When a ship takes hull damage, sacrifice either 1 crew member card or ship attachment card from the ship. Only do this once per strategy phase</t>
+  </si>
+  <si>
+    <t>Current player taps to use gun slots, announcing targets</t>
+  </si>
+  <si>
+    <t>Current player can play their cards, tap to gain department resourse or tap cards to use gun slots</t>
+  </si>
+  <si>
+    <t>Current player chooses to draw from their Strategy or Crew Deck</t>
+  </si>
+  <si>
+    <t>Current player untaps all their cards unless stated otherwise</t>
   </si>
 </sst>
 </file>
@@ -1040,7 +1052,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="54">
+  <cellXfs count="55">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1159,6 +1171,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -5307,7 +5320,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{91273792-62E9-442E-9CC7-E8C6E6BD4008}">
   <dimension ref="B1:V29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F26" sqref="F26"/>
     </sheetView>
   </sheetViews>
@@ -6284,13 +6297,13 @@
     <row r="16" spans="2:19" x14ac:dyDescent="0.25">
       <c r="P16">
         <f ca="1">RANDBETWEEN(0,123)</f>
-        <v>43</v>
+        <v>62</v>
       </c>
     </row>
     <row r="17" spans="2:16" x14ac:dyDescent="0.25">
       <c r="P17" s="46">
         <f ca="1">RANDBETWEEN(0,6)</f>
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="18" spans="2:16" x14ac:dyDescent="0.25">
@@ -6384,10 +6397,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F5EC53A5-8F19-4711-93EA-0F4CBD261EC8}">
-  <dimension ref="B2:B77"/>
+  <dimension ref="B2:B83"/>
   <sheetViews>
-    <sheetView topLeftCell="A51" workbookViewId="0">
-      <selection activeCell="L67" sqref="L67"/>
+    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
+      <selection activeCell="T29" sqref="T29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6497,227 +6510,250 @@
     </row>
     <row r="25" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B25" t="s">
-        <v>94</v>
+        <v>197</v>
       </c>
     </row>
     <row r="26" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B26" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="28" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B28" s="3" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="29" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B29" t="s">
-        <v>97</v>
+        <v>196</v>
       </c>
     </row>
     <row r="30" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B30" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
     </row>
     <row r="32" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B32" s="3" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
     </row>
     <row r="33" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B33" t="s">
-        <v>100</v>
+        <v>195</v>
       </c>
     </row>
     <row r="35" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B35" s="3" t="s">
-        <v>101</v>
+        <v>190</v>
       </c>
     </row>
     <row r="36" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B36" t="s">
-        <v>102</v>
+      <c r="B36" s="54" t="s">
+        <v>194</v>
       </c>
     </row>
     <row r="37" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B37" t="s">
-        <v>103</v>
+      <c r="B37" s="54"/>
+    </row>
+    <row r="38" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B38" s="3" t="s">
+        <v>191</v>
       </c>
     </row>
     <row r="39" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B39" s="3" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="40" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B40" t="s">
-        <v>105</v>
+      <c r="B39" s="54" t="s">
+        <v>192</v>
       </c>
     </row>
     <row r="41" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B41" t="s">
-        <v>106</v>
+      <c r="B41" s="3" t="s">
+        <v>98</v>
       </c>
     </row>
     <row r="42" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B42" t="s">
-        <v>107</v>
+        <v>99</v>
       </c>
     </row>
     <row r="43" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B43" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="44" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B44" t="s">
-        <v>109</v>
+        <v>100</v>
       </c>
     </row>
     <row r="45" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B45" t="s">
-        <v>110</v>
+      <c r="B45" s="3" t="s">
+        <v>101</v>
       </c>
     </row>
     <row r="46" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B46" t="s">
-        <v>111</v>
+        <v>102</v>
       </c>
     </row>
     <row r="47" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B47" t="s">
-        <v>112</v>
+        <v>103</v>
       </c>
     </row>
     <row r="48" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B48" t="s">
-        <v>113</v>
+        <v>104</v>
       </c>
     </row>
     <row r="49" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B49" t="s">
-        <v>114</v>
+        <v>105</v>
       </c>
     </row>
     <row r="50" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B50" t="s">
-        <v>115</v>
+        <v>106</v>
+      </c>
+    </row>
+    <row r="51" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B51" t="s">
+        <v>107</v>
       </c>
     </row>
     <row r="52" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B52" s="3" t="s">
-        <v>116</v>
+      <c r="B52" t="s">
+        <v>108</v>
       </c>
     </row>
     <row r="53" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B53" t="s">
-        <v>117</v>
+        <v>109</v>
       </c>
     </row>
     <row r="54" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B54" t="s">
-        <v>118</v>
+        <v>110</v>
       </c>
     </row>
     <row r="55" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B55" t="s">
-        <v>119</v>
+        <v>111</v>
       </c>
     </row>
     <row r="56" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B56" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="57" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B57" t="s">
-        <v>121</v>
+        <v>112</v>
       </c>
     </row>
     <row r="58" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B58" t="s">
-        <v>122</v>
+      <c r="B58" s="3" t="s">
+        <v>113</v>
       </c>
     </row>
     <row r="59" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B59" t="s">
-        <v>123</v>
+        <v>114</v>
       </c>
     </row>
     <row r="60" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B60" t="s">
-        <v>124</v>
+        <v>115</v>
+      </c>
+    </row>
+    <row r="61" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B61" t="s">
+        <v>116</v>
       </c>
     </row>
     <row r="62" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B62" s="3" t="s">
-        <v>125</v>
+      <c r="B62" t="s">
+        <v>117</v>
       </c>
     </row>
     <row r="63" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B63" t="s">
-        <v>126</v>
+        <v>118</v>
       </c>
     </row>
     <row r="64" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B64" t="s">
-        <v>127</v>
+        <v>119</v>
       </c>
     </row>
     <row r="65" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B65" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="67" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B67" s="3" t="s">
-        <v>129</v>
+        <v>120</v>
+      </c>
+    </row>
+    <row r="66" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B66" t="s">
+        <v>121</v>
       </c>
     </row>
     <row r="68" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B68" t="s">
-        <v>130</v>
+      <c r="B68" s="3" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="69" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B69" t="s">
+        <v>123</v>
       </c>
     </row>
     <row r="70" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B70" s="3" t="s">
-        <v>131</v>
+      <c r="B70" t="s">
+        <v>124</v>
       </c>
     </row>
     <row r="71" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B71" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="72" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B72" t="s">
-        <v>133</v>
+        <v>125</v>
       </c>
     </row>
     <row r="73" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B73" t="s">
-        <v>134</v>
+      <c r="B73" s="3" t="s">
+        <v>126</v>
       </c>
     </row>
     <row r="74" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B74" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="75" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B75" t="s">
-        <v>136</v>
+        <v>193</v>
       </c>
     </row>
     <row r="76" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B76" t="s">
-        <v>137</v>
+      <c r="B76" s="3" t="s">
+        <v>127</v>
       </c>
     </row>
     <row r="77" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B77" t="s">
-        <v>138</v>
+        <v>128</v>
+      </c>
+    </row>
+    <row r="78" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B78" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="79" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B79" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="80" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B80" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="81" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B81" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="82" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B82" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="83" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B83" t="s">
+        <v>134</v>
       </c>
     </row>
   </sheetData>
@@ -6738,52 +6774,52 @@
   <sheetData>
     <row r="2" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
     </row>
     <row r="3" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
     </row>
     <row r="4" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
     </row>
     <row r="5" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
     </row>
     <row r="6" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
     </row>
     <row r="7" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
     </row>
     <row r="8" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
     </row>
     <row r="9" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
     </row>
     <row r="10" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
     </row>
     <row r="11" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
     </row>
   </sheetData>
@@ -6795,7 +6831,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1CADF2F4-A124-44BC-8A72-4CE3F16F5D04}">
   <dimension ref="B2:D22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A9" workbookViewId="0">
       <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
@@ -6808,185 +6844,185 @@
   <sheetData>
     <row r="2" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B2" s="32" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="C2" s="32" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="D2" s="32" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
     </row>
     <row r="3" spans="2:4" ht="106.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="50" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="C3" s="48" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="D3" s="28" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
     </row>
     <row r="4" spans="2:4" ht="120" x14ac:dyDescent="0.25">
       <c r="B4" s="53"/>
       <c r="C4" s="52"/>
       <c r="D4" s="29" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
     </row>
     <row r="5" spans="2:4" ht="60" x14ac:dyDescent="0.25">
       <c r="B5" s="53"/>
       <c r="C5" s="52"/>
       <c r="D5" s="30" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
     </row>
     <row r="6" spans="2:4" ht="75" x14ac:dyDescent="0.25">
       <c r="B6" s="53"/>
       <c r="C6" s="52"/>
       <c r="D6" s="30" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
     </row>
     <row r="7" spans="2:4" ht="90" x14ac:dyDescent="0.25">
       <c r="B7" s="50" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="C7" s="48" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
       <c r="D7" s="28" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
     </row>
     <row r="8" spans="2:4" ht="90" x14ac:dyDescent="0.25">
       <c r="B8" s="53"/>
       <c r="C8" s="52"/>
       <c r="D8" s="30" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
     </row>
     <row r="9" spans="2:4" ht="75" x14ac:dyDescent="0.25">
       <c r="B9" s="50" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
       <c r="C9" s="48" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
       <c r="D9" s="28" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
     </row>
     <row r="10" spans="2:4" ht="30" x14ac:dyDescent="0.25">
       <c r="B10" s="51"/>
       <c r="C10" s="49"/>
       <c r="D10" s="31" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
     </row>
     <row r="11" spans="2:4" ht="76.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B11" s="50" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
       <c r="C11" s="48" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="D11" s="28" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
     </row>
     <row r="12" spans="2:4" ht="30" x14ac:dyDescent="0.25">
       <c r="B12" s="53"/>
       <c r="C12" s="52"/>
       <c r="D12" s="30" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
     </row>
     <row r="13" spans="2:4" ht="45" x14ac:dyDescent="0.25">
       <c r="B13" s="50" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
       <c r="C13" s="48" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="D13" s="28" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
     </row>
     <row r="14" spans="2:4" ht="30" x14ac:dyDescent="0.25">
       <c r="B14" s="53"/>
       <c r="C14" s="52"/>
       <c r="D14" s="30" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
     </row>
     <row r="15" spans="2:4" ht="45" x14ac:dyDescent="0.25">
       <c r="B15" s="53"/>
       <c r="C15" s="52"/>
       <c r="D15" s="30" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
     </row>
     <row r="16" spans="2:4" ht="60" x14ac:dyDescent="0.25">
       <c r="B16" s="53"/>
       <c r="C16" s="52"/>
       <c r="D16" s="30" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
     </row>
     <row r="17" spans="2:4" ht="45" x14ac:dyDescent="0.25">
       <c r="B17" s="50" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
       <c r="C17" s="48" t="s">
-        <v>177</v>
+        <v>173</v>
       </c>
       <c r="D17" s="28" t="s">
-        <v>178</v>
+        <v>174</v>
       </c>
     </row>
     <row r="18" spans="2:4" ht="45" x14ac:dyDescent="0.25">
       <c r="B18" s="53"/>
       <c r="C18" s="52"/>
       <c r="D18" s="30" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
     </row>
     <row r="19" spans="2:4" ht="60.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B19" s="50" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="C19" s="48" t="s">
-        <v>181</v>
+        <v>177</v>
       </c>
       <c r="D19" s="28" t="s">
-        <v>182</v>
+        <v>178</v>
       </c>
     </row>
     <row r="20" spans="2:4" ht="30" x14ac:dyDescent="0.25">
       <c r="B20" s="53"/>
       <c r="C20" s="52"/>
       <c r="D20" s="30" t="s">
-        <v>183</v>
+        <v>179</v>
       </c>
     </row>
     <row r="21" spans="2:4" ht="45" x14ac:dyDescent="0.25">
       <c r="B21" s="50" t="s">
-        <v>184</v>
+        <v>180</v>
       </c>
       <c r="C21" s="48" t="s">
-        <v>185</v>
+        <v>181</v>
       </c>
       <c r="D21" s="28" t="s">
-        <v>186</v>
+        <v>182</v>
       </c>
     </row>
     <row r="22" spans="2:4" ht="30" x14ac:dyDescent="0.25">
       <c r="B22" s="51"/>
       <c r="C22" s="49"/>
       <c r="D22" s="31" t="s">
-        <v>187</v>
+        <v>183</v>
       </c>
     </row>
   </sheetData>
@@ -7032,25 +7068,25 @@
   <sheetData>
     <row r="2" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A2" s="47" t="s">
-        <v>188</v>
+        <v>184</v>
       </c>
       <c r="B2" s="47"/>
       <c r="C2" s="47"/>
       <c r="F2" s="47" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="G2" s="47"/>
       <c r="H2" s="47"/>
     </row>
     <row r="3" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>190</v>
+        <v>186</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>21</v>
       </c>
       <c r="F3" t="s">
-        <v>190</v>
+        <v>186</v>
       </c>
       <c r="G3" s="1" t="s">
         <v>26</v>
@@ -7074,14 +7110,14 @@
     </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>191</v>
+        <v>187</v>
       </c>
       <c r="B5">
         <f>SUM(C10:C14)</f>
         <v>5000</v>
       </c>
       <c r="F5" t="s">
-        <v>191</v>
+        <v>187</v>
       </c>
       <c r="G5">
         <f>SUM(H10:H14)</f>
@@ -7090,14 +7126,14 @@
     </row>
     <row r="6" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
       <c r="B6">
         <f>SUM(C17:C19)</f>
         <v>2000</v>
       </c>
       <c r="F6" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
       <c r="G6">
         <f>SUM(H17:H19)</f>
@@ -7119,7 +7155,7 @@
         <v>2</v>
       </c>
       <c r="B9" s="17" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="C9" s="17" t="s">
         <v>3</v>
@@ -7128,7 +7164,7 @@
         <v>2</v>
       </c>
       <c r="G9" s="17" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="H9" s="17" t="s">
         <v>3</v>
@@ -7315,19 +7351,19 @@
     </row>
     <row r="16" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A16" s="17" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="B16" s="17" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="C16" t="s">
         <v>3</v>
       </c>
       <c r="F16" s="17" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="G16" s="17" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="H16" t="s">
         <v>3</v>

</xml_diff>

<commit_message>
Updated with new rules
Updated with new rules version 2 with department dice
</commit_message>
<xml_diff>
--- a/ShipCardGameCalcs.xlsx
+++ b/ShipCardGameCalcs.xlsx
@@ -1,28 +1,32 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27226"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MultiplayerGame\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2FDE9412-D2BF-4730-BF55-A39F428F72A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{46FE794F-886C-463B-B0ED-03A30A33612D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="3" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Values" sheetId="1" r:id="rId1"/>
     <sheet name="Ships and Crew Details" sheetId="3" r:id="rId2"/>
     <sheet name="Game Setup" sheetId="7" r:id="rId3"/>
     <sheet name="Game Rules and Turn Example" sheetId="4" r:id="rId4"/>
-    <sheet name="Ideas" sheetId="6" r:id="rId5"/>
-    <sheet name="Card Details" sheetId="5" r:id="rId6"/>
-    <sheet name="Comparison" sheetId="2" r:id="rId7"/>
+    <sheet name="Game Rules version 2" sheetId="8" r:id="rId5"/>
+    <sheet name="Ideas" sheetId="6" r:id="rId6"/>
+    <sheet name="Card Details" sheetId="5" r:id="rId7"/>
+    <sheet name="Comparison" sheetId="2" r:id="rId8"/>
   </sheets>
   <calcPr calcId="191028"/>
   <extLst>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+      <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
@@ -39,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="406" uniqueCount="198">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="471" uniqueCount="246">
   <si>
     <t>Ship Parameters</t>
   </si>
@@ -364,18 +368,39 @@
     <t>Untap Phase</t>
   </si>
   <si>
+    <t>Current player untaps all their cards unless stated otherwise</t>
+  </si>
+  <si>
     <t>All player ships shield damaged, restore 100 shield</t>
   </si>
   <si>
     <t>Draw Phase</t>
   </si>
   <si>
+    <t>Current player chooses to draw from their Strategy or Crew Deck</t>
+  </si>
+  <si>
     <t>Players can draw either 1 card from the strategy deck, or they can choose the see the top 3 cards of the crew deck and then get to pick 1. The rest get sent to the bottom of the crew deck.</t>
   </si>
   <si>
     <t>Strategy Phase</t>
   </si>
   <si>
+    <t>Current player can play their cards, tap to gain department resourse or tap cards to use gun slots</t>
+  </si>
+  <si>
+    <t>Battle Phase</t>
+  </si>
+  <si>
+    <t>Current player taps to use gun slots, announcing targets</t>
+  </si>
+  <si>
+    <t>Reaction Phase</t>
+  </si>
+  <si>
+    <t>This is where any player can play cards to react to the battle phase, such as playing a tactic card to change the ships target</t>
+  </si>
+  <si>
     <t>End Phase</t>
   </si>
   <si>
@@ -463,6 +488,9 @@
     <t>Taking Damage</t>
   </si>
   <si>
+    <t>When a ship takes hull damage, sacrifice either 1 crew member card or ship attachment card from the ship. Only do this once per strategy phase</t>
+  </si>
+  <si>
     <t>Ship Destroyed</t>
   </si>
   <si>
@@ -487,6 +515,156 @@
     <t>When only 1 player remains in the game they win</t>
   </si>
   <si>
+    <t>Game Rules Version 2</t>
+  </si>
+  <si>
+    <t>In this version we have given each player dice to represent each of their chosen departments in their deck</t>
+  </si>
+  <si>
+    <t>By doing this means that players aren't fully reliant on their crew cards for resource</t>
+  </si>
+  <si>
+    <t>Setup</t>
+  </si>
+  <si>
+    <t>Players agree amount of ship points in the game, for example 2000 points</t>
+  </si>
+  <si>
+    <t>Players choose their ships up to the amount of points, with 2000 points player A could have 1 Capital Ship, whereas Player B could have 1 Cruiser and 1 Frigate</t>
+  </si>
+  <si>
+    <t>Note that when picking your ship layout you must have at least 1 ship that can hold a captain</t>
+  </si>
+  <si>
+    <t>Players will have 2 decks each, one being a Strategy card deck and the other being a crew card deck.</t>
+  </si>
+  <si>
+    <t>A strategy deck will consist of 40 cards</t>
+  </si>
+  <si>
+    <t>A crew deck will consist of 30 cards</t>
+  </si>
+  <si>
+    <t>Then players will have d20's (dice with 20 sides) to represent each department used in their decks. For example if Player A has Research and Handling departments in their deck then they will have 2 d20s.</t>
+  </si>
+  <si>
+    <t>There are a total of 5 different departments, Handling, Research, Engineer, Assault and Medic</t>
+  </si>
+  <si>
+    <t>Players will start by shuffling each of their decks, once shuffled their opponent will cut each deck.</t>
+  </si>
+  <si>
+    <t>Below is an example layout of the play area also known as the "Space Zone"</t>
+  </si>
+  <si>
+    <t>The Space Field is where players place their chosen ship cards and play all their cards</t>
+  </si>
+  <si>
+    <t>The Junkyard Zone are where Strategy cards go after they have been played (Note that some Strategy cards can stay on the Ships Zone)</t>
+  </si>
+  <si>
+    <t>The Stasis Zone are where Crew cards go after they have been played and destroyed</t>
+  </si>
+  <si>
+    <t>Player A</t>
+  </si>
+  <si>
+    <t>Space FIeld</t>
+  </si>
+  <si>
+    <t>Junkyard Zone</t>
+  </si>
+  <si>
+    <t>Stasis Zone</t>
+  </si>
+  <si>
+    <t>Department Dice</t>
+  </si>
+  <si>
+    <t>Player B</t>
+  </si>
+  <si>
+    <t>Players will now draw 2 cards from their crew deck and 3 from their strategy deck</t>
+  </si>
+  <si>
+    <t>Each player may choose to have 1 free mulligen, after that if they mulligen anymore times then they reduce the amount of cards they get to keep in their hand by 1 each time. Down to a minimum of 1 strategy card and 1 crew card</t>
+  </si>
+  <si>
+    <t>Now the players will randomly pick which player goes first</t>
+  </si>
+  <si>
+    <t>Once players have setup each of their sides they are ready to play.</t>
+  </si>
+  <si>
+    <t>Game Start</t>
+  </si>
+  <si>
+    <t>There are different phases during each players turns which run in the following order which only the current player does on their turn:</t>
+  </si>
+  <si>
+    <t>Here you untap any cards out on the space field unless stated otherwise</t>
+  </si>
+  <si>
+    <t>Crew Hire Phase</t>
+  </si>
+  <si>
+    <t>Increment 1 of your department dice by 1 (Note you start off at 0 and a department dice goes up to a max of 20 each)</t>
+  </si>
+  <si>
+    <t>Choose to draw from either the strategy deck or crew deck, note in a 1v1 the first player does not draw any cards on their first turn</t>
+  </si>
+  <si>
+    <t>You can start playing any amount of cards as long they meet the card cost, except for tier 1 crew cards as only 1 tier 1 crew card can be played on your turn.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Also there can only ever be 1 admiral card on your side of the space field at any one time. Certain cards can also be played during your opponents turn at different phases.</t>
+  </si>
+  <si>
+    <t>To pay for the cost to play cards you will need to either tap a crew card or use some of your department dice resource by decreasing the department dice. You can use the  combination of crew cards and department dice</t>
+  </si>
+  <si>
+    <t>Note that when using the department dice you don't regain what you had next turn.</t>
+  </si>
+  <si>
+    <t>You can only assign crew cards to a ship if there is a free crew slot available</t>
+  </si>
+  <si>
+    <t>If you have any tier 1,2 or 3 crew members untapped they can be used to tap and assigned to a gun slot and fire at an enemy ship.</t>
+  </si>
+  <si>
+    <t>If for example a ship has 3 gun slots, then only 3 crew cards can be assigned to a gun slot</t>
+  </si>
+  <si>
+    <t>Once you have assigned all targets, the assigned player can react with cards and use other ships to maneuver in front of the targeted ship making them the target (this requires at least 1 tier 1,2 or 3 crew member on that ship to tap).</t>
+  </si>
+  <si>
+    <t>Damage Phase</t>
+  </si>
+  <si>
+    <t>Calculate all the damage from the battle and reaction phase and remove any destroyed ship cards out of play.</t>
+  </si>
+  <si>
+    <t>When damaging ships players will first have to take out the ships shields before then taking out the ships hull.</t>
+  </si>
+  <si>
+    <t>Once the ships hull reaches 0 at any point it is destroyed</t>
+  </si>
+  <si>
+    <t>All other cards attached to the ship are sent to either Stasis or Junkyard</t>
+  </si>
+  <si>
+    <t xml:space="preserve">If you have the last remaining ship/s in play, you win. </t>
+  </si>
+  <si>
+    <t>Otherwise if you have more cards in your hand than your current max hand size then reduce down to your max hand size.</t>
+  </si>
+  <si>
+    <t>You keep any unspent dice department resource NOT crew card resource</t>
+  </si>
+  <si>
+    <t>Now the turn gets moved to the next player on your left and they start their untap phase.</t>
+  </si>
+  <si>
     <t>Controlled deck is the battlefield conditions which affects the battlefield</t>
   </si>
   <si>
@@ -634,12 +812,6 @@
     <t>Crew Attachment cards can only be played on your turn</t>
   </si>
   <si>
-    <t>Player A</t>
-  </si>
-  <si>
-    <t>Player B</t>
-  </si>
-  <si>
     <t>Fleet Option</t>
   </si>
   <si>
@@ -650,37 +822,13 @@
   </si>
   <si>
     <t>No. of</t>
-  </si>
-  <si>
-    <t>Battle Phase</t>
-  </si>
-  <si>
-    <t>Reaction Phase</t>
-  </si>
-  <si>
-    <t>This is where any player can play cards to react to the battle phase, such as playing a tactic card to change the ships target</t>
-  </si>
-  <si>
-    <t>When a ship takes hull damage, sacrifice either 1 crew member card or ship attachment card from the ship. Only do this once per strategy phase</t>
-  </si>
-  <si>
-    <t>Current player taps to use gun slots, announcing targets</t>
-  </si>
-  <si>
-    <t>Current player can play their cards, tap to gain department resourse or tap cards to use gun slots</t>
-  </si>
-  <si>
-    <t>Current player chooses to draw from their Strategy or Crew Deck</t>
-  </si>
-  <si>
-    <t>Current player untaps all their cards unless stated otherwise</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="10">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -737,8 +885,24 @@
       <family val="2"/>
       <charset val="1"/>
     </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="9">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -787,8 +951,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="23">
+  <borders count="25">
     <border>
       <left/>
       <right/>
@@ -1048,11 +1218,35 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="medium">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="55">
+  <cellXfs count="70">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1171,7 +1365,40 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="23" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="24" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1180,6 +1407,14 @@
     <dxf>
       <fill>
         <patternFill patternType="none">
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
           <fgColor indexed="64"/>
           <bgColor indexed="65"/>
         </patternFill>
@@ -1274,23 +1509,15 @@
     <dxf>
       <fill>
         <patternFill patternType="none">
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
     </dxf>
     <dxf>
       <fill>
         <patternFill patternType="none">
           <fgColor indexed="64"/>
           <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <bgColor auto="1"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1402,6 +1629,13 @@
     </dxf>
     <dxf>
       <border outline="0">
+        <bottom style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
         <left style="thin">
           <color theme="4" tint="0.39997558519241921"/>
         </left>
@@ -1420,13 +1654,6 @@
           <bgColor indexed="65"/>
         </patternFill>
       </fill>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <bottom style="thin">
-          <color theme="4" tint="0.39997558519241921"/>
-        </bottom>
-      </border>
     </dxf>
     <dxf>
       <font>
@@ -1742,6 +1969,13 @@
     </dxf>
     <dxf>
       <border outline="0">
+        <bottom style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
         <left style="thin">
           <color theme="4" tint="0.39997558519241921"/>
         </left>
@@ -1778,13 +2012,6 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <border outline="0">
-        <bottom style="thin">
-          <color theme="4" tint="0.39997558519241921"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
       <font>
         <b/>
         <i val="0"/>
@@ -1835,6 +2062,9 @@
       </border>
     </dxf>
     <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0" outline="0">
         <left/>
@@ -1856,6 +2086,7 @@
       </border>
     </dxf>
     <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -1866,10 +2097,6 @@
         <top/>
         <bottom/>
       </border>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <border diagonalUp="0" diagonalDown="0" outline="0">
@@ -1914,9 +2141,6 @@
       </border>
     </dxf>
     <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
@@ -1960,6 +2184,9 @@
     </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -2032,9 +2259,6 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -2049,6 +2273,9 @@
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -2085,6 +2312,7 @@
       </border>
     </dxf>
     <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
       <fill>
         <patternFill patternType="none">
           <fgColor indexed="64"/>
@@ -2094,7 +2322,6 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
       <fill>
         <patternFill patternType="none">
           <fgColor indexed="64"/>
@@ -2104,6 +2331,7 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
       <fill>
         <patternFill patternType="none">
           <fgColor indexed="64"/>
@@ -2113,7 +2341,6 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
       <fill>
         <patternFill patternType="none">
           <fgColor indexed="64"/>
@@ -2123,6 +2350,7 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
       <fill>
         <patternFill patternType="none">
           <fgColor indexed="64"/>
@@ -2132,7 +2360,6 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
       <fill>
         <patternFill patternType="none">
           <fgColor indexed="64"/>
@@ -2142,6 +2369,7 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
       <fill>
         <patternFill patternType="none">
           <fgColor indexed="64"/>
@@ -2151,7 +2379,6 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
       <fill>
         <patternFill patternType="none">
           <fgColor indexed="64"/>
@@ -2161,6 +2388,7 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
       <fill>
         <patternFill patternType="none">
           <fgColor indexed="64"/>
@@ -2170,7 +2398,6 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
       <fill>
         <patternFill patternType="none">
           <fgColor indexed="64"/>
@@ -2180,6 +2407,7 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
       <fill>
         <patternFill patternType="none">
           <fgColor indexed="64"/>
@@ -2189,7 +2417,6 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
       <fill>
         <patternFill patternType="none">
           <fgColor indexed="64"/>
@@ -2199,6 +2426,7 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
       <fill>
         <patternFill patternType="none">
           <fgColor indexed="64"/>
@@ -2208,7 +2436,6 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
       <fill>
         <patternFill patternType="none">
           <fgColor indexed="64"/>
@@ -2216,14 +2443,6 @@
         </patternFill>
       </fill>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
     </dxf>
     <dxf>
       <font>
@@ -2251,6 +2470,14 @@
     <dxf>
       <fill>
         <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
           <bgColor auto="1"/>
         </patternFill>
       </fill>
@@ -2355,6 +2582,14 @@
     <dxf>
       <fill>
         <patternFill patternType="none">
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
           <fgColor indexed="64"/>
           <bgColor indexed="65"/>
         </patternFill>
@@ -2447,6 +2682,7 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
       <fill>
         <patternFill patternType="none">
           <bgColor indexed="65"/>
@@ -2464,26 +2700,17 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill patternType="none">
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
     </dxf>
     <dxf>
       <fill>
         <patternFill patternType="none">
           <fgColor indexed="64"/>
           <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <bgColor auto="1"/>
         </patternFill>
       </fill>
     </dxf>
@@ -2527,9 +2754,6 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
       <fill>
         <patternFill patternType="none">
           <fgColor indexed="64"/>
@@ -2597,6 +2821,9 @@
         </patternFill>
       </fill>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <fill>
@@ -2732,12 +2959,12 @@
   <autoFilter ref="A9:G14" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="7">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Option" totalsRowLabel="Total" dataDxfId="129"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="A" totalsRowFunction="sum" dataDxfId="128" totalsRowDxfId="127"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="B" totalsRowFunction="sum" dataDxfId="126" totalsRowDxfId="125"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="C" totalsRowFunction="sum" dataDxfId="124" totalsRowDxfId="123"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="D" totalsRowFunction="sum" dataDxfId="122" totalsRowDxfId="121"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="E" totalsRowFunction="sum" dataDxfId="120" totalsRowDxfId="119"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="F" totalsRowFunction="sum" dataDxfId="118" totalsRowDxfId="117"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="A" totalsRowFunction="sum" dataDxfId="127" totalsRowDxfId="128"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="B" totalsRowFunction="sum" dataDxfId="125" totalsRowDxfId="126"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="C" totalsRowFunction="sum" dataDxfId="123" totalsRowDxfId="124"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="D" totalsRowFunction="sum" dataDxfId="121" totalsRowDxfId="122"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="E" totalsRowFunction="sum" dataDxfId="119" totalsRowDxfId="120"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="F" totalsRowFunction="sum" dataDxfId="117" totalsRowDxfId="118"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium15" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2747,23 +2974,23 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="14" xr:uid="{00000000-000C-0000-FFFF-FFFF09000000}" name="TblFltCrewSizes" displayName="TblFltCrewSizes" ref="A17:G21" totalsRowCount="1" headerRowDxfId="15" dataDxfId="14">
   <autoFilter ref="A17:G20" xr:uid="{00000000-0009-0000-0100-00000E000000}"/>
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0900-000001000000}" name="Option" totalsRowLabel="Total" dataDxfId="13" totalsRowDxfId="12"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0900-000002000000}" name="A" totalsRowFunction="custom" dataDxfId="11" totalsRowDxfId="10">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0900-000001000000}" name="Option" totalsRowLabel="Total" dataDxfId="12" totalsRowDxfId="13"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0900-000002000000}" name="A" totalsRowFunction="custom" dataDxfId="10" totalsRowDxfId="11">
       <totalsRowFormula>SUBTOTAL(109,TblFltCrewSizes[A])</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0900-000003000000}" name="B" totalsRowFunction="custom" dataDxfId="9" totalsRowDxfId="8">
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0900-000003000000}" name="B" totalsRowFunction="custom" dataDxfId="8" totalsRowDxfId="9">
       <totalsRowFormula>SUBTOTAL(109,TblFltCrewSizes[B])</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0900-000004000000}" name="C" totalsRowFunction="custom" dataDxfId="7" totalsRowDxfId="6">
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0900-000004000000}" name="C" totalsRowFunction="custom" dataDxfId="6" totalsRowDxfId="7">
       <totalsRowFormula>SUBTOTAL(109,TblFltCrewSizes[C])</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0900-000005000000}" name="D" totalsRowFunction="custom" dataDxfId="5" totalsRowDxfId="4">
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0900-000005000000}" name="D" totalsRowFunction="custom" dataDxfId="4" totalsRowDxfId="5">
       <totalsRowFormula>SUBTOTAL(109,TblFltCrewSizes[D])</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0900-000006000000}" name="E" totalsRowFunction="custom" dataDxfId="3" totalsRowDxfId="2">
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0900-000006000000}" name="E" totalsRowFunction="custom" dataDxfId="2" totalsRowDxfId="3">
       <totalsRowFormula>SUBTOTAL(109,TblFltCrewSizes[E])</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0900-000007000000}" name="F" totalsRowFunction="sum" dataDxfId="1" totalsRowDxfId="0"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0900-000007000000}" name="F" totalsRowFunction="sum" dataDxfId="0" totalsRowDxfId="1"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium13" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2773,26 +3000,26 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="TblFleetShipValues" displayName="TblFleetShipValues" ref="J9:Q15" totalsRowCount="1" headerRowDxfId="116" dataDxfId="115" totalsRowDxfId="114">
   <autoFilter ref="J9:Q14" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
   <tableColumns count="8">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="Option" totalsRowLabel="Total " dataDxfId="113" totalsRowDxfId="112"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="A" totalsRowFunction="sum" dataDxfId="111" totalsRowDxfId="110">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="Option" totalsRowLabel="Total " dataDxfId="112" totalsRowDxfId="113"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="A" totalsRowFunction="sum" dataDxfId="110" totalsRowDxfId="111">
       <calculatedColumnFormula>(INDEX(TblBattlefieldFlt[[A]:[F]],MATCH(TblFleetShipValues[[#This Row],[Option]],TblBattlefieldFlt[Option],0),MATCH(TblFleetShipValues[[#Headers],[A]],TblBattlefieldFlt[[#Headers],[A]:[F]],0)))*(INDEX(TblShipPoints[Points],MATCH(TblFleetShipValues[[#This Row],[Option]],TblShipPoints[Ships],0)))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0100-000003000000}" name="B" totalsRowFunction="sum" dataDxfId="109" totalsRowDxfId="108">
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0100-000003000000}" name="B" totalsRowFunction="sum" dataDxfId="108" totalsRowDxfId="109">
       <calculatedColumnFormula>C10*#REF!</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0100-000004000000}" name="C" totalsRowFunction="sum" dataDxfId="107" totalsRowDxfId="106">
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0100-000004000000}" name="C" totalsRowFunction="sum" dataDxfId="106" totalsRowDxfId="107">
       <calculatedColumnFormula>D10*#REF!</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0100-000005000000}" name="D" totalsRowFunction="sum" dataDxfId="105" totalsRowDxfId="104">
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0100-000005000000}" name="D" totalsRowFunction="sum" dataDxfId="104" totalsRowDxfId="105">
       <calculatedColumnFormula>E10*#REF!</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0100-000006000000}" name="E" totalsRowFunction="sum" dataDxfId="103" totalsRowDxfId="102">
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0100-000006000000}" name="E" totalsRowFunction="sum" dataDxfId="102" totalsRowDxfId="103">
       <calculatedColumnFormula>F10*#REF!</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0100-000007000000}" name="F" totalsRowFunction="sum" dataDxfId="101" totalsRowDxfId="100">
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0100-000007000000}" name="F" totalsRowFunction="sum" dataDxfId="100" totalsRowDxfId="101">
       <calculatedColumnFormula>G10*#REF!</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0100-000008000000}" name="Name" dataDxfId="99" totalsRowDxfId="98"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0100-000008000000}" name="Name" dataDxfId="98" totalsRowDxfId="99"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium13" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2815,26 +3042,26 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{00000000-000C-0000-FFFF-FFFF03000000}" name="TblAdjFleetRolesValues" displayName="TblAdjFleetRolesValues" ref="A24:H30" totalsRowCount="1" headerRowDxfId="91" dataDxfId="90" totalsRowDxfId="89">
   <autoFilter ref="A24:H29" xr:uid="{00000000-0009-0000-0100-000006000000}"/>
   <tableColumns count="8">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0300-000001000000}" name="Option" totalsRowLabel="Total" dataDxfId="88" totalsRowDxfId="87"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0300-000002000000}" name="A" totalsRowFunction="sum" dataDxfId="86" totalsRowDxfId="85">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0300-000001000000}" name="Option" totalsRowLabel="Total" dataDxfId="87" totalsRowDxfId="88"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0300-000002000000}" name="A" totalsRowFunction="sum" dataDxfId="85" totalsRowDxfId="86">
       <calculatedColumnFormula>(INDEX(TblBattlefieldFlt[[A]:[F]],MATCH($A25,TblBattlefieldFlt[Option],0),MATCH(B$24,TblBattlefieldFlt[[#Headers],[A]:[F]],0)))*(INDEX(TblShipCrew[Adjusted],MATCH($A25,TblShipCrew[Ships],0)))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0300-000003000000}" name="B" totalsRowFunction="sum" dataDxfId="84" totalsRowDxfId="83">
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0300-000003000000}" name="B" totalsRowFunction="sum" dataDxfId="83" totalsRowDxfId="84">
       <calculatedColumnFormula>(INDEX(TblBattlefieldFlt[[A]:[F]],MATCH($A25,TblBattlefieldFlt[Option],0),MATCH(C$24,TblBattlefieldFlt[[#Headers],[A]:[F]],0)))*(INDEX(TblShipCrew[Adjusted],MATCH($A25,TblShipCrew[Ships],0)))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0300-000004000000}" name="C" totalsRowFunction="sum" dataDxfId="82" totalsRowDxfId="81">
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0300-000004000000}" name="C" totalsRowFunction="sum" dataDxfId="81" totalsRowDxfId="82">
       <calculatedColumnFormula>(INDEX(TblBattlefieldFlt[[A]:[F]],MATCH($A25,TblBattlefieldFlt[Option],0),MATCH(D$24,TblBattlefieldFlt[[#Headers],[A]:[F]],0)))*(INDEX(TblShipCrew[Adjusted],MATCH($A25,TblShipCrew[Ships],0)))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0300-000005000000}" name="D" totalsRowFunction="sum" dataDxfId="80" totalsRowDxfId="79">
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0300-000005000000}" name="D" totalsRowFunction="sum" dataDxfId="79" totalsRowDxfId="80">
       <calculatedColumnFormula>(INDEX(TblBattlefieldFlt[[A]:[F]],MATCH($A25,TblBattlefieldFlt[Option],0),MATCH(E$24,TblBattlefieldFlt[[#Headers],[A]:[F]],0)))*(INDEX(TblShipCrew[Adjusted],MATCH($A25,TblShipCrew[Ships],0)))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0300-000006000000}" name="E" totalsRowFunction="sum" dataDxfId="78" totalsRowDxfId="77">
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0300-000006000000}" name="E" totalsRowFunction="sum" dataDxfId="77" totalsRowDxfId="78">
       <calculatedColumnFormula>(INDEX(TblBattlefieldFlt[[A]:[F]],MATCH($A25,TblBattlefieldFlt[Option],0),MATCH(F$24,TblBattlefieldFlt[[#Headers],[A]:[F]],0)))*(INDEX(TblShipCrew[Adjusted],MATCH($A25,TblShipCrew[Ships],0)))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0300-000007000000}" name="F" totalsRowFunction="sum" dataDxfId="76" totalsRowDxfId="75">
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0300-000007000000}" name="F" totalsRowFunction="sum" dataDxfId="75" totalsRowDxfId="76">
       <calculatedColumnFormula>(INDEX(TblBattlefieldFlt[[A]:[F]],MATCH($A25,TblBattlefieldFlt[Option],0),MATCH(G$24,TblBattlefieldFlt[[#Headers],[A]:[F]],0)))*(INDEX(TblShipCrew[Adjusted],MATCH($A25,TblShipCrew[Ships],0)))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0300-000008000000}" name="Name" dataDxfId="74" totalsRowDxfId="73"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0300-000008000000}" name="Name" dataDxfId="73" totalsRowDxfId="74"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium13" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2845,11 +3072,11 @@
   <autoFilter ref="A32:G42" xr:uid="{00000000-0009-0000-0100-000008000000}"/>
   <tableColumns count="7">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0400-000001000000}" name="Option" totalsRowLabel="Total"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0400-000002000000}" name="A" totalsRowFunction="sum" dataDxfId="71" totalsRowDxfId="70">
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0400-000002000000}" name="A" totalsRowFunction="sum" dataDxfId="70" totalsRowDxfId="71">
       <calculatedColumnFormula>K10</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0400-000003000000}" name="B" totalsRowFunction="sum" dataDxfId="69" totalsRowDxfId="68"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0400-000004000000}" name="C" totalsRowFunction="sum" dataDxfId="67" totalsRowDxfId="66"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0400-000003000000}" name="B" totalsRowFunction="sum" dataDxfId="68" totalsRowDxfId="69"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0400-000004000000}" name="C" totalsRowFunction="sum" dataDxfId="66" totalsRowDxfId="67"/>
     <tableColumn id="5" xr3:uid="{00000000-0010-0000-0400-000005000000}" name="D" totalsRowFunction="sum" totalsRowDxfId="65"/>
     <tableColumn id="6" xr3:uid="{00000000-0010-0000-0400-000006000000}" name="E" totalsRowFunction="sum" totalsRowDxfId="64"/>
     <tableColumn id="7" xr3:uid="{00000000-0010-0000-0400-000007000000}" name="F" totalsRowFunction="sum" totalsRowDxfId="63"/>
@@ -2863,25 +3090,25 @@
   <autoFilter ref="J24:Q29" xr:uid="{00000000-0009-0000-0100-000009000000}"/>
   <tableColumns count="8">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0500-000001000000}" name="Option" totalsRowLabel="Total" dataDxfId="60"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0500-000002000000}" name="A" totalsRowFunction="sum" dataDxfId="59" totalsRowDxfId="58">
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0500-000002000000}" name="A" totalsRowFunction="sum" dataDxfId="58" totalsRowDxfId="59">
       <calculatedColumnFormula>(INDEX(TblBattlefieldFlt[[A]:[F]],MATCH($J25,TblBattlefieldFlt[Option],0),MATCH(K$24,TblBattlefieldFlt[[#Headers],[A]:[F]],0)))*(INDEX(TblShipCrew[Generic (500)],MATCH($J25,TblShipCrew[Ships],0)))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0500-000003000000}" name="B" totalsRowFunction="sum" dataDxfId="57" totalsRowDxfId="56">
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0500-000003000000}" name="B" totalsRowFunction="sum" dataDxfId="56" totalsRowDxfId="57">
       <calculatedColumnFormula>(INDEX(TblBattlefieldFlt[[A]:[F]],MATCH($J25,TblBattlefieldFlt[Option],0),MATCH(L$24,TblBattlefieldFlt[[#Headers],[A]:[F]],0)))*(INDEX(TblShipCrew[Generic (500)],MATCH($J25,TblShipCrew[Ships],0)))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0500-000004000000}" name="C" totalsRowFunction="sum" dataDxfId="55" totalsRowDxfId="54">
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0500-000004000000}" name="C" totalsRowFunction="sum" dataDxfId="54" totalsRowDxfId="55">
       <calculatedColumnFormula>(INDEX(TblBattlefieldFlt[[A]:[F]],MATCH($J25,TblBattlefieldFlt[Option],0),MATCH(M$24,TblBattlefieldFlt[[#Headers],[A]:[F]],0)))*(INDEX(TblShipCrew[Generic (500)],MATCH($J25,TblShipCrew[Ships],0)))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0500-000005000000}" name="D" totalsRowFunction="sum" dataDxfId="53" totalsRowDxfId="52">
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0500-000005000000}" name="D" totalsRowFunction="sum" dataDxfId="52" totalsRowDxfId="53">
       <calculatedColumnFormula>(INDEX(TblBattlefieldFlt[[A]:[F]],MATCH($J25,TblBattlefieldFlt[Option],0),MATCH(N$24,TblBattlefieldFlt[[#Headers],[A]:[F]],0)))*(INDEX(TblShipCrew[Generic (500)],MATCH($J25,TblShipCrew[Ships],0)))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0500-000006000000}" name="E" totalsRowFunction="sum" dataDxfId="51" totalsRowDxfId="50">
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0500-000006000000}" name="E" totalsRowFunction="sum" dataDxfId="50" totalsRowDxfId="51">
       <calculatedColumnFormula>(INDEX(TblBattlefieldFlt[[A]:[F]],MATCH($J25,TblBattlefieldFlt[Option],0),MATCH(O$24,TblBattlefieldFlt[[#Headers],[A]:[F]],0)))*(INDEX(TblShipCrew[Generic (500)],MATCH($J25,TblShipCrew[Ships],0)))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0500-000007000000}" name="F" totalsRowFunction="sum" dataDxfId="49" totalsRowDxfId="48">
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0500-000007000000}" name="F" totalsRowFunction="sum" dataDxfId="48" totalsRowDxfId="49">
       <calculatedColumnFormula>(INDEX(TblBattlefieldFlt[[A]:[F]],MATCH($J25,TblBattlefieldFlt[Option],0),MATCH(P$24,TblBattlefieldFlt[[#Headers],[A]:[F]],0)))*(INDEX(TblShipCrew[Generic (500)],MATCH($J25,TblShipCrew[Ships],0)))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0500-000008000000}" name="Name" dataDxfId="47" totalsRowDxfId="46"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0500-000008000000}" name="Name" dataDxfId="46" totalsRowDxfId="47"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium10" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2892,11 +3119,11 @@
   <autoFilter ref="J32:P42" xr:uid="{00000000-0009-0000-0100-00000A000000}"/>
   <tableColumns count="7">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0600-000001000000}" name="Option" totalsRowLabel="Total" totalsRowDxfId="44"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0600-000002000000}" name="A" totalsRowFunction="sum" dataDxfId="43" totalsRowDxfId="42">
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0600-000002000000}" name="A" totalsRowFunction="sum" dataDxfId="42" totalsRowDxfId="43">
       <calculatedColumnFormula>T10</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0600-000003000000}" name="B" totalsRowFunction="sum" dataDxfId="41" totalsRowDxfId="40"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0600-000004000000}" name="C" totalsRowFunction="sum" dataDxfId="39" totalsRowDxfId="38"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0600-000003000000}" name="B" totalsRowFunction="sum" dataDxfId="40" totalsRowDxfId="41"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0600-000004000000}" name="C" totalsRowFunction="sum" dataDxfId="38" totalsRowDxfId="39"/>
     <tableColumn id="5" xr3:uid="{00000000-0010-0000-0600-000005000000}" name="D" totalsRowFunction="sum" totalsRowDxfId="37"/>
     <tableColumn id="6" xr3:uid="{00000000-0010-0000-0600-000006000000}" name="E" totalsRowFunction="sum" totalsRowDxfId="36"/>
     <tableColumn id="7" xr3:uid="{00000000-0010-0000-0600-000007000000}" name="F" totalsRowFunction="sum" totalsRowDxfId="35"/>
@@ -2906,7 +3133,7 @@
 </file>
 
 <file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="13" xr:uid="{00000000-000C-0000-FFFF-FFFF07000000}" name="TblShipCrew" displayName="TblShipCrew" ref="D2:L7" totalsRowShown="0" headerRowDxfId="34" dataDxfId="32" headerRowBorderDxfId="33" tableBorderDxfId="31">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="13" xr:uid="{00000000-000C-0000-FFFF-FFFF07000000}" name="TblShipCrew" displayName="TblShipCrew" ref="D2:L7" totalsRowShown="0" headerRowDxfId="34" dataDxfId="33" headerRowBorderDxfId="31" tableBorderDxfId="32">
   <autoFilter ref="D2:L7" xr:uid="{00000000-0009-0000-0100-00000D000000}"/>
   <tableColumns count="9">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0700-000001000000}" name="Ships" dataDxfId="30"/>
@@ -2934,7 +3161,7 @@
 </file>
 
 <file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="12" xr:uid="{00000000-000C-0000-FFFF-FFFF08000000}" name="TblShipPoints" displayName="TblShipPoints" ref="A2:B7" totalsRowShown="0" headerRowDxfId="21" dataDxfId="19" headerRowBorderDxfId="20" tableBorderDxfId="18">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="12" xr:uid="{00000000-000C-0000-FFFF-FFFF08000000}" name="TblShipPoints" displayName="TblShipPoints" ref="A2:B7" totalsRowShown="0" headerRowDxfId="21" dataDxfId="20" headerRowBorderDxfId="18" tableBorderDxfId="19">
   <autoFilter ref="A2:B7" xr:uid="{00000000-0009-0000-0100-00000C000000}"/>
   <tableColumns count="2">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0800-000001000000}" name="Ships" dataDxfId="17"/>
@@ -3247,7 +3474,7 @@
       <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="14.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="7" width="15.42578125" customWidth="1"/>
@@ -3265,7 +3492,7 @@
     <col min="24" max="24" width="10" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:17">
       <c r="A1" s="47" t="s">
         <v>0</v>
       </c>
@@ -3282,7 +3509,7 @@
       <c r="O1" s="47"/>
       <c r="P1" s="47"/>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:17">
       <c r="A2" s="9" t="s">
         <v>2</v>
       </c>
@@ -3329,7 +3556,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:17">
       <c r="A3" s="15" t="s">
         <v>13</v>
       </c>
@@ -3382,7 +3609,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:17">
       <c r="A4" s="10" t="s">
         <v>14</v>
       </c>
@@ -3423,7 +3650,7 @@
         <v>5500</v>
       </c>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:17">
       <c r="A5" s="10" t="s">
         <v>15</v>
       </c>
@@ -3464,7 +3691,7 @@
         <v>3500</v>
       </c>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:17">
       <c r="A6" s="10" t="s">
         <v>16</v>
       </c>
@@ -3505,7 +3732,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:17">
       <c r="A7" t="s">
         <v>17</v>
       </c>
@@ -3546,7 +3773,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:17">
       <c r="A8" s="47" t="s">
         <v>18</v>
       </c>
@@ -3567,7 +3794,7 @@
       <c r="P8" s="47"/>
       <c r="Q8" s="47"/>
     </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:17">
       <c r="A9" s="8" t="s">
         <v>20</v>
       </c>
@@ -3615,7 +3842,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:17">
       <c r="A10" t="s">
         <v>13</v>
       </c>
@@ -3659,7 +3886,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:17">
       <c r="A11" t="s">
         <v>14</v>
       </c>
@@ -3705,7 +3932,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:17">
       <c r="A12" t="s">
         <v>15</v>
       </c>
@@ -3753,7 +3980,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:17">
       <c r="A13" t="s">
         <v>16</v>
       </c>
@@ -3799,7 +4026,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:17">
       <c r="A14" t="s">
         <v>17</v>
       </c>
@@ -3847,7 +4074,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:17">
       <c r="A15" t="s">
         <v>33</v>
       </c>
@@ -3904,7 +4131,7 @@
       </c>
       <c r="Q15" s="1"/>
     </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:17">
       <c r="A16" s="47" t="s">
         <v>35</v>
       </c>
@@ -3922,7 +4149,7 @@
       <c r="P16" s="1"/>
       <c r="Q16" s="1"/>
     </row>
-    <row r="17" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:18">
       <c r="A17" t="s">
         <v>20</v>
       </c>
@@ -3955,7 +4182,7 @@
       <c r="P17" s="1"/>
       <c r="Q17" s="1"/>
     </row>
-    <row r="18" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:18">
       <c r="A18" t="s">
         <v>4</v>
       </c>
@@ -3994,7 +4221,7 @@
       <c r="P18" s="1"/>
       <c r="Q18" s="1"/>
     </row>
-    <row r="19" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:18">
       <c r="A19" t="s">
         <v>5</v>
       </c>
@@ -4033,7 +4260,7 @@
       <c r="P19" s="1"/>
       <c r="Q19" s="1"/>
     </row>
-    <row r="20" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:18">
       <c r="A20" t="s">
         <v>6</v>
       </c>
@@ -4072,7 +4299,7 @@
       <c r="P20" s="1"/>
       <c r="Q20" s="1"/>
     </row>
-    <row r="21" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:18">
       <c r="A21" t="s">
         <v>33</v>
       </c>
@@ -4109,7 +4336,7 @@
       <c r="P21" s="1"/>
       <c r="Q21" s="1"/>
     </row>
-    <row r="22" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:18">
       <c r="A22" s="4"/>
       <c r="B22" s="5"/>
       <c r="C22" s="5"/>
@@ -4129,7 +4356,7 @@
       <c r="Q22" s="4"/>
       <c r="R22" s="4"/>
     </row>
-    <row r="23" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:18">
       <c r="A23" s="47" t="s">
         <v>40</v>
       </c>
@@ -4152,7 +4379,7 @@
       <c r="P23" s="47"/>
       <c r="Q23" s="47"/>
     </row>
-    <row r="24" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:18">
       <c r="A24" s="8" t="s">
         <v>20</v>
       </c>
@@ -4203,7 +4430,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="25" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:18">
       <c r="A25" t="s">
         <v>13</v>
       </c>
@@ -4266,7 +4493,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="26" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:18">
       <c r="A26" t="s">
         <v>14</v>
       </c>
@@ -4329,7 +4556,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="27" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:18">
       <c r="A27" t="s">
         <v>15</v>
       </c>
@@ -4392,7 +4619,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="28" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:18">
       <c r="A28" t="s">
         <v>16</v>
       </c>
@@ -4455,7 +4682,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="29" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:18">
       <c r="A29" t="s">
         <v>17</v>
       </c>
@@ -4518,7 +4745,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="30" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:18">
       <c r="A30" t="s">
         <v>33</v>
       </c>
@@ -4577,7 +4804,7 @@
       </c>
       <c r="Q30" s="1"/>
     </row>
-    <row r="31" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:18">
       <c r="A31" s="47" t="s">
         <v>47</v>
       </c>
@@ -4598,7 +4825,7 @@
       <c r="O31" s="47"/>
       <c r="P31" s="47"/>
     </row>
-    <row r="32" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:18">
       <c r="A32" t="s">
         <v>20</v>
       </c>
@@ -4643,7 +4870,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="33" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:16">
       <c r="A33" t="s">
         <v>28</v>
       </c>
@@ -4700,7 +4927,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:16">
       <c r="A34" t="s">
         <v>42</v>
       </c>
@@ -4757,7 +4984,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:16">
       <c r="A35" t="s">
         <v>29</v>
       </c>
@@ -4814,7 +5041,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:16">
       <c r="A36" t="s">
         <v>43</v>
       </c>
@@ -4871,7 +5098,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:16">
       <c r="A37" t="s">
         <v>30</v>
       </c>
@@ -4928,7 +5155,7 @@
         <v>2500</v>
       </c>
     </row>
-    <row r="38" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:16">
       <c r="A38" t="s">
         <v>44</v>
       </c>
@@ -4985,7 +5212,7 @@
         <v>3500</v>
       </c>
     </row>
-    <row r="39" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:16">
       <c r="A39" t="s">
         <v>31</v>
       </c>
@@ -5042,7 +5269,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:16">
       <c r="A40" t="s">
         <v>45</v>
       </c>
@@ -5099,7 +5326,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:16">
       <c r="A41" t="s">
         <v>32</v>
       </c>
@@ -5156,7 +5383,7 @@
         <v>5000</v>
       </c>
     </row>
-    <row r="42" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:16">
       <c r="A42" t="s">
         <v>46</v>
       </c>
@@ -5213,7 +5440,7 @@
         <v>5000</v>
       </c>
     </row>
-    <row r="43" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:16">
       <c r="A43" t="s">
         <v>33</v>
       </c>
@@ -5270,17 +5497,17 @@
         <v>16000</v>
       </c>
     </row>
-    <row r="45" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:16">
       <c r="C45" s="1"/>
       <c r="D45" s="1"/>
       <c r="E45" s="1"/>
       <c r="F45" s="1"/>
       <c r="G45" s="1"/>
     </row>
-    <row r="50" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="50" spans="2:2">
       <c r="B50" s="1"/>
     </row>
-    <row r="51" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="51" spans="2:2">
       <c r="B51" s="1"/>
     </row>
   </sheetData>
@@ -5321,10 +5548,10 @@
   <dimension ref="B1:V29"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F26" sqref="F26"/>
+      <selection activeCell="J19" sqref="J19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="2" max="2" width="16.5703125" customWidth="1"/>
     <col min="3" max="3" width="18" customWidth="1"/>
@@ -5335,12 +5562,12 @@
     <col min="13" max="13" width="34" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:22" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:22">
       <c r="M1" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="2" spans="2:22" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:22">
       <c r="B2" s="21" t="s">
         <v>2</v>
       </c>
@@ -5381,7 +5608,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="3" spans="2:22" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:22">
       <c r="B3" s="25" t="s">
         <v>13</v>
       </c>
@@ -5442,7 +5669,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="2:22" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:22">
       <c r="B4" s="26" t="s">
         <v>14</v>
       </c>
@@ -5503,7 +5730,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="5" spans="2:22" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:22">
       <c r="B5" s="27" t="s">
         <v>15</v>
       </c>
@@ -5557,7 +5784,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="6" spans="2:22" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:22">
       <c r="B6" s="26" t="s">
         <v>16</v>
       </c>
@@ -5611,7 +5838,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="7" spans="2:22" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:22">
       <c r="B7" s="27" t="s">
         <v>17</v>
       </c>
@@ -5658,7 +5885,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="8" spans="2:22" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:22">
       <c r="L8">
         <v>6</v>
       </c>
@@ -5684,7 +5911,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="9" spans="2:22" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:22">
       <c r="L9">
         <v>7</v>
       </c>
@@ -5703,7 +5930,7 @@
         <v>600</v>
       </c>
     </row>
-    <row r="10" spans="2:22" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:22">
       <c r="B10" t="s">
         <v>56</v>
       </c>
@@ -5725,7 +5952,7 @@
         <v>700</v>
       </c>
     </row>
-    <row r="11" spans="2:22" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:22">
       <c r="B11" s="19" t="s">
         <v>57</v>
       </c>
@@ -5759,7 +5986,7 @@
         <v>800</v>
       </c>
     </row>
-    <row r="12" spans="2:22" ht="75" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:22" ht="75">
       <c r="B12" s="20" t="s">
         <v>62</v>
       </c>
@@ -5786,7 +6013,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="13" spans="2:22" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:22">
       <c r="L13">
         <v>11</v>
       </c>
@@ -5798,7 +6025,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="14" spans="2:22" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:22">
       <c r="L14">
         <v>12</v>
       </c>
@@ -5810,7 +6037,7 @@
         <v>1100</v>
       </c>
     </row>
-    <row r="15" spans="2:22" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:22">
       <c r="B15" s="21" t="s">
         <v>2</v>
       </c>
@@ -5827,7 +6054,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="16" spans="2:22" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:22">
       <c r="B16" s="22" t="s">
         <v>13</v>
       </c>
@@ -5844,7 +6071,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="17" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:12">
       <c r="B17" s="23" t="s">
         <v>14</v>
       </c>
@@ -5861,7 +6088,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="18" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:12">
       <c r="B18" s="22" t="s">
         <v>15</v>
       </c>
@@ -5878,7 +6105,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="19" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:12">
       <c r="B19" s="23" t="s">
         <v>16</v>
       </c>
@@ -5895,7 +6122,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="20" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:12">
       <c r="B20" s="22" t="s">
         <v>17</v>
       </c>
@@ -5912,17 +6139,17 @@
         <v>18</v>
       </c>
     </row>
-    <row r="21" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:12">
       <c r="L21">
         <v>19</v>
       </c>
     </row>
-    <row r="22" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:12">
       <c r="L22">
         <v>20</v>
       </c>
     </row>
-    <row r="23" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:12">
       <c r="B23" s="36" t="s">
         <v>20</v>
       </c>
@@ -5948,7 +6175,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="24" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:12">
       <c r="B24" s="38" t="s">
         <v>13</v>
       </c>
@@ -5964,7 +6191,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="25" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:12">
       <c r="B25" s="40" t="s">
         <v>14</v>
       </c>
@@ -5982,7 +6209,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="26" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:12">
       <c r="B26" s="38" t="s">
         <v>15</v>
       </c>
@@ -6002,7 +6229,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="27" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:12">
       <c r="B27" s="40" t="s">
         <v>16</v>
       </c>
@@ -6020,7 +6247,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="28" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:12">
       <c r="B28" s="38" t="s">
         <v>17</v>
       </c>
@@ -6040,7 +6267,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="29" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:12">
       <c r="C29">
         <f>C24*G3*F3</f>
         <v>1000</v>
@@ -6079,9 +6306,9 @@
       <selection activeCell="P25" sqref="P24:Q25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:19">
       <c r="D1">
         <v>38</v>
       </c>
@@ -6104,7 +6331,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:19">
       <c r="J2" t="s">
         <v>58</v>
       </c>
@@ -6112,7 +6339,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="3" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:19">
       <c r="B3" s="42"/>
       <c r="C3" s="42"/>
       <c r="D3" s="42"/>
@@ -6145,7 +6372,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="4" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:19">
       <c r="B4" s="45" t="s">
         <v>69</v>
       </c>
@@ -6168,7 +6395,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:19">
       <c r="B5" s="43" t="s">
         <v>70</v>
       </c>
@@ -6191,7 +6418,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:19">
       <c r="B6" s="45" t="s">
         <v>71</v>
       </c>
@@ -6214,7 +6441,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:19">
       <c r="B7" s="6" t="s">
         <v>72</v>
       </c>
@@ -6237,7 +6464,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:19">
       <c r="G8" s="6" t="s">
         <v>13</v>
       </c>
@@ -6260,7 +6487,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:19">
       <c r="N10" s="19" t="s">
         <v>57</v>
       </c>
@@ -6277,7 +6504,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="15" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:19">
       <c r="C15" s="44" t="s">
         <v>17</v>
       </c>
@@ -6294,19 +6521,19 @@
         <v>17</v>
       </c>
     </row>
-    <row r="16" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:19">
       <c r="P16">
         <f ca="1">RANDBETWEEN(0,123)</f>
-        <v>62</v>
-      </c>
-    </row>
-    <row r="17" spans="2:16" x14ac:dyDescent="0.25">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="17" spans="2:16">
       <c r="P17" s="46">
         <f ca="1">RANDBETWEEN(0,6)</f>
-        <v>3</v>
-      </c>
-    </row>
-    <row r="18" spans="2:16" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="18" spans="2:16">
       <c r="C18" s="44" t="s">
         <v>17</v>
       </c>
@@ -6323,12 +6550,12 @@
         <v>72</v>
       </c>
     </row>
-    <row r="19" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:16">
       <c r="L19" s="45" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="20" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:16">
       <c r="E20" s="44" t="s">
         <v>17</v>
       </c>
@@ -6339,12 +6566,12 @@
         <v>70</v>
       </c>
     </row>
-    <row r="21" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:16">
       <c r="L21" s="45" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="22" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:16">
       <c r="B22" s="2"/>
       <c r="C22" s="2"/>
       <c r="D22" s="2"/>
@@ -6359,7 +6586,7 @@
       <c r="K22" s="2"/>
       <c r="L22" s="2"/>
     </row>
-    <row r="24" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:16">
       <c r="E24">
         <v>64</v>
       </c>
@@ -6382,7 +6609,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="25" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:16">
       <c r="K25" t="s">
         <v>58</v>
       </c>
@@ -6399,361 +6626,358 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F5EC53A5-8F19-4711-93EA-0F4CBD261EC8}">
   <dimension ref="B2:B83"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
-      <selection activeCell="T29" sqref="T29"/>
+    <sheetView topLeftCell="A61" workbookViewId="0">
+      <selection activeCell="F83" sqref="F83"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="2" max="2" width="11.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:2">
       <c r="B2" s="21" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="3" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:2">
       <c r="B3" s="3" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="4" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:2">
       <c r="B4" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="5" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:2">
       <c r="B5" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="6" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:2">
       <c r="B6" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="7" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:2">
       <c r="B7" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="8" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:2">
       <c r="B8" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="9" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:2">
       <c r="B9" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="10" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:2">
       <c r="B10" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="11" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:2">
       <c r="B11" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="13" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:2">
       <c r="B13" s="3" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="14" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:2">
       <c r="B14" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="15" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:2">
       <c r="B15" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="17" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:2">
       <c r="B17" s="3" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="18" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:2">
       <c r="B18" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="19" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:2">
       <c r="B19" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="20" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:2">
       <c r="B20" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="21" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:2">
       <c r="B21" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="22" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:2">
       <c r="B22" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="24" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:2">
       <c r="B24" s="3" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="25" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:2">
       <c r="B25" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="26" spans="2:2" x14ac:dyDescent="0.25">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="26" spans="2:2">
       <c r="B26" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="28" spans="2:2" x14ac:dyDescent="0.25">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="28" spans="2:2">
       <c r="B28" s="3" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="29" spans="2:2" x14ac:dyDescent="0.25">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="29" spans="2:2">
       <c r="B29" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="30" spans="2:2" x14ac:dyDescent="0.25">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="30" spans="2:2">
       <c r="B30" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="32" spans="2:2" x14ac:dyDescent="0.25">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="32" spans="2:2">
       <c r="B32" s="3" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="33" spans="2:2" x14ac:dyDescent="0.25">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="33" spans="2:2">
       <c r="B33" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="35" spans="2:2" x14ac:dyDescent="0.25">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="35" spans="2:2">
       <c r="B35" s="3" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="36" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B36" s="54" t="s">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="37" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B37" s="54"/>
-    </row>
-    <row r="38" spans="2:2" x14ac:dyDescent="0.25">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="36" spans="2:2">
+      <c r="B36" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="38" spans="2:2">
       <c r="B38" s="3" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="39" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B39" s="54" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="41" spans="2:2" x14ac:dyDescent="0.25">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="39" spans="2:2">
+      <c r="B39" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="41" spans="2:2">
       <c r="B41" s="3" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="42" spans="2:2" x14ac:dyDescent="0.25">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="42" spans="2:2">
       <c r="B42" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="43" spans="2:2" x14ac:dyDescent="0.25">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="43" spans="2:2">
       <c r="B43" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="45" spans="2:2" x14ac:dyDescent="0.25">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="45" spans="2:2">
       <c r="B45" s="3" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="46" spans="2:2" x14ac:dyDescent="0.25">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="46" spans="2:2">
       <c r="B46" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="47" spans="2:2" x14ac:dyDescent="0.25">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="47" spans="2:2">
       <c r="B47" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="48" spans="2:2" x14ac:dyDescent="0.25">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="48" spans="2:2">
       <c r="B48" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="49" spans="2:2" x14ac:dyDescent="0.25">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="49" spans="2:2">
       <c r="B49" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="50" spans="2:2" x14ac:dyDescent="0.25">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="50" spans="2:2">
       <c r="B50" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="51" spans="2:2" x14ac:dyDescent="0.25">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="51" spans="2:2">
       <c r="B51" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="52" spans="2:2" x14ac:dyDescent="0.25">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="52" spans="2:2">
       <c r="B52" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="53" spans="2:2" x14ac:dyDescent="0.25">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="53" spans="2:2">
       <c r="B53" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="54" spans="2:2" x14ac:dyDescent="0.25">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="54" spans="2:2">
       <c r="B54" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="55" spans="2:2" x14ac:dyDescent="0.25">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="55" spans="2:2">
       <c r="B55" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="56" spans="2:2" x14ac:dyDescent="0.25">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="56" spans="2:2">
       <c r="B56" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="58" spans="2:2" x14ac:dyDescent="0.25">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="58" spans="2:2">
       <c r="B58" s="3" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="59" spans="2:2" x14ac:dyDescent="0.25">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="59" spans="2:2">
       <c r="B59" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="60" spans="2:2" x14ac:dyDescent="0.25">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="60" spans="2:2">
       <c r="B60" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="61" spans="2:2" x14ac:dyDescent="0.25">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="61" spans="2:2">
       <c r="B61" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="62" spans="2:2" x14ac:dyDescent="0.25">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="62" spans="2:2">
       <c r="B62" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="63" spans="2:2" x14ac:dyDescent="0.25">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="63" spans="2:2">
       <c r="B63" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="64" spans="2:2" x14ac:dyDescent="0.25">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="64" spans="2:2">
       <c r="B64" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="65" spans="2:2" x14ac:dyDescent="0.25">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="65" spans="2:2">
       <c r="B65" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="66" spans="2:2" x14ac:dyDescent="0.25">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="66" spans="2:2">
       <c r="B66" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="68" spans="2:2" x14ac:dyDescent="0.25">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="68" spans="2:2">
       <c r="B68" s="3" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="69" spans="2:2" x14ac:dyDescent="0.25">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="69" spans="2:2">
       <c r="B69" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="70" spans="2:2" x14ac:dyDescent="0.25">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="70" spans="2:2">
       <c r="B70" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="71" spans="2:2" x14ac:dyDescent="0.25">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="71" spans="2:2">
       <c r="B71" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="73" spans="2:2" x14ac:dyDescent="0.25">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="73" spans="2:2">
       <c r="B73" s="3" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="74" spans="2:2" x14ac:dyDescent="0.25">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="74" spans="2:2">
       <c r="B74" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="76" spans="2:2" x14ac:dyDescent="0.25">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="76" spans="2:2">
       <c r="B76" s="3" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="77" spans="2:2" x14ac:dyDescent="0.25">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="77" spans="2:2">
       <c r="B77" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="78" spans="2:2" x14ac:dyDescent="0.25">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="78" spans="2:2">
       <c r="B78" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="79" spans="2:2" x14ac:dyDescent="0.25">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="79" spans="2:2">
       <c r="B79" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="80" spans="2:2" x14ac:dyDescent="0.25">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="80" spans="2:2">
       <c r="B80" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="81" spans="2:2" x14ac:dyDescent="0.25">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="81" spans="2:2">
       <c r="B81" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="82" spans="2:2" x14ac:dyDescent="0.25">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="82" spans="2:2">
       <c r="B82" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="83" spans="2:2" x14ac:dyDescent="0.25">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="83" spans="2:2">
       <c r="B83" t="s">
-        <v>134</v>
+        <v>142</v>
       </c>
     </row>
   </sheetData>
@@ -6763,6 +6987,458 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{93013FD4-B940-4A70-A7DA-BF82FD0F616E}">
+  <dimension ref="A2:K81"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="P29" sqref="P29"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="2" max="2" width="16.140625" customWidth="1"/>
+    <col min="11" max="11" width="16" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:2" ht="23.25">
+      <c r="B2" s="54" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="4" spans="2:2">
+      <c r="B4" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="5" spans="2:2">
+      <c r="B5" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="7" spans="2:2" ht="18.75">
+      <c r="B7" s="68" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="8" spans="2:2">
+      <c r="B8" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="9" spans="2:2">
+      <c r="B9" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="10" spans="2:2">
+      <c r="B10" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="11" spans="2:2">
+      <c r="B11" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="12" spans="2:2">
+      <c r="B12" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="13" spans="2:2">
+      <c r="B13" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="14" spans="2:2">
+      <c r="B14" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="15" spans="2:2">
+      <c r="B15" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="16" spans="2:2">
+      <c r="B16" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11">
+      <c r="B17" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11">
+      <c r="B18" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11">
+      <c r="B19" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11">
+      <c r="B20" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11">
+      <c r="A23" t="s">
+        <v>160</v>
+      </c>
+      <c r="B23" s="58" t="s">
+        <v>70</v>
+      </c>
+      <c r="C23" s="55"/>
+      <c r="D23" s="59" t="s">
+        <v>161</v>
+      </c>
+      <c r="E23" s="60"/>
+      <c r="F23" s="60"/>
+      <c r="G23" s="60"/>
+      <c r="H23" s="60"/>
+      <c r="I23" s="61"/>
+      <c r="J23" s="55"/>
+      <c r="K23" s="58" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11">
+      <c r="B24" s="55"/>
+      <c r="C24" s="55"/>
+      <c r="D24" s="62"/>
+      <c r="E24" s="63"/>
+      <c r="F24" s="63"/>
+      <c r="G24" s="63"/>
+      <c r="H24" s="63"/>
+      <c r="I24" s="64"/>
+      <c r="J24" s="55"/>
+      <c r="K24" s="55"/>
+    </row>
+    <row r="25" spans="1:11">
+      <c r="B25" s="55"/>
+      <c r="C25" s="55"/>
+      <c r="D25" s="62"/>
+      <c r="E25" s="63"/>
+      <c r="F25" s="63"/>
+      <c r="G25" s="63"/>
+      <c r="H25" s="63"/>
+      <c r="I25" s="64"/>
+      <c r="J25" s="55"/>
+      <c r="K25" s="55"/>
+    </row>
+    <row r="26" spans="1:11">
+      <c r="B26" s="58" t="s">
+        <v>72</v>
+      </c>
+      <c r="C26" s="55"/>
+      <c r="D26" s="62"/>
+      <c r="E26" s="63"/>
+      <c r="F26" s="63"/>
+      <c r="G26" s="63"/>
+      <c r="H26" s="63"/>
+      <c r="I26" s="64"/>
+      <c r="J26" s="55"/>
+      <c r="K26" s="58" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11">
+      <c r="B27" s="55"/>
+      <c r="C27" s="55"/>
+      <c r="D27" s="62"/>
+      <c r="E27" s="63"/>
+      <c r="F27" s="63"/>
+      <c r="G27" s="63"/>
+      <c r="H27" s="63"/>
+      <c r="I27" s="64"/>
+      <c r="J27" s="55"/>
+      <c r="K27" s="55"/>
+    </row>
+    <row r="28" spans="1:11">
+      <c r="B28" s="58" t="s">
+        <v>164</v>
+      </c>
+      <c r="C28" s="56"/>
+      <c r="D28" s="65"/>
+      <c r="E28" s="66"/>
+      <c r="F28" s="66"/>
+      <c r="G28" s="66"/>
+      <c r="H28" s="66"/>
+      <c r="I28" s="67"/>
+      <c r="J28" s="56"/>
+      <c r="K28" s="55"/>
+    </row>
+    <row r="29" spans="1:11">
+      <c r="B29" s="57"/>
+      <c r="C29" s="57"/>
+      <c r="D29" s="59" t="s">
+        <v>161</v>
+      </c>
+      <c r="E29" s="60"/>
+      <c r="F29" s="60"/>
+      <c r="G29" s="60"/>
+      <c r="H29" s="60"/>
+      <c r="I29" s="61"/>
+      <c r="J29" s="57"/>
+      <c r="K29" s="58" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11">
+      <c r="B30" s="57"/>
+      <c r="C30" s="57"/>
+      <c r="D30" s="62"/>
+      <c r="E30" s="63"/>
+      <c r="F30" s="63"/>
+      <c r="G30" s="63"/>
+      <c r="H30" s="63"/>
+      <c r="I30" s="64"/>
+      <c r="J30" s="57"/>
+      <c r="K30" s="57"/>
+    </row>
+    <row r="31" spans="1:11">
+      <c r="B31" s="58" t="s">
+        <v>163</v>
+      </c>
+      <c r="C31" s="57"/>
+      <c r="D31" s="62"/>
+      <c r="E31" s="63"/>
+      <c r="F31" s="63"/>
+      <c r="G31" s="63"/>
+      <c r="H31" s="63"/>
+      <c r="I31" s="64"/>
+      <c r="J31" s="57"/>
+      <c r="K31" s="58" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11">
+      <c r="B32" s="57"/>
+      <c r="C32" s="57"/>
+      <c r="D32" s="62"/>
+      <c r="E32" s="63"/>
+      <c r="F32" s="63"/>
+      <c r="G32" s="63"/>
+      <c r="H32" s="63"/>
+      <c r="I32" s="64"/>
+      <c r="J32" s="57"/>
+      <c r="K32" s="57"/>
+    </row>
+    <row r="33" spans="1:11">
+      <c r="B33" s="57"/>
+      <c r="C33" s="57"/>
+      <c r="D33" s="62"/>
+      <c r="E33" s="63"/>
+      <c r="F33" s="63"/>
+      <c r="G33" s="63"/>
+      <c r="H33" s="63"/>
+      <c r="I33" s="64"/>
+      <c r="J33" s="57"/>
+      <c r="K33" s="57"/>
+    </row>
+    <row r="34" spans="1:11">
+      <c r="A34" t="s">
+        <v>165</v>
+      </c>
+      <c r="B34" s="58" t="s">
+        <v>162</v>
+      </c>
+      <c r="C34" s="57"/>
+      <c r="D34" s="65"/>
+      <c r="E34" s="66"/>
+      <c r="F34" s="66"/>
+      <c r="G34" s="66"/>
+      <c r="H34" s="66"/>
+      <c r="I34" s="67"/>
+      <c r="J34" s="57"/>
+      <c r="K34" s="58" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="37" spans="1:11">
+      <c r="B37" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="38" spans="1:11">
+      <c r="B38" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="39" spans="1:11">
+      <c r="B39" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="40" spans="1:11">
+      <c r="B40" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="43" spans="1:11" ht="18.75">
+      <c r="B43" s="68" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="44" spans="1:11">
+      <c r="B44" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="46" spans="1:11">
+      <c r="B46" s="3" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="47" spans="1:11">
+      <c r="B47" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="49" spans="2:2">
+      <c r="B49" s="3" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="50" spans="2:2">
+      <c r="B50" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="52" spans="2:2">
+      <c r="B52" s="3" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="53" spans="2:2">
+      <c r="B53" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="55" spans="2:2">
+      <c r="B55" s="3" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="56" spans="2:2">
+      <c r="B56" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="57" spans="2:2">
+      <c r="B57" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="58" spans="2:2">
+      <c r="B58" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="59" spans="2:2">
+      <c r="B59" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="60" spans="2:2">
+      <c r="B60" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="62" spans="2:2">
+      <c r="B62" s="3" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="63" spans="2:2">
+      <c r="B63" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="64" spans="2:2">
+      <c r="B64" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="67" spans="2:2">
+      <c r="B67" s="3" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="68" spans="2:2">
+      <c r="B68" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="70" spans="2:2">
+      <c r="B70" s="3" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="71" spans="2:2">
+      <c r="B71" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="72" spans="2:2">
+      <c r="B72" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="73" spans="2:2">
+      <c r="B73" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="74" spans="2:2">
+      <c r="B74" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="75" spans="2:2">
+      <c r="B75" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="77" spans="2:2">
+      <c r="B77" s="3" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="78" spans="2:2">
+      <c r="B78" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="79" spans="2:2">
+      <c r="B79" s="69" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="80" spans="2:2">
+      <c r="B80" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="81" spans="2:2">
+      <c r="B81" t="s">
+        <v>192</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="D29:I34"/>
+    <mergeCell ref="D23:I28"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6016CF9E-E144-48D8-959F-618B8D85D284}">
   <dimension ref="B2:B11"/>
   <sheetViews>
@@ -6770,56 +7446,56 @@
       <selection activeCell="J14" sqref="J14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="2" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:2">
       <c r="B2" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="3" spans="2:2" x14ac:dyDescent="0.25">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="3" spans="2:2">
       <c r="B3" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="4" spans="2:2" x14ac:dyDescent="0.25">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="4" spans="2:2">
       <c r="B4" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="5" spans="2:2" x14ac:dyDescent="0.25">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="5" spans="2:2">
       <c r="B5" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="6" spans="2:2" x14ac:dyDescent="0.25">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="6" spans="2:2">
       <c r="B6" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="7" spans="2:2" x14ac:dyDescent="0.25">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="7" spans="2:2">
       <c r="B7" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="8" spans="2:2" x14ac:dyDescent="0.25">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="8" spans="2:2">
       <c r="B8" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="9" spans="2:2" x14ac:dyDescent="0.25">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="9" spans="2:2">
       <c r="B9" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="10" spans="2:2" x14ac:dyDescent="0.25">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="10" spans="2:2">
       <c r="B10" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="11" spans="2:2" x14ac:dyDescent="0.25">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="11" spans="2:2">
       <c r="B11" t="s">
-        <v>144</v>
+        <v>202</v>
       </c>
     </row>
   </sheetData>
@@ -6827,202 +7503,202 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1CADF2F4-A124-44BC-8A72-4CE3F16F5D04}">
   <dimension ref="B2:D22"/>
   <sheetViews>
-    <sheetView topLeftCell="A9" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="2" max="2" width="18.28515625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="29.42578125" customWidth="1"/>
     <col min="4" max="4" width="27.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:4">
       <c r="B2" s="32" t="s">
-        <v>145</v>
+        <v>203</v>
       </c>
       <c r="C2" s="32" t="s">
-        <v>146</v>
+        <v>204</v>
       </c>
       <c r="D2" s="32" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="3" spans="2:4" ht="106.5" customHeight="1" x14ac:dyDescent="0.25">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="3" spans="2:4" ht="106.5" customHeight="1">
       <c r="B3" s="50" t="s">
-        <v>148</v>
+        <v>206</v>
       </c>
       <c r="C3" s="48" t="s">
-        <v>149</v>
+        <v>207</v>
       </c>
       <c r="D3" s="28" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="4" spans="2:4" ht="120" x14ac:dyDescent="0.25">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="4" spans="2:4" ht="120">
       <c r="B4" s="53"/>
       <c r="C4" s="52"/>
       <c r="D4" s="29" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="5" spans="2:4" ht="60" x14ac:dyDescent="0.25">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="5" spans="2:4" ht="60">
       <c r="B5" s="53"/>
       <c r="C5" s="52"/>
       <c r="D5" s="30" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="6" spans="2:4" ht="75" x14ac:dyDescent="0.25">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="6" spans="2:4" ht="75">
       <c r="B6" s="53"/>
       <c r="C6" s="52"/>
       <c r="D6" s="30" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="7" spans="2:4" ht="90" x14ac:dyDescent="0.25">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="7" spans="2:4" ht="90">
       <c r="B7" s="50" t="s">
-        <v>154</v>
+        <v>212</v>
       </c>
       <c r="C7" s="48" t="s">
-        <v>155</v>
+        <v>213</v>
       </c>
       <c r="D7" s="28" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="8" spans="2:4" ht="90" x14ac:dyDescent="0.25">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="8" spans="2:4" ht="90">
       <c r="B8" s="53"/>
       <c r="C8" s="52"/>
       <c r="D8" s="30" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="9" spans="2:4" ht="75" x14ac:dyDescent="0.25">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="9" spans="2:4" ht="75">
       <c r="B9" s="50" t="s">
-        <v>158</v>
+        <v>216</v>
       </c>
       <c r="C9" s="48" t="s">
-        <v>159</v>
+        <v>217</v>
       </c>
       <c r="D9" s="28" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="10" spans="2:4" ht="30" x14ac:dyDescent="0.25">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="10" spans="2:4" ht="30">
       <c r="B10" s="51"/>
       <c r="C10" s="49"/>
       <c r="D10" s="31" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="11" spans="2:4" ht="76.5" customHeight="1" x14ac:dyDescent="0.25">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="11" spans="2:4" ht="76.5" customHeight="1">
       <c r="B11" s="50" t="s">
-        <v>162</v>
+        <v>220</v>
       </c>
       <c r="C11" s="48" t="s">
-        <v>163</v>
+        <v>221</v>
       </c>
       <c r="D11" s="28" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="12" spans="2:4" ht="30" x14ac:dyDescent="0.25">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="12" spans="2:4" ht="30">
       <c r="B12" s="53"/>
       <c r="C12" s="52"/>
       <c r="D12" s="30" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="13" spans="2:4" ht="45" x14ac:dyDescent="0.25">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="13" spans="2:4" ht="45">
       <c r="B13" s="50" t="s">
-        <v>166</v>
+        <v>224</v>
       </c>
       <c r="C13" s="48" t="s">
-        <v>167</v>
+        <v>225</v>
       </c>
       <c r="D13" s="28" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="14" spans="2:4" ht="30" x14ac:dyDescent="0.25">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="14" spans="2:4" ht="30">
       <c r="B14" s="53"/>
       <c r="C14" s="52"/>
       <c r="D14" s="30" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="15" spans="2:4" ht="45" x14ac:dyDescent="0.25">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="15" spans="2:4" ht="45">
       <c r="B15" s="53"/>
       <c r="C15" s="52"/>
       <c r="D15" s="30" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="16" spans="2:4" ht="60" x14ac:dyDescent="0.25">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="16" spans="2:4" ht="60">
       <c r="B16" s="53"/>
       <c r="C16" s="52"/>
       <c r="D16" s="30" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="17" spans="2:4" ht="45" x14ac:dyDescent="0.25">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="17" spans="2:4" ht="45">
       <c r="B17" s="50" t="s">
-        <v>172</v>
+        <v>230</v>
       </c>
       <c r="C17" s="48" t="s">
-        <v>173</v>
+        <v>231</v>
       </c>
       <c r="D17" s="28" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="18" spans="2:4" ht="45" x14ac:dyDescent="0.25">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="18" spans="2:4" ht="45">
       <c r="B18" s="53"/>
       <c r="C18" s="52"/>
       <c r="D18" s="30" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="19" spans="2:4" ht="60.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="19" spans="2:4" ht="60.75" customHeight="1">
       <c r="B19" s="50" t="s">
-        <v>176</v>
+        <v>234</v>
       </c>
       <c r="C19" s="48" t="s">
-        <v>177</v>
+        <v>235</v>
       </c>
       <c r="D19" s="28" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="20" spans="2:4" ht="30" x14ac:dyDescent="0.25">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="20" spans="2:4" ht="30">
       <c r="B20" s="53"/>
       <c r="C20" s="52"/>
       <c r="D20" s="30" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="21" spans="2:4" ht="45" x14ac:dyDescent="0.25">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="21" spans="2:4" ht="45">
       <c r="B21" s="50" t="s">
-        <v>180</v>
+        <v>238</v>
       </c>
       <c r="C21" s="48" t="s">
-        <v>181</v>
+        <v>239</v>
       </c>
       <c r="D21" s="28" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="22" spans="2:4" ht="30" x14ac:dyDescent="0.25">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="22" spans="2:4" ht="30">
       <c r="B22" s="51"/>
       <c r="C22" s="49"/>
       <c r="D22" s="31" t="s">
-        <v>183</v>
+        <v>241</v>
       </c>
     </row>
   </sheetData>
@@ -7048,7 +7724,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A2:S19"/>
   <sheetViews>
@@ -7056,7 +7732,7 @@
       <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="12.140625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="10.5703125" bestFit="1" customWidth="1"/>
@@ -7066,33 +7742,33 @@
     <col min="11" max="11" width="9.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:19">
       <c r="A2" s="47" t="s">
-        <v>184</v>
+        <v>160</v>
       </c>
       <c r="B2" s="47"/>
       <c r="C2" s="47"/>
       <c r="F2" s="47" t="s">
-        <v>185</v>
+        <v>165</v>
       </c>
       <c r="G2" s="47"/>
       <c r="H2" s="47"/>
     </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:19">
       <c r="A3" t="s">
-        <v>186</v>
+        <v>242</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>21</v>
       </c>
       <c r="F3" t="s">
-        <v>186</v>
+        <v>242</v>
       </c>
       <c r="G3" s="1" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:19">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -7108,54 +7784,54 @@
         <v>9500</v>
       </c>
     </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:19">
       <c r="A5" t="s">
-        <v>187</v>
+        <v>243</v>
       </c>
       <c r="B5">
         <f>SUM(C10:C14)</f>
         <v>5000</v>
       </c>
       <c r="F5" t="s">
-        <v>187</v>
+        <v>243</v>
       </c>
       <c r="G5">
         <f>SUM(H10:H14)</f>
         <v>7500</v>
       </c>
     </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:19">
       <c r="A6" t="s">
-        <v>188</v>
+        <v>244</v>
       </c>
       <c r="B6">
         <f>SUM(C17:C19)</f>
         <v>2000</v>
       </c>
       <c r="F6" t="s">
-        <v>188</v>
+        <v>244</v>
       </c>
       <c r="G6">
         <f>SUM(H17:H19)</f>
         <v>2000</v>
       </c>
     </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:19">
       <c r="C7" s="17"/>
       <c r="H7" s="17"/>
     </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:19">
       <c r="C8" s="17"/>
       <c r="H8" s="17"/>
       <c r="Q8" s="3"/>
       <c r="S8" s="3"/>
     </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:19">
       <c r="A9" s="17" t="s">
         <v>2</v>
       </c>
       <c r="B9" s="17" t="s">
-        <v>189</v>
+        <v>245</v>
       </c>
       <c r="C9" s="17" t="s">
         <v>3</v>
@@ -7164,7 +7840,7 @@
         <v>2</v>
       </c>
       <c r="G9" s="17" t="s">
-        <v>189</v>
+        <v>245</v>
       </c>
       <c r="H9" s="17" t="s">
         <v>3</v>
@@ -7181,7 +7857,7 @@
       <c r="R9" s="1"/>
       <c r="S9" s="7"/>
     </row>
-    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:19">
       <c r="A10" s="17" t="s">
         <v>13</v>
       </c>
@@ -7216,7 +7892,7 @@
       <c r="R10" s="1"/>
       <c r="S10" s="7"/>
     </row>
-    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:19">
       <c r="A11" s="17" t="s">
         <v>14</v>
       </c>
@@ -7253,7 +7929,7 @@
       <c r="R11" s="1"/>
       <c r="S11" s="7"/>
     </row>
-    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:19">
       <c r="A12" s="17" t="s">
         <v>15</v>
       </c>
@@ -7290,7 +7966,7 @@
       <c r="R12" s="1"/>
       <c r="S12" s="7"/>
     </row>
-    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:19">
       <c r="A13" s="17" t="s">
         <v>16</v>
       </c>
@@ -7325,7 +8001,7 @@
       <c r="R13" s="1"/>
       <c r="S13" s="7"/>
     </row>
-    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:19">
       <c r="A14" s="17" t="s">
         <v>17</v>
       </c>
@@ -7349,27 +8025,27 @@
         <v>5000</v>
       </c>
     </row>
-    <row r="16" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:19">
       <c r="A16" s="17" t="s">
-        <v>148</v>
+        <v>206</v>
       </c>
       <c r="B16" s="17" t="s">
-        <v>189</v>
+        <v>245</v>
       </c>
       <c r="C16" t="s">
         <v>3</v>
       </c>
       <c r="F16" s="17" t="s">
-        <v>148</v>
+        <v>206</v>
       </c>
       <c r="G16" s="17" t="s">
-        <v>189</v>
+        <v>245</v>
       </c>
       <c r="H16" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8">
       <c r="A17" s="17" t="s">
         <v>4</v>
       </c>
@@ -7393,7 +8069,7 @@
         <v>1500</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:8">
       <c r="A18" s="17" t="s">
         <v>5</v>
       </c>
@@ -7417,7 +8093,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:8">
       <c r="A19" s="17" t="s">
         <v>6</v>
       </c>

</xml_diff>

<commit_message>
Figuring out new mechanics and cards
Figuring out new mechanics and cards
</commit_message>
<xml_diff>
--- a/ShipCardGameCalcs.xlsx
+++ b/ShipCardGameCalcs.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27226"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27230"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MultiplayerGame\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{46FE794F-886C-463B-B0ED-03A30A33612D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{7C940714-625D-4C48-A3A9-03623713CFAE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="3" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="4" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Values" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,8 @@
     <sheet name="Game Rules version 2" sheetId="8" r:id="rId5"/>
     <sheet name="Ideas" sheetId="6" r:id="rId6"/>
     <sheet name="Card Details" sheetId="5" r:id="rId7"/>
-    <sheet name="Comparison" sheetId="2" r:id="rId8"/>
+    <sheet name="Card Mechanics" sheetId="9" r:id="rId8"/>
+    <sheet name="Comparison" sheetId="2" r:id="rId9"/>
   </sheets>
   <calcPr calcId="191028"/>
   <extLst>
@@ -43,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="471" uniqueCount="246">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="497" uniqueCount="261">
   <si>
     <t>Ship Parameters</t>
   </si>
@@ -749,13 +750,13 @@
     <t>Event</t>
   </si>
   <si>
-    <t>Research project cards are ways for the player to potentially change the tide of battle with either basic card drawing to removing a ships upgrade.</t>
+    <t>Event cards are ways for the player to potentially change the tide of battle with either basic card drawing to removing a ships upgrade.</t>
   </si>
   <si>
     <t>You can play as many Research Project cards as long you can pay their cost</t>
   </si>
   <si>
-    <t>Research Project cards can only be played on your turn</t>
+    <t>Can only be played on your turn</t>
   </si>
   <si>
     <t>Ship Upgrade</t>
@@ -767,9 +768,6 @@
     <t>You can play as manyShip Upgrade cards as long you can pay their cost</t>
   </si>
   <si>
-    <t>Ship Upgrade cards can only be played on your turn</t>
-  </si>
-  <si>
     <t>You can't move a ship upgrade from one ship to another once attached</t>
   </si>
   <si>
@@ -797,9 +795,6 @@
     <t>You can play a many On Going Event cards as long as you can pay their cost</t>
   </si>
   <si>
-    <t>On Going Event cards can only be played on your turn</t>
-  </si>
-  <si>
     <t>Crew Attachment</t>
   </si>
   <si>
@@ -809,7 +804,58 @@
     <t>You can play a many Crew Attachment cards as long as you can pay their cost</t>
   </si>
   <si>
-    <t>Crew Attachment cards can only be played on your turn</t>
+    <t>Private Mission</t>
+  </si>
+  <si>
+    <t>Played to the field that has a mission only the player who played it can do and gain the rewards for</t>
+  </si>
+  <si>
+    <t>You can play as many Private Mission cards as long as you can pay their cost</t>
+  </si>
+  <si>
+    <t>Once the mission is complete then remove private mission card from field and send to the scrapyard</t>
+  </si>
+  <si>
+    <t>Galaxy Mission</t>
+  </si>
+  <si>
+    <t>Played to the field that has a mission that any player can do and gain the rewards for</t>
+  </si>
+  <si>
+    <t>Dangerous Mission</t>
+  </si>
+  <si>
+    <t>Played to the field that has a mission only the player who played it can do and gain the rewards for, however after a certain amount of turns it will have consequences</t>
+  </si>
+  <si>
+    <t>If the missions runs out of turns the it will activate the consequence affect and then get sent to the scrapyard</t>
+  </si>
+  <si>
+    <t>Detail</t>
+  </si>
+  <si>
+    <t>Piercing Round</t>
+  </si>
+  <si>
+    <t>Deals damage straight to hull from gun slot</t>
+  </si>
+  <si>
+    <t>Corrosion</t>
+  </si>
+  <si>
+    <t>Deals damage straight to hull over time</t>
+  </si>
+  <si>
+    <t>Swarm</t>
+  </si>
+  <si>
+    <t>Create X pod ship/s with 100 hull and can tap to deal 100 damage to enemy ship</t>
+  </si>
+  <si>
+    <t>Infection</t>
+  </si>
+  <si>
+    <t>Sacrifice 1 crew</t>
   </si>
   <si>
     <t>Fleet Option</t>
@@ -1246,7 +1292,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="70">
+  <cellXfs count="73">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1344,8 +1390,41 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="23" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="24" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1365,40 +1444,18 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="23" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="24" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -3493,21 +3550,21 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17">
-      <c r="A1" s="47" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="47"/>
-      <c r="C1" s="47"/>
-      <c r="D1" s="47"/>
-      <c r="E1" s="47"/>
-      <c r="F1" s="47"/>
-      <c r="G1" s="47"/>
-      <c r="H1" s="47"/>
-      <c r="N1" s="47" t="s">
+      <c r="A1" s="53" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="53"/>
+      <c r="C1" s="53"/>
+      <c r="D1" s="53"/>
+      <c r="E1" s="53"/>
+      <c r="F1" s="53"/>
+      <c r="G1" s="53"/>
+      <c r="H1" s="53"/>
+      <c r="N1" s="53" t="s">
         <v>1</v>
       </c>
-      <c r="O1" s="47"/>
-      <c r="P1" s="47"/>
+      <c r="O1" s="53"/>
+      <c r="P1" s="53"/>
     </row>
     <row r="2" spans="1:17">
       <c r="A2" s="9" t="s">
@@ -3774,25 +3831,25 @@
       </c>
     </row>
     <row r="8" spans="1:17">
-      <c r="A8" s="47" t="s">
+      <c r="A8" s="53" t="s">
         <v>18</v>
       </c>
-      <c r="B8" s="47"/>
-      <c r="C8" s="47"/>
-      <c r="D8" s="47"/>
-      <c r="E8" s="47"/>
-      <c r="F8" s="47"/>
-      <c r="G8" s="47"/>
-      <c r="J8" s="47" t="s">
+      <c r="B8" s="53"/>
+      <c r="C8" s="53"/>
+      <c r="D8" s="53"/>
+      <c r="E8" s="53"/>
+      <c r="F8" s="53"/>
+      <c r="G8" s="53"/>
+      <c r="J8" s="53" t="s">
         <v>19</v>
       </c>
-      <c r="K8" s="47"/>
-      <c r="L8" s="47"/>
-      <c r="M8" s="47"/>
-      <c r="N8" s="47"/>
-      <c r="O8" s="47"/>
-      <c r="P8" s="47"/>
-      <c r="Q8" s="47"/>
+      <c r="K8" s="53"/>
+      <c r="L8" s="53"/>
+      <c r="M8" s="53"/>
+      <c r="N8" s="53"/>
+      <c r="O8" s="53"/>
+      <c r="P8" s="53"/>
+      <c r="Q8" s="53"/>
     </row>
     <row r="9" spans="1:17">
       <c r="A9" s="8" t="s">
@@ -4132,15 +4189,15 @@
       <c r="Q15" s="1"/>
     </row>
     <row r="16" spans="1:17">
-      <c r="A16" s="47" t="s">
+      <c r="A16" s="53" t="s">
         <v>35</v>
       </c>
-      <c r="B16" s="47"/>
-      <c r="C16" s="47"/>
-      <c r="D16" s="47"/>
-      <c r="E16" s="47"/>
-      <c r="F16" s="47"/>
-      <c r="G16" s="47"/>
+      <c r="B16" s="53"/>
+      <c r="C16" s="53"/>
+      <c r="D16" s="53"/>
+      <c r="E16" s="53"/>
+      <c r="F16" s="53"/>
+      <c r="G16" s="53"/>
       <c r="K16" s="1"/>
       <c r="L16" s="1"/>
       <c r="M16" s="1"/>
@@ -4357,27 +4414,27 @@
       <c r="R22" s="4"/>
     </row>
     <row r="23" spans="1:18">
-      <c r="A23" s="47" t="s">
+      <c r="A23" s="53" t="s">
         <v>40</v>
       </c>
-      <c r="B23" s="47"/>
-      <c r="C23" s="47"/>
-      <c r="D23" s="47"/>
-      <c r="E23" s="47"/>
-      <c r="F23" s="47"/>
-      <c r="G23" s="47"/>
-      <c r="H23" s="47"/>
+      <c r="B23" s="53"/>
+      <c r="C23" s="53"/>
+      <c r="D23" s="53"/>
+      <c r="E23" s="53"/>
+      <c r="F23" s="53"/>
+      <c r="G23" s="53"/>
+      <c r="H23" s="53"/>
       <c r="I23" s="4"/>
-      <c r="J23" s="47" t="s">
+      <c r="J23" s="53" t="s">
         <v>41</v>
       </c>
-      <c r="K23" s="47"/>
-      <c r="L23" s="47"/>
-      <c r="M23" s="47"/>
-      <c r="N23" s="47"/>
-      <c r="O23" s="47"/>
-      <c r="P23" s="47"/>
-      <c r="Q23" s="47"/>
+      <c r="K23" s="53"/>
+      <c r="L23" s="53"/>
+      <c r="M23" s="53"/>
+      <c r="N23" s="53"/>
+      <c r="O23" s="53"/>
+      <c r="P23" s="53"/>
+      <c r="Q23" s="53"/>
     </row>
     <row r="24" spans="1:18">
       <c r="A24" s="8" t="s">
@@ -4805,25 +4862,25 @@
       <c r="Q30" s="1"/>
     </row>
     <row r="31" spans="1:18">
-      <c r="A31" s="47" t="s">
+      <c r="A31" s="53" t="s">
         <v>47</v>
       </c>
-      <c r="B31" s="47"/>
-      <c r="C31" s="47"/>
-      <c r="D31" s="47"/>
-      <c r="E31" s="47"/>
-      <c r="F31" s="47"/>
-      <c r="G31" s="47"/>
+      <c r="B31" s="53"/>
+      <c r="C31" s="53"/>
+      <c r="D31" s="53"/>
+      <c r="E31" s="53"/>
+      <c r="F31" s="53"/>
+      <c r="G31" s="53"/>
       <c r="I31" s="4"/>
-      <c r="J31" s="47" t="s">
+      <c r="J31" s="53" t="s">
         <v>48</v>
       </c>
-      <c r="K31" s="47"/>
-      <c r="L31" s="47"/>
-      <c r="M31" s="47"/>
-      <c r="N31" s="47"/>
-      <c r="O31" s="47"/>
-      <c r="P31" s="47"/>
+      <c r="K31" s="53"/>
+      <c r="L31" s="53"/>
+      <c r="M31" s="53"/>
+      <c r="N31" s="53"/>
+      <c r="O31" s="53"/>
+      <c r="P31" s="53"/>
     </row>
     <row r="32" spans="1:18">
       <c r="A32" t="s">
@@ -6524,13 +6581,13 @@
     <row r="16" spans="2:19">
       <c r="P16">
         <f ca="1">RANDBETWEEN(0,123)</f>
-        <v>76</v>
+        <v>113</v>
       </c>
     </row>
     <row r="17" spans="2:16">
       <c r="P17" s="46">
         <f ca="1">RANDBETWEEN(0,6)</f>
-        <v>5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="18" spans="2:16">
@@ -6990,8 +7047,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{93013FD4-B940-4A70-A7DA-BF82FD0F616E}">
   <dimension ref="A2:K81"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="P29" sqref="P29"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="L71" sqref="L71"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -7001,7 +7058,7 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:2" ht="23.25">
-      <c r="B2" s="54" t="s">
+      <c r="B2" s="47" t="s">
         <v>143</v>
       </c>
     </row>
@@ -7016,7 +7073,7 @@
       </c>
     </row>
     <row r="7" spans="2:2" ht="18.75">
-      <c r="B7" s="68" t="s">
+      <c r="B7" s="51" t="s">
         <v>146</v>
       </c>
     </row>
@@ -7089,173 +7146,173 @@
       <c r="A23" t="s">
         <v>160</v>
       </c>
-      <c r="B23" s="58" t="s">
+      <c r="B23" s="50" t="s">
         <v>70</v>
       </c>
-      <c r="C23" s="55"/>
-      <c r="D23" s="59" t="s">
+      <c r="C23" s="48"/>
+      <c r="D23" s="54" t="s">
         <v>161</v>
       </c>
-      <c r="E23" s="60"/>
-      <c r="F23" s="60"/>
-      <c r="G23" s="60"/>
-      <c r="H23" s="60"/>
-      <c r="I23" s="61"/>
-      <c r="J23" s="55"/>
-      <c r="K23" s="58" t="s">
+      <c r="E23" s="55"/>
+      <c r="F23" s="55"/>
+      <c r="G23" s="55"/>
+      <c r="H23" s="55"/>
+      <c r="I23" s="56"/>
+      <c r="J23" s="48"/>
+      <c r="K23" s="50" t="s">
         <v>162</v>
       </c>
     </row>
     <row r="24" spans="1:11">
-      <c r="B24" s="55"/>
-      <c r="C24" s="55"/>
-      <c r="D24" s="62"/>
-      <c r="E24" s="63"/>
-      <c r="F24" s="63"/>
-      <c r="G24" s="63"/>
-      <c r="H24" s="63"/>
-      <c r="I24" s="64"/>
-      <c r="J24" s="55"/>
-      <c r="K24" s="55"/>
+      <c r="B24" s="48"/>
+      <c r="C24" s="48"/>
+      <c r="D24" s="57"/>
+      <c r="E24" s="58"/>
+      <c r="F24" s="58"/>
+      <c r="G24" s="58"/>
+      <c r="H24" s="58"/>
+      <c r="I24" s="59"/>
+      <c r="J24" s="48"/>
+      <c r="K24" s="48"/>
     </row>
     <row r="25" spans="1:11">
-      <c r="B25" s="55"/>
-      <c r="C25" s="55"/>
-      <c r="D25" s="62"/>
-      <c r="E25" s="63"/>
-      <c r="F25" s="63"/>
-      <c r="G25" s="63"/>
-      <c r="H25" s="63"/>
-      <c r="I25" s="64"/>
-      <c r="J25" s="55"/>
-      <c r="K25" s="55"/>
+      <c r="B25" s="48"/>
+      <c r="C25" s="48"/>
+      <c r="D25" s="57"/>
+      <c r="E25" s="58"/>
+      <c r="F25" s="58"/>
+      <c r="G25" s="58"/>
+      <c r="H25" s="58"/>
+      <c r="I25" s="59"/>
+      <c r="J25" s="48"/>
+      <c r="K25" s="48"/>
     </row>
     <row r="26" spans="1:11">
-      <c r="B26" s="58" t="s">
+      <c r="B26" s="50" t="s">
         <v>72</v>
       </c>
-      <c r="C26" s="55"/>
-      <c r="D26" s="62"/>
-      <c r="E26" s="63"/>
-      <c r="F26" s="63"/>
-      <c r="G26" s="63"/>
-      <c r="H26" s="63"/>
-      <c r="I26" s="64"/>
-      <c r="J26" s="55"/>
-      <c r="K26" s="58" t="s">
+      <c r="C26" s="48"/>
+      <c r="D26" s="57"/>
+      <c r="E26" s="58"/>
+      <c r="F26" s="58"/>
+      <c r="G26" s="58"/>
+      <c r="H26" s="58"/>
+      <c r="I26" s="59"/>
+      <c r="J26" s="48"/>
+      <c r="K26" s="50" t="s">
         <v>163</v>
       </c>
     </row>
     <row r="27" spans="1:11">
-      <c r="B27" s="55"/>
-      <c r="C27" s="55"/>
-      <c r="D27" s="62"/>
-      <c r="E27" s="63"/>
-      <c r="F27" s="63"/>
-      <c r="G27" s="63"/>
-      <c r="H27" s="63"/>
-      <c r="I27" s="64"/>
-      <c r="J27" s="55"/>
-      <c r="K27" s="55"/>
+      <c r="B27" s="48"/>
+      <c r="C27" s="48"/>
+      <c r="D27" s="57"/>
+      <c r="E27" s="58"/>
+      <c r="F27" s="58"/>
+      <c r="G27" s="58"/>
+      <c r="H27" s="58"/>
+      <c r="I27" s="59"/>
+      <c r="J27" s="48"/>
+      <c r="K27" s="48"/>
     </row>
     <row r="28" spans="1:11">
-      <c r="B28" s="58" t="s">
+      <c r="B28" s="50" t="s">
         <v>164</v>
       </c>
-      <c r="C28" s="56"/>
-      <c r="D28" s="65"/>
-      <c r="E28" s="66"/>
-      <c r="F28" s="66"/>
-      <c r="G28" s="66"/>
-      <c r="H28" s="66"/>
-      <c r="I28" s="67"/>
-      <c r="J28" s="56"/>
-      <c r="K28" s="55"/>
+      <c r="C28" s="49"/>
+      <c r="D28" s="60"/>
+      <c r="E28" s="61"/>
+      <c r="F28" s="61"/>
+      <c r="G28" s="61"/>
+      <c r="H28" s="61"/>
+      <c r="I28" s="62"/>
+      <c r="J28" s="49"/>
+      <c r="K28" s="48"/>
     </row>
     <row r="29" spans="1:11">
-      <c r="B29" s="57"/>
-      <c r="C29" s="57"/>
-      <c r="D29" s="59" t="s">
+      <c r="B29" s="48"/>
+      <c r="C29" s="48"/>
+      <c r="D29" s="54" t="s">
         <v>161</v>
       </c>
-      <c r="E29" s="60"/>
-      <c r="F29" s="60"/>
-      <c r="G29" s="60"/>
-      <c r="H29" s="60"/>
-      <c r="I29" s="61"/>
-      <c r="J29" s="57"/>
-      <c r="K29" s="58" t="s">
+      <c r="E29" s="55"/>
+      <c r="F29" s="55"/>
+      <c r="G29" s="55"/>
+      <c r="H29" s="55"/>
+      <c r="I29" s="56"/>
+      <c r="J29" s="48"/>
+      <c r="K29" s="50" t="s">
         <v>164</v>
       </c>
     </row>
     <row r="30" spans="1:11">
-      <c r="B30" s="57"/>
-      <c r="C30" s="57"/>
-      <c r="D30" s="62"/>
-      <c r="E30" s="63"/>
-      <c r="F30" s="63"/>
-      <c r="G30" s="63"/>
-      <c r="H30" s="63"/>
-      <c r="I30" s="64"/>
-      <c r="J30" s="57"/>
-      <c r="K30" s="57"/>
+      <c r="B30" s="48"/>
+      <c r="C30" s="48"/>
+      <c r="D30" s="57"/>
+      <c r="E30" s="58"/>
+      <c r="F30" s="58"/>
+      <c r="G30" s="58"/>
+      <c r="H30" s="58"/>
+      <c r="I30" s="59"/>
+      <c r="J30" s="48"/>
+      <c r="K30" s="48"/>
     </row>
     <row r="31" spans="1:11">
-      <c r="B31" s="58" t="s">
+      <c r="B31" s="50" t="s">
         <v>163</v>
       </c>
-      <c r="C31" s="57"/>
-      <c r="D31" s="62"/>
-      <c r="E31" s="63"/>
-      <c r="F31" s="63"/>
-      <c r="G31" s="63"/>
-      <c r="H31" s="63"/>
-      <c r="I31" s="64"/>
-      <c r="J31" s="57"/>
-      <c r="K31" s="58" t="s">
+      <c r="C31" s="48"/>
+      <c r="D31" s="57"/>
+      <c r="E31" s="58"/>
+      <c r="F31" s="58"/>
+      <c r="G31" s="58"/>
+      <c r="H31" s="58"/>
+      <c r="I31" s="59"/>
+      <c r="J31" s="48"/>
+      <c r="K31" s="50" t="s">
         <v>72</v>
       </c>
     </row>
     <row r="32" spans="1:11">
-      <c r="B32" s="57"/>
-      <c r="C32" s="57"/>
-      <c r="D32" s="62"/>
-      <c r="E32" s="63"/>
-      <c r="F32" s="63"/>
-      <c r="G32" s="63"/>
-      <c r="H32" s="63"/>
-      <c r="I32" s="64"/>
-      <c r="J32" s="57"/>
-      <c r="K32" s="57"/>
+      <c r="B32" s="48"/>
+      <c r="C32" s="48"/>
+      <c r="D32" s="57"/>
+      <c r="E32" s="58"/>
+      <c r="F32" s="58"/>
+      <c r="G32" s="58"/>
+      <c r="H32" s="58"/>
+      <c r="I32" s="59"/>
+      <c r="J32" s="48"/>
+      <c r="K32" s="48"/>
     </row>
     <row r="33" spans="1:11">
-      <c r="B33" s="57"/>
-      <c r="C33" s="57"/>
-      <c r="D33" s="62"/>
-      <c r="E33" s="63"/>
-      <c r="F33" s="63"/>
-      <c r="G33" s="63"/>
-      <c r="H33" s="63"/>
-      <c r="I33" s="64"/>
-      <c r="J33" s="57"/>
-      <c r="K33" s="57"/>
+      <c r="B33" s="48"/>
+      <c r="C33" s="48"/>
+      <c r="D33" s="57"/>
+      <c r="E33" s="58"/>
+      <c r="F33" s="58"/>
+      <c r="G33" s="58"/>
+      <c r="H33" s="58"/>
+      <c r="I33" s="59"/>
+      <c r="J33" s="48"/>
+      <c r="K33" s="48"/>
     </row>
     <row r="34" spans="1:11">
       <c r="A34" t="s">
         <v>165</v>
       </c>
-      <c r="B34" s="58" t="s">
+      <c r="B34" s="50" t="s">
         <v>162</v>
       </c>
-      <c r="C34" s="57"/>
-      <c r="D34" s="65"/>
-      <c r="E34" s="66"/>
-      <c r="F34" s="66"/>
-      <c r="G34" s="66"/>
-      <c r="H34" s="66"/>
-      <c r="I34" s="67"/>
-      <c r="J34" s="57"/>
-      <c r="K34" s="58" t="s">
+      <c r="C34" s="48"/>
+      <c r="D34" s="60"/>
+      <c r="E34" s="61"/>
+      <c r="F34" s="61"/>
+      <c r="G34" s="61"/>
+      <c r="H34" s="61"/>
+      <c r="I34" s="62"/>
+      <c r="J34" s="48"/>
+      <c r="K34" s="50" t="s">
         <v>70</v>
       </c>
     </row>
@@ -7280,7 +7337,7 @@
       </c>
     </row>
     <row r="43" spans="1:11" ht="18.75">
-      <c r="B43" s="68" t="s">
+      <c r="B43" s="51" t="s">
         <v>170</v>
       </c>
     </row>
@@ -7415,7 +7472,7 @@
       </c>
     </row>
     <row r="79" spans="2:2">
-      <c r="B79" s="69" t="s">
+      <c r="B79" s="52" t="s">
         <v>190</v>
       </c>
     </row>
@@ -7505,10 +7562,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1CADF2F4-A124-44BC-8A72-4CE3F16F5D04}">
-  <dimension ref="B2:D22"/>
+  <dimension ref="B2:D32"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+    <sheetView tabSelected="1" topLeftCell="A24" workbookViewId="0">
+      <selection activeCell="D32" sqref="B29:D32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -7530,10 +7587,10 @@
       </c>
     </row>
     <row r="3" spans="2:4" ht="106.5" customHeight="1">
-      <c r="B3" s="50" t="s">
+      <c r="B3" s="65" t="s">
         <v>206</v>
       </c>
-      <c r="C3" s="48" t="s">
+      <c r="C3" s="63" t="s">
         <v>207</v>
       </c>
       <c r="D3" s="28" t="s">
@@ -7541,31 +7598,31 @@
       </c>
     </row>
     <row r="4" spans="2:4" ht="120">
-      <c r="B4" s="53"/>
-      <c r="C4" s="52"/>
+      <c r="B4" s="68"/>
+      <c r="C4" s="67"/>
       <c r="D4" s="29" t="s">
         <v>209</v>
       </c>
     </row>
     <row r="5" spans="2:4" ht="60">
-      <c r="B5" s="53"/>
-      <c r="C5" s="52"/>
+      <c r="B5" s="68"/>
+      <c r="C5" s="67"/>
       <c r="D5" s="30" t="s">
         <v>210</v>
       </c>
     </row>
     <row r="6" spans="2:4" ht="75">
-      <c r="B6" s="53"/>
-      <c r="C6" s="52"/>
+      <c r="B6" s="68"/>
+      <c r="C6" s="67"/>
       <c r="D6" s="30" t="s">
         <v>211</v>
       </c>
     </row>
     <row r="7" spans="2:4" ht="90">
-      <c r="B7" s="50" t="s">
+      <c r="B7" s="65" t="s">
         <v>212</v>
       </c>
-      <c r="C7" s="48" t="s">
+      <c r="C7" s="63" t="s">
         <v>213</v>
       </c>
       <c r="D7" s="28" t="s">
@@ -7573,17 +7630,17 @@
       </c>
     </row>
     <row r="8" spans="2:4" ht="90">
-      <c r="B8" s="53"/>
-      <c r="C8" s="52"/>
+      <c r="B8" s="68"/>
+      <c r="C8" s="67"/>
       <c r="D8" s="30" t="s">
         <v>215</v>
       </c>
     </row>
     <row r="9" spans="2:4" ht="75">
-      <c r="B9" s="50" t="s">
+      <c r="B9" s="65" t="s">
         <v>216</v>
       </c>
-      <c r="C9" s="48" t="s">
+      <c r="C9" s="63" t="s">
         <v>217</v>
       </c>
       <c r="D9" s="28" t="s">
@@ -7591,118 +7648,206 @@
       </c>
     </row>
     <row r="10" spans="2:4" ht="30">
-      <c r="B10" s="51"/>
-      <c r="C10" s="49"/>
+      <c r="B10" s="66"/>
+      <c r="C10" s="64"/>
       <c r="D10" s="31" t="s">
         <v>219</v>
       </c>
     </row>
     <row r="11" spans="2:4" ht="76.5" customHeight="1">
-      <c r="B11" s="50" t="s">
+      <c r="B11" s="65" t="s">
         <v>220</v>
       </c>
-      <c r="C11" s="48" t="s">
+      <c r="C11" s="63" t="s">
         <v>221</v>
       </c>
       <c r="D11" s="28" t="s">
         <v>222</v>
       </c>
     </row>
-    <row r="12" spans="2:4" ht="30">
-      <c r="B12" s="53"/>
-      <c r="C12" s="52"/>
-      <c r="D12" s="30" t="s">
+    <row r="12" spans="2:4" ht="30.75">
+      <c r="B12" s="68"/>
+      <c r="C12" s="67"/>
+      <c r="D12" s="31" t="s">
         <v>223</v>
       </c>
     </row>
-    <row r="13" spans="2:4" ht="45">
-      <c r="B13" s="50" t="s">
+    <row r="13" spans="2:4" ht="45.75">
+      <c r="B13" s="65" t="s">
         <v>224</v>
       </c>
-      <c r="C13" s="48" t="s">
+      <c r="C13" s="63" t="s">
         <v>225</v>
       </c>
       <c r="D13" s="28" t="s">
         <v>226</v>
       </c>
     </row>
-    <row r="14" spans="2:4" ht="30">
-      <c r="B14" s="53"/>
-      <c r="C14" s="52"/>
-      <c r="D14" s="30" t="s">
+    <row r="14" spans="2:4" ht="30.75">
+      <c r="B14" s="68"/>
+      <c r="C14" s="67"/>
+      <c r="D14" s="31" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="15" spans="2:4" ht="45.75">
+      <c r="B15" s="68"/>
+      <c r="C15" s="67"/>
+      <c r="D15" s="30" t="s">
         <v>227</v>
       </c>
     </row>
-    <row r="15" spans="2:4" ht="45">
-      <c r="B15" s="53"/>
-      <c r="C15" s="52"/>
-      <c r="D15" s="30" t="s">
+    <row r="16" spans="2:4" ht="60">
+      <c r="B16" s="68"/>
+      <c r="C16" s="67"/>
+      <c r="D16" s="30" t="s">
         <v>228</v>
       </c>
     </row>
-    <row r="16" spans="2:4" ht="60">
-      <c r="B16" s="53"/>
-      <c r="C16" s="52"/>
-      <c r="D16" s="30" t="s">
+    <row r="17" spans="2:4" ht="45">
+      <c r="B17" s="65" t="s">
         <v>229</v>
       </c>
-    </row>
-    <row r="17" spans="2:4" ht="45">
-      <c r="B17" s="50" t="s">
+      <c r="C17" s="63" t="s">
         <v>230</v>
       </c>
-      <c r="C17" s="48" t="s">
+      <c r="D17" s="28" t="s">
         <v>231</v>
       </c>
-      <c r="D17" s="28" t="s">
+    </row>
+    <row r="18" spans="2:4" ht="45">
+      <c r="B18" s="68"/>
+      <c r="C18" s="67"/>
+      <c r="D18" s="30" t="s">
         <v>232</v>
       </c>
     </row>
-    <row r="18" spans="2:4" ht="45">
-      <c r="B18" s="53"/>
-      <c r="C18" s="52"/>
-      <c r="D18" s="30" t="s">
+    <row r="19" spans="2:4" ht="60.75" customHeight="1">
+      <c r="B19" s="65" t="s">
         <v>233</v>
       </c>
-    </row>
-    <row r="19" spans="2:4" ht="60.75" customHeight="1">
-      <c r="B19" s="50" t="s">
+      <c r="C19" s="63" t="s">
         <v>234</v>
       </c>
-      <c r="C19" s="48" t="s">
+      <c r="D19" s="28" t="s">
         <v>235</v>
       </c>
-      <c r="D19" s="28" t="s">
+    </row>
+    <row r="20" spans="2:4" ht="30.75">
+      <c r="B20" s="68"/>
+      <c r="C20" s="67"/>
+      <c r="D20" s="31" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="21" spans="2:4" ht="45.75">
+      <c r="B21" s="65" t="s">
         <v>236</v>
       </c>
-    </row>
-    <row r="20" spans="2:4" ht="30">
-      <c r="B20" s="53"/>
-      <c r="C20" s="52"/>
-      <c r="D20" s="30" t="s">
+      <c r="C21" s="63" t="s">
         <v>237</v>
       </c>
-    </row>
-    <row r="21" spans="2:4" ht="45">
-      <c r="B21" s="50" t="s">
+      <c r="D21" s="28" t="s">
         <v>238</v>
       </c>
-      <c r="C21" s="48" t="s">
+    </row>
+    <row r="22" spans="2:4" ht="30.75">
+      <c r="B22" s="68"/>
+      <c r="C22" s="69"/>
+      <c r="D22" s="31" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="23" spans="2:4" ht="62.25" customHeight="1">
+      <c r="B23" s="65" t="s">
         <v>239</v>
       </c>
-      <c r="D21" s="28" t="s">
+      <c r="C23" s="63" t="s">
         <v>240</v>
       </c>
-    </row>
-    <row r="22" spans="2:4" ht="30">
-      <c r="B22" s="51"/>
-      <c r="C22" s="49"/>
-      <c r="D22" s="31" t="s">
+      <c r="D23" s="28" t="s">
         <v>241</v>
       </c>
     </row>
+    <row r="24" spans="2:4" ht="62.25" customHeight="1">
+      <c r="B24" s="68"/>
+      <c r="C24" s="69"/>
+      <c r="D24" s="30" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="25" spans="2:4" ht="30.75">
+      <c r="B25" s="66"/>
+      <c r="C25" s="64"/>
+      <c r="D25" s="30" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="26" spans="2:4" ht="45.75">
+      <c r="B26" s="65" t="s">
+        <v>243</v>
+      </c>
+      <c r="C26" s="63" t="s">
+        <v>244</v>
+      </c>
+      <c r="D26" s="28" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="27" spans="2:4" ht="60.75">
+      <c r="B27" s="68"/>
+      <c r="C27" s="69"/>
+      <c r="D27" s="30" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="28" spans="2:4" ht="30.75">
+      <c r="B28" s="68"/>
+      <c r="C28" s="69"/>
+      <c r="D28" s="30" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="29" spans="2:4" ht="45.75">
+      <c r="B29" s="70" t="s">
+        <v>245</v>
+      </c>
+      <c r="C29" s="63" t="s">
+        <v>246</v>
+      </c>
+      <c r="D29" s="28" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="30" spans="2:4" ht="60.75">
+      <c r="B30" s="71"/>
+      <c r="C30" s="69"/>
+      <c r="D30" s="30" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="31" spans="2:4" ht="30.75">
+      <c r="B31" s="71"/>
+      <c r="C31" s="69"/>
+      <c r="D31" s="30" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="32" spans="2:4" ht="60.75">
+      <c r="B32" s="72"/>
+      <c r="C32" s="64"/>
+      <c r="D32" s="31" t="s">
+        <v>247</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="16">
+  <mergeCells count="22">
+    <mergeCell ref="C29:C32"/>
+    <mergeCell ref="B29:B32"/>
+    <mergeCell ref="C23:C25"/>
+    <mergeCell ref="B23:B25"/>
+    <mergeCell ref="C26:C28"/>
+    <mergeCell ref="B26:B28"/>
     <mergeCell ref="C21:C22"/>
     <mergeCell ref="B21:B22"/>
     <mergeCell ref="C19:C20"/>
@@ -7725,6 +7870,65 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1914FF74-0E8B-4E92-8BDD-103E839E1854}">
+  <dimension ref="B3:C7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E9" sqref="E9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="2" max="2" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="73.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="2:3" ht="23.25">
+      <c r="B3" s="47" t="s">
+        <v>27</v>
+      </c>
+      <c r="C3" s="47" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="4" spans="2:3">
+      <c r="B4" s="3" t="s">
+        <v>249</v>
+      </c>
+      <c r="C4" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="5" spans="2:3">
+      <c r="B5" s="3" t="s">
+        <v>251</v>
+      </c>
+      <c r="C5" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="6" spans="2:3">
+      <c r="B6" s="3" t="s">
+        <v>253</v>
+      </c>
+      <c r="C6" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="7" spans="2:3">
+      <c r="B7" s="3" t="s">
+        <v>255</v>
+      </c>
+      <c r="C7" t="s">
+        <v>256</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A2:S19"/>
   <sheetViews>
@@ -7743,26 +7947,26 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:19">
-      <c r="A2" s="47" t="s">
+      <c r="A2" s="53" t="s">
         <v>160</v>
       </c>
-      <c r="B2" s="47"/>
-      <c r="C2" s="47"/>
-      <c r="F2" s="47" t="s">
+      <c r="B2" s="53"/>
+      <c r="C2" s="53"/>
+      <c r="F2" s="53" t="s">
         <v>165</v>
       </c>
-      <c r="G2" s="47"/>
-      <c r="H2" s="47"/>
+      <c r="G2" s="53"/>
+      <c r="H2" s="53"/>
     </row>
     <row r="3" spans="1:19">
       <c r="A3" t="s">
-        <v>242</v>
+        <v>257</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>21</v>
       </c>
       <c r="F3" t="s">
-        <v>242</v>
+        <v>257</v>
       </c>
       <c r="G3" s="1" t="s">
         <v>26</v>
@@ -7786,14 +7990,14 @@
     </row>
     <row r="5" spans="1:19">
       <c r="A5" t="s">
-        <v>243</v>
+        <v>258</v>
       </c>
       <c r="B5">
         <f>SUM(C10:C14)</f>
         <v>5000</v>
       </c>
       <c r="F5" t="s">
-        <v>243</v>
+        <v>258</v>
       </c>
       <c r="G5">
         <f>SUM(H10:H14)</f>
@@ -7802,14 +8006,14 @@
     </row>
     <row r="6" spans="1:19">
       <c r="A6" t="s">
-        <v>244</v>
+        <v>259</v>
       </c>
       <c r="B6">
         <f>SUM(C17:C19)</f>
         <v>2000</v>
       </c>
       <c r="F6" t="s">
-        <v>244</v>
+        <v>259</v>
       </c>
       <c r="G6">
         <f>SUM(H17:H19)</f>
@@ -7831,7 +8035,7 @@
         <v>2</v>
       </c>
       <c r="B9" s="17" t="s">
-        <v>245</v>
+        <v>260</v>
       </c>
       <c r="C9" s="17" t="s">
         <v>3</v>
@@ -7840,7 +8044,7 @@
         <v>2</v>
       </c>
       <c r="G9" s="17" t="s">
-        <v>245</v>
+        <v>260</v>
       </c>
       <c r="H9" s="17" t="s">
         <v>3</v>
@@ -8030,7 +8234,7 @@
         <v>206</v>
       </c>
       <c r="B16" s="17" t="s">
-        <v>245</v>
+        <v>260</v>
       </c>
       <c r="C16" t="s">
         <v>3</v>
@@ -8039,7 +8243,7 @@
         <v>206</v>
       </c>
       <c r="G16" s="17" t="s">
-        <v>245</v>
+        <v>260</v>
       </c>
       <c r="H16" t="s">
         <v>3</v>

</xml_diff>

<commit_message>
Added few more cards with Pierce mechanic
Added few more cards with Pierce mechanic
</commit_message>
<xml_diff>
--- a/ShipCardGameCalcs.xlsx
+++ b/ShipCardGameCalcs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MultiplayerGame\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{7C940714-625D-4C48-A3A9-03623713CFAE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{1A0DFE89-4D13-4BBE-8BF3-FD4398C4F847}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="4" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="6" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Values" sheetId="1" r:id="rId1"/>
@@ -843,7 +843,7 @@
     <t>Corrosion</t>
   </si>
   <si>
-    <t>Deals damage straight to hull over time</t>
+    <t>Deals damage straight to hull at the start of target players turn</t>
   </si>
   <si>
     <t>Swarm</t>
@@ -1292,7 +1292,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="73">
+  <cellXfs count="72">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1429,22 +1429,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1455,6 +1443,15 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -6581,7 +6578,7 @@
     <row r="16" spans="2:19">
       <c r="P16">
         <f ca="1">RANDBETWEEN(0,123)</f>
-        <v>113</v>
+        <v>58</v>
       </c>
     </row>
     <row r="17" spans="2:16">
@@ -7564,7 +7561,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1CADF2F4-A124-44BC-8A72-4CE3F16F5D04}">
   <dimension ref="B2:D32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A24" workbookViewId="0">
+    <sheetView topLeftCell="A23" workbookViewId="0">
       <selection activeCell="D32" sqref="B29:D32"/>
     </sheetView>
   </sheetViews>
@@ -7587,7 +7584,7 @@
       </c>
     </row>
     <row r="3" spans="2:4" ht="106.5" customHeight="1">
-      <c r="B3" s="65" t="s">
+      <c r="B3" s="69" t="s">
         <v>206</v>
       </c>
       <c r="C3" s="63" t="s">
@@ -7598,28 +7595,28 @@
       </c>
     </row>
     <row r="4" spans="2:4" ht="120">
-      <c r="B4" s="68"/>
-      <c r="C4" s="67"/>
+      <c r="B4" s="70"/>
+      <c r="C4" s="64"/>
       <c r="D4" s="29" t="s">
         <v>209</v>
       </c>
     </row>
     <row r="5" spans="2:4" ht="60">
-      <c r="B5" s="68"/>
-      <c r="C5" s="67"/>
+      <c r="B5" s="70"/>
+      <c r="C5" s="64"/>
       <c r="D5" s="30" t="s">
         <v>210</v>
       </c>
     </row>
     <row r="6" spans="2:4" ht="75">
-      <c r="B6" s="68"/>
-      <c r="C6" s="67"/>
+      <c r="B6" s="70"/>
+      <c r="C6" s="64"/>
       <c r="D6" s="30" t="s">
         <v>211</v>
       </c>
     </row>
     <row r="7" spans="2:4" ht="90">
-      <c r="B7" s="65" t="s">
+      <c r="B7" s="69" t="s">
         <v>212</v>
       </c>
       <c r="C7" s="63" t="s">
@@ -7630,14 +7627,14 @@
       </c>
     </row>
     <row r="8" spans="2:4" ht="90">
-      <c r="B8" s="68"/>
-      <c r="C8" s="67"/>
+      <c r="B8" s="70"/>
+      <c r="C8" s="64"/>
       <c r="D8" s="30" t="s">
         <v>215</v>
       </c>
     </row>
     <row r="9" spans="2:4" ht="75">
-      <c r="B9" s="65" t="s">
+      <c r="B9" s="69" t="s">
         <v>216</v>
       </c>
       <c r="C9" s="63" t="s">
@@ -7648,14 +7645,14 @@
       </c>
     </row>
     <row r="10" spans="2:4" ht="30">
-      <c r="B10" s="66"/>
-      <c r="C10" s="64"/>
+      <c r="B10" s="71"/>
+      <c r="C10" s="65"/>
       <c r="D10" s="31" t="s">
         <v>219</v>
       </c>
     </row>
     <row r="11" spans="2:4" ht="76.5" customHeight="1">
-      <c r="B11" s="65" t="s">
+      <c r="B11" s="69" t="s">
         <v>220</v>
       </c>
       <c r="C11" s="63" t="s">
@@ -7666,14 +7663,14 @@
       </c>
     </row>
     <row r="12" spans="2:4" ht="30.75">
-      <c r="B12" s="68"/>
-      <c r="C12" s="67"/>
+      <c r="B12" s="70"/>
+      <c r="C12" s="64"/>
       <c r="D12" s="31" t="s">
         <v>223</v>
       </c>
     </row>
     <row r="13" spans="2:4" ht="45.75">
-      <c r="B13" s="65" t="s">
+      <c r="B13" s="69" t="s">
         <v>224</v>
       </c>
       <c r="C13" s="63" t="s">
@@ -7684,28 +7681,28 @@
       </c>
     </row>
     <row r="14" spans="2:4" ht="30.75">
-      <c r="B14" s="68"/>
-      <c r="C14" s="67"/>
+      <c r="B14" s="70"/>
+      <c r="C14" s="64"/>
       <c r="D14" s="31" t="s">
         <v>223</v>
       </c>
     </row>
     <row r="15" spans="2:4" ht="45.75">
-      <c r="B15" s="68"/>
-      <c r="C15" s="67"/>
+      <c r="B15" s="70"/>
+      <c r="C15" s="64"/>
       <c r="D15" s="30" t="s">
         <v>227</v>
       </c>
     </row>
     <row r="16" spans="2:4" ht="60">
-      <c r="B16" s="68"/>
-      <c r="C16" s="67"/>
+      <c r="B16" s="70"/>
+      <c r="C16" s="64"/>
       <c r="D16" s="30" t="s">
         <v>228</v>
       </c>
     </row>
     <row r="17" spans="2:4" ht="45">
-      <c r="B17" s="65" t="s">
+      <c r="B17" s="69" t="s">
         <v>229</v>
       </c>
       <c r="C17" s="63" t="s">
@@ -7716,14 +7713,14 @@
       </c>
     </row>
     <row r="18" spans="2:4" ht="45">
-      <c r="B18" s="68"/>
-      <c r="C18" s="67"/>
+      <c r="B18" s="70"/>
+      <c r="C18" s="64"/>
       <c r="D18" s="30" t="s">
         <v>232</v>
       </c>
     </row>
     <row r="19" spans="2:4" ht="60.75" customHeight="1">
-      <c r="B19" s="65" t="s">
+      <c r="B19" s="69" t="s">
         <v>233</v>
       </c>
       <c r="C19" s="63" t="s">
@@ -7734,14 +7731,14 @@
       </c>
     </row>
     <row r="20" spans="2:4" ht="30.75">
-      <c r="B20" s="68"/>
-      <c r="C20" s="67"/>
+      <c r="B20" s="70"/>
+      <c r="C20" s="64"/>
       <c r="D20" s="31" t="s">
         <v>223</v>
       </c>
     </row>
     <row r="21" spans="2:4" ht="45.75">
-      <c r="B21" s="65" t="s">
+      <c r="B21" s="69" t="s">
         <v>236</v>
       </c>
       <c r="C21" s="63" t="s">
@@ -7752,14 +7749,14 @@
       </c>
     </row>
     <row r="22" spans="2:4" ht="30.75">
-      <c r="B22" s="68"/>
-      <c r="C22" s="69"/>
+      <c r="B22" s="70"/>
+      <c r="C22" s="64"/>
       <c r="D22" s="31" t="s">
         <v>223</v>
       </c>
     </row>
     <row r="23" spans="2:4" ht="62.25" customHeight="1">
-      <c r="B23" s="65" t="s">
+      <c r="B23" s="69" t="s">
         <v>239</v>
       </c>
       <c r="C23" s="63" t="s">
@@ -7770,21 +7767,21 @@
       </c>
     </row>
     <row r="24" spans="2:4" ht="62.25" customHeight="1">
-      <c r="B24" s="68"/>
-      <c r="C24" s="69"/>
+      <c r="B24" s="70"/>
+      <c r="C24" s="64"/>
       <c r="D24" s="30" t="s">
         <v>242</v>
       </c>
     </row>
     <row r="25" spans="2:4" ht="30.75">
-      <c r="B25" s="66"/>
-      <c r="C25" s="64"/>
+      <c r="B25" s="71"/>
+      <c r="C25" s="65"/>
       <c r="D25" s="30" t="s">
         <v>223</v>
       </c>
     </row>
     <row r="26" spans="2:4" ht="45.75">
-      <c r="B26" s="65" t="s">
+      <c r="B26" s="69" t="s">
         <v>243</v>
       </c>
       <c r="C26" s="63" t="s">
@@ -7795,21 +7792,21 @@
       </c>
     </row>
     <row r="27" spans="2:4" ht="60.75">
-      <c r="B27" s="68"/>
-      <c r="C27" s="69"/>
+      <c r="B27" s="70"/>
+      <c r="C27" s="64"/>
       <c r="D27" s="30" t="s">
         <v>242</v>
       </c>
     </row>
     <row r="28" spans="2:4" ht="30.75">
-      <c r="B28" s="68"/>
-      <c r="C28" s="69"/>
+      <c r="B28" s="70"/>
+      <c r="C28" s="64"/>
       <c r="D28" s="30" t="s">
         <v>223</v>
       </c>
     </row>
     <row r="29" spans="2:4" ht="45.75">
-      <c r="B29" s="70" t="s">
+      <c r="B29" s="66" t="s">
         <v>245</v>
       </c>
       <c r="C29" s="63" t="s">
@@ -7820,34 +7817,28 @@
       </c>
     </row>
     <row r="30" spans="2:4" ht="60.75">
-      <c r="B30" s="71"/>
-      <c r="C30" s="69"/>
+      <c r="B30" s="67"/>
+      <c r="C30" s="64"/>
       <c r="D30" s="30" t="s">
         <v>242</v>
       </c>
     </row>
     <row r="31" spans="2:4" ht="30.75">
-      <c r="B31" s="71"/>
-      <c r="C31" s="69"/>
+      <c r="B31" s="67"/>
+      <c r="C31" s="64"/>
       <c r="D31" s="30" t="s">
         <v>223</v>
       </c>
     </row>
     <row r="32" spans="2:4" ht="60.75">
-      <c r="B32" s="72"/>
-      <c r="C32" s="64"/>
+      <c r="B32" s="68"/>
+      <c r="C32" s="65"/>
       <c r="D32" s="31" t="s">
         <v>247</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="22">
-    <mergeCell ref="C29:C32"/>
-    <mergeCell ref="B29:B32"/>
-    <mergeCell ref="C23:C25"/>
-    <mergeCell ref="B23:B25"/>
-    <mergeCell ref="C26:C28"/>
-    <mergeCell ref="B26:B28"/>
     <mergeCell ref="C21:C22"/>
     <mergeCell ref="B21:B22"/>
     <mergeCell ref="C19:C20"/>
@@ -7864,6 +7855,12 @@
     <mergeCell ref="B13:B16"/>
     <mergeCell ref="C17:C18"/>
     <mergeCell ref="B17:B18"/>
+    <mergeCell ref="C29:C32"/>
+    <mergeCell ref="B29:B32"/>
+    <mergeCell ref="C23:C25"/>
+    <mergeCell ref="B23:B25"/>
+    <mergeCell ref="C26:C28"/>
+    <mergeCell ref="B26:B28"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -7873,8 +7870,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1914FF74-0E8B-4E92-8BDD-103E839E1854}">
   <dimension ref="B3:C7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>

</xml_diff>

<commit_message>
Ironed out mechanics for each department
Ironed out mechanics for each department and added cards. Also named core mechanics and game phases more
</commit_message>
<xml_diff>
--- a/ShipCardGameCalcs.xlsx
+++ b/ShipCardGameCalcs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MultiplayerGame\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{1A0DFE89-4D13-4BBE-8BF3-FD4398C4F847}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{A4EFA6C7-89AA-4E42-B8B0-9C8437321480}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="6" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="4" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Values" sheetId="1" r:id="rId1"/>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="497" uniqueCount="261">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="534" uniqueCount="288">
   <si>
     <t>Ship Parameters</t>
   </si>
@@ -288,6 +288,21 @@
     <t>Points towards cards based around enemy crew</t>
   </si>
   <si>
+    <t>Starter Recommended</t>
+  </si>
+  <si>
+    <t>Medic/Research</t>
+  </si>
+  <si>
+    <t>Research/Engineering</t>
+  </si>
+  <si>
+    <t>Assault/Handling</t>
+  </si>
+  <si>
+    <t>Engineering/Medic</t>
+  </si>
+  <si>
     <t>Assault</t>
   </si>
   <si>
@@ -603,10 +618,13 @@
     <t>There are different phases during each players turns which run in the following order which only the current player does on their turn:</t>
   </si>
   <si>
-    <t>Here you untap any cards out on the space field unless stated otherwise</t>
-  </si>
-  <si>
-    <t>Crew Hire Phase</t>
+    <t>Disengage Phase</t>
+  </si>
+  <si>
+    <t>Here you Disengage (Turn any cards back to an upright position) any cards out on the space field unless stated otherwise and can choose to deploy to a different owned ship</t>
+  </si>
+  <si>
+    <t>Resource Allocation Phase</t>
   </si>
   <si>
     <t>Increment 1 of your department dice by 1 (Note you start off at 0 and a department dice goes up to a max of 20 each)</t>
@@ -621,7 +639,7 @@
     <t xml:space="preserve"> Also there can only ever be 1 admiral card on your side of the space field at any one time. Certain cards can also be played during your opponents turn at different phases.</t>
   </si>
   <si>
-    <t>To pay for the cost to play cards you will need to either tap a crew card or use some of your department dice resource by decreasing the department dice. You can use the  combination of crew cards and department dice</t>
+    <t>To pay for the cost to play cards you will need to either Engage a crew card or use some of your department dice resource by decreasing the department dice. You can use the  combination of crew cards and department dice</t>
   </si>
   <si>
     <t>Note that when using the department dice you don't regain what you had next turn.</t>
@@ -630,13 +648,13 @@
     <t>You can only assign crew cards to a ship if there is a free crew slot available</t>
   </si>
   <si>
-    <t>If you have any tier 1,2 or 3 crew members untapped they can be used to tap and assigned to a gun slot and fire at an enemy ship.</t>
+    <t>If you have any tier 1,2 or 3 crew members Disengagedthey can be used to Engage and assigned to a gun slot and fire at an enemy ship.</t>
   </si>
   <si>
     <t>If for example a ship has 3 gun slots, then only 3 crew cards can be assigned to a gun slot</t>
   </si>
   <si>
-    <t>Once you have assigned all targets, the assigned player can react with cards and use other ships to maneuver in front of the targeted ship making them the target (this requires at least 1 tier 1,2 or 3 crew member on that ship to tap).</t>
+    <t>Once you have assigned all targets, the assigned player can react with cards and use other ships to maneuver in front of the targeted ship making them the target (this requires at least 1 tier 1,2 or 3 crew member on that ship to Engage).</t>
   </si>
   <si>
     <t>Damage Phase</t>
@@ -663,7 +681,7 @@
     <t>You keep any unspent dice department resource NOT crew card resource</t>
   </si>
   <si>
-    <t>Now the turn gets moved to the next player on your left and they start their untap phase.</t>
+    <t>Now the turn gets moved to the next player on your left and they start their Disengage phase.</t>
   </si>
   <si>
     <t>Controlled deck is the battlefield conditions which affects the battlefield</t>
@@ -714,10 +732,10 @@
     <t>A crew card can only be played to fill A ships service slot. Only one crew card can be played per turn.</t>
   </si>
   <si>
-    <t>On tap a crew type card can be used to either provide a given department point used to play other cards or activate card abilities. Amount and Department point/s are defined on the card</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Any crew card can be tapped and assigned to their ships gun slot and shoot an enemy target ship </t>
+    <t>On Engage, a crew type card can be used to either provide a given department point used to play other cards or activate card abilities. Amount and Department point/s are defined on the card</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Any crew card can be Engaged and assigned to their ships gun slot and shoot an enemy target ship </t>
   </si>
   <si>
     <t>Crew cards will have a given Rank, Rank 1 can be played for free to a ship. Ranks higher than 1 will require a cost to be played</t>
@@ -834,12 +852,18 @@
     <t>Detail</t>
   </si>
   <si>
+    <t>Department Specific</t>
+  </si>
+  <si>
     <t>Piercing Round</t>
   </si>
   <si>
     <t>Deals damage straight to hull from gun slot</t>
   </si>
   <si>
+    <t>Engineering</t>
+  </si>
+  <si>
     <t>Corrosion</t>
   </si>
   <si>
@@ -855,7 +879,64 @@
     <t>Infection</t>
   </si>
   <si>
-    <t>Sacrifice 1 crew</t>
+    <t>Enemy ship Sacrifice 1 crew</t>
+  </si>
+  <si>
+    <t>Medic</t>
+  </si>
+  <si>
+    <t>Engage</t>
+  </si>
+  <si>
+    <t>To Engage a card the player must turn the card 90 degrees. Once this is done the card can't engage again until they are turned back facing the correct way. This can happen during the Disengage phase</t>
+  </si>
+  <si>
+    <t>Disengage</t>
+  </si>
+  <si>
+    <t>Turn card back to upright position</t>
+  </si>
+  <si>
+    <t>Sacrifice</t>
+  </si>
+  <si>
+    <t>Send target crew to Stasis</t>
+  </si>
+  <si>
+    <t>Evasion</t>
+  </si>
+  <si>
+    <t>Evade attack when targetted</t>
+  </si>
+  <si>
+    <t>Formation</t>
+  </si>
+  <si>
+    <t>When multiple of your ships attack</t>
+  </si>
+  <si>
+    <t>Repair</t>
+  </si>
+  <si>
+    <t>Repair ship by X amount</t>
+  </si>
+  <si>
+    <t>Invade</t>
+  </si>
+  <si>
+    <t>Disable enemy crew</t>
+  </si>
+  <si>
+    <t>Science</t>
+  </si>
+  <si>
+    <t>Draw/scry from Strategy deck</t>
+  </si>
+  <si>
+    <t>Revive</t>
+  </si>
+  <si>
+    <t>Return target crew from stasis</t>
   </si>
   <si>
     <t>Fleet Option</t>
@@ -1292,7 +1373,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="72">
+  <cellXfs count="73">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1396,6 +1477,9 @@
     <xf numFmtId="0" fontId="0" fillId="9" borderId="24" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -3547,21 +3631,21 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17">
-      <c r="A1" s="53" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="53"/>
-      <c r="C1" s="53"/>
-      <c r="D1" s="53"/>
-      <c r="E1" s="53"/>
-      <c r="F1" s="53"/>
-      <c r="G1" s="53"/>
-      <c r="H1" s="53"/>
-      <c r="N1" s="53" t="s">
+      <c r="A1" s="54" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="54"/>
+      <c r="C1" s="54"/>
+      <c r="D1" s="54"/>
+      <c r="E1" s="54"/>
+      <c r="F1" s="54"/>
+      <c r="G1" s="54"/>
+      <c r="H1" s="54"/>
+      <c r="N1" s="54" t="s">
         <v>1</v>
       </c>
-      <c r="O1" s="53"/>
-      <c r="P1" s="53"/>
+      <c r="O1" s="54"/>
+      <c r="P1" s="54"/>
     </row>
     <row r="2" spans="1:17">
       <c r="A2" s="9" t="s">
@@ -3828,25 +3912,25 @@
       </c>
     </row>
     <row r="8" spans="1:17">
-      <c r="A8" s="53" t="s">
+      <c r="A8" s="54" t="s">
         <v>18</v>
       </c>
-      <c r="B8" s="53"/>
-      <c r="C8" s="53"/>
-      <c r="D8" s="53"/>
-      <c r="E8" s="53"/>
-      <c r="F8" s="53"/>
-      <c r="G8" s="53"/>
-      <c r="J8" s="53" t="s">
+      <c r="B8" s="54"/>
+      <c r="C8" s="54"/>
+      <c r="D8" s="54"/>
+      <c r="E8" s="54"/>
+      <c r="F8" s="54"/>
+      <c r="G8" s="54"/>
+      <c r="J8" s="54" t="s">
         <v>19</v>
       </c>
-      <c r="K8" s="53"/>
-      <c r="L8" s="53"/>
-      <c r="M8" s="53"/>
-      <c r="N8" s="53"/>
-      <c r="O8" s="53"/>
-      <c r="P8" s="53"/>
-      <c r="Q8" s="53"/>
+      <c r="K8" s="54"/>
+      <c r="L8" s="54"/>
+      <c r="M8" s="54"/>
+      <c r="N8" s="54"/>
+      <c r="O8" s="54"/>
+      <c r="P8" s="54"/>
+      <c r="Q8" s="54"/>
     </row>
     <row r="9" spans="1:17">
       <c r="A9" s="8" t="s">
@@ -4186,15 +4270,15 @@
       <c r="Q15" s="1"/>
     </row>
     <row r="16" spans="1:17">
-      <c r="A16" s="53" t="s">
+      <c r="A16" s="54" t="s">
         <v>35</v>
       </c>
-      <c r="B16" s="53"/>
-      <c r="C16" s="53"/>
-      <c r="D16" s="53"/>
-      <c r="E16" s="53"/>
-      <c r="F16" s="53"/>
-      <c r="G16" s="53"/>
+      <c r="B16" s="54"/>
+      <c r="C16" s="54"/>
+      <c r="D16" s="54"/>
+      <c r="E16" s="54"/>
+      <c r="F16" s="54"/>
+      <c r="G16" s="54"/>
       <c r="K16" s="1"/>
       <c r="L16" s="1"/>
       <c r="M16" s="1"/>
@@ -4411,27 +4495,27 @@
       <c r="R22" s="4"/>
     </row>
     <row r="23" spans="1:18">
-      <c r="A23" s="53" t="s">
+      <c r="A23" s="54" t="s">
         <v>40</v>
       </c>
-      <c r="B23" s="53"/>
-      <c r="C23" s="53"/>
-      <c r="D23" s="53"/>
-      <c r="E23" s="53"/>
-      <c r="F23" s="53"/>
-      <c r="G23" s="53"/>
-      <c r="H23" s="53"/>
+      <c r="B23" s="54"/>
+      <c r="C23" s="54"/>
+      <c r="D23" s="54"/>
+      <c r="E23" s="54"/>
+      <c r="F23" s="54"/>
+      <c r="G23" s="54"/>
+      <c r="H23" s="54"/>
       <c r="I23" s="4"/>
-      <c r="J23" s="53" t="s">
+      <c r="J23" s="54" t="s">
         <v>41</v>
       </c>
-      <c r="K23" s="53"/>
-      <c r="L23" s="53"/>
-      <c r="M23" s="53"/>
-      <c r="N23" s="53"/>
-      <c r="O23" s="53"/>
-      <c r="P23" s="53"/>
-      <c r="Q23" s="53"/>
+      <c r="K23" s="54"/>
+      <c r="L23" s="54"/>
+      <c r="M23" s="54"/>
+      <c r="N23" s="54"/>
+      <c r="O23" s="54"/>
+      <c r="P23" s="54"/>
+      <c r="Q23" s="54"/>
     </row>
     <row r="24" spans="1:18">
       <c r="A24" s="8" t="s">
@@ -4859,25 +4943,25 @@
       <c r="Q30" s="1"/>
     </row>
     <row r="31" spans="1:18">
-      <c r="A31" s="53" t="s">
+      <c r="A31" s="54" t="s">
         <v>47</v>
       </c>
-      <c r="B31" s="53"/>
-      <c r="C31" s="53"/>
-      <c r="D31" s="53"/>
-      <c r="E31" s="53"/>
-      <c r="F31" s="53"/>
-      <c r="G31" s="53"/>
+      <c r="B31" s="54"/>
+      <c r="C31" s="54"/>
+      <c r="D31" s="54"/>
+      <c r="E31" s="54"/>
+      <c r="F31" s="54"/>
+      <c r="G31" s="54"/>
       <c r="I31" s="4"/>
-      <c r="J31" s="53" t="s">
+      <c r="J31" s="54" t="s">
         <v>48</v>
       </c>
-      <c r="K31" s="53"/>
-      <c r="L31" s="53"/>
-      <c r="M31" s="53"/>
-      <c r="N31" s="53"/>
-      <c r="O31" s="53"/>
-      <c r="P31" s="53"/>
+      <c r="K31" s="54"/>
+      <c r="L31" s="54"/>
+      <c r="M31" s="54"/>
+      <c r="N31" s="54"/>
+      <c r="O31" s="54"/>
+      <c r="P31" s="54"/>
     </row>
     <row r="32" spans="1:18">
       <c r="A32" t="s">
@@ -5599,10 +5683,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{91273792-62E9-442E-9CC7-E8C6E6BD4008}">
-  <dimension ref="B1:V29"/>
+  <dimension ref="B1:V32"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J19" sqref="J19"/>
+      <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -6345,6 +6429,31 @@
       <c r="H29">
         <f>(H26*G5*F5)+(H28*G7*F7)</f>
         <v>1500</v>
+      </c>
+    </row>
+    <row r="31" spans="2:12">
+      <c r="C31" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="32" spans="2:12">
+      <c r="C32" t="s">
+        <v>68</v>
+      </c>
+      <c r="D32" t="s">
+        <v>69</v>
+      </c>
+      <c r="E32" t="s">
+        <v>70</v>
+      </c>
+      <c r="F32" t="s">
+        <v>71</v>
+      </c>
+      <c r="G32" t="s">
+        <v>70</v>
+      </c>
+      <c r="H32" t="s">
+        <v>58</v>
       </c>
     </row>
   </sheetData>
@@ -6390,7 +6499,7 @@
         <v>58</v>
       </c>
       <c r="K2" t="s">
-        <v>67</v>
+        <v>72</v>
       </c>
     </row>
     <row r="3" spans="2:19">
@@ -6400,7 +6509,7 @@
       <c r="E3" s="42"/>
       <c r="F3" s="42"/>
       <c r="G3" s="42" t="s">
-        <v>68</v>
+        <v>73</v>
       </c>
       <c r="H3" s="42"/>
       <c r="I3" s="42"/>
@@ -6428,7 +6537,7 @@
     </row>
     <row r="4" spans="2:19">
       <c r="B4" s="45" t="s">
-        <v>69</v>
+        <v>74</v>
       </c>
       <c r="N4" s="25" t="s">
         <v>13</v>
@@ -6451,7 +6560,7 @@
     </row>
     <row r="5" spans="2:19">
       <c r="B5" s="43" t="s">
-        <v>70</v>
+        <v>75</v>
       </c>
       <c r="N5" s="26" t="s">
         <v>14</v>
@@ -6474,7 +6583,7 @@
     </row>
     <row r="6" spans="2:19">
       <c r="B6" s="45" t="s">
-        <v>71</v>
+        <v>76</v>
       </c>
       <c r="N6" s="27" t="s">
         <v>15</v>
@@ -6497,7 +6606,7 @@
     </row>
     <row r="7" spans="2:19">
       <c r="B7" s="6" t="s">
-        <v>72</v>
+        <v>77</v>
       </c>
       <c r="N7" s="26" t="s">
         <v>16</v>
@@ -6578,13 +6687,13 @@
     <row r="16" spans="2:19">
       <c r="P16">
         <f ca="1">RANDBETWEEN(0,123)</f>
-        <v>58</v>
+        <v>64</v>
       </c>
     </row>
     <row r="17" spans="2:16">
       <c r="P17" s="46">
         <f ca="1">RANDBETWEEN(0,6)</f>
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="18" spans="2:16">
@@ -6601,12 +6710,12 @@
         <v>17</v>
       </c>
       <c r="L18" s="6" t="s">
-        <v>72</v>
+        <v>77</v>
       </c>
     </row>
     <row r="19" spans="2:16">
       <c r="L19" s="45" t="s">
-        <v>71</v>
+        <v>76</v>
       </c>
     </row>
     <row r="20" spans="2:16">
@@ -6617,12 +6726,12 @@
         <v>17</v>
       </c>
       <c r="L20" s="43" t="s">
-        <v>70</v>
+        <v>75</v>
       </c>
     </row>
     <row r="21" spans="2:16">
       <c r="L21" s="45" t="s">
-        <v>69</v>
+        <v>74</v>
       </c>
     </row>
     <row r="22" spans="2:16">
@@ -6632,7 +6741,7 @@
       <c r="E22" s="2"/>
       <c r="F22" s="2"/>
       <c r="G22" s="2" t="s">
-        <v>73</v>
+        <v>78</v>
       </c>
       <c r="H22" s="2"/>
       <c r="I22" s="2"/>
@@ -6668,7 +6777,7 @@
         <v>58</v>
       </c>
       <c r="L25" t="s">
-        <v>67</v>
+        <v>72</v>
       </c>
     </row>
   </sheetData>
@@ -6680,8 +6789,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F5EC53A5-8F19-4711-93EA-0F4CBD261EC8}">
   <dimension ref="B2:B83"/>
   <sheetViews>
-    <sheetView topLeftCell="A61" workbookViewId="0">
-      <selection activeCell="F83" sqref="F83"/>
+    <sheetView topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="H25" sqref="H25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -6691,347 +6800,347 @@
   <sheetData>
     <row r="2" spans="2:2">
       <c r="B2" s="21" t="s">
-        <v>74</v>
+        <v>79</v>
       </c>
     </row>
     <row r="3" spans="2:2">
       <c r="B3" s="3" t="s">
-        <v>75</v>
+        <v>80</v>
       </c>
     </row>
     <row r="4" spans="2:2">
       <c r="B4" t="s">
-        <v>76</v>
+        <v>81</v>
       </c>
     </row>
     <row r="5" spans="2:2">
       <c r="B5" t="s">
-        <v>77</v>
+        <v>82</v>
       </c>
     </row>
     <row r="6" spans="2:2">
       <c r="B6" t="s">
-        <v>78</v>
+        <v>83</v>
       </c>
     </row>
     <row r="7" spans="2:2">
       <c r="B7" t="s">
-        <v>79</v>
+        <v>84</v>
       </c>
     </row>
     <row r="8" spans="2:2">
       <c r="B8" t="s">
-        <v>80</v>
+        <v>85</v>
       </c>
     </row>
     <row r="9" spans="2:2">
       <c r="B9" t="s">
-        <v>81</v>
+        <v>86</v>
       </c>
     </row>
     <row r="10" spans="2:2">
       <c r="B10" t="s">
-        <v>82</v>
+        <v>87</v>
       </c>
     </row>
     <row r="11" spans="2:2">
       <c r="B11" t="s">
-        <v>83</v>
+        <v>88</v>
       </c>
     </row>
     <row r="13" spans="2:2">
       <c r="B13" s="3" t="s">
-        <v>84</v>
+        <v>89</v>
       </c>
     </row>
     <row r="14" spans="2:2">
       <c r="B14" t="s">
-        <v>85</v>
+        <v>90</v>
       </c>
     </row>
     <row r="15" spans="2:2">
       <c r="B15" t="s">
-        <v>86</v>
+        <v>91</v>
       </c>
     </row>
     <row r="17" spans="2:2">
       <c r="B17" s="3" t="s">
-        <v>87</v>
+        <v>92</v>
       </c>
     </row>
     <row r="18" spans="2:2">
       <c r="B18" t="s">
-        <v>88</v>
+        <v>93</v>
       </c>
     </row>
     <row r="19" spans="2:2">
       <c r="B19" t="s">
-        <v>89</v>
+        <v>94</v>
       </c>
     </row>
     <row r="20" spans="2:2">
       <c r="B20" t="s">
-        <v>90</v>
+        <v>95</v>
       </c>
     </row>
     <row r="21" spans="2:2">
       <c r="B21" t="s">
-        <v>91</v>
+        <v>96</v>
       </c>
     </row>
     <row r="22" spans="2:2">
       <c r="B22" t="s">
-        <v>92</v>
+        <v>97</v>
       </c>
     </row>
     <row r="24" spans="2:2">
       <c r="B24" s="3" t="s">
-        <v>93</v>
+        <v>98</v>
       </c>
     </row>
     <row r="25" spans="2:2">
       <c r="B25" t="s">
-        <v>94</v>
+        <v>99</v>
       </c>
     </row>
     <row r="26" spans="2:2">
       <c r="B26" t="s">
-        <v>95</v>
+        <v>100</v>
       </c>
     </row>
     <row r="28" spans="2:2">
       <c r="B28" s="3" t="s">
-        <v>96</v>
+        <v>101</v>
       </c>
     </row>
     <row r="29" spans="2:2">
       <c r="B29" t="s">
-        <v>97</v>
+        <v>102</v>
       </c>
     </row>
     <row r="30" spans="2:2">
       <c r="B30" t="s">
-        <v>98</v>
+        <v>103</v>
       </c>
     </row>
     <row r="32" spans="2:2">
       <c r="B32" s="3" t="s">
-        <v>99</v>
+        <v>104</v>
       </c>
     </row>
     <row r="33" spans="2:2">
       <c r="B33" t="s">
-        <v>100</v>
+        <v>105</v>
       </c>
     </row>
     <row r="35" spans="2:2">
       <c r="B35" s="3" t="s">
-        <v>101</v>
+        <v>106</v>
       </c>
     </row>
     <row r="36" spans="2:2">
       <c r="B36" t="s">
-        <v>102</v>
+        <v>107</v>
       </c>
     </row>
     <row r="38" spans="2:2">
       <c r="B38" s="3" t="s">
-        <v>103</v>
+        <v>108</v>
       </c>
     </row>
     <row r="39" spans="2:2">
       <c r="B39" t="s">
-        <v>104</v>
+        <v>109</v>
       </c>
     </row>
     <row r="41" spans="2:2">
       <c r="B41" s="3" t="s">
-        <v>105</v>
+        <v>110</v>
       </c>
     </row>
     <row r="42" spans="2:2">
       <c r="B42" t="s">
-        <v>106</v>
+        <v>111</v>
       </c>
     </row>
     <row r="43" spans="2:2">
       <c r="B43" t="s">
-        <v>107</v>
+        <v>112</v>
       </c>
     </row>
     <row r="45" spans="2:2">
       <c r="B45" s="3" t="s">
-        <v>108</v>
+        <v>113</v>
       </c>
     </row>
     <row r="46" spans="2:2">
       <c r="B46" t="s">
-        <v>109</v>
+        <v>114</v>
       </c>
     </row>
     <row r="47" spans="2:2">
       <c r="B47" t="s">
-        <v>110</v>
+        <v>115</v>
       </c>
     </row>
     <row r="48" spans="2:2">
       <c r="B48" t="s">
-        <v>111</v>
+        <v>116</v>
       </c>
     </row>
     <row r="49" spans="2:2">
       <c r="B49" t="s">
-        <v>112</v>
+        <v>117</v>
       </c>
     </row>
     <row r="50" spans="2:2">
       <c r="B50" t="s">
-        <v>113</v>
+        <v>118</v>
       </c>
     </row>
     <row r="51" spans="2:2">
       <c r="B51" t="s">
-        <v>114</v>
+        <v>119</v>
       </c>
     </row>
     <row r="52" spans="2:2">
       <c r="B52" t="s">
-        <v>115</v>
+        <v>120</v>
       </c>
     </row>
     <row r="53" spans="2:2">
       <c r="B53" t="s">
-        <v>116</v>
+        <v>121</v>
       </c>
     </row>
     <row r="54" spans="2:2">
       <c r="B54" t="s">
-        <v>117</v>
+        <v>122</v>
       </c>
     </row>
     <row r="55" spans="2:2">
       <c r="B55" t="s">
-        <v>118</v>
+        <v>123</v>
       </c>
     </row>
     <row r="56" spans="2:2">
       <c r="B56" t="s">
-        <v>119</v>
+        <v>124</v>
       </c>
     </row>
     <row r="58" spans="2:2">
       <c r="B58" s="3" t="s">
-        <v>120</v>
+        <v>125</v>
       </c>
     </row>
     <row r="59" spans="2:2">
       <c r="B59" t="s">
-        <v>121</v>
+        <v>126</v>
       </c>
     </row>
     <row r="60" spans="2:2">
       <c r="B60" t="s">
-        <v>122</v>
+        <v>127</v>
       </c>
     </row>
     <row r="61" spans="2:2">
       <c r="B61" t="s">
-        <v>123</v>
+        <v>128</v>
       </c>
     </row>
     <row r="62" spans="2:2">
       <c r="B62" t="s">
-        <v>124</v>
+        <v>129</v>
       </c>
     </row>
     <row r="63" spans="2:2">
       <c r="B63" t="s">
-        <v>125</v>
+        <v>130</v>
       </c>
     </row>
     <row r="64" spans="2:2">
       <c r="B64" t="s">
-        <v>126</v>
+        <v>131</v>
       </c>
     </row>
     <row r="65" spans="2:2">
       <c r="B65" t="s">
-        <v>127</v>
+        <v>132</v>
       </c>
     </row>
     <row r="66" spans="2:2">
       <c r="B66" t="s">
-        <v>128</v>
+        <v>133</v>
       </c>
     </row>
     <row r="68" spans="2:2">
       <c r="B68" s="3" t="s">
-        <v>129</v>
+        <v>134</v>
       </c>
     </row>
     <row r="69" spans="2:2">
       <c r="B69" t="s">
-        <v>130</v>
+        <v>135</v>
       </c>
     </row>
     <row r="70" spans="2:2">
       <c r="B70" t="s">
-        <v>131</v>
+        <v>136</v>
       </c>
     </row>
     <row r="71" spans="2:2">
       <c r="B71" t="s">
-        <v>132</v>
+        <v>137</v>
       </c>
     </row>
     <row r="73" spans="2:2">
       <c r="B73" s="3" t="s">
-        <v>133</v>
+        <v>138</v>
       </c>
     </row>
     <row r="74" spans="2:2">
       <c r="B74" t="s">
-        <v>134</v>
+        <v>139</v>
       </c>
     </row>
     <row r="76" spans="2:2">
       <c r="B76" s="3" t="s">
-        <v>135</v>
+        <v>140</v>
       </c>
     </row>
     <row r="77" spans="2:2">
       <c r="B77" t="s">
-        <v>136</v>
+        <v>141</v>
       </c>
     </row>
     <row r="78" spans="2:2">
       <c r="B78" t="s">
-        <v>137</v>
+        <v>142</v>
       </c>
     </row>
     <row r="79" spans="2:2">
       <c r="B79" t="s">
-        <v>138</v>
+        <v>143</v>
       </c>
     </row>
     <row r="80" spans="2:2">
       <c r="B80" t="s">
-        <v>139</v>
+        <v>144</v>
       </c>
     </row>
     <row r="81" spans="2:2">
       <c r="B81" t="s">
-        <v>140</v>
+        <v>145</v>
       </c>
     </row>
     <row r="82" spans="2:2">
       <c r="B82" t="s">
-        <v>141</v>
+        <v>146</v>
       </c>
     </row>
     <row r="83" spans="2:2">
       <c r="B83" t="s">
-        <v>142</v>
+        <v>147</v>
       </c>
     </row>
   </sheetData>
@@ -7044,8 +7153,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{93013FD4-B940-4A70-A7DA-BF82FD0F616E}">
   <dimension ref="A2:K81"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="L71" sqref="L71"/>
+    <sheetView tabSelected="1" topLeftCell="A44" workbookViewId="0">
+      <selection activeCell="B50" sqref="B50:B65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -7056,431 +7165,436 @@
   <sheetData>
     <row r="2" spans="2:2" ht="23.25">
       <c r="B2" s="47" t="s">
-        <v>143</v>
+        <v>148</v>
       </c>
     </row>
     <row r="4" spans="2:2">
       <c r="B4" t="s">
-        <v>144</v>
+        <v>149</v>
       </c>
     </row>
     <row r="5" spans="2:2">
       <c r="B5" t="s">
-        <v>145</v>
+        <v>150</v>
       </c>
     </row>
     <row r="7" spans="2:2" ht="18.75">
       <c r="B7" s="51" t="s">
-        <v>146</v>
+        <v>151</v>
       </c>
     </row>
     <row r="8" spans="2:2">
       <c r="B8" t="s">
-        <v>147</v>
+        <v>152</v>
       </c>
     </row>
     <row r="9" spans="2:2">
       <c r="B9" t="s">
-        <v>148</v>
+        <v>153</v>
       </c>
     </row>
     <row r="10" spans="2:2">
       <c r="B10" t="s">
-        <v>149</v>
+        <v>154</v>
       </c>
     </row>
     <row r="11" spans="2:2">
       <c r="B11" t="s">
-        <v>150</v>
+        <v>155</v>
       </c>
     </row>
     <row r="12" spans="2:2">
       <c r="B12" t="s">
-        <v>151</v>
+        <v>156</v>
       </c>
     </row>
     <row r="13" spans="2:2">
       <c r="B13" t="s">
-        <v>152</v>
+        <v>157</v>
       </c>
     </row>
     <row r="14" spans="2:2">
       <c r="B14" t="s">
-        <v>153</v>
+        <v>158</v>
       </c>
     </row>
     <row r="15" spans="2:2">
       <c r="B15" t="s">
-        <v>154</v>
+        <v>159</v>
       </c>
     </row>
     <row r="16" spans="2:2">
       <c r="B16" t="s">
-        <v>155</v>
+        <v>160</v>
       </c>
     </row>
     <row r="17" spans="1:11">
       <c r="B17" t="s">
-        <v>156</v>
+        <v>161</v>
       </c>
     </row>
     <row r="18" spans="1:11">
       <c r="B18" t="s">
-        <v>157</v>
+        <v>162</v>
       </c>
     </row>
     <row r="19" spans="1:11">
       <c r="B19" t="s">
-        <v>158</v>
+        <v>163</v>
       </c>
     </row>
     <row r="20" spans="1:11">
       <c r="B20" t="s">
-        <v>159</v>
+        <v>164</v>
       </c>
     </row>
     <row r="23" spans="1:11">
       <c r="A23" t="s">
-        <v>160</v>
+        <v>165</v>
       </c>
       <c r="B23" s="50" t="s">
-        <v>70</v>
+        <v>75</v>
       </c>
       <c r="C23" s="48"/>
-      <c r="D23" s="54" t="s">
-        <v>161</v>
-      </c>
-      <c r="E23" s="55"/>
-      <c r="F23" s="55"/>
-      <c r="G23" s="55"/>
-      <c r="H23" s="55"/>
-      <c r="I23" s="56"/>
+      <c r="D23" s="55" t="s">
+        <v>166</v>
+      </c>
+      <c r="E23" s="56"/>
+      <c r="F23" s="56"/>
+      <c r="G23" s="56"/>
+      <c r="H23" s="56"/>
+      <c r="I23" s="57"/>
       <c r="J23" s="48"/>
       <c r="K23" s="50" t="s">
-        <v>162</v>
+        <v>167</v>
       </c>
     </row>
     <row r="24" spans="1:11">
       <c r="B24" s="48"/>
       <c r="C24" s="48"/>
-      <c r="D24" s="57"/>
-      <c r="E24" s="58"/>
-      <c r="F24" s="58"/>
-      <c r="G24" s="58"/>
-      <c r="H24" s="58"/>
-      <c r="I24" s="59"/>
+      <c r="D24" s="58"/>
+      <c r="E24" s="59"/>
+      <c r="F24" s="59"/>
+      <c r="G24" s="59"/>
+      <c r="H24" s="59"/>
+      <c r="I24" s="60"/>
       <c r="J24" s="48"/>
       <c r="K24" s="48"/>
     </row>
     <row r="25" spans="1:11">
       <c r="B25" s="48"/>
       <c r="C25" s="48"/>
-      <c r="D25" s="57"/>
-      <c r="E25" s="58"/>
-      <c r="F25" s="58"/>
-      <c r="G25" s="58"/>
-      <c r="H25" s="58"/>
-      <c r="I25" s="59"/>
+      <c r="D25" s="58"/>
+      <c r="E25" s="59"/>
+      <c r="F25" s="59"/>
+      <c r="G25" s="59"/>
+      <c r="H25" s="59"/>
+      <c r="I25" s="60"/>
       <c r="J25" s="48"/>
       <c r="K25" s="48"/>
     </row>
     <row r="26" spans="1:11">
       <c r="B26" s="50" t="s">
-        <v>72</v>
+        <v>77</v>
       </c>
       <c r="C26" s="48"/>
-      <c r="D26" s="57"/>
-      <c r="E26" s="58"/>
-      <c r="F26" s="58"/>
-      <c r="G26" s="58"/>
-      <c r="H26" s="58"/>
-      <c r="I26" s="59"/>
+      <c r="D26" s="58"/>
+      <c r="E26" s="59"/>
+      <c r="F26" s="59"/>
+      <c r="G26" s="59"/>
+      <c r="H26" s="59"/>
+      <c r="I26" s="60"/>
       <c r="J26" s="48"/>
       <c r="K26" s="50" t="s">
-        <v>163</v>
+        <v>168</v>
       </c>
     </row>
     <row r="27" spans="1:11">
       <c r="B27" s="48"/>
       <c r="C27" s="48"/>
-      <c r="D27" s="57"/>
-      <c r="E27" s="58"/>
-      <c r="F27" s="58"/>
-      <c r="G27" s="58"/>
-      <c r="H27" s="58"/>
-      <c r="I27" s="59"/>
+      <c r="D27" s="58"/>
+      <c r="E27" s="59"/>
+      <c r="F27" s="59"/>
+      <c r="G27" s="59"/>
+      <c r="H27" s="59"/>
+      <c r="I27" s="60"/>
       <c r="J27" s="48"/>
       <c r="K27" s="48"/>
     </row>
     <row r="28" spans="1:11">
       <c r="B28" s="50" t="s">
-        <v>164</v>
+        <v>169</v>
       </c>
       <c r="C28" s="49"/>
-      <c r="D28" s="60"/>
-      <c r="E28" s="61"/>
-      <c r="F28" s="61"/>
-      <c r="G28" s="61"/>
-      <c r="H28" s="61"/>
-      <c r="I28" s="62"/>
+      <c r="D28" s="61"/>
+      <c r="E28" s="62"/>
+      <c r="F28" s="62"/>
+      <c r="G28" s="62"/>
+      <c r="H28" s="62"/>
+      <c r="I28" s="63"/>
       <c r="J28" s="49"/>
       <c r="K28" s="48"/>
     </row>
     <row r="29" spans="1:11">
       <c r="B29" s="48"/>
       <c r="C29" s="48"/>
-      <c r="D29" s="54" t="s">
-        <v>161</v>
-      </c>
-      <c r="E29" s="55"/>
-      <c r="F29" s="55"/>
-      <c r="G29" s="55"/>
-      <c r="H29" s="55"/>
-      <c r="I29" s="56"/>
+      <c r="D29" s="55" t="s">
+        <v>166</v>
+      </c>
+      <c r="E29" s="56"/>
+      <c r="F29" s="56"/>
+      <c r="G29" s="56"/>
+      <c r="H29" s="56"/>
+      <c r="I29" s="57"/>
       <c r="J29" s="48"/>
       <c r="K29" s="50" t="s">
-        <v>164</v>
+        <v>169</v>
       </c>
     </row>
     <row r="30" spans="1:11">
       <c r="B30" s="48"/>
       <c r="C30" s="48"/>
-      <c r="D30" s="57"/>
-      <c r="E30" s="58"/>
-      <c r="F30" s="58"/>
-      <c r="G30" s="58"/>
-      <c r="H30" s="58"/>
-      <c r="I30" s="59"/>
+      <c r="D30" s="58"/>
+      <c r="E30" s="59"/>
+      <c r="F30" s="59"/>
+      <c r="G30" s="59"/>
+      <c r="H30" s="59"/>
+      <c r="I30" s="60"/>
       <c r="J30" s="48"/>
       <c r="K30" s="48"/>
     </row>
     <row r="31" spans="1:11">
       <c r="B31" s="50" t="s">
-        <v>163</v>
+        <v>168</v>
       </c>
       <c r="C31" s="48"/>
-      <c r="D31" s="57"/>
-      <c r="E31" s="58"/>
-      <c r="F31" s="58"/>
-      <c r="G31" s="58"/>
-      <c r="H31" s="58"/>
-      <c r="I31" s="59"/>
+      <c r="D31" s="58"/>
+      <c r="E31" s="59"/>
+      <c r="F31" s="59"/>
+      <c r="G31" s="59"/>
+      <c r="H31" s="59"/>
+      <c r="I31" s="60"/>
       <c r="J31" s="48"/>
       <c r="K31" s="50" t="s">
-        <v>72</v>
+        <v>77</v>
       </c>
     </row>
     <row r="32" spans="1:11">
       <c r="B32" s="48"/>
       <c r="C32" s="48"/>
-      <c r="D32" s="57"/>
-      <c r="E32" s="58"/>
-      <c r="F32" s="58"/>
-      <c r="G32" s="58"/>
-      <c r="H32" s="58"/>
-      <c r="I32" s="59"/>
+      <c r="D32" s="58"/>
+      <c r="E32" s="59"/>
+      <c r="F32" s="59"/>
+      <c r="G32" s="59"/>
+      <c r="H32" s="59"/>
+      <c r="I32" s="60"/>
       <c r="J32" s="48"/>
       <c r="K32" s="48"/>
     </row>
     <row r="33" spans="1:11">
       <c r="B33" s="48"/>
       <c r="C33" s="48"/>
-      <c r="D33" s="57"/>
-      <c r="E33" s="58"/>
-      <c r="F33" s="58"/>
-      <c r="G33" s="58"/>
-      <c r="H33" s="58"/>
-      <c r="I33" s="59"/>
+      <c r="D33" s="58"/>
+      <c r="E33" s="59"/>
+      <c r="F33" s="59"/>
+      <c r="G33" s="59"/>
+      <c r="H33" s="59"/>
+      <c r="I33" s="60"/>
       <c r="J33" s="48"/>
       <c r="K33" s="48"/>
     </row>
     <row r="34" spans="1:11">
       <c r="A34" t="s">
-        <v>165</v>
+        <v>170</v>
       </c>
       <c r="B34" s="50" t="s">
-        <v>162</v>
+        <v>167</v>
       </c>
       <c r="C34" s="48"/>
-      <c r="D34" s="60"/>
-      <c r="E34" s="61"/>
-      <c r="F34" s="61"/>
-      <c r="G34" s="61"/>
-      <c r="H34" s="61"/>
-      <c r="I34" s="62"/>
+      <c r="D34" s="61"/>
+      <c r="E34" s="62"/>
+      <c r="F34" s="62"/>
+      <c r="G34" s="62"/>
+      <c r="H34" s="62"/>
+      <c r="I34" s="63"/>
       <c r="J34" s="48"/>
       <c r="K34" s="50" t="s">
-        <v>70</v>
+        <v>75</v>
       </c>
     </row>
     <row r="37" spans="1:11">
       <c r="B37" t="s">
-        <v>166</v>
+        <v>171</v>
       </c>
     </row>
     <row r="38" spans="1:11">
       <c r="B38" t="s">
-        <v>167</v>
+        <v>172</v>
       </c>
     </row>
     <row r="39" spans="1:11">
       <c r="B39" t="s">
-        <v>168</v>
+        <v>173</v>
       </c>
     </row>
     <row r="40" spans="1:11">
       <c r="B40" t="s">
-        <v>169</v>
+        <v>174</v>
       </c>
     </row>
     <row r="43" spans="1:11" ht="18.75">
       <c r="B43" s="51" t="s">
-        <v>170</v>
+        <v>175</v>
       </c>
     </row>
     <row r="44" spans="1:11">
       <c r="B44" t="s">
-        <v>171</v>
+        <v>176</v>
       </c>
     </row>
     <row r="46" spans="1:11">
       <c r="B46" s="3" t="s">
-        <v>93</v>
+        <v>177</v>
       </c>
     </row>
     <row r="47" spans="1:11">
       <c r="B47" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="49" spans="2:2">
-      <c r="B49" s="3" t="s">
-        <v>173</v>
+        <v>178</v>
+      </c>
+    </row>
+    <row r="48" spans="1:11">
+      <c r="B48" t="s">
+        <v>100</v>
       </c>
     </row>
     <row r="50" spans="2:2">
-      <c r="B50" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="52" spans="2:2">
-      <c r="B52" s="3" t="s">
-        <v>96</v>
+      <c r="B50" s="3" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="51" spans="2:2">
+      <c r="B51" t="s">
+        <v>180</v>
       </c>
     </row>
     <row r="53" spans="2:2">
-      <c r="B53" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="55" spans="2:2">
-      <c r="B55" s="3" t="s">
-        <v>99</v>
+      <c r="B53" s="3" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="54" spans="2:2">
+      <c r="B54" t="s">
+        <v>181</v>
       </c>
     </row>
     <row r="56" spans="2:2">
-      <c r="B56" t="s">
-        <v>176</v>
+      <c r="B56" s="3" t="s">
+        <v>104</v>
       </c>
     </row>
     <row r="57" spans="2:2">
       <c r="B57" t="s">
-        <v>177</v>
+        <v>182</v>
       </c>
     </row>
     <row r="58" spans="2:2">
       <c r="B58" t="s">
-        <v>178</v>
+        <v>183</v>
       </c>
     </row>
     <row r="59" spans="2:2">
       <c r="B59" t="s">
-        <v>179</v>
+        <v>184</v>
       </c>
     </row>
     <row r="60" spans="2:2">
       <c r="B60" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="62" spans="2:2">
-      <c r="B62" s="3" t="s">
-        <v>101</v>
+        <v>185</v>
+      </c>
+    </row>
+    <row r="61" spans="2:2">
+      <c r="B61" t="s">
+        <v>186</v>
       </c>
     </row>
     <row r="63" spans="2:2">
-      <c r="B63" t="s">
-        <v>181</v>
+      <c r="B63" s="3" t="s">
+        <v>106</v>
       </c>
     </row>
     <row r="64" spans="2:2">
       <c r="B64" t="s">
-        <v>182</v>
+        <v>187</v>
+      </c>
+    </row>
+    <row r="65" spans="2:2">
+      <c r="B65" t="s">
+        <v>188</v>
       </c>
     </row>
     <row r="67" spans="2:2">
       <c r="B67" s="3" t="s">
-        <v>103</v>
+        <v>108</v>
       </c>
     </row>
     <row r="68" spans="2:2">
       <c r="B68" t="s">
-        <v>183</v>
+        <v>189</v>
       </c>
     </row>
     <row r="70" spans="2:2">
       <c r="B70" s="3" t="s">
-        <v>184</v>
+        <v>190</v>
       </c>
     </row>
     <row r="71" spans="2:2">
       <c r="B71" t="s">
-        <v>185</v>
+        <v>191</v>
       </c>
     </row>
     <row r="72" spans="2:2">
       <c r="B72" t="s">
-        <v>186</v>
+        <v>192</v>
       </c>
     </row>
     <row r="73" spans="2:2">
       <c r="B73" t="s">
-        <v>187</v>
+        <v>193</v>
       </c>
     </row>
     <row r="74" spans="2:2">
       <c r="B74" t="s">
-        <v>139</v>
+        <v>144</v>
       </c>
     </row>
     <row r="75" spans="2:2">
       <c r="B75" t="s">
-        <v>188</v>
+        <v>194</v>
       </c>
     </row>
     <row r="77" spans="2:2">
       <c r="B77" s="3" t="s">
-        <v>105</v>
+        <v>110</v>
       </c>
     </row>
     <row r="78" spans="2:2">
       <c r="B78" t="s">
-        <v>189</v>
+        <v>195</v>
       </c>
     </row>
     <row r="79" spans="2:2">
       <c r="B79" s="52" t="s">
-        <v>190</v>
+        <v>196</v>
       </c>
     </row>
     <row r="80" spans="2:2">
       <c r="B80" t="s">
-        <v>191</v>
+        <v>197</v>
       </c>
     </row>
     <row r="81" spans="2:2">
       <c r="B81" t="s">
-        <v>192</v>
+        <v>198</v>
       </c>
     </row>
   </sheetData>
@@ -7504,52 +7618,52 @@
   <sheetData>
     <row r="2" spans="2:2">
       <c r="B2" t="s">
-        <v>193</v>
+        <v>199</v>
       </c>
     </row>
     <row r="3" spans="2:2">
       <c r="B3" t="s">
-        <v>194</v>
+        <v>200</v>
       </c>
     </row>
     <row r="4" spans="2:2">
       <c r="B4" t="s">
-        <v>195</v>
+        <v>201</v>
       </c>
     </row>
     <row r="5" spans="2:2">
       <c r="B5" t="s">
-        <v>196</v>
+        <v>202</v>
       </c>
     </row>
     <row r="6" spans="2:2">
       <c r="B6" t="s">
-        <v>197</v>
+        <v>203</v>
       </c>
     </row>
     <row r="7" spans="2:2">
       <c r="B7" t="s">
-        <v>198</v>
+        <v>204</v>
       </c>
     </row>
     <row r="8" spans="2:2">
       <c r="B8" t="s">
-        <v>199</v>
+        <v>205</v>
       </c>
     </row>
     <row r="9" spans="2:2">
       <c r="B9" t="s">
-        <v>200</v>
+        <v>206</v>
       </c>
     </row>
     <row r="10" spans="2:2">
       <c r="B10" t="s">
-        <v>201</v>
+        <v>207</v>
       </c>
     </row>
     <row r="11" spans="2:2">
       <c r="B11" t="s">
-        <v>202</v>
+        <v>208</v>
       </c>
     </row>
   </sheetData>
@@ -7561,8 +7675,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1CADF2F4-A124-44BC-8A72-4CE3F16F5D04}">
   <dimension ref="B2:D32"/>
   <sheetViews>
-    <sheetView topLeftCell="A23" workbookViewId="0">
-      <selection activeCell="D32" sqref="B29:D32"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -7574,267 +7688,267 @@
   <sheetData>
     <row r="2" spans="2:4">
       <c r="B2" s="32" t="s">
-        <v>203</v>
+        <v>209</v>
       </c>
       <c r="C2" s="32" t="s">
-        <v>204</v>
+        <v>210</v>
       </c>
       <c r="D2" s="32" t="s">
-        <v>205</v>
+        <v>211</v>
       </c>
     </row>
     <row r="3" spans="2:4" ht="106.5" customHeight="1">
-      <c r="B3" s="69" t="s">
-        <v>206</v>
-      </c>
-      <c r="C3" s="63" t="s">
-        <v>207</v>
+      <c r="B3" s="70" t="s">
+        <v>212</v>
+      </c>
+      <c r="C3" s="64" t="s">
+        <v>213</v>
       </c>
       <c r="D3" s="28" t="s">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="4" spans="2:4" ht="120">
-      <c r="B4" s="70"/>
-      <c r="C4" s="64"/>
+        <v>214</v>
+      </c>
+    </row>
+    <row r="4" spans="2:4" ht="106.5">
+      <c r="B4" s="71"/>
+      <c r="C4" s="65"/>
       <c r="D4" s="29" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="5" spans="2:4" ht="60">
-      <c r="B5" s="70"/>
-      <c r="C5" s="64"/>
+        <v>215</v>
+      </c>
+    </row>
+    <row r="5" spans="2:4" ht="60.75">
+      <c r="B5" s="71"/>
+      <c r="C5" s="65"/>
       <c r="D5" s="30" t="s">
-        <v>210</v>
+        <v>216</v>
       </c>
     </row>
     <row r="6" spans="2:4" ht="75">
-      <c r="B6" s="70"/>
-      <c r="C6" s="64"/>
+      <c r="B6" s="71"/>
+      <c r="C6" s="65"/>
       <c r="D6" s="30" t="s">
-        <v>211</v>
+        <v>217</v>
       </c>
     </row>
     <row r="7" spans="2:4" ht="90">
-      <c r="B7" s="69" t="s">
-        <v>212</v>
-      </c>
-      <c r="C7" s="63" t="s">
-        <v>213</v>
+      <c r="B7" s="70" t="s">
+        <v>218</v>
+      </c>
+      <c r="C7" s="64" t="s">
+        <v>219</v>
       </c>
       <c r="D7" s="28" t="s">
-        <v>214</v>
+        <v>220</v>
       </c>
     </row>
     <row r="8" spans="2:4" ht="90">
-      <c r="B8" s="70"/>
-      <c r="C8" s="64"/>
+      <c r="B8" s="71"/>
+      <c r="C8" s="65"/>
       <c r="D8" s="30" t="s">
-        <v>215</v>
+        <v>221</v>
       </c>
     </row>
     <row r="9" spans="2:4" ht="75">
-      <c r="B9" s="69" t="s">
-        <v>216</v>
-      </c>
-      <c r="C9" s="63" t="s">
-        <v>217</v>
+      <c r="B9" s="70" t="s">
+        <v>222</v>
+      </c>
+      <c r="C9" s="64" t="s">
+        <v>223</v>
       </c>
       <c r="D9" s="28" t="s">
-        <v>218</v>
+        <v>224</v>
       </c>
     </row>
     <row r="10" spans="2:4" ht="30">
-      <c r="B10" s="71"/>
-      <c r="C10" s="65"/>
+      <c r="B10" s="72"/>
+      <c r="C10" s="66"/>
       <c r="D10" s="31" t="s">
-        <v>219</v>
+        <v>225</v>
       </c>
     </row>
     <row r="11" spans="2:4" ht="76.5" customHeight="1">
-      <c r="B11" s="69" t="s">
-        <v>220</v>
-      </c>
-      <c r="C11" s="63" t="s">
-        <v>221</v>
+      <c r="B11" s="70" t="s">
+        <v>226</v>
+      </c>
+      <c r="C11" s="64" t="s">
+        <v>227</v>
       </c>
       <c r="D11" s="28" t="s">
-        <v>222</v>
+        <v>228</v>
       </c>
     </row>
     <row r="12" spans="2:4" ht="30.75">
-      <c r="B12" s="70"/>
-      <c r="C12" s="64"/>
+      <c r="B12" s="71"/>
+      <c r="C12" s="65"/>
       <c r="D12" s="31" t="s">
-        <v>223</v>
+        <v>229</v>
       </c>
     </row>
     <row r="13" spans="2:4" ht="45.75">
-      <c r="B13" s="69" t="s">
-        <v>224</v>
-      </c>
-      <c r="C13" s="63" t="s">
-        <v>225</v>
+      <c r="B13" s="70" t="s">
+        <v>230</v>
+      </c>
+      <c r="C13" s="64" t="s">
+        <v>231</v>
       </c>
       <c r="D13" s="28" t="s">
-        <v>226</v>
+        <v>232</v>
       </c>
     </row>
     <row r="14" spans="2:4" ht="30.75">
-      <c r="B14" s="70"/>
-      <c r="C14" s="64"/>
+      <c r="B14" s="71"/>
+      <c r="C14" s="65"/>
       <c r="D14" s="31" t="s">
-        <v>223</v>
+        <v>229</v>
       </c>
     </row>
     <row r="15" spans="2:4" ht="45.75">
-      <c r="B15" s="70"/>
-      <c r="C15" s="64"/>
+      <c r="B15" s="71"/>
+      <c r="C15" s="65"/>
       <c r="D15" s="30" t="s">
-        <v>227</v>
+        <v>233</v>
       </c>
     </row>
     <row r="16" spans="2:4" ht="60">
-      <c r="B16" s="70"/>
-      <c r="C16" s="64"/>
+      <c r="B16" s="71"/>
+      <c r="C16" s="65"/>
       <c r="D16" s="30" t="s">
-        <v>228</v>
+        <v>234</v>
       </c>
     </row>
     <row r="17" spans="2:4" ht="45">
-      <c r="B17" s="69" t="s">
+      <c r="B17" s="70" t="s">
+        <v>235</v>
+      </c>
+      <c r="C17" s="64" t="s">
+        <v>236</v>
+      </c>
+      <c r="D17" s="28" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="18" spans="2:4" ht="45">
+      <c r="B18" s="71"/>
+      <c r="C18" s="65"/>
+      <c r="D18" s="30" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="19" spans="2:4" ht="60.75" customHeight="1">
+      <c r="B19" s="70" t="s">
+        <v>239</v>
+      </c>
+      <c r="C19" s="64" t="s">
+        <v>240</v>
+      </c>
+      <c r="D19" s="28" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="20" spans="2:4" ht="30.75">
+      <c r="B20" s="71"/>
+      <c r="C20" s="65"/>
+      <c r="D20" s="31" t="s">
         <v>229</v>
       </c>
-      <c r="C17" s="63" t="s">
-        <v>230</v>
-      </c>
-      <c r="D17" s="28" t="s">
-        <v>231</v>
-      </c>
-    </row>
-    <row r="18" spans="2:4" ht="45">
-      <c r="B18" s="70"/>
-      <c r="C18" s="64"/>
-      <c r="D18" s="30" t="s">
-        <v>232</v>
-      </c>
-    </row>
-    <row r="19" spans="2:4" ht="60.75" customHeight="1">
-      <c r="B19" s="69" t="s">
-        <v>233</v>
-      </c>
-      <c r="C19" s="63" t="s">
-        <v>234</v>
-      </c>
-      <c r="D19" s="28" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="20" spans="2:4" ht="30.75">
-      <c r="B20" s="70"/>
-      <c r="C20" s="64"/>
-      <c r="D20" s="31" t="s">
-        <v>223</v>
-      </c>
     </row>
     <row r="21" spans="2:4" ht="45.75">
-      <c r="B21" s="69" t="s">
-        <v>236</v>
-      </c>
-      <c r="C21" s="63" t="s">
-        <v>237</v>
+      <c r="B21" s="70" t="s">
+        <v>242</v>
+      </c>
+      <c r="C21" s="64" t="s">
+        <v>243</v>
       </c>
       <c r="D21" s="28" t="s">
-        <v>238</v>
+        <v>244</v>
       </c>
     </row>
     <row r="22" spans="2:4" ht="30.75">
-      <c r="B22" s="70"/>
-      <c r="C22" s="64"/>
+      <c r="B22" s="71"/>
+      <c r="C22" s="65"/>
       <c r="D22" s="31" t="s">
-        <v>223</v>
+        <v>229</v>
       </c>
     </row>
     <row r="23" spans="2:4" ht="62.25" customHeight="1">
-      <c r="B23" s="69" t="s">
-        <v>239</v>
-      </c>
-      <c r="C23" s="63" t="s">
-        <v>240</v>
+      <c r="B23" s="70" t="s">
+        <v>245</v>
+      </c>
+      <c r="C23" s="64" t="s">
+        <v>246</v>
       </c>
       <c r="D23" s="28" t="s">
-        <v>241</v>
+        <v>247</v>
       </c>
     </row>
     <row r="24" spans="2:4" ht="62.25" customHeight="1">
-      <c r="B24" s="70"/>
-      <c r="C24" s="64"/>
+      <c r="B24" s="71"/>
+      <c r="C24" s="65"/>
       <c r="D24" s="30" t="s">
-        <v>242</v>
+        <v>248</v>
       </c>
     </row>
     <row r="25" spans="2:4" ht="30.75">
-      <c r="B25" s="71"/>
-      <c r="C25" s="65"/>
+      <c r="B25" s="72"/>
+      <c r="C25" s="66"/>
       <c r="D25" s="30" t="s">
-        <v>223</v>
+        <v>229</v>
       </c>
     </row>
     <row r="26" spans="2:4" ht="45.75">
-      <c r="B26" s="69" t="s">
-        <v>243</v>
-      </c>
-      <c r="C26" s="63" t="s">
-        <v>244</v>
+      <c r="B26" s="70" t="s">
+        <v>249</v>
+      </c>
+      <c r="C26" s="64" t="s">
+        <v>250</v>
       </c>
       <c r="D26" s="28" t="s">
-        <v>241</v>
+        <v>247</v>
       </c>
     </row>
     <row r="27" spans="2:4" ht="60.75">
-      <c r="B27" s="70"/>
-      <c r="C27" s="64"/>
+      <c r="B27" s="71"/>
+      <c r="C27" s="65"/>
       <c r="D27" s="30" t="s">
-        <v>242</v>
+        <v>248</v>
       </c>
     </row>
     <row r="28" spans="2:4" ht="30.75">
-      <c r="B28" s="70"/>
-      <c r="C28" s="64"/>
+      <c r="B28" s="71"/>
+      <c r="C28" s="65"/>
       <c r="D28" s="30" t="s">
-        <v>223</v>
+        <v>229</v>
       </c>
     </row>
     <row r="29" spans="2:4" ht="45.75">
-      <c r="B29" s="66" t="s">
-        <v>245</v>
-      </c>
-      <c r="C29" s="63" t="s">
-        <v>246</v>
+      <c r="B29" s="67" t="s">
+        <v>251</v>
+      </c>
+      <c r="C29" s="64" t="s">
+        <v>252</v>
       </c>
       <c r="D29" s="28" t="s">
-        <v>241</v>
+        <v>247</v>
       </c>
     </row>
     <row r="30" spans="2:4" ht="60.75">
-      <c r="B30" s="67"/>
-      <c r="C30" s="64"/>
+      <c r="B30" s="68"/>
+      <c r="C30" s="65"/>
       <c r="D30" s="30" t="s">
-        <v>242</v>
+        <v>248</v>
       </c>
     </row>
     <row r="31" spans="2:4" ht="30.75">
-      <c r="B31" s="67"/>
-      <c r="C31" s="64"/>
+      <c r="B31" s="68"/>
+      <c r="C31" s="65"/>
       <c r="D31" s="30" t="s">
-        <v>223</v>
+        <v>229</v>
       </c>
     </row>
     <row r="32" spans="2:4" ht="60.75">
-      <c r="B32" s="68"/>
-      <c r="C32" s="65"/>
+      <c r="B32" s="69"/>
+      <c r="C32" s="66"/>
       <c r="D32" s="31" t="s">
-        <v>247</v>
+        <v>253</v>
       </c>
     </row>
   </sheetData>
@@ -7868,10 +7982,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1914FF74-0E8B-4E92-8BDD-103E839E1854}">
-  <dimension ref="B3:C7"/>
+  <dimension ref="B3:D29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -7880,45 +7994,189 @@
     <col min="3" max="3" width="73.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:3" ht="23.25">
+    <row r="3" spans="2:4" ht="23.25">
       <c r="B3" s="47" t="s">
         <v>27</v>
       </c>
       <c r="C3" s="47" t="s">
-        <v>248</v>
-      </c>
-    </row>
-    <row r="4" spans="2:3">
+        <v>254</v>
+      </c>
+      <c r="D3" s="51" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="4" spans="2:4">
       <c r="B4" s="3" t="s">
-        <v>249</v>
+        <v>256</v>
       </c>
       <c r="C4" t="s">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="5" spans="2:3">
+        <v>257</v>
+      </c>
+      <c r="D4" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="5" spans="2:4">
       <c r="B5" s="3" t="s">
-        <v>251</v>
+        <v>259</v>
       </c>
       <c r="C5" t="s">
-        <v>252</v>
-      </c>
-    </row>
-    <row r="6" spans="2:3">
+        <v>260</v>
+      </c>
+      <c r="D5" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="6" spans="2:4">
       <c r="B6" s="3" t="s">
-        <v>253</v>
+        <v>261</v>
       </c>
       <c r="C6" t="s">
-        <v>254</v>
-      </c>
-    </row>
-    <row r="7" spans="2:3">
+        <v>262</v>
+      </c>
+      <c r="D6" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="7" spans="2:4">
       <c r="B7" s="3" t="s">
-        <v>255</v>
+        <v>263</v>
       </c>
       <c r="C7" t="s">
-        <v>256</v>
-      </c>
+        <v>264</v>
+      </c>
+      <c r="D7" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="8" spans="2:4" ht="45.75">
+      <c r="B8" s="3" t="s">
+        <v>266</v>
+      </c>
+      <c r="C8" s="53" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="9" spans="2:4">
+      <c r="B9" s="3" t="s">
+        <v>268</v>
+      </c>
+      <c r="C9" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="10" spans="2:4">
+      <c r="B10" s="3" t="s">
+        <v>270</v>
+      </c>
+      <c r="C10" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="11" spans="2:4">
+      <c r="B11" s="3" t="s">
+        <v>272</v>
+      </c>
+      <c r="C11" t="s">
+        <v>273</v>
+      </c>
+      <c r="D11" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="12" spans="2:4">
+      <c r="B12" s="3" t="s">
+        <v>274</v>
+      </c>
+      <c r="C12" t="s">
+        <v>275</v>
+      </c>
+      <c r="D12" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="13" spans="2:4">
+      <c r="B13" s="3" t="s">
+        <v>276</v>
+      </c>
+      <c r="C13" t="s">
+        <v>277</v>
+      </c>
+      <c r="D13" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="14" spans="2:4">
+      <c r="B14" s="3" t="s">
+        <v>278</v>
+      </c>
+      <c r="C14" t="s">
+        <v>279</v>
+      </c>
+      <c r="D14" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="15" spans="2:4">
+      <c r="B15" s="3" t="s">
+        <v>280</v>
+      </c>
+      <c r="C15" t="s">
+        <v>281</v>
+      </c>
+      <c r="D15" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="16" spans="2:4">
+      <c r="B16" s="3" t="s">
+        <v>282</v>
+      </c>
+      <c r="C16" t="s">
+        <v>283</v>
+      </c>
+      <c r="D16" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="17" spans="2:2">
+      <c r="B17" s="3"/>
+    </row>
+    <row r="18" spans="2:2">
+      <c r="B18" s="3"/>
+    </row>
+    <row r="19" spans="2:2">
+      <c r="B19" s="3"/>
+    </row>
+    <row r="20" spans="2:2">
+      <c r="B20" s="3"/>
+    </row>
+    <row r="21" spans="2:2">
+      <c r="B21" s="3"/>
+    </row>
+    <row r="22" spans="2:2">
+      <c r="B22" s="3"/>
+    </row>
+    <row r="23" spans="2:2">
+      <c r="B23" s="3"/>
+    </row>
+    <row r="24" spans="2:2">
+      <c r="B24" s="3"/>
+    </row>
+    <row r="25" spans="2:2">
+      <c r="B25" s="3"/>
+    </row>
+    <row r="26" spans="2:2">
+      <c r="B26" s="3"/>
+    </row>
+    <row r="27" spans="2:2">
+      <c r="B27" s="3"/>
+    </row>
+    <row r="28" spans="2:2">
+      <c r="B28" s="3"/>
+    </row>
+    <row r="29" spans="2:2">
+      <c r="B29" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -7944,26 +8202,26 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:19">
-      <c r="A2" s="53" t="s">
-        <v>160</v>
-      </c>
-      <c r="B2" s="53"/>
-      <c r="C2" s="53"/>
-      <c r="F2" s="53" t="s">
+      <c r="A2" s="54" t="s">
         <v>165</v>
       </c>
-      <c r="G2" s="53"/>
-      <c r="H2" s="53"/>
+      <c r="B2" s="54"/>
+      <c r="C2" s="54"/>
+      <c r="F2" s="54" t="s">
+        <v>170</v>
+      </c>
+      <c r="G2" s="54"/>
+      <c r="H2" s="54"/>
     </row>
     <row r="3" spans="1:19">
       <c r="A3" t="s">
-        <v>257</v>
+        <v>284</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>21</v>
       </c>
       <c r="F3" t="s">
-        <v>257</v>
+        <v>284</v>
       </c>
       <c r="G3" s="1" t="s">
         <v>26</v>
@@ -7987,14 +8245,14 @@
     </row>
     <row r="5" spans="1:19">
       <c r="A5" t="s">
-        <v>258</v>
+        <v>285</v>
       </c>
       <c r="B5">
         <f>SUM(C10:C14)</f>
         <v>5000</v>
       </c>
       <c r="F5" t="s">
-        <v>258</v>
+        <v>285</v>
       </c>
       <c r="G5">
         <f>SUM(H10:H14)</f>
@@ -8003,14 +8261,14 @@
     </row>
     <row r="6" spans="1:19">
       <c r="A6" t="s">
-        <v>259</v>
+        <v>286</v>
       </c>
       <c r="B6">
         <f>SUM(C17:C19)</f>
         <v>2000</v>
       </c>
       <c r="F6" t="s">
-        <v>259</v>
+        <v>286</v>
       </c>
       <c r="G6">
         <f>SUM(H17:H19)</f>
@@ -8032,7 +8290,7 @@
         <v>2</v>
       </c>
       <c r="B9" s="17" t="s">
-        <v>260</v>
+        <v>287</v>
       </c>
       <c r="C9" s="17" t="s">
         <v>3</v>
@@ -8041,7 +8299,7 @@
         <v>2</v>
       </c>
       <c r="G9" s="17" t="s">
-        <v>260</v>
+        <v>287</v>
       </c>
       <c r="H9" s="17" t="s">
         <v>3</v>
@@ -8228,19 +8486,19 @@
     </row>
     <row r="16" spans="1:19">
       <c r="A16" s="17" t="s">
-        <v>206</v>
+        <v>212</v>
       </c>
       <c r="B16" s="17" t="s">
-        <v>260</v>
+        <v>287</v>
       </c>
       <c r="C16" t="s">
         <v>3</v>
       </c>
       <c r="F16" s="17" t="s">
-        <v>206</v>
+        <v>212</v>
       </c>
       <c r="G16" s="17" t="s">
-        <v>260</v>
+        <v>287</v>
       </c>
       <c r="H16" t="s">
         <v>3</v>

</xml_diff>

<commit_message>
Updated card mechanics and added Krileon Species
Updated card mechanics and added Krileon Species
</commit_message>
<xml_diff>
--- a/ShipCardGameCalcs.xlsx
+++ b/ShipCardGameCalcs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MultiplayerGame\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{A4EFA6C7-89AA-4E42-B8B0-9C8437321480}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{7C10CB07-5693-44A5-B180-0F0EDA992F21}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="4" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="1" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Values" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,8 @@
     <sheet name="Ideas" sheetId="6" r:id="rId6"/>
     <sheet name="Card Details" sheetId="5" r:id="rId7"/>
     <sheet name="Card Mechanics" sheetId="9" r:id="rId8"/>
-    <sheet name="Comparison" sheetId="2" r:id="rId9"/>
+    <sheet name="Species" sheetId="10" r:id="rId9"/>
+    <sheet name="Comparison" sheetId="2" r:id="rId10"/>
   </sheets>
   <calcPr calcId="191028"/>
   <extLst>
@@ -44,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="534" uniqueCount="288">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="586" uniqueCount="325">
   <si>
     <t>Ship Parameters</t>
   </si>
@@ -648,7 +649,7 @@
     <t>You can only assign crew cards to a ship if there is a free crew slot available</t>
   </si>
   <si>
-    <t>If you have any tier 1,2 or 3 crew members Disengagedthey can be used to Engage and assigned to a gun slot and fire at an enemy ship.</t>
+    <t>If you have any tier 1,2 or 3 crew members Disengaged they can be used to Engage and assigned to a gun slot and fire at an enemy ship.</t>
   </si>
   <si>
     <t>If for example a ship has 3 gun slots, then only 3 crew cards can be assigned to a gun slot</t>
@@ -747,7 +748,7 @@
     <t xml:space="preserve">Captain and Leuitenant cards will have their own unique benefits and abilities to their assigned ship. </t>
   </si>
   <si>
-    <t>A Captain and Leuitenant card can only be played to fill a Captain or Leuitenant slot. Only one Captain or Leuitenant card can be played per turn.</t>
+    <t>A Captain and Leuitenant card can only be played to fill a Captain or Leuitenant slot. Only one Captain or Leuitenant card can be played per turn. You can't have duplicates in your deck.</t>
   </si>
   <si>
     <t>A captain and leuitenant triggered and payed abilities can only be used for their assigned ship or for ships that can't have a captain or leuitenant</t>
@@ -762,7 +763,7 @@
     <t>There can only be one admiral card in play at any one time on your side of the battlefield as long as you can pay their cost</t>
   </si>
   <si>
-    <t>Admiral cards can only be played on your turn</t>
+    <t>Admiral cards can only be played on your turn and you can't have duplicates in your deck</t>
   </si>
   <si>
     <t>Event</t>
@@ -849,12 +850,33 @@
     <t>If the missions runs out of turns the it will activate the consequence affect and then get sent to the scrapyard</t>
   </si>
   <si>
+    <t>Ship</t>
+  </si>
+  <si>
+    <t>Each player will have Ships at the start of the game on the space field. The objective of the game is to destroy the opponents ships before they destroy yours.</t>
+  </si>
+  <si>
+    <t>You can have any amount of ships as long as the total points worth is not greater than the agreed play points</t>
+  </si>
+  <si>
+    <t>You must have at least one ship that can hold a Captain</t>
+  </si>
+  <si>
+    <t>To destroy a ship you have to deplete their Hull to 0.</t>
+  </si>
+  <si>
+    <t>You can only hit a ships Hull if its Shield has been depleted to 0 first, unless stated otherwise</t>
+  </si>
+  <si>
     <t>Detail</t>
   </si>
   <si>
     <t>Department Specific</t>
   </si>
   <si>
+    <t>Department Type Overview</t>
+  </si>
+  <si>
     <t>Piercing Round</t>
   </si>
   <si>
@@ -864,39 +886,57 @@
     <t>Engineering</t>
   </si>
   <si>
+    <t>Department</t>
+  </si>
+  <si>
     <t>Corrosion</t>
   </si>
   <si>
     <t>Deals damage straight to hull at the start of target players turn</t>
   </si>
   <si>
+    <t>Like to have the most upgraded ships out there. Using ship upgrades and advance technology to bypass the enemy ships shields and keep their ship under repair. They aren't one for early game but late game they can be tough to overcome</t>
+  </si>
+  <si>
     <t>Swarm</t>
   </si>
   <si>
     <t>Create X pod ship/s with 100 hull and can tap to deal 100 damage to enemy ship</t>
   </si>
   <si>
+    <t>One to keep the enemy under pressure invading their ships during the early game. They will call for help from their swarm and become burtal in the early game, however during the late game they fall off.</t>
+  </si>
+  <si>
     <t>Infection</t>
   </si>
   <si>
-    <t>Enemy ship Sacrifice 1 crew</t>
+    <t>Target Enemy ship Sacrifice 1 crew at the start of their Disengage Phase</t>
   </si>
   <si>
     <t>Medic</t>
   </si>
   <si>
+    <t>Keeping the enemy crew down to a minimum and able to revive their own. They will use disease to their advantage against enemy ships and stasis. Known for having the most "unique" crew with all their upgrades they have a lot up their sleeves. They strive in the mid game</t>
+  </si>
+  <si>
     <t>Engage</t>
   </si>
   <si>
     <t>To Engage a card the player must turn the card 90 degrees. Once this is done the card can't engage again until they are turned back facing the correct way. This can happen during the Disengage phase</t>
   </si>
   <si>
+    <t>Being most knowledgable to get the cards they want when they need it using it to deal a lot of damage with cosmic cards. They are known for their mid/late game</t>
+  </si>
+  <si>
     <t>Disengage</t>
   </si>
   <si>
     <t>Turn card back to upright position</t>
   </si>
   <si>
+    <t>The tricksters of departments, maneuvering out the way of potential threat and normally played with a widespread of ships. Their formation and tactics are like no other when flying their ships on the space field. They strive in the early/mid game but fall off in the late game</t>
+  </si>
+  <si>
     <t>Sacrifice</t>
   </si>
   <si>
@@ -918,25 +958,98 @@
     <t>Repair</t>
   </si>
   <si>
-    <t>Repair ship by X amount</t>
+    <t>Repair ship/s by X amount</t>
   </si>
   <si>
     <t>Invade</t>
   </si>
   <si>
-    <t>Disable enemy crew</t>
-  </si>
-  <si>
-    <t>Science</t>
-  </si>
-  <si>
-    <t>Draw/scry from Strategy deck</t>
+    <t>Disable enemy crew card/s on target ship/s</t>
   </si>
   <si>
     <t>Revive</t>
   </si>
   <si>
-    <t>Return target crew from stasis</t>
+    <t>Return target crew card from stasis and assign to target ship</t>
+  </si>
+  <si>
+    <t>Study</t>
+  </si>
+  <si>
+    <t>View cards on top of your Strategy deck, pick X amount to place in your hand and put the rest in any order on top of your strategy deck</t>
+  </si>
+  <si>
+    <t>Disease spread</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Deal damage to enemy ship based off cards in their stasis. </t>
+  </si>
+  <si>
+    <t>Cosmic Knowledge</t>
+  </si>
+  <si>
+    <t>Deal damage to enemy ship based off Event and on Going Event cards played this turn</t>
+  </si>
+  <si>
+    <t>Counter Attack</t>
+  </si>
+  <si>
+    <t>For each attack evaded this turn deal X amount of damage to target ship</t>
+  </si>
+  <si>
+    <t>Mutiny</t>
+  </si>
+  <si>
+    <t>If you control all crew slots on enemy ship for X amount of turns then you take control of that ship.</t>
+  </si>
+  <si>
+    <t>Powering Up</t>
+  </si>
+  <si>
+    <t>Target ship gains X amount of shield at start of your Disengage Phase</t>
+  </si>
+  <si>
+    <t>Discard</t>
+  </si>
+  <si>
+    <t>Send card/s from your hand to the Junkyard/Stasis</t>
+  </si>
+  <si>
+    <t>Special features</t>
+  </si>
+  <si>
+    <t>Human</t>
+  </si>
+  <si>
+    <t>Humans have had their fair share off space wars against their own which has also meant for eventual peace across their systems. Since then most are very open to various species in their crew but some still hold strength and prefer to stick to their own.</t>
+  </si>
+  <si>
+    <t>Robot</t>
+  </si>
+  <si>
+    <t>A lot of robots respect and work for the species that created them and are one of the most advanced in thei ship understanding. But there are some who left and rebelled against their masters, looking to convert any none Robots species as their own</t>
+  </si>
+  <si>
+    <t>Engage: Repair ship by 100</t>
+  </si>
+  <si>
+    <t>Cyborg</t>
+  </si>
+  <si>
+    <t>Some species have needed to under go so much operation that they are more machine than what they once were. These have become known as cyborgs and are known for being very multitalented in departments.</t>
+  </si>
+  <si>
+    <t>Engage: Get +1 to one of two different departments. For example "Enters Engaged or attached ship takes 200 damage
+Engage: Medic or Handling + 1"</t>
+  </si>
+  <si>
+    <t>Krileon</t>
+  </si>
+  <si>
+    <t>These huge crab like species are known for their size and brute strength. Having huge claws they normally frighten most at first sight, however having as an ally can really change the tides of a battle.</t>
+  </si>
+  <si>
+    <t>Engage: Engage 1 enemy crew member until start of your next turn</t>
   </si>
   <si>
     <t>Fleet Option</t>
@@ -1085,7 +1198,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="25">
+  <borders count="27">
     <border>
       <left/>
       <right/>
@@ -1369,11 +1482,37 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color rgb="FF000000"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="medium">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="73">
+  <cellXfs count="82">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1481,6 +1620,9 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1516,8 +1658,17 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1528,20 +1679,58 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="140">
+  <dxfs count="144">
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <border>
+        <bottom style="medium">
+          <color rgb="FF000000"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <left style="medium">
+          <color rgb="FF000000"/>
+        </left>
+        <right style="medium">
+          <color rgb="FF000000"/>
+        </right>
+        <top style="medium">
+          <color rgb="FF000000"/>
+        </top>
+        <bottom style="medium">
+          <color rgb="FF000000"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+      </font>
+    </dxf>
     <dxf>
       <fill>
         <patternFill patternType="none">
@@ -3072,13 +3261,13 @@
   </dxfs>
   <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9">
     <tableStyle name="TableStyleMedium2 2" pivot="0" count="7" xr9:uid="{00000000-0011-0000-FFFF-FFFF00000000}">
-      <tableStyleElement type="wholeTable" dxfId="139"/>
-      <tableStyleElement type="headerRow" dxfId="138"/>
-      <tableStyleElement type="totalRow" dxfId="137"/>
-      <tableStyleElement type="firstColumn" dxfId="136"/>
-      <tableStyleElement type="lastColumn" dxfId="135"/>
-      <tableStyleElement type="firstColumnStripe" dxfId="134"/>
-      <tableStyleElement type="secondColumnStripe" dxfId="133"/>
+      <tableStyleElement type="wholeTable" dxfId="143"/>
+      <tableStyleElement type="headerRow" dxfId="142"/>
+      <tableStyleElement type="totalRow" dxfId="141"/>
+      <tableStyleElement type="firstColumn" dxfId="140"/>
+      <tableStyleElement type="lastColumn" dxfId="139"/>
+      <tableStyleElement type="firstColumnStripe" dxfId="138"/>
+      <tableStyleElement type="secondColumnStripe" dxfId="137"/>
     </tableStyle>
   </tableStyles>
   <extLst>
@@ -3093,204 +3282,215 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="TblBattlefieldFlt" displayName="TblBattlefieldFlt" ref="A9:G15" totalsRowCount="1" headerRowDxfId="132" dataDxfId="131" totalsRowDxfId="130">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="TblBattlefieldFlt" displayName="TblBattlefieldFlt" ref="A9:G15" totalsRowCount="1" headerRowDxfId="136" dataDxfId="135" totalsRowDxfId="134">
   <autoFilter ref="A9:G14" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Option" totalsRowLabel="Total" dataDxfId="129"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="A" totalsRowFunction="sum" dataDxfId="127" totalsRowDxfId="128"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="B" totalsRowFunction="sum" dataDxfId="125" totalsRowDxfId="126"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="C" totalsRowFunction="sum" dataDxfId="123" totalsRowDxfId="124"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="D" totalsRowFunction="sum" dataDxfId="121" totalsRowDxfId="122"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="E" totalsRowFunction="sum" dataDxfId="119" totalsRowDxfId="120"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="F" totalsRowFunction="sum" dataDxfId="117" totalsRowDxfId="118"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Option" totalsRowLabel="Total" dataDxfId="133"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="A" totalsRowFunction="sum" dataDxfId="131" totalsRowDxfId="132"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="B" totalsRowFunction="sum" dataDxfId="129" totalsRowDxfId="130"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="C" totalsRowFunction="sum" dataDxfId="127" totalsRowDxfId="128"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="D" totalsRowFunction="sum" dataDxfId="125" totalsRowDxfId="126"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="E" totalsRowFunction="sum" dataDxfId="123" totalsRowDxfId="124"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="F" totalsRowFunction="sum" dataDxfId="121" totalsRowDxfId="122"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium15" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table10.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="14" xr:uid="{00000000-000C-0000-FFFF-FFFF09000000}" name="TblFltCrewSizes" displayName="TblFltCrewSizes" ref="A17:G21" totalsRowCount="1" headerRowDxfId="15" dataDxfId="14">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="14" xr:uid="{00000000-000C-0000-FFFF-FFFF09000000}" name="TblFltCrewSizes" displayName="TblFltCrewSizes" ref="A17:G21" totalsRowCount="1" headerRowDxfId="19" dataDxfId="18">
   <autoFilter ref="A17:G20" xr:uid="{00000000-0009-0000-0100-00000E000000}"/>
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0900-000001000000}" name="Option" totalsRowLabel="Total" dataDxfId="12" totalsRowDxfId="13"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0900-000002000000}" name="A" totalsRowFunction="custom" dataDxfId="10" totalsRowDxfId="11">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0900-000001000000}" name="Option" totalsRowLabel="Total" dataDxfId="16" totalsRowDxfId="17"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0900-000002000000}" name="A" totalsRowFunction="custom" dataDxfId="14" totalsRowDxfId="15">
       <totalsRowFormula>SUBTOTAL(109,TblFltCrewSizes[A])</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0900-000003000000}" name="B" totalsRowFunction="custom" dataDxfId="8" totalsRowDxfId="9">
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0900-000003000000}" name="B" totalsRowFunction="custom" dataDxfId="12" totalsRowDxfId="13">
       <totalsRowFormula>SUBTOTAL(109,TblFltCrewSizes[B])</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0900-000004000000}" name="C" totalsRowFunction="custom" dataDxfId="6" totalsRowDxfId="7">
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0900-000004000000}" name="C" totalsRowFunction="custom" dataDxfId="10" totalsRowDxfId="11">
       <totalsRowFormula>SUBTOTAL(109,TblFltCrewSizes[C])</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0900-000005000000}" name="D" totalsRowFunction="custom" dataDxfId="4" totalsRowDxfId="5">
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0900-000005000000}" name="D" totalsRowFunction="custom" dataDxfId="8" totalsRowDxfId="9">
       <totalsRowFormula>SUBTOTAL(109,TblFltCrewSizes[D])</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0900-000006000000}" name="E" totalsRowFunction="custom" dataDxfId="2" totalsRowDxfId="3">
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0900-000006000000}" name="E" totalsRowFunction="custom" dataDxfId="6" totalsRowDxfId="7">
       <totalsRowFormula>SUBTOTAL(109,TblFltCrewSizes[E])</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0900-000007000000}" name="F" totalsRowFunction="sum" dataDxfId="0" totalsRowDxfId="1"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0900-000007000000}" name="F" totalsRowFunction="sum" dataDxfId="4" totalsRowDxfId="5"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium13" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
+<file path=xl/tables/table11.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{186E891F-CC1D-4ED6-98A6-972A212A6308}" name="Table3" displayName="Table3" ref="I4:J9" totalsRowShown="0" headerRowDxfId="3" headerRowBorderDxfId="1" tableBorderDxfId="2">
+  <autoFilter ref="I4:J9" xr:uid="{186E891F-CC1D-4ED6-98A6-972A212A6308}"/>
+  <tableColumns count="2">
+    <tableColumn id="1" xr3:uid="{C81D7C06-9F89-4717-99F4-FA4E60C3BBF7}" name="Department"/>
+    <tableColumn id="2" xr3:uid="{EE9AB412-432D-45A0-92A5-DA3A84572278}" name="Description" dataDxfId="0"/>
+  </tableColumns>
+  <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="TblFleetShipValues" displayName="TblFleetShipValues" ref="J9:Q15" totalsRowCount="1" headerRowDxfId="116" dataDxfId="115" totalsRowDxfId="114">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="TblFleetShipValues" displayName="TblFleetShipValues" ref="J9:Q15" totalsRowCount="1" headerRowDxfId="120" dataDxfId="119" totalsRowDxfId="118">
   <autoFilter ref="J9:Q14" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
   <tableColumns count="8">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="Option" totalsRowLabel="Total " dataDxfId="112" totalsRowDxfId="113"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="A" totalsRowFunction="sum" dataDxfId="110" totalsRowDxfId="111">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="Option" totalsRowLabel="Total " dataDxfId="116" totalsRowDxfId="117"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="A" totalsRowFunction="sum" dataDxfId="114" totalsRowDxfId="115">
       <calculatedColumnFormula>(INDEX(TblBattlefieldFlt[[A]:[F]],MATCH(TblFleetShipValues[[#This Row],[Option]],TblBattlefieldFlt[Option],0),MATCH(TblFleetShipValues[[#Headers],[A]],TblBattlefieldFlt[[#Headers],[A]:[F]],0)))*(INDEX(TblShipPoints[Points],MATCH(TblFleetShipValues[[#This Row],[Option]],TblShipPoints[Ships],0)))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0100-000003000000}" name="B" totalsRowFunction="sum" dataDxfId="108" totalsRowDxfId="109">
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0100-000003000000}" name="B" totalsRowFunction="sum" dataDxfId="112" totalsRowDxfId="113">
       <calculatedColumnFormula>C10*#REF!</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0100-000004000000}" name="C" totalsRowFunction="sum" dataDxfId="106" totalsRowDxfId="107">
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0100-000004000000}" name="C" totalsRowFunction="sum" dataDxfId="110" totalsRowDxfId="111">
       <calculatedColumnFormula>D10*#REF!</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0100-000005000000}" name="D" totalsRowFunction="sum" dataDxfId="104" totalsRowDxfId="105">
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0100-000005000000}" name="D" totalsRowFunction="sum" dataDxfId="108" totalsRowDxfId="109">
       <calculatedColumnFormula>E10*#REF!</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0100-000006000000}" name="E" totalsRowFunction="sum" dataDxfId="102" totalsRowDxfId="103">
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0100-000006000000}" name="E" totalsRowFunction="sum" dataDxfId="106" totalsRowDxfId="107">
       <calculatedColumnFormula>F10*#REF!</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0100-000007000000}" name="F" totalsRowFunction="sum" dataDxfId="100" totalsRowDxfId="101">
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0100-000007000000}" name="F" totalsRowFunction="sum" dataDxfId="104" totalsRowDxfId="105">
       <calculatedColumnFormula>G10*#REF!</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0100-000008000000}" name="Name" dataDxfId="98" totalsRowDxfId="99"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0100-000008000000}" name="Name" dataDxfId="102" totalsRowDxfId="103"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium13" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{00000000-000C-0000-FFFF-FFFF02000000}" name="TblRoleControlValues" displayName="TblRoleControlValues" ref="N2:Q3" totalsRowShown="0" headerRowDxfId="97" dataDxfId="96">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{00000000-000C-0000-FFFF-FFFF02000000}" name="TblRoleControlValues" displayName="TblRoleControlValues" ref="N2:Q3" totalsRowShown="0" headerRowDxfId="101" dataDxfId="100">
   <autoFilter ref="N2:Q3" xr:uid="{00000000-0009-0000-0100-000005000000}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0200-000001000000}" name="Generic" dataDxfId="95"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0200-000002000000}" name="Service" dataDxfId="94"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0200-000003000000}" name="Lieutenant" dataDxfId="93"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0200-000004000000}" name="Captain" dataDxfId="92"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0200-000001000000}" name="Generic" dataDxfId="99"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0200-000002000000}" name="Service" dataDxfId="98"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0200-000003000000}" name="Lieutenant" dataDxfId="97"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0200-000004000000}" name="Captain" dataDxfId="96"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{00000000-000C-0000-FFFF-FFFF03000000}" name="TblAdjFleetRolesValues" displayName="TblAdjFleetRolesValues" ref="A24:H30" totalsRowCount="1" headerRowDxfId="91" dataDxfId="90" totalsRowDxfId="89">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{00000000-000C-0000-FFFF-FFFF03000000}" name="TblAdjFleetRolesValues" displayName="TblAdjFleetRolesValues" ref="A24:H30" totalsRowCount="1" headerRowDxfId="95" dataDxfId="94" totalsRowDxfId="93">
   <autoFilter ref="A24:H29" xr:uid="{00000000-0009-0000-0100-000006000000}"/>
   <tableColumns count="8">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0300-000001000000}" name="Option" totalsRowLabel="Total" dataDxfId="87" totalsRowDxfId="88"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0300-000002000000}" name="A" totalsRowFunction="sum" dataDxfId="85" totalsRowDxfId="86">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0300-000001000000}" name="Option" totalsRowLabel="Total" dataDxfId="91" totalsRowDxfId="92"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0300-000002000000}" name="A" totalsRowFunction="sum" dataDxfId="89" totalsRowDxfId="90">
       <calculatedColumnFormula>(INDEX(TblBattlefieldFlt[[A]:[F]],MATCH($A25,TblBattlefieldFlt[Option],0),MATCH(B$24,TblBattlefieldFlt[[#Headers],[A]:[F]],0)))*(INDEX(TblShipCrew[Adjusted],MATCH($A25,TblShipCrew[Ships],0)))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0300-000003000000}" name="B" totalsRowFunction="sum" dataDxfId="83" totalsRowDxfId="84">
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0300-000003000000}" name="B" totalsRowFunction="sum" dataDxfId="87" totalsRowDxfId="88">
       <calculatedColumnFormula>(INDEX(TblBattlefieldFlt[[A]:[F]],MATCH($A25,TblBattlefieldFlt[Option],0),MATCH(C$24,TblBattlefieldFlt[[#Headers],[A]:[F]],0)))*(INDEX(TblShipCrew[Adjusted],MATCH($A25,TblShipCrew[Ships],0)))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0300-000004000000}" name="C" totalsRowFunction="sum" dataDxfId="81" totalsRowDxfId="82">
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0300-000004000000}" name="C" totalsRowFunction="sum" dataDxfId="85" totalsRowDxfId="86">
       <calculatedColumnFormula>(INDEX(TblBattlefieldFlt[[A]:[F]],MATCH($A25,TblBattlefieldFlt[Option],0),MATCH(D$24,TblBattlefieldFlt[[#Headers],[A]:[F]],0)))*(INDEX(TblShipCrew[Adjusted],MATCH($A25,TblShipCrew[Ships],0)))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0300-000005000000}" name="D" totalsRowFunction="sum" dataDxfId="79" totalsRowDxfId="80">
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0300-000005000000}" name="D" totalsRowFunction="sum" dataDxfId="83" totalsRowDxfId="84">
       <calculatedColumnFormula>(INDEX(TblBattlefieldFlt[[A]:[F]],MATCH($A25,TblBattlefieldFlt[Option],0),MATCH(E$24,TblBattlefieldFlt[[#Headers],[A]:[F]],0)))*(INDEX(TblShipCrew[Adjusted],MATCH($A25,TblShipCrew[Ships],0)))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0300-000006000000}" name="E" totalsRowFunction="sum" dataDxfId="77" totalsRowDxfId="78">
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0300-000006000000}" name="E" totalsRowFunction="sum" dataDxfId="81" totalsRowDxfId="82">
       <calculatedColumnFormula>(INDEX(TblBattlefieldFlt[[A]:[F]],MATCH($A25,TblBattlefieldFlt[Option],0),MATCH(F$24,TblBattlefieldFlt[[#Headers],[A]:[F]],0)))*(INDEX(TblShipCrew[Adjusted],MATCH($A25,TblShipCrew[Ships],0)))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0300-000007000000}" name="F" totalsRowFunction="sum" dataDxfId="75" totalsRowDxfId="76">
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0300-000007000000}" name="F" totalsRowFunction="sum" dataDxfId="79" totalsRowDxfId="80">
       <calculatedColumnFormula>(INDEX(TblBattlefieldFlt[[A]:[F]],MATCH($A25,TblBattlefieldFlt[Option],0),MATCH(G$24,TblBattlefieldFlt[[#Headers],[A]:[F]],0)))*(INDEX(TblShipCrew[Adjusted],MATCH($A25,TblShipCrew[Ships],0)))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0300-000008000000}" name="Name" dataDxfId="73" totalsRowDxfId="74"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0300-000008000000}" name="Name" dataDxfId="77" totalsRowDxfId="78"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium13" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{00000000-000C-0000-FFFF-FFFF04000000}" name="TblCombinedAdjFltValues" displayName="TblCombinedAdjFltValues" ref="A32:G43" totalsRowCount="1" headerRowDxfId="72">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{00000000-000C-0000-FFFF-FFFF04000000}" name="TblCombinedAdjFltValues" displayName="TblCombinedAdjFltValues" ref="A32:G43" totalsRowCount="1" headerRowDxfId="76">
   <autoFilter ref="A32:G42" xr:uid="{00000000-0009-0000-0100-000008000000}"/>
   <tableColumns count="7">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0400-000001000000}" name="Option" totalsRowLabel="Total"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0400-000002000000}" name="A" totalsRowFunction="sum" dataDxfId="70" totalsRowDxfId="71">
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0400-000002000000}" name="A" totalsRowFunction="sum" dataDxfId="74" totalsRowDxfId="75">
       <calculatedColumnFormula>K10</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0400-000003000000}" name="B" totalsRowFunction="sum" dataDxfId="68" totalsRowDxfId="69"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0400-000004000000}" name="C" totalsRowFunction="sum" dataDxfId="66" totalsRowDxfId="67"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0400-000005000000}" name="D" totalsRowFunction="sum" totalsRowDxfId="65"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0400-000006000000}" name="E" totalsRowFunction="sum" totalsRowDxfId="64"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0400-000007000000}" name="F" totalsRowFunction="sum" totalsRowDxfId="63"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0400-000003000000}" name="B" totalsRowFunction="sum" dataDxfId="72" totalsRowDxfId="73"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0400-000004000000}" name="C" totalsRowFunction="sum" dataDxfId="70" totalsRowDxfId="71"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0400-000005000000}" name="D" totalsRowFunction="sum" totalsRowDxfId="69"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0400-000006000000}" name="E" totalsRowFunction="sum" totalsRowDxfId="68"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0400-000007000000}" name="F" totalsRowFunction="sum" totalsRowDxfId="67"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium13" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{00000000-000C-0000-FFFF-FFFF05000000}" name="TblGenFleetRolesValues" displayName="TblGenFleetRolesValues" ref="J24:Q30" totalsRowCount="1" headerRowDxfId="62" dataDxfId="61">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{00000000-000C-0000-FFFF-FFFF05000000}" name="TblGenFleetRolesValues" displayName="TblGenFleetRolesValues" ref="J24:Q30" totalsRowCount="1" headerRowDxfId="66" dataDxfId="65">
   <autoFilter ref="J24:Q29" xr:uid="{00000000-0009-0000-0100-000009000000}"/>
   <tableColumns count="8">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0500-000001000000}" name="Option" totalsRowLabel="Total" dataDxfId="60"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0500-000002000000}" name="A" totalsRowFunction="sum" dataDxfId="58" totalsRowDxfId="59">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0500-000001000000}" name="Option" totalsRowLabel="Total" dataDxfId="64"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0500-000002000000}" name="A" totalsRowFunction="sum" dataDxfId="62" totalsRowDxfId="63">
       <calculatedColumnFormula>(INDEX(TblBattlefieldFlt[[A]:[F]],MATCH($J25,TblBattlefieldFlt[Option],0),MATCH(K$24,TblBattlefieldFlt[[#Headers],[A]:[F]],0)))*(INDEX(TblShipCrew[Generic (500)],MATCH($J25,TblShipCrew[Ships],0)))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0500-000003000000}" name="B" totalsRowFunction="sum" dataDxfId="56" totalsRowDxfId="57">
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0500-000003000000}" name="B" totalsRowFunction="sum" dataDxfId="60" totalsRowDxfId="61">
       <calculatedColumnFormula>(INDEX(TblBattlefieldFlt[[A]:[F]],MATCH($J25,TblBattlefieldFlt[Option],0),MATCH(L$24,TblBattlefieldFlt[[#Headers],[A]:[F]],0)))*(INDEX(TblShipCrew[Generic (500)],MATCH($J25,TblShipCrew[Ships],0)))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0500-000004000000}" name="C" totalsRowFunction="sum" dataDxfId="54" totalsRowDxfId="55">
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0500-000004000000}" name="C" totalsRowFunction="sum" dataDxfId="58" totalsRowDxfId="59">
       <calculatedColumnFormula>(INDEX(TblBattlefieldFlt[[A]:[F]],MATCH($J25,TblBattlefieldFlt[Option],0),MATCH(M$24,TblBattlefieldFlt[[#Headers],[A]:[F]],0)))*(INDEX(TblShipCrew[Generic (500)],MATCH($J25,TblShipCrew[Ships],0)))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0500-000005000000}" name="D" totalsRowFunction="sum" dataDxfId="52" totalsRowDxfId="53">
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0500-000005000000}" name="D" totalsRowFunction="sum" dataDxfId="56" totalsRowDxfId="57">
       <calculatedColumnFormula>(INDEX(TblBattlefieldFlt[[A]:[F]],MATCH($J25,TblBattlefieldFlt[Option],0),MATCH(N$24,TblBattlefieldFlt[[#Headers],[A]:[F]],0)))*(INDEX(TblShipCrew[Generic (500)],MATCH($J25,TblShipCrew[Ships],0)))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0500-000006000000}" name="E" totalsRowFunction="sum" dataDxfId="50" totalsRowDxfId="51">
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0500-000006000000}" name="E" totalsRowFunction="sum" dataDxfId="54" totalsRowDxfId="55">
       <calculatedColumnFormula>(INDEX(TblBattlefieldFlt[[A]:[F]],MATCH($J25,TblBattlefieldFlt[Option],0),MATCH(O$24,TblBattlefieldFlt[[#Headers],[A]:[F]],0)))*(INDEX(TblShipCrew[Generic (500)],MATCH($J25,TblShipCrew[Ships],0)))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0500-000007000000}" name="F" totalsRowFunction="sum" dataDxfId="48" totalsRowDxfId="49">
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0500-000007000000}" name="F" totalsRowFunction="sum" dataDxfId="52" totalsRowDxfId="53">
       <calculatedColumnFormula>(INDEX(TblBattlefieldFlt[[A]:[F]],MATCH($J25,TblBattlefieldFlt[Option],0),MATCH(P$24,TblBattlefieldFlt[[#Headers],[A]:[F]],0)))*(INDEX(TblShipCrew[Generic (500)],MATCH($J25,TblShipCrew[Ships],0)))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0500-000008000000}" name="Name" dataDxfId="46" totalsRowDxfId="47"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0500-000008000000}" name="Name" dataDxfId="50" totalsRowDxfId="51"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium10" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{00000000-000C-0000-FFFF-FFFF06000000}" name="TblCombinedGenFltValues" displayName="TblCombinedGenFltValues" ref="J32:P43" totalsRowCount="1" headerRowDxfId="45">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{00000000-000C-0000-FFFF-FFFF06000000}" name="TblCombinedGenFltValues" displayName="TblCombinedGenFltValues" ref="J32:P43" totalsRowCount="1" headerRowDxfId="49">
   <autoFilter ref="J32:P42" xr:uid="{00000000-0009-0000-0100-00000A000000}"/>
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0600-000001000000}" name="Option" totalsRowLabel="Total" totalsRowDxfId="44"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0600-000002000000}" name="A" totalsRowFunction="sum" dataDxfId="42" totalsRowDxfId="43">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0600-000001000000}" name="Option" totalsRowLabel="Total" totalsRowDxfId="48"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0600-000002000000}" name="A" totalsRowFunction="sum" dataDxfId="46" totalsRowDxfId="47">
       <calculatedColumnFormula>T10</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0600-000003000000}" name="B" totalsRowFunction="sum" dataDxfId="40" totalsRowDxfId="41"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0600-000004000000}" name="C" totalsRowFunction="sum" dataDxfId="38" totalsRowDxfId="39"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0600-000005000000}" name="D" totalsRowFunction="sum" totalsRowDxfId="37"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0600-000006000000}" name="E" totalsRowFunction="sum" totalsRowDxfId="36"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0600-000007000000}" name="F" totalsRowFunction="sum" totalsRowDxfId="35"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0600-000003000000}" name="B" totalsRowFunction="sum" dataDxfId="44" totalsRowDxfId="45"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0600-000004000000}" name="C" totalsRowFunction="sum" dataDxfId="42" totalsRowDxfId="43"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0600-000005000000}" name="D" totalsRowFunction="sum" totalsRowDxfId="41"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0600-000006000000}" name="E" totalsRowFunction="sum" totalsRowDxfId="40"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0600-000007000000}" name="F" totalsRowFunction="sum" totalsRowDxfId="39"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium10" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="13" xr:uid="{00000000-000C-0000-FFFF-FFFF07000000}" name="TblShipCrew" displayName="TblShipCrew" ref="D2:L7" totalsRowShown="0" headerRowDxfId="34" dataDxfId="33" headerRowBorderDxfId="31" tableBorderDxfId="32">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="13" xr:uid="{00000000-000C-0000-FFFF-FFFF07000000}" name="TblShipCrew" displayName="TblShipCrew" ref="D2:L7" totalsRowShown="0" headerRowDxfId="38" dataDxfId="37" headerRowBorderDxfId="35" tableBorderDxfId="36">
   <autoFilter ref="D2:L7" xr:uid="{00000000-0009-0000-0100-00000D000000}"/>
   <tableColumns count="9">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0700-000001000000}" name="Ships" dataDxfId="30"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0700-000002000000}" name="Service" dataDxfId="29"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0700-000003000000}" name="Lieutenant" dataDxfId="28"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0700-000004000000}" name="Captain" dataDxfId="27"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0700-000005000000}" name="Service Value" dataDxfId="26">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0700-000001000000}" name="Ships" dataDxfId="34"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0700-000002000000}" name="Service" dataDxfId="33"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0700-000003000000}" name="Lieutenant" dataDxfId="32"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0700-000004000000}" name="Captain" dataDxfId="31"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0700-000005000000}" name="Service Value" dataDxfId="30">
       <calculatedColumnFormula>TblShipCrew[[#This Row],[Service]]*TblRoleControlValues[Service]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0700-000006000000}" name="Lt Value" dataDxfId="25">
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0700-000006000000}" name="Lt Value" dataDxfId="29">
       <calculatedColumnFormula>TblShipCrew[[#This Row],[Lieutenant]]*TblRoleControlValues[Lieutenant]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0700-000007000000}" name="Cpt Value" dataDxfId="24">
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0700-000007000000}" name="Cpt Value" dataDxfId="28">
       <calculatedColumnFormula>TblShipCrew[[#This Row],[Captain]]*TblRoleControlValues[Captain]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0700-000008000000}" name="Adjusted" dataDxfId="23">
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0700-000008000000}" name="Adjusted" dataDxfId="27">
       <calculatedColumnFormula>SUM(TblShipCrew[[#This Row],[Service Value]:[Cpt Value]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0700-000009000000}" name="Generic (500)" dataDxfId="22">
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0700-000009000000}" name="Generic (500)" dataDxfId="26">
       <calculatedColumnFormula>SUM(TblShipCrew[[#This Row],[Service]:[Captain]])*TblRoleControlValues[Generic]</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -3299,11 +3499,11 @@
 </file>
 
 <file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="12" xr:uid="{00000000-000C-0000-FFFF-FFFF08000000}" name="TblShipPoints" displayName="TblShipPoints" ref="A2:B7" totalsRowShown="0" headerRowDxfId="21" dataDxfId="20" headerRowBorderDxfId="18" tableBorderDxfId="19">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="12" xr:uid="{00000000-000C-0000-FFFF-FFFF08000000}" name="TblShipPoints" displayName="TblShipPoints" ref="A2:B7" totalsRowShown="0" headerRowDxfId="25" dataDxfId="24" headerRowBorderDxfId="22" tableBorderDxfId="23">
   <autoFilter ref="A2:B7" xr:uid="{00000000-0009-0000-0100-00000C000000}"/>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0800-000001000000}" name="Ships" dataDxfId="17"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0800-000002000000}" name="Points" dataDxfId="16"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0800-000001000000}" name="Ships" dataDxfId="21"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0800-000002000000}" name="Points" dataDxfId="20"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -3631,21 +3831,21 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17">
-      <c r="A1" s="54" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="54"/>
-      <c r="C1" s="54"/>
-      <c r="D1" s="54"/>
-      <c r="E1" s="54"/>
-      <c r="F1" s="54"/>
-      <c r="G1" s="54"/>
-      <c r="H1" s="54"/>
-      <c r="N1" s="54" t="s">
+      <c r="A1" s="55" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="55"/>
+      <c r="C1" s="55"/>
+      <c r="D1" s="55"/>
+      <c r="E1" s="55"/>
+      <c r="F1" s="55"/>
+      <c r="G1" s="55"/>
+      <c r="H1" s="55"/>
+      <c r="N1" s="55" t="s">
         <v>1</v>
       </c>
-      <c r="O1" s="54"/>
-      <c r="P1" s="54"/>
+      <c r="O1" s="55"/>
+      <c r="P1" s="55"/>
     </row>
     <row r="2" spans="1:17">
       <c r="A2" s="9" t="s">
@@ -3912,25 +4112,25 @@
       </c>
     </row>
     <row r="8" spans="1:17">
-      <c r="A8" s="54" t="s">
+      <c r="A8" s="55" t="s">
         <v>18</v>
       </c>
-      <c r="B8" s="54"/>
-      <c r="C8" s="54"/>
-      <c r="D8" s="54"/>
-      <c r="E8" s="54"/>
-      <c r="F8" s="54"/>
-      <c r="G8" s="54"/>
-      <c r="J8" s="54" t="s">
+      <c r="B8" s="55"/>
+      <c r="C8" s="55"/>
+      <c r="D8" s="55"/>
+      <c r="E8" s="55"/>
+      <c r="F8" s="55"/>
+      <c r="G8" s="55"/>
+      <c r="J8" s="55" t="s">
         <v>19</v>
       </c>
-      <c r="K8" s="54"/>
-      <c r="L8" s="54"/>
-      <c r="M8" s="54"/>
-      <c r="N8" s="54"/>
-      <c r="O8" s="54"/>
-      <c r="P8" s="54"/>
-      <c r="Q8" s="54"/>
+      <c r="K8" s="55"/>
+      <c r="L8" s="55"/>
+      <c r="M8" s="55"/>
+      <c r="N8" s="55"/>
+      <c r="O8" s="55"/>
+      <c r="P8" s="55"/>
+      <c r="Q8" s="55"/>
     </row>
     <row r="9" spans="1:17">
       <c r="A9" s="8" t="s">
@@ -4270,15 +4470,15 @@
       <c r="Q15" s="1"/>
     </row>
     <row r="16" spans="1:17">
-      <c r="A16" s="54" t="s">
+      <c r="A16" s="55" t="s">
         <v>35</v>
       </c>
-      <c r="B16" s="54"/>
-      <c r="C16" s="54"/>
-      <c r="D16" s="54"/>
-      <c r="E16" s="54"/>
-      <c r="F16" s="54"/>
-      <c r="G16" s="54"/>
+      <c r="B16" s="55"/>
+      <c r="C16" s="55"/>
+      <c r="D16" s="55"/>
+      <c r="E16" s="55"/>
+      <c r="F16" s="55"/>
+      <c r="G16" s="55"/>
       <c r="K16" s="1"/>
       <c r="L16" s="1"/>
       <c r="M16" s="1"/>
@@ -4495,27 +4695,27 @@
       <c r="R22" s="4"/>
     </row>
     <row r="23" spans="1:18">
-      <c r="A23" s="54" t="s">
+      <c r="A23" s="55" t="s">
         <v>40</v>
       </c>
-      <c r="B23" s="54"/>
-      <c r="C23" s="54"/>
-      <c r="D23" s="54"/>
-      <c r="E23" s="54"/>
-      <c r="F23" s="54"/>
-      <c r="G23" s="54"/>
-      <c r="H23" s="54"/>
+      <c r="B23" s="55"/>
+      <c r="C23" s="55"/>
+      <c r="D23" s="55"/>
+      <c r="E23" s="55"/>
+      <c r="F23" s="55"/>
+      <c r="G23" s="55"/>
+      <c r="H23" s="55"/>
       <c r="I23" s="4"/>
-      <c r="J23" s="54" t="s">
+      <c r="J23" s="55" t="s">
         <v>41</v>
       </c>
-      <c r="K23" s="54"/>
-      <c r="L23" s="54"/>
-      <c r="M23" s="54"/>
-      <c r="N23" s="54"/>
-      <c r="O23" s="54"/>
-      <c r="P23" s="54"/>
-      <c r="Q23" s="54"/>
+      <c r="K23" s="55"/>
+      <c r="L23" s="55"/>
+      <c r="M23" s="55"/>
+      <c r="N23" s="55"/>
+      <c r="O23" s="55"/>
+      <c r="P23" s="55"/>
+      <c r="Q23" s="55"/>
     </row>
     <row r="24" spans="1:18">
       <c r="A24" s="8" t="s">
@@ -4943,25 +5143,25 @@
       <c r="Q30" s="1"/>
     </row>
     <row r="31" spans="1:18">
-      <c r="A31" s="54" t="s">
+      <c r="A31" s="55" t="s">
         <v>47</v>
       </c>
-      <c r="B31" s="54"/>
-      <c r="C31" s="54"/>
-      <c r="D31" s="54"/>
-      <c r="E31" s="54"/>
-      <c r="F31" s="54"/>
-      <c r="G31" s="54"/>
+      <c r="B31" s="55"/>
+      <c r="C31" s="55"/>
+      <c r="D31" s="55"/>
+      <c r="E31" s="55"/>
+      <c r="F31" s="55"/>
+      <c r="G31" s="55"/>
       <c r="I31" s="4"/>
-      <c r="J31" s="54" t="s">
+      <c r="J31" s="55" t="s">
         <v>48</v>
       </c>
-      <c r="K31" s="54"/>
-      <c r="L31" s="54"/>
-      <c r="M31" s="54"/>
-      <c r="N31" s="54"/>
-      <c r="O31" s="54"/>
-      <c r="P31" s="54"/>
+      <c r="K31" s="55"/>
+      <c r="L31" s="55"/>
+      <c r="M31" s="55"/>
+      <c r="N31" s="55"/>
+      <c r="O31" s="55"/>
+      <c r="P31" s="55"/>
     </row>
     <row r="32" spans="1:18">
       <c r="A32" t="s">
@@ -5681,6 +5881,408 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A2:S19"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.5703125" customWidth="1"/>
+    <col min="10" max="10" width="12.7109375" customWidth="1"/>
+    <col min="11" max="11" width="9.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:19">
+      <c r="A2" s="55" t="s">
+        <v>165</v>
+      </c>
+      <c r="B2" s="55"/>
+      <c r="C2" s="55"/>
+      <c r="F2" s="55" t="s">
+        <v>170</v>
+      </c>
+      <c r="G2" s="55"/>
+      <c r="H2" s="55"/>
+    </row>
+    <row r="3" spans="1:19">
+      <c r="A3" t="s">
+        <v>321</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="F3" t="s">
+        <v>321</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="4" spans="1:19">
+      <c r="A4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4">
+        <f>INDEX(TblCombinedAdjFltValues[[#Totals],[A]:[F]],MATCH(Comparison!$B$3,TblCombinedAdjFltValues[[#Headers],[A]:[F]]))</f>
+        <v>7000</v>
+      </c>
+      <c r="F4" t="s">
+        <v>3</v>
+      </c>
+      <c r="G4">
+        <f>INDEX(TblCombinedAdjFltValues[[#Totals],[A]:[F]],MATCH(Comparison!$G$3,TblCombinedAdjFltValues[[#Headers],[A]:[F]]))</f>
+        <v>9500</v>
+      </c>
+    </row>
+    <row r="5" spans="1:19">
+      <c r="A5" t="s">
+        <v>322</v>
+      </c>
+      <c r="B5">
+        <f>SUM(C10:C14)</f>
+        <v>5000</v>
+      </c>
+      <c r="F5" t="s">
+        <v>322</v>
+      </c>
+      <c r="G5">
+        <f>SUM(H10:H14)</f>
+        <v>7500</v>
+      </c>
+    </row>
+    <row r="6" spans="1:19">
+      <c r="A6" t="s">
+        <v>323</v>
+      </c>
+      <c r="B6">
+        <f>SUM(C17:C19)</f>
+        <v>2000</v>
+      </c>
+      <c r="F6" t="s">
+        <v>323</v>
+      </c>
+      <c r="G6">
+        <f>SUM(H17:H19)</f>
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="7" spans="1:19">
+      <c r="C7" s="17"/>
+      <c r="H7" s="17"/>
+    </row>
+    <row r="8" spans="1:19">
+      <c r="C8" s="17"/>
+      <c r="H8" s="17"/>
+      <c r="Q8" s="3"/>
+      <c r="S8" s="3"/>
+    </row>
+    <row r="9" spans="1:19">
+      <c r="A9" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="B9" s="17" t="s">
+        <v>324</v>
+      </c>
+      <c r="C9" s="17" t="s">
+        <v>3</v>
+      </c>
+      <c r="F9" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="G9" s="17" t="s">
+        <v>324</v>
+      </c>
+      <c r="H9" s="17" t="s">
+        <v>3</v>
+      </c>
+      <c r="I9" s="1"/>
+      <c r="J9" s="1"/>
+      <c r="K9" s="1"/>
+      <c r="L9" s="1"/>
+      <c r="M9" s="1"/>
+      <c r="N9" s="1"/>
+      <c r="O9" s="1"/>
+      <c r="P9" s="1"/>
+      <c r="Q9" s="7"/>
+      <c r="R9" s="1"/>
+      <c r="S9" s="7"/>
+    </row>
+    <row r="10" spans="1:19">
+      <c r="A10" s="17" t="s">
+        <v>13</v>
+      </c>
+      <c r="B10" s="18">
+        <f>INDEX(TblBattlefieldFlt[[A]:[F]],MATCH($A10,TblBattlefieldFlt[Option],0),MATCH($B$3,TblBattlefieldFlt[[#Headers],[A]:[F]],0))</f>
+        <v>1</v>
+      </c>
+      <c r="C10" s="17">
+        <f>INDEX(TblShipPoints[Points],MATCH(A10,TblShipPoints[Ships],0))*B10</f>
+        <v>5000</v>
+      </c>
+      <c r="F10" s="17" t="s">
+        <v>13</v>
+      </c>
+      <c r="G10" s="18">
+        <f>INDEX(TblBattlefieldFlt[[A]:[F]],MATCH($F10,TblBattlefieldFlt[Option],0),MATCH($G$3,TblBattlefieldFlt[[#Headers],[A]:[F]],0))</f>
+        <v>0</v>
+      </c>
+      <c r="H10" s="17">
+        <f>INDEX(TblShipPoints[Points],MATCH(F10,TblShipPoints[Ships],0))*G10</f>
+        <v>0</v>
+      </c>
+      <c r="I10" s="1"/>
+      <c r="J10" s="1"/>
+      <c r="K10" s="1"/>
+      <c r="L10" s="1"/>
+      <c r="M10" s="1"/>
+      <c r="N10" s="1"/>
+      <c r="O10" s="1"/>
+      <c r="P10" s="1"/>
+      <c r="Q10" s="7"/>
+      <c r="R10" s="1"/>
+      <c r="S10" s="7"/>
+    </row>
+    <row r="11" spans="1:19">
+      <c r="A11" s="17" t="s">
+        <v>14</v>
+      </c>
+      <c r="B11" s="18">
+        <f>INDEX(TblBattlefieldFlt[[A]:[F]],MATCH($A11,TblBattlefieldFlt[Option],0),MATCH($B$3,TblBattlefieldFlt[[#Headers],[A]:[F]],0))</f>
+        <v>0</v>
+      </c>
+      <c r="C11" s="17">
+        <f>INDEX(TblShipPoints[Points],MATCH(A11,TblShipPoints[Ships],0))*B11</f>
+        <v>0</v>
+      </c>
+      <c r="D11" s="17"/>
+      <c r="E11" s="17"/>
+      <c r="F11" s="17" t="s">
+        <v>14</v>
+      </c>
+      <c r="G11" s="18">
+        <f>INDEX(TblBattlefieldFlt[[A]:[F]],MATCH($F11,TblBattlefieldFlt[Option],0),MATCH($G$3,TblBattlefieldFlt[[#Headers],[A]:[F]],0))</f>
+        <v>0</v>
+      </c>
+      <c r="H11" s="17">
+        <f>INDEX(TblShipPoints[Points],MATCH(F11,TblShipPoints[Ships],0))*G11</f>
+        <v>0</v>
+      </c>
+      <c r="I11" s="1"/>
+      <c r="J11" s="1"/>
+      <c r="K11" s="1"/>
+      <c r="L11" s="1"/>
+      <c r="M11" s="1"/>
+      <c r="N11" s="1"/>
+      <c r="O11" s="1"/>
+      <c r="P11" s="1"/>
+      <c r="Q11" s="7"/>
+      <c r="R11" s="1"/>
+      <c r="S11" s="7"/>
+    </row>
+    <row r="12" spans="1:19">
+      <c r="A12" s="17" t="s">
+        <v>15</v>
+      </c>
+      <c r="B12" s="18">
+        <f>INDEX(TblBattlefieldFlt[[A]:[F]],MATCH($A12,TblBattlefieldFlt[Option],0),MATCH($B$3,TblBattlefieldFlt[[#Headers],[A]:[F]],0))</f>
+        <v>0</v>
+      </c>
+      <c r="C12" s="17">
+        <f>INDEX(TblShipPoints[Points],MATCH(A12,TblShipPoints[Ships],0))*B12</f>
+        <v>0</v>
+      </c>
+      <c r="D12" s="17"/>
+      <c r="E12" s="17"/>
+      <c r="F12" s="17" t="s">
+        <v>15</v>
+      </c>
+      <c r="G12" s="18">
+        <f>INDEX(TblBattlefieldFlt[[A]:[F]],MATCH($F12,TblBattlefieldFlt[Option],0),MATCH($G$3,TblBattlefieldFlt[[#Headers],[A]:[F]],0))</f>
+        <v>1</v>
+      </c>
+      <c r="H12" s="17">
+        <f>INDEX(TblShipPoints[Points],MATCH(F12,TblShipPoints[Ships],0))*G12</f>
+        <v>2500</v>
+      </c>
+      <c r="I12" s="1"/>
+      <c r="J12" s="1"/>
+      <c r="K12" s="1"/>
+      <c r="L12" s="1"/>
+      <c r="M12" s="1"/>
+      <c r="N12" s="1"/>
+      <c r="O12" s="1"/>
+      <c r="P12" s="1"/>
+      <c r="Q12" s="7"/>
+      <c r="R12" s="1"/>
+      <c r="S12" s="7"/>
+    </row>
+    <row r="13" spans="1:19">
+      <c r="A13" s="17" t="s">
+        <v>16</v>
+      </c>
+      <c r="B13" s="18">
+        <f>INDEX(TblBattlefieldFlt[[A]:[F]],MATCH($A13,TblBattlefieldFlt[Option],0),MATCH($B$3,TblBattlefieldFlt[[#Headers],[A]:[F]],0))</f>
+        <v>0</v>
+      </c>
+      <c r="C13" s="17">
+        <f>INDEX(TblShipPoints[Points],MATCH(A13,TblShipPoints[Ships],0))*B13</f>
+        <v>0</v>
+      </c>
+      <c r="F13" s="17" t="s">
+        <v>16</v>
+      </c>
+      <c r="G13" s="18">
+        <f>INDEX(TblBattlefieldFlt[[A]:[F]],MATCH($F13,TblBattlefieldFlt[Option],0),MATCH($G$3,TblBattlefieldFlt[[#Headers],[A]:[F]],0))</f>
+        <v>0</v>
+      </c>
+      <c r="H13" s="17">
+        <f>INDEX(TblShipPoints[Points],MATCH(F13,TblShipPoints[Ships],0))*G13</f>
+        <v>0</v>
+      </c>
+      <c r="I13" s="1"/>
+      <c r="J13" s="1"/>
+      <c r="K13" s="1"/>
+      <c r="L13" s="1"/>
+      <c r="M13" s="1"/>
+      <c r="N13" s="1"/>
+      <c r="O13" s="1"/>
+      <c r="P13" s="1"/>
+      <c r="Q13" s="7"/>
+      <c r="R13" s="1"/>
+      <c r="S13" s="7"/>
+    </row>
+    <row r="14" spans="1:19">
+      <c r="A14" s="17" t="s">
+        <v>17</v>
+      </c>
+      <c r="B14" s="18">
+        <f>INDEX(TblBattlefieldFlt[[A]:[F]],MATCH($A14,TblBattlefieldFlt[Option],0),MATCH($B$3,TblBattlefieldFlt[[#Headers],[A]:[F]],0))</f>
+        <v>0</v>
+      </c>
+      <c r="C14" s="17">
+        <f>INDEX(TblShipPoints[Points],MATCH(A14,TblShipPoints[Ships],0))*B14</f>
+        <v>0</v>
+      </c>
+      <c r="F14" s="17" t="s">
+        <v>17</v>
+      </c>
+      <c r="G14" s="18">
+        <f>INDEX(TblBattlefieldFlt[[A]:[F]],MATCH($F14,TblBattlefieldFlt[Option],0),MATCH($G$3,TblBattlefieldFlt[[#Headers],[A]:[F]],0))</f>
+        <v>10</v>
+      </c>
+      <c r="H14" s="17">
+        <f>INDEX(TblShipPoints[Points],MATCH(F14,TblShipPoints[Ships],0))*G14</f>
+        <v>5000</v>
+      </c>
+    </row>
+    <row r="16" spans="1:19">
+      <c r="A16" s="17" t="s">
+        <v>212</v>
+      </c>
+      <c r="B16" s="17" t="s">
+        <v>324</v>
+      </c>
+      <c r="C16" t="s">
+        <v>3</v>
+      </c>
+      <c r="F16" s="17" t="s">
+        <v>212</v>
+      </c>
+      <c r="G16" s="17" t="s">
+        <v>324</v>
+      </c>
+      <c r="H16" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8">
+      <c r="A17" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="B17" s="18">
+        <f>SUMPRODUCT($B$10:$B$14,TblShipCrew[Service])</f>
+        <v>11</v>
+      </c>
+      <c r="C17">
+        <f>TblRoleControlValues[Service]*B17</f>
+        <v>1100</v>
+      </c>
+      <c r="F17" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="G17" s="18">
+        <f>SUMPRODUCT($G$10:$G$14,TblShipCrew[Service])</f>
+        <v>15</v>
+      </c>
+      <c r="H17">
+        <f>TblRoleControlValues[Service]*G17</f>
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8">
+      <c r="A18" s="17" t="s">
+        <v>5</v>
+      </c>
+      <c r="B18" s="18">
+        <f>SUMPRODUCT($B$10:$B$14,TblShipCrew[Lieutenant])</f>
+        <v>3</v>
+      </c>
+      <c r="C18">
+        <f>TblRoleControlValues[Lieutenant]*B18</f>
+        <v>600</v>
+      </c>
+      <c r="F18" s="17" t="s">
+        <v>5</v>
+      </c>
+      <c r="G18" s="18">
+        <f>SUMPRODUCT($G$10:$G$14,TblShipCrew[Lieutenant])</f>
+        <v>1</v>
+      </c>
+      <c r="H18">
+        <f>TblRoleControlValues[Lieutenant]*G18</f>
+        <v>200</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8">
+      <c r="A19" s="17" t="s">
+        <v>6</v>
+      </c>
+      <c r="B19" s="18">
+        <f>SUMPRODUCT($B$10:$B$14,TblShipCrew[Captain])</f>
+        <v>1</v>
+      </c>
+      <c r="C19">
+        <f>TblRoleControlValues[Captain]*B19</f>
+        <v>300</v>
+      </c>
+      <c r="F19" s="17" t="s">
+        <v>6</v>
+      </c>
+      <c r="G19" s="18">
+        <f>SUMPRODUCT($G$10:$G$14,TblShipCrew[Captain])</f>
+        <v>1</v>
+      </c>
+      <c r="H19">
+        <f>TblRoleControlValues[Captain]*G19</f>
+        <v>300</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A2:C2"/>
+    <mergeCell ref="F2:H2"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{91273792-62E9-442E-9CC7-E8C6E6BD4008}">
   <dimension ref="B1:V32"/>
@@ -6687,7 +7289,7 @@
     <row r="16" spans="2:19">
       <c r="P16">
         <f ca="1">RANDBETWEEN(0,123)</f>
-        <v>64</v>
+        <v>77</v>
       </c>
     </row>
     <row r="17" spans="2:16">
@@ -7153,8 +7755,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{93013FD4-B940-4A70-A7DA-BF82FD0F616E}">
   <dimension ref="A2:K81"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A44" workbookViewId="0">
-      <selection activeCell="B50" sqref="B50:B65"/>
+    <sheetView topLeftCell="A35" workbookViewId="0">
+      <selection activeCell="B64" sqref="B64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -7256,14 +7858,14 @@
         <v>75</v>
       </c>
       <c r="C23" s="48"/>
-      <c r="D23" s="55" t="s">
+      <c r="D23" s="56" t="s">
         <v>166</v>
       </c>
-      <c r="E23" s="56"/>
-      <c r="F23" s="56"/>
-      <c r="G23" s="56"/>
-      <c r="H23" s="56"/>
-      <c r="I23" s="57"/>
+      <c r="E23" s="57"/>
+      <c r="F23" s="57"/>
+      <c r="G23" s="57"/>
+      <c r="H23" s="57"/>
+      <c r="I23" s="58"/>
       <c r="J23" s="48"/>
       <c r="K23" s="50" t="s">
         <v>167</v>
@@ -7272,24 +7874,24 @@
     <row r="24" spans="1:11">
       <c r="B24" s="48"/>
       <c r="C24" s="48"/>
-      <c r="D24" s="58"/>
-      <c r="E24" s="59"/>
-      <c r="F24" s="59"/>
-      <c r="G24" s="59"/>
-      <c r="H24" s="59"/>
-      <c r="I24" s="60"/>
+      <c r="D24" s="59"/>
+      <c r="E24" s="60"/>
+      <c r="F24" s="60"/>
+      <c r="G24" s="60"/>
+      <c r="H24" s="60"/>
+      <c r="I24" s="61"/>
       <c r="J24" s="48"/>
       <c r="K24" s="48"/>
     </row>
     <row r="25" spans="1:11">
       <c r="B25" s="48"/>
       <c r="C25" s="48"/>
-      <c r="D25" s="58"/>
-      <c r="E25" s="59"/>
-      <c r="F25" s="59"/>
-      <c r="G25" s="59"/>
-      <c r="H25" s="59"/>
-      <c r="I25" s="60"/>
+      <c r="D25" s="59"/>
+      <c r="E25" s="60"/>
+      <c r="F25" s="60"/>
+      <c r="G25" s="60"/>
+      <c r="H25" s="60"/>
+      <c r="I25" s="61"/>
       <c r="J25" s="48"/>
       <c r="K25" s="48"/>
     </row>
@@ -7298,12 +7900,12 @@
         <v>77</v>
       </c>
       <c r="C26" s="48"/>
-      <c r="D26" s="58"/>
-      <c r="E26" s="59"/>
-      <c r="F26" s="59"/>
-      <c r="G26" s="59"/>
-      <c r="H26" s="59"/>
-      <c r="I26" s="60"/>
+      <c r="D26" s="59"/>
+      <c r="E26" s="60"/>
+      <c r="F26" s="60"/>
+      <c r="G26" s="60"/>
+      <c r="H26" s="60"/>
+      <c r="I26" s="61"/>
       <c r="J26" s="48"/>
       <c r="K26" s="50" t="s">
         <v>168</v>
@@ -7312,12 +7914,12 @@
     <row r="27" spans="1:11">
       <c r="B27" s="48"/>
       <c r="C27" s="48"/>
-      <c r="D27" s="58"/>
-      <c r="E27" s="59"/>
-      <c r="F27" s="59"/>
-      <c r="G27" s="59"/>
-      <c r="H27" s="59"/>
-      <c r="I27" s="60"/>
+      <c r="D27" s="59"/>
+      <c r="E27" s="60"/>
+      <c r="F27" s="60"/>
+      <c r="G27" s="60"/>
+      <c r="H27" s="60"/>
+      <c r="I27" s="61"/>
       <c r="J27" s="48"/>
       <c r="K27" s="48"/>
     </row>
@@ -7326,26 +7928,26 @@
         <v>169</v>
       </c>
       <c r="C28" s="49"/>
-      <c r="D28" s="61"/>
-      <c r="E28" s="62"/>
-      <c r="F28" s="62"/>
-      <c r="G28" s="62"/>
-      <c r="H28" s="62"/>
-      <c r="I28" s="63"/>
+      <c r="D28" s="62"/>
+      <c r="E28" s="63"/>
+      <c r="F28" s="63"/>
+      <c r="G28" s="63"/>
+      <c r="H28" s="63"/>
+      <c r="I28" s="64"/>
       <c r="J28" s="49"/>
       <c r="K28" s="48"/>
     </row>
     <row r="29" spans="1:11">
       <c r="B29" s="48"/>
       <c r="C29" s="48"/>
-      <c r="D29" s="55" t="s">
+      <c r="D29" s="56" t="s">
         <v>166</v>
       </c>
-      <c r="E29" s="56"/>
-      <c r="F29" s="56"/>
-      <c r="G29" s="56"/>
-      <c r="H29" s="56"/>
-      <c r="I29" s="57"/>
+      <c r="E29" s="57"/>
+      <c r="F29" s="57"/>
+      <c r="G29" s="57"/>
+      <c r="H29" s="57"/>
+      <c r="I29" s="58"/>
       <c r="J29" s="48"/>
       <c r="K29" s="50" t="s">
         <v>169</v>
@@ -7354,12 +7956,12 @@
     <row r="30" spans="1:11">
       <c r="B30" s="48"/>
       <c r="C30" s="48"/>
-      <c r="D30" s="58"/>
-      <c r="E30" s="59"/>
-      <c r="F30" s="59"/>
-      <c r="G30" s="59"/>
-      <c r="H30" s="59"/>
-      <c r="I30" s="60"/>
+      <c r="D30" s="59"/>
+      <c r="E30" s="60"/>
+      <c r="F30" s="60"/>
+      <c r="G30" s="60"/>
+      <c r="H30" s="60"/>
+      <c r="I30" s="61"/>
       <c r="J30" s="48"/>
       <c r="K30" s="48"/>
     </row>
@@ -7368,12 +7970,12 @@
         <v>168</v>
       </c>
       <c r="C31" s="48"/>
-      <c r="D31" s="58"/>
-      <c r="E31" s="59"/>
-      <c r="F31" s="59"/>
-      <c r="G31" s="59"/>
-      <c r="H31" s="59"/>
-      <c r="I31" s="60"/>
+      <c r="D31" s="59"/>
+      <c r="E31" s="60"/>
+      <c r="F31" s="60"/>
+      <c r="G31" s="60"/>
+      <c r="H31" s="60"/>
+      <c r="I31" s="61"/>
       <c r="J31" s="48"/>
       <c r="K31" s="50" t="s">
         <v>77</v>
@@ -7382,24 +7984,24 @@
     <row r="32" spans="1:11">
       <c r="B32" s="48"/>
       <c r="C32" s="48"/>
-      <c r="D32" s="58"/>
-      <c r="E32" s="59"/>
-      <c r="F32" s="59"/>
-      <c r="G32" s="59"/>
-      <c r="H32" s="59"/>
-      <c r="I32" s="60"/>
+      <c r="D32" s="59"/>
+      <c r="E32" s="60"/>
+      <c r="F32" s="60"/>
+      <c r="G32" s="60"/>
+      <c r="H32" s="60"/>
+      <c r="I32" s="61"/>
       <c r="J32" s="48"/>
       <c r="K32" s="48"/>
     </row>
     <row r="33" spans="1:11">
       <c r="B33" s="48"/>
       <c r="C33" s="48"/>
-      <c r="D33" s="58"/>
-      <c r="E33" s="59"/>
-      <c r="F33" s="59"/>
-      <c r="G33" s="59"/>
-      <c r="H33" s="59"/>
-      <c r="I33" s="60"/>
+      <c r="D33" s="59"/>
+      <c r="E33" s="60"/>
+      <c r="F33" s="60"/>
+      <c r="G33" s="60"/>
+      <c r="H33" s="60"/>
+      <c r="I33" s="61"/>
       <c r="J33" s="48"/>
       <c r="K33" s="48"/>
     </row>
@@ -7411,12 +8013,12 @@
         <v>167</v>
       </c>
       <c r="C34" s="48"/>
-      <c r="D34" s="61"/>
-      <c r="E34" s="62"/>
-      <c r="F34" s="62"/>
-      <c r="G34" s="62"/>
-      <c r="H34" s="62"/>
-      <c r="I34" s="63"/>
+      <c r="D34" s="62"/>
+      <c r="E34" s="63"/>
+      <c r="F34" s="63"/>
+      <c r="G34" s="63"/>
+      <c r="H34" s="63"/>
+      <c r="I34" s="64"/>
       <c r="J34" s="48"/>
       <c r="K34" s="50" t="s">
         <v>75</v>
@@ -7673,10 +8275,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1CADF2F4-A124-44BC-8A72-4CE3F16F5D04}">
-  <dimension ref="B2:D32"/>
+  <dimension ref="B2:D39"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H4" sqref="H4"/>
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -7698,10 +8300,10 @@
       </c>
     </row>
     <row r="3" spans="2:4" ht="106.5" customHeight="1">
-      <c r="B3" s="70" t="s">
+      <c r="B3" s="67" t="s">
         <v>212</v>
       </c>
-      <c r="C3" s="64" t="s">
+      <c r="C3" s="65" t="s">
         <v>213</v>
       </c>
       <c r="D3" s="28" t="s">
@@ -7709,31 +8311,31 @@
       </c>
     </row>
     <row r="4" spans="2:4" ht="106.5">
-      <c r="B4" s="71"/>
-      <c r="C4" s="65"/>
+      <c r="B4" s="68"/>
+      <c r="C4" s="66"/>
       <c r="D4" s="29" t="s">
         <v>215</v>
       </c>
     </row>
     <row r="5" spans="2:4" ht="60.75">
-      <c r="B5" s="71"/>
-      <c r="C5" s="65"/>
+      <c r="B5" s="68"/>
+      <c r="C5" s="66"/>
       <c r="D5" s="30" t="s">
         <v>216</v>
       </c>
     </row>
     <row r="6" spans="2:4" ht="75">
-      <c r="B6" s="71"/>
-      <c r="C6" s="65"/>
+      <c r="B6" s="68"/>
+      <c r="C6" s="66"/>
       <c r="D6" s="30" t="s">
         <v>217</v>
       </c>
     </row>
-    <row r="7" spans="2:4" ht="90">
-      <c r="B7" s="70" t="s">
+    <row r="7" spans="2:4" ht="106.5">
+      <c r="B7" s="67" t="s">
         <v>218</v>
       </c>
-      <c r="C7" s="64" t="s">
+      <c r="C7" s="65" t="s">
         <v>219</v>
       </c>
       <c r="D7" s="28" t="s">
@@ -7741,35 +8343,35 @@
       </c>
     </row>
     <row r="8" spans="2:4" ht="90">
-      <c r="B8" s="71"/>
-      <c r="C8" s="65"/>
+      <c r="B8" s="68"/>
+      <c r="C8" s="66"/>
       <c r="D8" s="30" t="s">
         <v>221</v>
       </c>
     </row>
     <row r="9" spans="2:4" ht="75">
-      <c r="B9" s="70" t="s">
+      <c r="B9" s="67" t="s">
         <v>222</v>
       </c>
-      <c r="C9" s="64" t="s">
+      <c r="C9" s="65" t="s">
         <v>223</v>
       </c>
       <c r="D9" s="28" t="s">
         <v>224</v>
       </c>
     </row>
-    <row r="10" spans="2:4" ht="30">
-      <c r="B10" s="72"/>
-      <c r="C10" s="66"/>
+    <row r="10" spans="2:4" ht="60.75">
+      <c r="B10" s="70"/>
+      <c r="C10" s="69"/>
       <c r="D10" s="31" t="s">
         <v>225</v>
       </c>
     </row>
     <row r="11" spans="2:4" ht="76.5" customHeight="1">
-      <c r="B11" s="70" t="s">
+      <c r="B11" s="67" t="s">
         <v>226</v>
       </c>
-      <c r="C11" s="64" t="s">
+      <c r="C11" s="65" t="s">
         <v>227</v>
       </c>
       <c r="D11" s="28" t="s">
@@ -7777,17 +8379,17 @@
       </c>
     </row>
     <row r="12" spans="2:4" ht="30.75">
-      <c r="B12" s="71"/>
-      <c r="C12" s="65"/>
+      <c r="B12" s="68"/>
+      <c r="C12" s="66"/>
       <c r="D12" s="31" t="s">
         <v>229</v>
       </c>
     </row>
     <row r="13" spans="2:4" ht="45.75">
-      <c r="B13" s="70" t="s">
+      <c r="B13" s="67" t="s">
         <v>230</v>
       </c>
-      <c r="C13" s="64" t="s">
+      <c r="C13" s="65" t="s">
         <v>231</v>
       </c>
       <c r="D13" s="28" t="s">
@@ -7795,31 +8397,31 @@
       </c>
     </row>
     <row r="14" spans="2:4" ht="30.75">
-      <c r="B14" s="71"/>
-      <c r="C14" s="65"/>
+      <c r="B14" s="68"/>
+      <c r="C14" s="66"/>
       <c r="D14" s="31" t="s">
         <v>229</v>
       </c>
     </row>
     <row r="15" spans="2:4" ht="45.75">
-      <c r="B15" s="71"/>
-      <c r="C15" s="65"/>
+      <c r="B15" s="68"/>
+      <c r="C15" s="66"/>
       <c r="D15" s="30" t="s">
         <v>233</v>
       </c>
     </row>
     <row r="16" spans="2:4" ht="60">
-      <c r="B16" s="71"/>
-      <c r="C16" s="65"/>
+      <c r="B16" s="68"/>
+      <c r="C16" s="66"/>
       <c r="D16" s="30" t="s">
         <v>234</v>
       </c>
     </row>
     <row r="17" spans="2:4" ht="45">
-      <c r="B17" s="70" t="s">
+      <c r="B17" s="67" t="s">
         <v>235</v>
       </c>
-      <c r="C17" s="64" t="s">
+      <c r="C17" s="65" t="s">
         <v>236</v>
       </c>
       <c r="D17" s="28" t="s">
@@ -7827,17 +8429,17 @@
       </c>
     </row>
     <row r="18" spans="2:4" ht="45">
-      <c r="B18" s="71"/>
-      <c r="C18" s="65"/>
+      <c r="B18" s="68"/>
+      <c r="C18" s="66"/>
       <c r="D18" s="30" t="s">
         <v>238</v>
       </c>
     </row>
     <row r="19" spans="2:4" ht="60.75" customHeight="1">
-      <c r="B19" s="70" t="s">
+      <c r="B19" s="67" t="s">
         <v>239</v>
       </c>
-      <c r="C19" s="64" t="s">
+      <c r="C19" s="65" t="s">
         <v>240</v>
       </c>
       <c r="D19" s="28" t="s">
@@ -7845,17 +8447,17 @@
       </c>
     </row>
     <row r="20" spans="2:4" ht="30.75">
-      <c r="B20" s="71"/>
-      <c r="C20" s="65"/>
+      <c r="B20" s="68"/>
+      <c r="C20" s="66"/>
       <c r="D20" s="31" t="s">
         <v>229</v>
       </c>
     </row>
     <row r="21" spans="2:4" ht="45.75">
-      <c r="B21" s="70" t="s">
+      <c r="B21" s="67" t="s">
         <v>242</v>
       </c>
-      <c r="C21" s="64" t="s">
+      <c r="C21" s="65" t="s">
         <v>243</v>
       </c>
       <c r="D21" s="28" t="s">
@@ -7863,17 +8465,17 @@
       </c>
     </row>
     <row r="22" spans="2:4" ht="30.75">
-      <c r="B22" s="71"/>
-      <c r="C22" s="65"/>
+      <c r="B22" s="68"/>
+      <c r="C22" s="66"/>
       <c r="D22" s="31" t="s">
         <v>229</v>
       </c>
     </row>
     <row r="23" spans="2:4" ht="62.25" customHeight="1">
-      <c r="B23" s="70" t="s">
+      <c r="B23" s="67" t="s">
         <v>245</v>
       </c>
-      <c r="C23" s="64" t="s">
+      <c r="C23" s="65" t="s">
         <v>246</v>
       </c>
       <c r="D23" s="28" t="s">
@@ -7881,24 +8483,24 @@
       </c>
     </row>
     <row r="24" spans="2:4" ht="62.25" customHeight="1">
-      <c r="B24" s="71"/>
-      <c r="C24" s="65"/>
+      <c r="B24" s="68"/>
+      <c r="C24" s="66"/>
       <c r="D24" s="30" t="s">
         <v>248</v>
       </c>
     </row>
     <row r="25" spans="2:4" ht="30.75">
-      <c r="B25" s="72"/>
-      <c r="C25" s="66"/>
+      <c r="B25" s="70"/>
+      <c r="C25" s="69"/>
       <c r="D25" s="30" t="s">
         <v>229</v>
       </c>
     </row>
     <row r="26" spans="2:4" ht="45.75">
-      <c r="B26" s="70" t="s">
+      <c r="B26" s="67" t="s">
         <v>249</v>
       </c>
-      <c r="C26" s="64" t="s">
+      <c r="C26" s="65" t="s">
         <v>250</v>
       </c>
       <c r="D26" s="28" t="s">
@@ -7906,24 +8508,24 @@
       </c>
     </row>
     <row r="27" spans="2:4" ht="60.75">
-      <c r="B27" s="71"/>
-      <c r="C27" s="65"/>
+      <c r="B27" s="68"/>
+      <c r="C27" s="66"/>
       <c r="D27" s="30" t="s">
         <v>248</v>
       </c>
     </row>
     <row r="28" spans="2:4" ht="30.75">
-      <c r="B28" s="71"/>
-      <c r="C28" s="65"/>
+      <c r="B28" s="68"/>
+      <c r="C28" s="66"/>
       <c r="D28" s="30" t="s">
         <v>229</v>
       </c>
     </row>
     <row r="29" spans="2:4" ht="45.75">
-      <c r="B29" s="67" t="s">
+      <c r="B29" s="71" t="s">
         <v>251</v>
       </c>
-      <c r="C29" s="64" t="s">
+      <c r="C29" s="65" t="s">
         <v>252</v>
       </c>
       <c r="D29" s="28" t="s">
@@ -7931,28 +8533,85 @@
       </c>
     </row>
     <row r="30" spans="2:4" ht="60.75">
-      <c r="B30" s="68"/>
-      <c r="C30" s="65"/>
+      <c r="B30" s="72"/>
+      <c r="C30" s="66"/>
       <c r="D30" s="30" t="s">
         <v>248</v>
       </c>
     </row>
     <row r="31" spans="2:4" ht="30.75">
-      <c r="B31" s="68"/>
-      <c r="C31" s="65"/>
+      <c r="B31" s="72"/>
+      <c r="C31" s="66"/>
       <c r="D31" s="30" t="s">
         <v>229</v>
       </c>
     </row>
     <row r="32" spans="2:4" ht="60.75">
-      <c r="B32" s="69"/>
-      <c r="C32" s="66"/>
-      <c r="D32" s="31" t="s">
+      <c r="B32" s="72"/>
+      <c r="C32" s="76"/>
+      <c r="D32" s="30" t="s">
         <v>253</v>
       </c>
     </row>
+    <row r="33" spans="2:4" ht="76.5" customHeight="1">
+      <c r="B33" s="71" t="s">
+        <v>254</v>
+      </c>
+      <c r="C33" s="65" t="s">
+        <v>255</v>
+      </c>
+      <c r="D33" s="28" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="34" spans="2:4" ht="30.75">
+      <c r="B34" s="72"/>
+      <c r="C34" s="76"/>
+      <c r="D34" s="30" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="35" spans="2:4" ht="30.75">
+      <c r="B35" s="72"/>
+      <c r="C35" s="76"/>
+      <c r="D35" s="30" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="36" spans="2:4" ht="60.75">
+      <c r="B36" s="72"/>
+      <c r="C36" s="76"/>
+      <c r="D36" s="30" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="37" spans="2:4" ht="137.25">
+      <c r="B37" s="72"/>
+      <c r="C37" s="76"/>
+      <c r="D37" s="30" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="38" spans="2:4" ht="45.75">
+      <c r="B38" s="73"/>
+      <c r="C38" s="69"/>
+      <c r="D38" s="31" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="39" spans="2:4">
+      <c r="D39" s="53"/>
+    </row>
   </sheetData>
-  <mergeCells count="22">
+  <mergeCells count="24">
+    <mergeCell ref="C33:C38"/>
+    <mergeCell ref="B33:B38"/>
+    <mergeCell ref="C29:C32"/>
+    <mergeCell ref="B29:B32"/>
+    <mergeCell ref="C23:C25"/>
+    <mergeCell ref="B23:B25"/>
+    <mergeCell ref="C26:C28"/>
+    <mergeCell ref="B26:B28"/>
     <mergeCell ref="C21:C22"/>
     <mergeCell ref="B21:B22"/>
     <mergeCell ref="C19:C20"/>
@@ -7969,12 +8628,6 @@
     <mergeCell ref="B13:B16"/>
     <mergeCell ref="C17:C18"/>
     <mergeCell ref="B17:B18"/>
-    <mergeCell ref="C29:C32"/>
-    <mergeCell ref="B29:B32"/>
-    <mergeCell ref="C23:C25"/>
-    <mergeCell ref="B23:B25"/>
-    <mergeCell ref="C26:C28"/>
-    <mergeCell ref="B26:B28"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -7982,16 +8635,306 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1914FF74-0E8B-4E92-8BDD-103E839E1854}">
-  <dimension ref="B3:D29"/>
+  <dimension ref="B3:J28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="73.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="33.140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="31.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="2:10" ht="23.25">
+      <c r="B3" s="47" t="s">
+        <v>27</v>
+      </c>
+      <c r="C3" s="47" t="s">
+        <v>260</v>
+      </c>
+      <c r="D3" s="51" t="s">
+        <v>261</v>
+      </c>
+      <c r="I3" s="51" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="4" spans="2:10">
+      <c r="B4" s="3" t="s">
+        <v>263</v>
+      </c>
+      <c r="C4" t="s">
+        <v>264</v>
+      </c>
+      <c r="D4" t="s">
+        <v>265</v>
+      </c>
+      <c r="I4" s="78" t="s">
+        <v>266</v>
+      </c>
+      <c r="J4" s="79" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="5" spans="2:10" ht="121.5">
+      <c r="B5" s="3" t="s">
+        <v>267</v>
+      </c>
+      <c r="C5" t="s">
+        <v>268</v>
+      </c>
+      <c r="D5" t="s">
+        <v>57</v>
+      </c>
+      <c r="I5" s="75" t="s">
+        <v>265</v>
+      </c>
+      <c r="J5" s="77" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="6" spans="2:10" ht="91.5">
+      <c r="B6" s="3" t="s">
+        <v>270</v>
+      </c>
+      <c r="C6" t="s">
+        <v>271</v>
+      </c>
+      <c r="D6" t="s">
+        <v>72</v>
+      </c>
+      <c r="I6" s="75" t="s">
+        <v>72</v>
+      </c>
+      <c r="J6" s="77" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="7" spans="2:10" ht="137.25">
+      <c r="B7" s="3" t="s">
+        <v>273</v>
+      </c>
+      <c r="C7" t="s">
+        <v>274</v>
+      </c>
+      <c r="D7" t="s">
+        <v>275</v>
+      </c>
+      <c r="I7" s="75" t="s">
+        <v>275</v>
+      </c>
+      <c r="J7" s="77" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="8" spans="2:10" ht="76.5">
+      <c r="B8" s="3" t="s">
+        <v>277</v>
+      </c>
+      <c r="C8" s="53" t="s">
+        <v>278</v>
+      </c>
+      <c r="I8" s="75" t="s">
+        <v>57</v>
+      </c>
+      <c r="J8" s="77" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="9" spans="2:10" ht="137.25">
+      <c r="B9" s="3" t="s">
+        <v>280</v>
+      </c>
+      <c r="C9" t="s">
+        <v>281</v>
+      </c>
+      <c r="I9" s="75" t="s">
+        <v>58</v>
+      </c>
+      <c r="J9" s="77" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="10" spans="2:10">
+      <c r="B10" s="3" t="s">
+        <v>283</v>
+      </c>
+      <c r="C10" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="11" spans="2:10">
+      <c r="B11" s="3" t="s">
+        <v>285</v>
+      </c>
+      <c r="C11" t="s">
+        <v>286</v>
+      </c>
+      <c r="D11" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="12" spans="2:10">
+      <c r="B12" s="3" t="s">
+        <v>287</v>
+      </c>
+      <c r="C12" t="s">
+        <v>288</v>
+      </c>
+      <c r="D12" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="13" spans="2:10">
+      <c r="B13" s="3" t="s">
+        <v>289</v>
+      </c>
+      <c r="C13" t="s">
+        <v>290</v>
+      </c>
+      <c r="D13" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="14" spans="2:10">
+      <c r="B14" s="3" t="s">
+        <v>291</v>
+      </c>
+      <c r="C14" t="s">
+        <v>292</v>
+      </c>
+      <c r="D14" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="15" spans="2:10">
+      <c r="B15" s="3" t="s">
+        <v>293</v>
+      </c>
+      <c r="C15" t="s">
+        <v>294</v>
+      </c>
+      <c r="D15" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="16" spans="2:10" ht="30.75">
+      <c r="B16" s="3" t="s">
+        <v>295</v>
+      </c>
+      <c r="C16" s="53" t="s">
+        <v>296</v>
+      </c>
+      <c r="D16" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="17" spans="2:4">
+      <c r="B17" s="3" t="s">
+        <v>297</v>
+      </c>
+      <c r="C17" t="s">
+        <v>298</v>
+      </c>
+      <c r="D17" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="18" spans="2:4">
+      <c r="B18" s="3" t="s">
+        <v>299</v>
+      </c>
+      <c r="C18" t="s">
+        <v>300</v>
+      </c>
+      <c r="D18" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="19" spans="2:4">
+      <c r="B19" s="3" t="s">
+        <v>301</v>
+      </c>
+      <c r="C19" t="s">
+        <v>302</v>
+      </c>
+      <c r="D19" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="20" spans="2:4" ht="30.75">
+      <c r="B20" s="80" t="s">
+        <v>303</v>
+      </c>
+      <c r="C20" s="81" t="s">
+        <v>304</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="21" spans="2:4">
+      <c r="B21" s="3" t="s">
+        <v>305</v>
+      </c>
+      <c r="C21" t="s">
+        <v>306</v>
+      </c>
+      <c r="D21" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="22" spans="2:4">
+      <c r="B22" s="3" t="s">
+        <v>307</v>
+      </c>
+      <c r="C22" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="23" spans="2:4">
+      <c r="B23" s="3"/>
+    </row>
+    <row r="24" spans="2:4">
+      <c r="B24" s="3"/>
+    </row>
+    <row r="25" spans="2:4">
+      <c r="B25" s="3"/>
+    </row>
+    <row r="26" spans="2:4">
+      <c r="B26" s="3"/>
+    </row>
+    <row r="27" spans="2:4">
+      <c r="B27" s="3"/>
+    </row>
+    <row r="28" spans="2:4">
+      <c r="B28" s="3"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D3CDE875-88F5-4F85-ACCD-AF4C3075C97E}">
+  <dimension ref="B3:D30"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="2" max="2" width="24.140625" customWidth="1"/>
+    <col min="3" max="3" width="45.42578125" customWidth="1"/>
+    <col min="4" max="4" width="34.28515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="3" spans="2:4" ht="23.25">
@@ -7999,588 +8942,161 @@
         <v>27</v>
       </c>
       <c r="C3" s="47" t="s">
-        <v>254</v>
-      </c>
-      <c r="D3" s="51" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="4" spans="2:4">
-      <c r="B4" s="3" t="s">
-        <v>256</v>
-      </c>
-      <c r="C4" t="s">
-        <v>257</v>
-      </c>
-      <c r="D4" t="s">
-        <v>258</v>
-      </c>
-    </row>
-    <row r="5" spans="2:4">
-      <c r="B5" s="3" t="s">
-        <v>259</v>
-      </c>
-      <c r="C5" t="s">
         <v>260</v>
       </c>
-      <c r="D5" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="6" spans="2:4">
-      <c r="B6" s="3" t="s">
-        <v>261</v>
-      </c>
-      <c r="C6" t="s">
-        <v>262</v>
-      </c>
-      <c r="D6" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="7" spans="2:4">
-      <c r="B7" s="3" t="s">
-        <v>263</v>
-      </c>
-      <c r="C7" t="s">
-        <v>264</v>
-      </c>
-      <c r="D7" t="s">
-        <v>265</v>
-      </c>
-    </row>
-    <row r="8" spans="2:4" ht="45.75">
-      <c r="B8" s="3" t="s">
-        <v>266</v>
-      </c>
-      <c r="C8" s="53" t="s">
-        <v>267</v>
-      </c>
+      <c r="D3" s="47" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="4" spans="2:4" ht="91.5">
+      <c r="B4" s="74" t="s">
+        <v>310</v>
+      </c>
+      <c r="C4" s="54" t="s">
+        <v>311</v>
+      </c>
+      <c r="D4" s="54"/>
+    </row>
+    <row r="5" spans="2:4" ht="91.5">
+      <c r="B5" s="74" t="s">
+        <v>312</v>
+      </c>
+      <c r="C5" s="54" t="s">
+        <v>313</v>
+      </c>
+      <c r="D5" s="54" t="s">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="6" spans="2:4" ht="76.5">
+      <c r="B6" s="74" t="s">
+        <v>315</v>
+      </c>
+      <c r="C6" s="54" t="s">
+        <v>316</v>
+      </c>
+      <c r="D6" s="54" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="7" spans="2:4" ht="76.5">
+      <c r="B7" s="74" t="s">
+        <v>318</v>
+      </c>
+      <c r="C7" s="54" t="s">
+        <v>319</v>
+      </c>
+      <c r="D7" s="54" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="8" spans="2:4">
+      <c r="B8" s="74"/>
+      <c r="C8" s="74"/>
+      <c r="D8" s="54"/>
     </row>
     <row r="9" spans="2:4">
-      <c r="B9" s="3" t="s">
-        <v>268</v>
-      </c>
-      <c r="C9" t="s">
-        <v>269</v>
-      </c>
+      <c r="B9" s="74"/>
+      <c r="C9" s="74"/>
+      <c r="D9" s="54"/>
     </row>
     <row r="10" spans="2:4">
-      <c r="B10" s="3" t="s">
-        <v>270</v>
-      </c>
-      <c r="C10" t="s">
-        <v>271</v>
-      </c>
+      <c r="B10" s="74"/>
+      <c r="C10" s="74"/>
+      <c r="D10" s="54"/>
     </row>
     <row r="11" spans="2:4">
-      <c r="B11" s="3" t="s">
-        <v>272</v>
-      </c>
-      <c r="C11" t="s">
-        <v>273</v>
-      </c>
-      <c r="D11" t="s">
-        <v>58</v>
-      </c>
+      <c r="B11" s="74"/>
+      <c r="C11" s="74"/>
+      <c r="D11" s="54"/>
     </row>
     <row r="12" spans="2:4">
-      <c r="B12" s="3" t="s">
-        <v>274</v>
-      </c>
-      <c r="C12" t="s">
-        <v>275</v>
-      </c>
-      <c r="D12" t="s">
-        <v>58</v>
-      </c>
+      <c r="B12" s="74"/>
+      <c r="C12" s="74"/>
+      <c r="D12" s="54"/>
     </row>
     <row r="13" spans="2:4">
-      <c r="B13" s="3" t="s">
-        <v>276</v>
-      </c>
-      <c r="C13" t="s">
-        <v>277</v>
-      </c>
-      <c r="D13" t="s">
-        <v>258</v>
-      </c>
+      <c r="B13" s="74"/>
+      <c r="C13" s="74"/>
+      <c r="D13" s="54"/>
     </row>
     <row r="14" spans="2:4">
-      <c r="B14" s="3" t="s">
-        <v>278</v>
-      </c>
-      <c r="C14" t="s">
-        <v>279</v>
-      </c>
-      <c r="D14" t="s">
-        <v>72</v>
-      </c>
+      <c r="B14" s="74"/>
+      <c r="C14" s="74"/>
+      <c r="D14" s="54"/>
     </row>
     <row r="15" spans="2:4">
-      <c r="B15" s="3" t="s">
-        <v>280</v>
-      </c>
-      <c r="C15" t="s">
-        <v>281</v>
-      </c>
-      <c r="D15" t="s">
-        <v>57</v>
-      </c>
+      <c r="B15" s="74"/>
+      <c r="C15" s="74"/>
+      <c r="D15" s="54"/>
     </row>
     <row r="16" spans="2:4">
-      <c r="B16" s="3" t="s">
-        <v>282</v>
-      </c>
-      <c r="C16" t="s">
-        <v>283</v>
-      </c>
-      <c r="D16" t="s">
-        <v>265</v>
-      </c>
-    </row>
-    <row r="17" spans="2:2">
-      <c r="B17" s="3"/>
-    </row>
-    <row r="18" spans="2:2">
-      <c r="B18" s="3"/>
-    </row>
-    <row r="19" spans="2:2">
-      <c r="B19" s="3"/>
-    </row>
-    <row r="20" spans="2:2">
-      <c r="B20" s="3"/>
-    </row>
-    <row r="21" spans="2:2">
-      <c r="B21" s="3"/>
-    </row>
-    <row r="22" spans="2:2">
-      <c r="B22" s="3"/>
-    </row>
-    <row r="23" spans="2:2">
-      <c r="B23" s="3"/>
-    </row>
-    <row r="24" spans="2:2">
-      <c r="B24" s="3"/>
-    </row>
-    <row r="25" spans="2:2">
-      <c r="B25" s="3"/>
-    </row>
-    <row r="26" spans="2:2">
-      <c r="B26" s="3"/>
-    </row>
-    <row r="27" spans="2:2">
-      <c r="B27" s="3"/>
-    </row>
-    <row r="28" spans="2:2">
-      <c r="B28" s="3"/>
-    </row>
-    <row r="29" spans="2:2">
-      <c r="B29" s="3"/>
+      <c r="B16" s="74"/>
+      <c r="C16" s="74"/>
+      <c r="D16" s="54"/>
+    </row>
+    <row r="17" spans="2:4">
+      <c r="B17" s="74"/>
+      <c r="C17" s="74"/>
+      <c r="D17" s="54"/>
+    </row>
+    <row r="18" spans="2:4">
+      <c r="B18" s="74"/>
+      <c r="C18" s="74"/>
+      <c r="D18" s="54"/>
+    </row>
+    <row r="19" spans="2:4">
+      <c r="B19" s="74"/>
+      <c r="C19" s="74"/>
+      <c r="D19" s="54"/>
+    </row>
+    <row r="20" spans="2:4">
+      <c r="B20" s="74"/>
+      <c r="C20" s="74"/>
+      <c r="D20" s="54"/>
+    </row>
+    <row r="21" spans="2:4">
+      <c r="B21" s="74"/>
+      <c r="C21" s="74"/>
+      <c r="D21" s="54"/>
+    </row>
+    <row r="22" spans="2:4">
+      <c r="B22" s="74"/>
+      <c r="C22" s="74"/>
+      <c r="D22" s="54"/>
+    </row>
+    <row r="23" spans="2:4">
+      <c r="B23" s="74"/>
+      <c r="C23" s="74"/>
+      <c r="D23" s="54"/>
+    </row>
+    <row r="24" spans="2:4">
+      <c r="B24" s="74"/>
+      <c r="C24" s="74"/>
+      <c r="D24" s="54"/>
+    </row>
+    <row r="25" spans="2:4">
+      <c r="C25" s="74"/>
+      <c r="D25" s="54"/>
+    </row>
+    <row r="26" spans="2:4">
+      <c r="C26" s="74"/>
+      <c r="D26" s="54"/>
+    </row>
+    <row r="27" spans="2:4">
+      <c r="C27" s="74"/>
+      <c r="D27" s="54"/>
+    </row>
+    <row r="28" spans="2:4">
+      <c r="D28" s="54"/>
+    </row>
+    <row r="29" spans="2:4">
+      <c r="D29" s="54"/>
+    </row>
+    <row r="30" spans="2:4">
+      <c r="D30" s="54"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A2:S19"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <cols>
-    <col min="1" max="1" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="9.5703125" customWidth="1"/>
-    <col min="10" max="10" width="12.7109375" customWidth="1"/>
-    <col min="11" max="11" width="9.85546875" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="2" spans="1:19">
-      <c r="A2" s="54" t="s">
-        <v>165</v>
-      </c>
-      <c r="B2" s="54"/>
-      <c r="C2" s="54"/>
-      <c r="F2" s="54" t="s">
-        <v>170</v>
-      </c>
-      <c r="G2" s="54"/>
-      <c r="H2" s="54"/>
-    </row>
-    <row r="3" spans="1:19">
-      <c r="A3" t="s">
-        <v>284</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="F3" t="s">
-        <v>284</v>
-      </c>
-      <c r="G3" s="1" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="4" spans="1:19">
-      <c r="A4" t="s">
-        <v>3</v>
-      </c>
-      <c r="B4">
-        <f>INDEX(TblCombinedAdjFltValues[[#Totals],[A]:[F]],MATCH(Comparison!$B$3,TblCombinedAdjFltValues[[#Headers],[A]:[F]]))</f>
-        <v>7000</v>
-      </c>
-      <c r="F4" t="s">
-        <v>3</v>
-      </c>
-      <c r="G4">
-        <f>INDEX(TblCombinedAdjFltValues[[#Totals],[A]:[F]],MATCH(Comparison!$G$3,TblCombinedAdjFltValues[[#Headers],[A]:[F]]))</f>
-        <v>9500</v>
-      </c>
-    </row>
-    <row r="5" spans="1:19">
-      <c r="A5" t="s">
-        <v>285</v>
-      </c>
-      <c r="B5">
-        <f>SUM(C10:C14)</f>
-        <v>5000</v>
-      </c>
-      <c r="F5" t="s">
-        <v>285</v>
-      </c>
-      <c r="G5">
-        <f>SUM(H10:H14)</f>
-        <v>7500</v>
-      </c>
-    </row>
-    <row r="6" spans="1:19">
-      <c r="A6" t="s">
-        <v>286</v>
-      </c>
-      <c r="B6">
-        <f>SUM(C17:C19)</f>
-        <v>2000</v>
-      </c>
-      <c r="F6" t="s">
-        <v>286</v>
-      </c>
-      <c r="G6">
-        <f>SUM(H17:H19)</f>
-        <v>2000</v>
-      </c>
-    </row>
-    <row r="7" spans="1:19">
-      <c r="C7" s="17"/>
-      <c r="H7" s="17"/>
-    </row>
-    <row r="8" spans="1:19">
-      <c r="C8" s="17"/>
-      <c r="H8" s="17"/>
-      <c r="Q8" s="3"/>
-      <c r="S8" s="3"/>
-    </row>
-    <row r="9" spans="1:19">
-      <c r="A9" s="17" t="s">
-        <v>2</v>
-      </c>
-      <c r="B9" s="17" t="s">
-        <v>287</v>
-      </c>
-      <c r="C9" s="17" t="s">
-        <v>3</v>
-      </c>
-      <c r="F9" s="17" t="s">
-        <v>2</v>
-      </c>
-      <c r="G9" s="17" t="s">
-        <v>287</v>
-      </c>
-      <c r="H9" s="17" t="s">
-        <v>3</v>
-      </c>
-      <c r="I9" s="1"/>
-      <c r="J9" s="1"/>
-      <c r="K9" s="1"/>
-      <c r="L9" s="1"/>
-      <c r="M9" s="1"/>
-      <c r="N9" s="1"/>
-      <c r="O9" s="1"/>
-      <c r="P9" s="1"/>
-      <c r="Q9" s="7"/>
-      <c r="R9" s="1"/>
-      <c r="S9" s="7"/>
-    </row>
-    <row r="10" spans="1:19">
-      <c r="A10" s="17" t="s">
-        <v>13</v>
-      </c>
-      <c r="B10" s="18">
-        <f>INDEX(TblBattlefieldFlt[[A]:[F]],MATCH($A10,TblBattlefieldFlt[Option],0),MATCH($B$3,TblBattlefieldFlt[[#Headers],[A]:[F]],0))</f>
-        <v>1</v>
-      </c>
-      <c r="C10" s="17">
-        <f>INDEX(TblShipPoints[Points],MATCH(A10,TblShipPoints[Ships],0))*B10</f>
-        <v>5000</v>
-      </c>
-      <c r="F10" s="17" t="s">
-        <v>13</v>
-      </c>
-      <c r="G10" s="18">
-        <f>INDEX(TblBattlefieldFlt[[A]:[F]],MATCH($F10,TblBattlefieldFlt[Option],0),MATCH($G$3,TblBattlefieldFlt[[#Headers],[A]:[F]],0))</f>
-        <v>0</v>
-      </c>
-      <c r="H10" s="17">
-        <f>INDEX(TblShipPoints[Points],MATCH(F10,TblShipPoints[Ships],0))*G10</f>
-        <v>0</v>
-      </c>
-      <c r="I10" s="1"/>
-      <c r="J10" s="1"/>
-      <c r="K10" s="1"/>
-      <c r="L10" s="1"/>
-      <c r="M10" s="1"/>
-      <c r="N10" s="1"/>
-      <c r="O10" s="1"/>
-      <c r="P10" s="1"/>
-      <c r="Q10" s="7"/>
-      <c r="R10" s="1"/>
-      <c r="S10" s="7"/>
-    </row>
-    <row r="11" spans="1:19">
-      <c r="A11" s="17" t="s">
-        <v>14</v>
-      </c>
-      <c r="B11" s="18">
-        <f>INDEX(TblBattlefieldFlt[[A]:[F]],MATCH($A11,TblBattlefieldFlt[Option],0),MATCH($B$3,TblBattlefieldFlt[[#Headers],[A]:[F]],0))</f>
-        <v>0</v>
-      </c>
-      <c r="C11" s="17">
-        <f>INDEX(TblShipPoints[Points],MATCH(A11,TblShipPoints[Ships],0))*B11</f>
-        <v>0</v>
-      </c>
-      <c r="D11" s="17"/>
-      <c r="E11" s="17"/>
-      <c r="F11" s="17" t="s">
-        <v>14</v>
-      </c>
-      <c r="G11" s="18">
-        <f>INDEX(TblBattlefieldFlt[[A]:[F]],MATCH($F11,TblBattlefieldFlt[Option],0),MATCH($G$3,TblBattlefieldFlt[[#Headers],[A]:[F]],0))</f>
-        <v>0</v>
-      </c>
-      <c r="H11" s="17">
-        <f>INDEX(TblShipPoints[Points],MATCH(F11,TblShipPoints[Ships],0))*G11</f>
-        <v>0</v>
-      </c>
-      <c r="I11" s="1"/>
-      <c r="J11" s="1"/>
-      <c r="K11" s="1"/>
-      <c r="L11" s="1"/>
-      <c r="M11" s="1"/>
-      <c r="N11" s="1"/>
-      <c r="O11" s="1"/>
-      <c r="P11" s="1"/>
-      <c r="Q11" s="7"/>
-      <c r="R11" s="1"/>
-      <c r="S11" s="7"/>
-    </row>
-    <row r="12" spans="1:19">
-      <c r="A12" s="17" t="s">
-        <v>15</v>
-      </c>
-      <c r="B12" s="18">
-        <f>INDEX(TblBattlefieldFlt[[A]:[F]],MATCH($A12,TblBattlefieldFlt[Option],0),MATCH($B$3,TblBattlefieldFlt[[#Headers],[A]:[F]],0))</f>
-        <v>0</v>
-      </c>
-      <c r="C12" s="17">
-        <f>INDEX(TblShipPoints[Points],MATCH(A12,TblShipPoints[Ships],0))*B12</f>
-        <v>0</v>
-      </c>
-      <c r="D12" s="17"/>
-      <c r="E12" s="17"/>
-      <c r="F12" s="17" t="s">
-        <v>15</v>
-      </c>
-      <c r="G12" s="18">
-        <f>INDEX(TblBattlefieldFlt[[A]:[F]],MATCH($F12,TblBattlefieldFlt[Option],0),MATCH($G$3,TblBattlefieldFlt[[#Headers],[A]:[F]],0))</f>
-        <v>1</v>
-      </c>
-      <c r="H12" s="17">
-        <f>INDEX(TblShipPoints[Points],MATCH(F12,TblShipPoints[Ships],0))*G12</f>
-        <v>2500</v>
-      </c>
-      <c r="I12" s="1"/>
-      <c r="J12" s="1"/>
-      <c r="K12" s="1"/>
-      <c r="L12" s="1"/>
-      <c r="M12" s="1"/>
-      <c r="N12" s="1"/>
-      <c r="O12" s="1"/>
-      <c r="P12" s="1"/>
-      <c r="Q12" s="7"/>
-      <c r="R12" s="1"/>
-      <c r="S12" s="7"/>
-    </row>
-    <row r="13" spans="1:19">
-      <c r="A13" s="17" t="s">
-        <v>16</v>
-      </c>
-      <c r="B13" s="18">
-        <f>INDEX(TblBattlefieldFlt[[A]:[F]],MATCH($A13,TblBattlefieldFlt[Option],0),MATCH($B$3,TblBattlefieldFlt[[#Headers],[A]:[F]],0))</f>
-        <v>0</v>
-      </c>
-      <c r="C13" s="17">
-        <f>INDEX(TblShipPoints[Points],MATCH(A13,TblShipPoints[Ships],0))*B13</f>
-        <v>0</v>
-      </c>
-      <c r="F13" s="17" t="s">
-        <v>16</v>
-      </c>
-      <c r="G13" s="18">
-        <f>INDEX(TblBattlefieldFlt[[A]:[F]],MATCH($F13,TblBattlefieldFlt[Option],0),MATCH($G$3,TblBattlefieldFlt[[#Headers],[A]:[F]],0))</f>
-        <v>0</v>
-      </c>
-      <c r="H13" s="17">
-        <f>INDEX(TblShipPoints[Points],MATCH(F13,TblShipPoints[Ships],0))*G13</f>
-        <v>0</v>
-      </c>
-      <c r="I13" s="1"/>
-      <c r="J13" s="1"/>
-      <c r="K13" s="1"/>
-      <c r="L13" s="1"/>
-      <c r="M13" s="1"/>
-      <c r="N13" s="1"/>
-      <c r="O13" s="1"/>
-      <c r="P13" s="1"/>
-      <c r="Q13" s="7"/>
-      <c r="R13" s="1"/>
-      <c r="S13" s="7"/>
-    </row>
-    <row r="14" spans="1:19">
-      <c r="A14" s="17" t="s">
-        <v>17</v>
-      </c>
-      <c r="B14" s="18">
-        <f>INDEX(TblBattlefieldFlt[[A]:[F]],MATCH($A14,TblBattlefieldFlt[Option],0),MATCH($B$3,TblBattlefieldFlt[[#Headers],[A]:[F]],0))</f>
-        <v>0</v>
-      </c>
-      <c r="C14" s="17">
-        <f>INDEX(TblShipPoints[Points],MATCH(A14,TblShipPoints[Ships],0))*B14</f>
-        <v>0</v>
-      </c>
-      <c r="F14" s="17" t="s">
-        <v>17</v>
-      </c>
-      <c r="G14" s="18">
-        <f>INDEX(TblBattlefieldFlt[[A]:[F]],MATCH($F14,TblBattlefieldFlt[Option],0),MATCH($G$3,TblBattlefieldFlt[[#Headers],[A]:[F]],0))</f>
-        <v>10</v>
-      </c>
-      <c r="H14" s="17">
-        <f>INDEX(TblShipPoints[Points],MATCH(F14,TblShipPoints[Ships],0))*G14</f>
-        <v>5000</v>
-      </c>
-    </row>
-    <row r="16" spans="1:19">
-      <c r="A16" s="17" t="s">
-        <v>212</v>
-      </c>
-      <c r="B16" s="17" t="s">
-        <v>287</v>
-      </c>
-      <c r="C16" t="s">
-        <v>3</v>
-      </c>
-      <c r="F16" s="17" t="s">
-        <v>212</v>
-      </c>
-      <c r="G16" s="17" t="s">
-        <v>287</v>
-      </c>
-      <c r="H16" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8">
-      <c r="A17" s="17" t="s">
-        <v>4</v>
-      </c>
-      <c r="B17" s="18">
-        <f>SUMPRODUCT($B$10:$B$14,TblShipCrew[Service])</f>
-        <v>11</v>
-      </c>
-      <c r="C17">
-        <f>TblRoleControlValues[Service]*B17</f>
-        <v>1100</v>
-      </c>
-      <c r="F17" s="17" t="s">
-        <v>4</v>
-      </c>
-      <c r="G17" s="18">
-        <f>SUMPRODUCT($G$10:$G$14,TblShipCrew[Service])</f>
-        <v>15</v>
-      </c>
-      <c r="H17">
-        <f>TblRoleControlValues[Service]*G17</f>
-        <v>1500</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8">
-      <c r="A18" s="17" t="s">
-        <v>5</v>
-      </c>
-      <c r="B18" s="18">
-        <f>SUMPRODUCT($B$10:$B$14,TblShipCrew[Lieutenant])</f>
-        <v>3</v>
-      </c>
-      <c r="C18">
-        <f>TblRoleControlValues[Lieutenant]*B18</f>
-        <v>600</v>
-      </c>
-      <c r="F18" s="17" t="s">
-        <v>5</v>
-      </c>
-      <c r="G18" s="18">
-        <f>SUMPRODUCT($G$10:$G$14,TblShipCrew[Lieutenant])</f>
-        <v>1</v>
-      </c>
-      <c r="H18">
-        <f>TblRoleControlValues[Lieutenant]*G18</f>
-        <v>200</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8">
-      <c r="A19" s="17" t="s">
-        <v>6</v>
-      </c>
-      <c r="B19" s="18">
-        <f>SUMPRODUCT($B$10:$B$14,TblShipCrew[Captain])</f>
-        <v>1</v>
-      </c>
-      <c r="C19">
-        <f>TblRoleControlValues[Captain]*B19</f>
-        <v>300</v>
-      </c>
-      <c r="F19" s="17" t="s">
-        <v>6</v>
-      </c>
-      <c r="G19" s="18">
-        <f>SUMPRODUCT($G$10:$G$14,TblShipCrew[Captain])</f>
-        <v>1</v>
-      </c>
-      <c r="H19">
-        <f>TblRoleControlValues[Captain]*G19</f>
-        <v>300</v>
-      </c>
-    </row>
-  </sheetData>
-  <mergeCells count="2">
-    <mergeCell ref="A2:C2"/>
-    <mergeCell ref="F2:H2"/>
-  </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
Started first Ancient Cards
Started first Ancient Cards
</commit_message>
<xml_diff>
--- a/ShipCardGameCalcs.xlsx
+++ b/ShipCardGameCalcs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MultiplayerGame\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{D33C5C3D-8994-4A59-9ADC-34F4C96C60A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{EDEDB9CE-C3E6-46CD-ABB2-921E734D71CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="8" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="7" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Values" sheetId="1" r:id="rId1"/>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="593" uniqueCount="331">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="595" uniqueCount="333">
   <si>
     <t>Ship Parameters</t>
   </si>
@@ -1031,6 +1031,12 @@
   </si>
   <si>
     <t>Reduce target ships shield to 0</t>
+  </si>
+  <si>
+    <t>Ancient</t>
+  </si>
+  <si>
+    <t>If this card is to be sent to the Junkyard, place it on the bottom of the owners Strategy/Crew deck instead</t>
   </si>
   <si>
     <t>Special features</t>
@@ -1685,8 +1691,17 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1696,15 +1711,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -5924,13 +5930,13 @@
     </row>
     <row r="3" spans="1:19">
       <c r="A3" t="s">
-        <v>327</v>
+        <v>329</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>21</v>
       </c>
       <c r="F3" t="s">
-        <v>327</v>
+        <v>329</v>
       </c>
       <c r="G3" s="1" t="s">
         <v>26</v>
@@ -5954,14 +5960,14 @@
     </row>
     <row r="5" spans="1:19">
       <c r="A5" t="s">
-        <v>328</v>
+        <v>330</v>
       </c>
       <c r="B5">
         <f>SUM(C10:C14)</f>
         <v>5000</v>
       </c>
       <c r="F5" t="s">
-        <v>328</v>
+        <v>330</v>
       </c>
       <c r="G5">
         <f>SUM(H10:H14)</f>
@@ -5970,14 +5976,14 @@
     </row>
     <row r="6" spans="1:19">
       <c r="A6" t="s">
-        <v>329</v>
+        <v>331</v>
       </c>
       <c r="B6">
         <f>SUM(C17:C19)</f>
         <v>2000</v>
       </c>
       <c r="F6" t="s">
-        <v>329</v>
+        <v>331</v>
       </c>
       <c r="G6">
         <f>SUM(H17:H19)</f>
@@ -5999,7 +6005,7 @@
         <v>2</v>
       </c>
       <c r="B9" s="17" t="s">
-        <v>330</v>
+        <v>332</v>
       </c>
       <c r="C9" s="17" t="s">
         <v>3</v>
@@ -6008,7 +6014,7 @@
         <v>2</v>
       </c>
       <c r="G9" s="17" t="s">
-        <v>330</v>
+        <v>332</v>
       </c>
       <c r="H9" s="17" t="s">
         <v>3</v>
@@ -6198,7 +6204,7 @@
         <v>212</v>
       </c>
       <c r="B16" s="17" t="s">
-        <v>330</v>
+        <v>332</v>
       </c>
       <c r="C16" t="s">
         <v>3</v>
@@ -6207,7 +6213,7 @@
         <v>212</v>
       </c>
       <c r="G16" s="17" t="s">
-        <v>330</v>
+        <v>332</v>
       </c>
       <c r="H16" t="s">
         <v>3</v>
@@ -7300,13 +7306,13 @@
     <row r="16" spans="2:19">
       <c r="P16">
         <f ca="1">RANDBETWEEN(0,123)</f>
-        <v>106</v>
+        <v>109</v>
       </c>
     </row>
     <row r="17" spans="2:16">
       <c r="P17" s="46">
         <f ca="1">RANDBETWEEN(0,6)</f>
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="18" spans="2:16">
@@ -7766,7 +7772,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{93013FD4-B940-4A70-A7DA-BF82FD0F616E}">
   <dimension ref="A2:K81"/>
   <sheetViews>
-    <sheetView topLeftCell="A49" workbookViewId="0">
+    <sheetView topLeftCell="A34" workbookViewId="0">
       <selection activeCell="B64" sqref="B64"/>
     </sheetView>
   </sheetViews>
@@ -8311,7 +8317,7 @@
       </c>
     </row>
     <row r="3" spans="2:4" ht="106.5" customHeight="1">
-      <c r="B3" s="76" t="s">
+      <c r="B3" s="72" t="s">
         <v>212</v>
       </c>
       <c r="C3" s="70" t="s">
@@ -8322,28 +8328,28 @@
       </c>
     </row>
     <row r="4" spans="2:4" ht="106.5">
-      <c r="B4" s="77"/>
+      <c r="B4" s="73"/>
       <c r="C4" s="71"/>
       <c r="D4" s="29" t="s">
         <v>215</v>
       </c>
     </row>
     <row r="5" spans="2:4" ht="60.75">
-      <c r="B5" s="77"/>
+      <c r="B5" s="73"/>
       <c r="C5" s="71"/>
       <c r="D5" s="30" t="s">
         <v>216</v>
       </c>
     </row>
     <row r="6" spans="2:4" ht="75">
-      <c r="B6" s="77"/>
+      <c r="B6" s="73"/>
       <c r="C6" s="71"/>
       <c r="D6" s="30" t="s">
         <v>217</v>
       </c>
     </row>
     <row r="7" spans="2:4" ht="106.5">
-      <c r="B7" s="76" t="s">
+      <c r="B7" s="72" t="s">
         <v>218</v>
       </c>
       <c r="C7" s="70" t="s">
@@ -8354,14 +8360,14 @@
       </c>
     </row>
     <row r="8" spans="2:4" ht="90">
-      <c r="B8" s="77"/>
+      <c r="B8" s="73"/>
       <c r="C8" s="71"/>
       <c r="D8" s="30" t="s">
         <v>221</v>
       </c>
     </row>
     <row r="9" spans="2:4" ht="75">
-      <c r="B9" s="76" t="s">
+      <c r="B9" s="72" t="s">
         <v>222</v>
       </c>
       <c r="C9" s="70" t="s">
@@ -8372,14 +8378,14 @@
       </c>
     </row>
     <row r="10" spans="2:4" ht="60.75">
-      <c r="B10" s="78"/>
-      <c r="C10" s="72"/>
+      <c r="B10" s="75"/>
+      <c r="C10" s="74"/>
       <c r="D10" s="31" t="s">
         <v>225</v>
       </c>
     </row>
     <row r="11" spans="2:4" ht="76.5" customHeight="1">
-      <c r="B11" s="76" t="s">
+      <c r="B11" s="72" t="s">
         <v>226</v>
       </c>
       <c r="C11" s="70" t="s">
@@ -8390,14 +8396,14 @@
       </c>
     </row>
     <row r="12" spans="2:4" ht="30.75">
-      <c r="B12" s="77"/>
+      <c r="B12" s="73"/>
       <c r="C12" s="71"/>
       <c r="D12" s="31" t="s">
         <v>229</v>
       </c>
     </row>
     <row r="13" spans="2:4" ht="45.75">
-      <c r="B13" s="76" t="s">
+      <c r="B13" s="72" t="s">
         <v>230</v>
       </c>
       <c r="C13" s="70" t="s">
@@ -8408,28 +8414,28 @@
       </c>
     </row>
     <row r="14" spans="2:4" ht="30.75">
-      <c r="B14" s="77"/>
+      <c r="B14" s="73"/>
       <c r="C14" s="71"/>
       <c r="D14" s="31" t="s">
         <v>229</v>
       </c>
     </row>
     <row r="15" spans="2:4" ht="45.75">
-      <c r="B15" s="77"/>
+      <c r="B15" s="73"/>
       <c r="C15" s="71"/>
       <c r="D15" s="30" t="s">
         <v>233</v>
       </c>
     </row>
     <row r="16" spans="2:4" ht="60">
-      <c r="B16" s="77"/>
+      <c r="B16" s="73"/>
       <c r="C16" s="71"/>
       <c r="D16" s="30" t="s">
         <v>234</v>
       </c>
     </row>
     <row r="17" spans="2:4" ht="45">
-      <c r="B17" s="76" t="s">
+      <c r="B17" s="72" t="s">
         <v>235</v>
       </c>
       <c r="C17" s="70" t="s">
@@ -8440,14 +8446,14 @@
       </c>
     </row>
     <row r="18" spans="2:4" ht="45">
-      <c r="B18" s="77"/>
+      <c r="B18" s="73"/>
       <c r="C18" s="71"/>
       <c r="D18" s="30" t="s">
         <v>238</v>
       </c>
     </row>
     <row r="19" spans="2:4" ht="60.75" customHeight="1">
-      <c r="B19" s="76" t="s">
+      <c r="B19" s="72" t="s">
         <v>239</v>
       </c>
       <c r="C19" s="70" t="s">
@@ -8458,14 +8464,14 @@
       </c>
     </row>
     <row r="20" spans="2:4" ht="30.75">
-      <c r="B20" s="77"/>
+      <c r="B20" s="73"/>
       <c r="C20" s="71"/>
       <c r="D20" s="31" t="s">
         <v>229</v>
       </c>
     </row>
     <row r="21" spans="2:4" ht="45.75">
-      <c r="B21" s="76" t="s">
+      <c r="B21" s="72" t="s">
         <v>242</v>
       </c>
       <c r="C21" s="70" t="s">
@@ -8476,14 +8482,14 @@
       </c>
     </row>
     <row r="22" spans="2:4" ht="30.75">
-      <c r="B22" s="77"/>
+      <c r="B22" s="73"/>
       <c r="C22" s="71"/>
       <c r="D22" s="31" t="s">
         <v>229</v>
       </c>
     </row>
     <row r="23" spans="2:4" ht="62.25" customHeight="1">
-      <c r="B23" s="76" t="s">
+      <c r="B23" s="72" t="s">
         <v>245</v>
       </c>
       <c r="C23" s="70" t="s">
@@ -8494,21 +8500,21 @@
       </c>
     </row>
     <row r="24" spans="2:4" ht="62.25" customHeight="1">
-      <c r="B24" s="77"/>
+      <c r="B24" s="73"/>
       <c r="C24" s="71"/>
       <c r="D24" s="30" t="s">
         <v>248</v>
       </c>
     </row>
     <row r="25" spans="2:4" ht="30.75">
-      <c r="B25" s="78"/>
-      <c r="C25" s="72"/>
+      <c r="B25" s="75"/>
+      <c r="C25" s="74"/>
       <c r="D25" s="30" t="s">
         <v>229</v>
       </c>
     </row>
     <row r="26" spans="2:4" ht="45.75">
-      <c r="B26" s="76" t="s">
+      <c r="B26" s="72" t="s">
         <v>249</v>
       </c>
       <c r="C26" s="70" t="s">
@@ -8519,21 +8525,21 @@
       </c>
     </row>
     <row r="27" spans="2:4" ht="60.75">
-      <c r="B27" s="77"/>
+      <c r="B27" s="73"/>
       <c r="C27" s="71"/>
       <c r="D27" s="30" t="s">
         <v>248</v>
       </c>
     </row>
     <row r="28" spans="2:4" ht="30.75">
-      <c r="B28" s="77"/>
+      <c r="B28" s="73"/>
       <c r="C28" s="71"/>
       <c r="D28" s="30" t="s">
         <v>229</v>
       </c>
     </row>
     <row r="29" spans="2:4" ht="45.75">
-      <c r="B29" s="73" t="s">
+      <c r="B29" s="76" t="s">
         <v>251</v>
       </c>
       <c r="C29" s="70" t="s">
@@ -8544,28 +8550,28 @@
       </c>
     </row>
     <row r="30" spans="2:4" ht="60.75">
-      <c r="B30" s="74"/>
+      <c r="B30" s="77"/>
       <c r="C30" s="71"/>
       <c r="D30" s="30" t="s">
         <v>248</v>
       </c>
     </row>
     <row r="31" spans="2:4" ht="30.75">
-      <c r="B31" s="74"/>
+      <c r="B31" s="77"/>
       <c r="C31" s="71"/>
       <c r="D31" s="30" t="s">
         <v>229</v>
       </c>
     </row>
     <row r="32" spans="2:4" ht="60.75">
-      <c r="B32" s="74"/>
+      <c r="B32" s="77"/>
       <c r="C32" s="71"/>
       <c r="D32" s="30" t="s">
         <v>253</v>
       </c>
     </row>
     <row r="33" spans="2:4" ht="76.5" customHeight="1">
-      <c r="B33" s="73" t="s">
+      <c r="B33" s="76" t="s">
         <v>254</v>
       </c>
       <c r="C33" s="70" t="s">
@@ -8576,36 +8582,36 @@
       </c>
     </row>
     <row r="34" spans="2:4" ht="30.75">
-      <c r="B34" s="74"/>
+      <c r="B34" s="77"/>
       <c r="C34" s="71"/>
       <c r="D34" s="30" t="s">
         <v>257</v>
       </c>
     </row>
     <row r="35" spans="2:4" ht="30.75">
-      <c r="B35" s="74"/>
+      <c r="B35" s="77"/>
       <c r="C35" s="71"/>
       <c r="D35" s="30" t="s">
         <v>258</v>
       </c>
     </row>
     <row r="36" spans="2:4" ht="60.75">
-      <c r="B36" s="74"/>
+      <c r="B36" s="77"/>
       <c r="C36" s="71"/>
       <c r="D36" s="30" t="s">
         <v>259</v>
       </c>
     </row>
     <row r="37" spans="2:4" ht="137.25">
-      <c r="B37" s="74"/>
+      <c r="B37" s="77"/>
       <c r="C37" s="71"/>
       <c r="D37" s="30" t="s">
         <v>144</v>
       </c>
     </row>
     <row r="38" spans="2:4" ht="45.75">
-      <c r="B38" s="75"/>
-      <c r="C38" s="72"/>
+      <c r="B38" s="78"/>
+      <c r="C38" s="74"/>
       <c r="D38" s="31" t="s">
         <v>194</v>
       </c>
@@ -8615,6 +8621,14 @@
     </row>
   </sheetData>
   <mergeCells count="24">
+    <mergeCell ref="C33:C38"/>
+    <mergeCell ref="B33:B38"/>
+    <mergeCell ref="C29:C32"/>
+    <mergeCell ref="B29:B32"/>
+    <mergeCell ref="C23:C25"/>
+    <mergeCell ref="B23:B25"/>
+    <mergeCell ref="C26:C28"/>
+    <mergeCell ref="B26:B28"/>
     <mergeCell ref="C21:C22"/>
     <mergeCell ref="B21:B22"/>
     <mergeCell ref="C19:C20"/>
@@ -8631,14 +8645,6 @@
     <mergeCell ref="B13:B16"/>
     <mergeCell ref="C17:C18"/>
     <mergeCell ref="B17:B18"/>
-    <mergeCell ref="C33:C38"/>
-    <mergeCell ref="B33:B38"/>
-    <mergeCell ref="C29:C32"/>
-    <mergeCell ref="B29:B32"/>
-    <mergeCell ref="C23:C25"/>
-    <mergeCell ref="B23:B25"/>
-    <mergeCell ref="C26:C28"/>
-    <mergeCell ref="B26:B28"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -8649,7 +8655,7 @@
   <dimension ref="B3:J28"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="D25" sqref="D25"/>
+      <selection activeCell="C27" sqref="C27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -8935,7 +8941,12 @@
       </c>
     </row>
     <row r="26" spans="2:4">
-      <c r="B26" s="3"/>
+      <c r="B26" s="3" t="s">
+        <v>315</v>
+      </c>
+      <c r="C26" t="s">
+        <v>316</v>
+      </c>
     </row>
     <row r="27" spans="2:4">
       <c r="B27" s="3"/>
@@ -8974,49 +8985,49 @@
         <v>260</v>
       </c>
       <c r="D3" s="47" t="s">
-        <v>315</v>
+        <v>317</v>
       </c>
     </row>
     <row r="4" spans="2:4" ht="91.5">
       <c r="B4" s="55" t="s">
-        <v>316</v>
+        <v>318</v>
       </c>
       <c r="C4" s="54" t="s">
-        <v>317</v>
+        <v>319</v>
       </c>
       <c r="D4" s="54"/>
     </row>
     <row r="5" spans="2:4" ht="91.5">
       <c r="B5" s="55" t="s">
-        <v>318</v>
+        <v>320</v>
       </c>
       <c r="C5" s="54" t="s">
-        <v>319</v>
+        <v>321</v>
       </c>
       <c r="D5" s="54" t="s">
-        <v>320</v>
+        <v>322</v>
       </c>
     </row>
     <row r="6" spans="2:4" ht="76.5">
       <c r="B6" s="55" t="s">
-        <v>321</v>
+        <v>323</v>
       </c>
       <c r="C6" s="54" t="s">
-        <v>322</v>
+        <v>324</v>
       </c>
       <c r="D6" s="54" t="s">
-        <v>323</v>
+        <v>325</v>
       </c>
     </row>
     <row r="7" spans="2:4" ht="76.5">
       <c r="B7" s="55" t="s">
-        <v>324</v>
+        <v>326</v>
       </c>
       <c r="C7" s="54" t="s">
-        <v>325</v>
+        <v>327</v>
       </c>
       <c r="D7" s="54" t="s">
-        <v>326</v>
+        <v>328</v>
       </c>
     </row>
     <row r="8" spans="2:4">

</xml_diff>

<commit_message>
Added few more captain cards
Added few more captain cards
</commit_message>
<xml_diff>
--- a/ShipCardGameCalcs.xlsx
+++ b/ShipCardGameCalcs.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27230"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27307"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MultiplayerGame\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{EDEDB9CE-C3E6-46CD-ABB2-921E734D71CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{8A97E62D-71EF-464E-A7D9-4491D7CC38FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="7" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -946,7 +946,7 @@
     <t>Evasion</t>
   </si>
   <si>
-    <t>Evade attack when targetted</t>
+    <t>Evade X attacks when targetted during the battle phase</t>
   </si>
   <si>
     <t>Formation</t>
@@ -7306,13 +7306,13 @@
     <row r="16" spans="2:19">
       <c r="P16">
         <f ca="1">RANDBETWEEN(0,123)</f>
-        <v>109</v>
+        <v>44</v>
       </c>
     </row>
     <row r="17" spans="2:16">
       <c r="P17" s="46">
         <f ca="1">RANDBETWEEN(0,6)</f>
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="18" spans="2:16">
@@ -8294,7 +8294,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1CADF2F4-A124-44BC-8A72-4CE3F16F5D04}">
   <dimension ref="B2:D39"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A18" workbookViewId="0">
       <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
@@ -8654,8 +8654,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1914FF74-0E8B-4E92-8BDD-103E839E1854}">
   <dimension ref="B3:J28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="C27" sqref="C27"/>
+    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>

</xml_diff>

<commit_message>
Added Multiply and ship cards
Added Multiply and ship cards
</commit_message>
<xml_diff>
--- a/ShipCardGameCalcs.xlsx
+++ b/ShipCardGameCalcs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MultiplayerGame\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{46C53E0E-506E-4574-87A1-4DECB806DC73}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{03D89E1D-F14A-4765-81B9-B9E033D6D618}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="7" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="598" uniqueCount="335">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="600" uniqueCount="337">
   <si>
     <t>Ship Parameters</t>
   </si>
@@ -901,7 +901,7 @@
     <t>Swarm</t>
   </si>
   <si>
-    <t>Create X pod ship/s with 100 hull and can tap to deal 100 damage to enemy ship, they can also be used to block a gun slot</t>
+    <t>Create X pod ship/s with 100 hull and can engage to deal 100 damage to enemy ship, they can also be used to block a gun slot</t>
   </si>
   <si>
     <t>One to keep the enemy under pressure invading their ships during the early game. They will call for help from their swarm and become burtal in the early game, however during the late game they fall off.</t>
@@ -1043,6 +1043,12 @@
   </si>
   <si>
     <t>Deal Double damage</t>
+  </si>
+  <si>
+    <t>Multiply</t>
+  </si>
+  <si>
+    <t>Create a copy</t>
   </si>
   <si>
     <t>Special features</t>
@@ -1697,8 +1703,17 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1708,15 +1723,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -5936,13 +5942,13 @@
     </row>
     <row r="3" spans="1:19">
       <c r="A3" t="s">
-        <v>331</v>
+        <v>333</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>21</v>
       </c>
       <c r="F3" t="s">
-        <v>331</v>
+        <v>333</v>
       </c>
       <c r="G3" s="1" t="s">
         <v>26</v>
@@ -5966,14 +5972,14 @@
     </row>
     <row r="5" spans="1:19">
       <c r="A5" t="s">
-        <v>332</v>
+        <v>334</v>
       </c>
       <c r="B5">
         <f>SUM(C10:C14)</f>
         <v>5000</v>
       </c>
       <c r="F5" t="s">
-        <v>332</v>
+        <v>334</v>
       </c>
       <c r="G5">
         <f>SUM(H10:H14)</f>
@@ -5982,14 +5988,14 @@
     </row>
     <row r="6" spans="1:19">
       <c r="A6" t="s">
-        <v>333</v>
+        <v>335</v>
       </c>
       <c r="B6">
         <f>SUM(C17:C19)</f>
         <v>2000</v>
       </c>
       <c r="F6" t="s">
-        <v>333</v>
+        <v>335</v>
       </c>
       <c r="G6">
         <f>SUM(H17:H19)</f>
@@ -6011,7 +6017,7 @@
         <v>2</v>
       </c>
       <c r="B9" s="17" t="s">
-        <v>334</v>
+        <v>336</v>
       </c>
       <c r="C9" s="17" t="s">
         <v>3</v>
@@ -6020,7 +6026,7 @@
         <v>2</v>
       </c>
       <c r="G9" s="17" t="s">
-        <v>334</v>
+        <v>336</v>
       </c>
       <c r="H9" s="17" t="s">
         <v>3</v>
@@ -6210,7 +6216,7 @@
         <v>212</v>
       </c>
       <c r="B16" s="17" t="s">
-        <v>334</v>
+        <v>336</v>
       </c>
       <c r="C16" t="s">
         <v>3</v>
@@ -6219,7 +6225,7 @@
         <v>212</v>
       </c>
       <c r="G16" s="17" t="s">
-        <v>334</v>
+        <v>336</v>
       </c>
       <c r="H16" t="s">
         <v>3</v>
@@ -7312,13 +7318,13 @@
     <row r="16" spans="2:19">
       <c r="P16">
         <f ca="1">RANDBETWEEN(0,123)</f>
-        <v>121</v>
+        <v>90</v>
       </c>
     </row>
     <row r="17" spans="2:16">
       <c r="P17" s="46">
         <f ca="1">RANDBETWEEN(0,6)</f>
-        <v>6</v>
+        <v>1</v>
       </c>
     </row>
     <row r="18" spans="2:16">
@@ -7778,7 +7784,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{93013FD4-B940-4A70-A7DA-BF82FD0F616E}">
   <dimension ref="A2:K81"/>
   <sheetViews>
-    <sheetView topLeftCell="A34" workbookViewId="0">
+    <sheetView topLeftCell="A29" workbookViewId="0">
       <selection activeCell="H53" sqref="H53"/>
     </sheetView>
   </sheetViews>
@@ -8300,7 +8306,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1CADF2F4-A124-44BC-8A72-4CE3F16F5D04}">
   <dimension ref="B2:D39"/>
   <sheetViews>
-    <sheetView topLeftCell="G10" workbookViewId="0">
+    <sheetView topLeftCell="A10" workbookViewId="0">
       <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
@@ -8323,7 +8329,7 @@
       </c>
     </row>
     <row r="3" spans="2:4" ht="106.5" customHeight="1">
-      <c r="B3" s="76" t="s">
+      <c r="B3" s="72" t="s">
         <v>212</v>
       </c>
       <c r="C3" s="70" t="s">
@@ -8334,28 +8340,28 @@
       </c>
     </row>
     <row r="4" spans="2:4" ht="106.5">
-      <c r="B4" s="77"/>
+      <c r="B4" s="73"/>
       <c r="C4" s="71"/>
       <c r="D4" s="29" t="s">
         <v>215</v>
       </c>
     </row>
     <row r="5" spans="2:4" ht="60.75">
-      <c r="B5" s="77"/>
+      <c r="B5" s="73"/>
       <c r="C5" s="71"/>
       <c r="D5" s="30" t="s">
         <v>216</v>
       </c>
     </row>
     <row r="6" spans="2:4" ht="75">
-      <c r="B6" s="77"/>
+      <c r="B6" s="73"/>
       <c r="C6" s="71"/>
       <c r="D6" s="30" t="s">
         <v>217</v>
       </c>
     </row>
     <row r="7" spans="2:4" ht="106.5">
-      <c r="B7" s="76" t="s">
+      <c r="B7" s="72" t="s">
         <v>218</v>
       </c>
       <c r="C7" s="70" t="s">
@@ -8366,14 +8372,14 @@
       </c>
     </row>
     <row r="8" spans="2:4" ht="90">
-      <c r="B8" s="77"/>
+      <c r="B8" s="73"/>
       <c r="C8" s="71"/>
       <c r="D8" s="30" t="s">
         <v>221</v>
       </c>
     </row>
     <row r="9" spans="2:4" ht="75">
-      <c r="B9" s="76" t="s">
+      <c r="B9" s="72" t="s">
         <v>222</v>
       </c>
       <c r="C9" s="70" t="s">
@@ -8384,14 +8390,14 @@
       </c>
     </row>
     <row r="10" spans="2:4" ht="60.75">
-      <c r="B10" s="78"/>
-      <c r="C10" s="72"/>
+      <c r="B10" s="75"/>
+      <c r="C10" s="74"/>
       <c r="D10" s="31" t="s">
         <v>225</v>
       </c>
     </row>
     <row r="11" spans="2:4" ht="76.5" customHeight="1">
-      <c r="B11" s="76" t="s">
+      <c r="B11" s="72" t="s">
         <v>226</v>
       </c>
       <c r="C11" s="70" t="s">
@@ -8402,14 +8408,14 @@
       </c>
     </row>
     <row r="12" spans="2:4" ht="30.75">
-      <c r="B12" s="77"/>
+      <c r="B12" s="73"/>
       <c r="C12" s="71"/>
       <c r="D12" s="31" t="s">
         <v>229</v>
       </c>
     </row>
     <row r="13" spans="2:4" ht="45.75">
-      <c r="B13" s="76" t="s">
+      <c r="B13" s="72" t="s">
         <v>230</v>
       </c>
       <c r="C13" s="70" t="s">
@@ -8420,28 +8426,28 @@
       </c>
     </row>
     <row r="14" spans="2:4" ht="30.75">
-      <c r="B14" s="77"/>
+      <c r="B14" s="73"/>
       <c r="C14" s="71"/>
       <c r="D14" s="31" t="s">
         <v>229</v>
       </c>
     </row>
     <row r="15" spans="2:4" ht="45.75">
-      <c r="B15" s="77"/>
+      <c r="B15" s="73"/>
       <c r="C15" s="71"/>
       <c r="D15" s="30" t="s">
         <v>233</v>
       </c>
     </row>
     <row r="16" spans="2:4" ht="60">
-      <c r="B16" s="77"/>
+      <c r="B16" s="73"/>
       <c r="C16" s="71"/>
       <c r="D16" s="30" t="s">
         <v>234</v>
       </c>
     </row>
     <row r="17" spans="2:4" ht="45">
-      <c r="B17" s="76" t="s">
+      <c r="B17" s="72" t="s">
         <v>235</v>
       </c>
       <c r="C17" s="70" t="s">
@@ -8452,14 +8458,14 @@
       </c>
     </row>
     <row r="18" spans="2:4" ht="45">
-      <c r="B18" s="77"/>
+      <c r="B18" s="73"/>
       <c r="C18" s="71"/>
       <c r="D18" s="30" t="s">
         <v>238</v>
       </c>
     </row>
     <row r="19" spans="2:4" ht="60.75" customHeight="1">
-      <c r="B19" s="76" t="s">
+      <c r="B19" s="72" t="s">
         <v>239</v>
       </c>
       <c r="C19" s="70" t="s">
@@ -8470,14 +8476,14 @@
       </c>
     </row>
     <row r="20" spans="2:4" ht="30.75">
-      <c r="B20" s="77"/>
+      <c r="B20" s="73"/>
       <c r="C20" s="71"/>
       <c r="D20" s="31" t="s">
         <v>229</v>
       </c>
     </row>
     <row r="21" spans="2:4" ht="45.75">
-      <c r="B21" s="76" t="s">
+      <c r="B21" s="72" t="s">
         <v>242</v>
       </c>
       <c r="C21" s="70" t="s">
@@ -8488,14 +8494,14 @@
       </c>
     </row>
     <row r="22" spans="2:4" ht="30.75">
-      <c r="B22" s="77"/>
+      <c r="B22" s="73"/>
       <c r="C22" s="71"/>
       <c r="D22" s="31" t="s">
         <v>229</v>
       </c>
     </row>
     <row r="23" spans="2:4" ht="62.25" customHeight="1">
-      <c r="B23" s="76" t="s">
+      <c r="B23" s="72" t="s">
         <v>245</v>
       </c>
       <c r="C23" s="70" t="s">
@@ -8506,21 +8512,21 @@
       </c>
     </row>
     <row r="24" spans="2:4" ht="62.25" customHeight="1">
-      <c r="B24" s="77"/>
+      <c r="B24" s="73"/>
       <c r="C24" s="71"/>
       <c r="D24" s="30" t="s">
         <v>248</v>
       </c>
     </row>
     <row r="25" spans="2:4" ht="30.75">
-      <c r="B25" s="78"/>
-      <c r="C25" s="72"/>
+      <c r="B25" s="75"/>
+      <c r="C25" s="74"/>
       <c r="D25" s="30" t="s">
         <v>229</v>
       </c>
     </row>
     <row r="26" spans="2:4" ht="45.75">
-      <c r="B26" s="76" t="s">
+      <c r="B26" s="72" t="s">
         <v>249</v>
       </c>
       <c r="C26" s="70" t="s">
@@ -8531,21 +8537,21 @@
       </c>
     </row>
     <row r="27" spans="2:4" ht="60.75">
-      <c r="B27" s="77"/>
+      <c r="B27" s="73"/>
       <c r="C27" s="71"/>
       <c r="D27" s="30" t="s">
         <v>248</v>
       </c>
     </row>
     <row r="28" spans="2:4" ht="30.75">
-      <c r="B28" s="77"/>
+      <c r="B28" s="73"/>
       <c r="C28" s="71"/>
       <c r="D28" s="30" t="s">
         <v>229</v>
       </c>
     </row>
     <row r="29" spans="2:4" ht="45.75">
-      <c r="B29" s="73" t="s">
+      <c r="B29" s="76" t="s">
         <v>251</v>
       </c>
       <c r="C29" s="70" t="s">
@@ -8556,28 +8562,28 @@
       </c>
     </row>
     <row r="30" spans="2:4" ht="60.75">
-      <c r="B30" s="74"/>
+      <c r="B30" s="77"/>
       <c r="C30" s="71"/>
       <c r="D30" s="30" t="s">
         <v>248</v>
       </c>
     </row>
     <row r="31" spans="2:4" ht="30.75">
-      <c r="B31" s="74"/>
+      <c r="B31" s="77"/>
       <c r="C31" s="71"/>
       <c r="D31" s="30" t="s">
         <v>229</v>
       </c>
     </row>
     <row r="32" spans="2:4" ht="60.75">
-      <c r="B32" s="74"/>
+      <c r="B32" s="77"/>
       <c r="C32" s="71"/>
       <c r="D32" s="30" t="s">
         <v>253</v>
       </c>
     </row>
     <row r="33" spans="2:4" ht="76.5" customHeight="1">
-      <c r="B33" s="73" t="s">
+      <c r="B33" s="76" t="s">
         <v>254</v>
       </c>
       <c r="C33" s="70" t="s">
@@ -8588,36 +8594,36 @@
       </c>
     </row>
     <row r="34" spans="2:4" ht="30.75">
-      <c r="B34" s="74"/>
+      <c r="B34" s="77"/>
       <c r="C34" s="71"/>
       <c r="D34" s="30" t="s">
         <v>257</v>
       </c>
     </row>
     <row r="35" spans="2:4" ht="30.75">
-      <c r="B35" s="74"/>
+      <c r="B35" s="77"/>
       <c r="C35" s="71"/>
       <c r="D35" s="30" t="s">
         <v>258</v>
       </c>
     </row>
     <row r="36" spans="2:4" ht="60.75">
-      <c r="B36" s="74"/>
+      <c r="B36" s="77"/>
       <c r="C36" s="71"/>
       <c r="D36" s="30" t="s">
         <v>259</v>
       </c>
     </row>
     <row r="37" spans="2:4" ht="137.25">
-      <c r="B37" s="74"/>
+      <c r="B37" s="77"/>
       <c r="C37" s="71"/>
       <c r="D37" s="30" t="s">
         <v>144</v>
       </c>
     </row>
     <row r="38" spans="2:4" ht="45.75">
-      <c r="B38" s="75"/>
-      <c r="C38" s="72"/>
+      <c r="B38" s="78"/>
+      <c r="C38" s="74"/>
       <c r="D38" s="31" t="s">
         <v>194</v>
       </c>
@@ -8627,6 +8633,14 @@
     </row>
   </sheetData>
   <mergeCells count="24">
+    <mergeCell ref="C33:C38"/>
+    <mergeCell ref="B33:B38"/>
+    <mergeCell ref="C29:C32"/>
+    <mergeCell ref="B29:B32"/>
+    <mergeCell ref="C23:C25"/>
+    <mergeCell ref="B23:B25"/>
+    <mergeCell ref="C26:C28"/>
+    <mergeCell ref="B26:B28"/>
     <mergeCell ref="C21:C22"/>
     <mergeCell ref="B21:B22"/>
     <mergeCell ref="C19:C20"/>
@@ -8643,14 +8657,6 @@
     <mergeCell ref="B13:B16"/>
     <mergeCell ref="C17:C18"/>
     <mergeCell ref="B17:B18"/>
-    <mergeCell ref="C33:C38"/>
-    <mergeCell ref="B33:B38"/>
-    <mergeCell ref="C29:C32"/>
-    <mergeCell ref="B29:B32"/>
-    <mergeCell ref="C23:C25"/>
-    <mergeCell ref="B23:B25"/>
-    <mergeCell ref="C26:C28"/>
-    <mergeCell ref="B26:B28"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -8661,7 +8667,7 @@
   <dimension ref="B3:J28"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="C30" sqref="C30"/>
+      <selection activeCell="D28" sqref="D28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -8724,7 +8730,7 @@
       <c r="B6" s="3" t="s">
         <v>270</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C6" s="53" t="s">
         <v>271</v>
       </c>
       <c r="D6" t="s">
@@ -8966,7 +8972,12 @@
       </c>
     </row>
     <row r="28" spans="2:4">
-      <c r="B28" s="3"/>
+      <c r="B28" s="3" t="s">
+        <v>319</v>
+      </c>
+      <c r="C28" t="s">
+        <v>320</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -8999,49 +9010,49 @@
         <v>260</v>
       </c>
       <c r="D3" s="47" t="s">
-        <v>319</v>
+        <v>321</v>
       </c>
     </row>
     <row r="4" spans="2:4" ht="91.5">
       <c r="B4" s="55" t="s">
-        <v>320</v>
+        <v>322</v>
       </c>
       <c r="C4" s="54" t="s">
-        <v>321</v>
+        <v>323</v>
       </c>
       <c r="D4" s="54"/>
     </row>
     <row r="5" spans="2:4" ht="91.5">
       <c r="B5" s="55" t="s">
-        <v>322</v>
+        <v>324</v>
       </c>
       <c r="C5" s="54" t="s">
-        <v>323</v>
+        <v>325</v>
       </c>
       <c r="D5" s="54" t="s">
-        <v>324</v>
+        <v>326</v>
       </c>
     </row>
     <row r="6" spans="2:4" ht="76.5">
       <c r="B6" s="55" t="s">
-        <v>325</v>
+        <v>327</v>
       </c>
       <c r="C6" s="54" t="s">
-        <v>326</v>
+        <v>328</v>
       </c>
       <c r="D6" s="54" t="s">
-        <v>327</v>
+        <v>329</v>
       </c>
     </row>
     <row r="7" spans="2:4" ht="76.5">
       <c r="B7" s="55" t="s">
-        <v>328</v>
+        <v>330</v>
       </c>
       <c r="C7" s="54" t="s">
-        <v>329</v>
+        <v>331</v>
       </c>
       <c r="D7" s="54" t="s">
-        <v>330</v>
+        <v>332</v>
       </c>
     </row>
     <row r="8" spans="2:4">

</xml_diff>

<commit_message>
Hit 300 card designs and 20 ship card designs
Hit 300 card designs and 20 ship card designs, including various mechanics added and tweaked as well as existing card changes
</commit_message>
<xml_diff>
--- a/ShipCardGameCalcs.xlsx
+++ b/ShipCardGameCalcs.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27307"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27321"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MultiplayerGame\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{03D89E1D-F14A-4765-81B9-B9E033D6D618}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{4E65C079-02EE-4F6D-9EE7-E529B63EEBE3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="7" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="600" uniqueCount="337">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="614" uniqueCount="350">
   <si>
     <t>Ship Parameters</t>
   </si>
@@ -685,6 +685,9 @@
     <t>Now the turn gets moved to the next player on your left and they start their Disengage phase.</t>
   </si>
   <si>
+    <t>Currently Max hand size 8</t>
+  </si>
+  <si>
     <t>Controlled deck is the battlefield conditions which affects the battlefield</t>
   </si>
   <si>
@@ -841,12 +844,18 @@
     <t>Played to the field that has a mission that any player can do and gain the rewards for</t>
   </si>
   <si>
+    <t>You can play as many Galaxy Mission cards as long as you can pay their cost</t>
+  </si>
+  <si>
     <t>Dangerous Mission</t>
   </si>
   <si>
     <t>Played to the field that has a mission only the player who played it can do and gain the rewards for, however after a certain amount of turns it will have consequences</t>
   </si>
   <si>
+    <t>You can play as many Dangerous Mission cards as long as you can pay their cost</t>
+  </si>
+  <si>
     <t>If the missions runs out of turns the it will activate the consequence affect and then get sent to the scrapyard</t>
   </si>
   <si>
@@ -904,7 +913,7 @@
     <t>Create X pod ship/s with 100 hull and can engage to deal 100 damage to enemy ship, they can also be used to block a gun slot</t>
   </si>
   <si>
-    <t>One to keep the enemy under pressure invading their ships during the early game. They will call for help from their swarm and become burtal in the early game, however during the late game they fall off.</t>
+    <t>One to keep the enemy under pressure invading their ships during the early game. They will call for help from their swarm and become brutal in the early game, however during the late game they fall off.</t>
   </si>
   <si>
     <t>Infection</t>
@@ -925,7 +934,7 @@
     <t>To Engage a card the player must turn the card 90 degrees. Once this is done the card can't engage again until they are turned back facing the correct way. This can happen during the Disengage phase</t>
   </si>
   <si>
-    <t>Being most knowledgable to get the cards they want when they need it using it to deal a lot of damage with cosmic cards. They are known for their mid/late game</t>
+    <t>Being most knowledgable to get the cards they want when they need it using it to deal a lot of damage with cosmic cards and cosmic creatures. They are known for their mid/late game</t>
   </si>
   <si>
     <t>Disengage</t>
@@ -952,7 +961,7 @@
     <t>Formation</t>
   </si>
   <si>
-    <t>When multiple of your ships attack</t>
+    <t>When X or more of your ships attack</t>
   </si>
   <si>
     <t>Repair</t>
@@ -979,7 +988,7 @@
     <t>View cards on top of your Strategy deck, pick X amount to place in your hand and put the rest in any order on top of your strategy deck</t>
   </si>
   <si>
-    <t>Disease spread</t>
+    <t>Viral Sabotage</t>
   </si>
   <si>
     <t>Deal X damage to assigned ship when this crew member is Engaged</t>
@@ -1049,6 +1058,36 @@
   </si>
   <si>
     <t>Create a copy</t>
+  </si>
+  <si>
+    <t>Crew Promotion</t>
+  </si>
+  <si>
+    <t>Upgrade X crew card/s by looking through your crew deck for the next tier up. Then play the new crew card in place of the upgrade crew. Shuffle your crew deck and send the original to stasis.</t>
+  </si>
+  <si>
+    <t>Cosmic Creatures</t>
+  </si>
+  <si>
+    <t>Create x Health and X damage Creature with effect cosmic energy</t>
+  </si>
+  <si>
+    <t>Cosmic Energy</t>
+  </si>
+  <si>
+    <t>Any excess damage hits next ship</t>
+  </si>
+  <si>
+    <t>Cloak</t>
+  </si>
+  <si>
+    <t xml:space="preserve">the Ship and its assigned crew, attachments can't be the target. If an assigned crew member on the cloaked ship is engaged or disengaged or if the player uses a department dice then the ship loses Cloak </t>
+  </si>
+  <si>
+    <t>Velocity Precision</t>
+  </si>
+  <si>
+    <t>Enemy ships can't maneuver in front of this ships target</t>
   </si>
   <si>
     <t>Special features</t>
@@ -1104,7 +1143,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
-  <fonts count="10">
+  <fonts count="11">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1176,6 +1215,13 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="10">
@@ -1548,7 +1594,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="79">
+  <cellXfs count="80">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1667,6 +1713,7 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1703,17 +1750,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1723,6 +1761,15 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -3860,21 +3907,21 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17">
-      <c r="A1" s="60" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="60"/>
-      <c r="C1" s="60"/>
-      <c r="D1" s="60"/>
-      <c r="E1" s="60"/>
-      <c r="F1" s="60"/>
-      <c r="G1" s="60"/>
-      <c r="H1" s="60"/>
-      <c r="N1" s="60" t="s">
+      <c r="A1" s="61" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="61"/>
+      <c r="C1" s="61"/>
+      <c r="D1" s="61"/>
+      <c r="E1" s="61"/>
+      <c r="F1" s="61"/>
+      <c r="G1" s="61"/>
+      <c r="H1" s="61"/>
+      <c r="N1" s="61" t="s">
         <v>1</v>
       </c>
-      <c r="O1" s="60"/>
-      <c r="P1" s="60"/>
+      <c r="O1" s="61"/>
+      <c r="P1" s="61"/>
     </row>
     <row r="2" spans="1:17">
       <c r="A2" s="9" t="s">
@@ -4141,25 +4188,25 @@
       </c>
     </row>
     <row r="8" spans="1:17">
-      <c r="A8" s="60" t="s">
+      <c r="A8" s="61" t="s">
         <v>18</v>
       </c>
-      <c r="B8" s="60"/>
-      <c r="C8" s="60"/>
-      <c r="D8" s="60"/>
-      <c r="E8" s="60"/>
-      <c r="F8" s="60"/>
-      <c r="G8" s="60"/>
-      <c r="J8" s="60" t="s">
+      <c r="B8" s="61"/>
+      <c r="C8" s="61"/>
+      <c r="D8" s="61"/>
+      <c r="E8" s="61"/>
+      <c r="F8" s="61"/>
+      <c r="G8" s="61"/>
+      <c r="J8" s="61" t="s">
         <v>19</v>
       </c>
-      <c r="K8" s="60"/>
-      <c r="L8" s="60"/>
-      <c r="M8" s="60"/>
-      <c r="N8" s="60"/>
-      <c r="O8" s="60"/>
-      <c r="P8" s="60"/>
-      <c r="Q8" s="60"/>
+      <c r="K8" s="61"/>
+      <c r="L8" s="61"/>
+      <c r="M8" s="61"/>
+      <c r="N8" s="61"/>
+      <c r="O8" s="61"/>
+      <c r="P8" s="61"/>
+      <c r="Q8" s="61"/>
     </row>
     <row r="9" spans="1:17">
       <c r="A9" s="8" t="s">
@@ -4499,15 +4546,15 @@
       <c r="Q15" s="1"/>
     </row>
     <row r="16" spans="1:17">
-      <c r="A16" s="60" t="s">
+      <c r="A16" s="61" t="s">
         <v>35</v>
       </c>
-      <c r="B16" s="60"/>
-      <c r="C16" s="60"/>
-      <c r="D16" s="60"/>
-      <c r="E16" s="60"/>
-      <c r="F16" s="60"/>
-      <c r="G16" s="60"/>
+      <c r="B16" s="61"/>
+      <c r="C16" s="61"/>
+      <c r="D16" s="61"/>
+      <c r="E16" s="61"/>
+      <c r="F16" s="61"/>
+      <c r="G16" s="61"/>
       <c r="K16" s="1"/>
       <c r="L16" s="1"/>
       <c r="M16" s="1"/>
@@ -4724,27 +4771,27 @@
       <c r="R22" s="4"/>
     </row>
     <row r="23" spans="1:18">
-      <c r="A23" s="60" t="s">
+      <c r="A23" s="61" t="s">
         <v>40</v>
       </c>
-      <c r="B23" s="60"/>
-      <c r="C23" s="60"/>
-      <c r="D23" s="60"/>
-      <c r="E23" s="60"/>
-      <c r="F23" s="60"/>
-      <c r="G23" s="60"/>
-      <c r="H23" s="60"/>
+      <c r="B23" s="61"/>
+      <c r="C23" s="61"/>
+      <c r="D23" s="61"/>
+      <c r="E23" s="61"/>
+      <c r="F23" s="61"/>
+      <c r="G23" s="61"/>
+      <c r="H23" s="61"/>
       <c r="I23" s="4"/>
-      <c r="J23" s="60" t="s">
+      <c r="J23" s="61" t="s">
         <v>41</v>
       </c>
-      <c r="K23" s="60"/>
-      <c r="L23" s="60"/>
-      <c r="M23" s="60"/>
-      <c r="N23" s="60"/>
-      <c r="O23" s="60"/>
-      <c r="P23" s="60"/>
-      <c r="Q23" s="60"/>
+      <c r="K23" s="61"/>
+      <c r="L23" s="61"/>
+      <c r="M23" s="61"/>
+      <c r="N23" s="61"/>
+      <c r="O23" s="61"/>
+      <c r="P23" s="61"/>
+      <c r="Q23" s="61"/>
     </row>
     <row r="24" spans="1:18">
       <c r="A24" s="8" t="s">
@@ -5172,25 +5219,25 @@
       <c r="Q30" s="1"/>
     </row>
     <row r="31" spans="1:18">
-      <c r="A31" s="60" t="s">
+      <c r="A31" s="61" t="s">
         <v>47</v>
       </c>
-      <c r="B31" s="60"/>
-      <c r="C31" s="60"/>
-      <c r="D31" s="60"/>
-      <c r="E31" s="60"/>
-      <c r="F31" s="60"/>
-      <c r="G31" s="60"/>
+      <c r="B31" s="61"/>
+      <c r="C31" s="61"/>
+      <c r="D31" s="61"/>
+      <c r="E31" s="61"/>
+      <c r="F31" s="61"/>
+      <c r="G31" s="61"/>
       <c r="I31" s="4"/>
-      <c r="J31" s="60" t="s">
+      <c r="J31" s="61" t="s">
         <v>48</v>
       </c>
-      <c r="K31" s="60"/>
-      <c r="L31" s="60"/>
-      <c r="M31" s="60"/>
-      <c r="N31" s="60"/>
-      <c r="O31" s="60"/>
-      <c r="P31" s="60"/>
+      <c r="K31" s="61"/>
+      <c r="L31" s="61"/>
+      <c r="M31" s="61"/>
+      <c r="N31" s="61"/>
+      <c r="O31" s="61"/>
+      <c r="P31" s="61"/>
     </row>
     <row r="32" spans="1:18">
       <c r="A32" t="s">
@@ -5929,26 +5976,26 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:19">
-      <c r="A2" s="60" t="s">
+      <c r="A2" s="61" t="s">
         <v>165</v>
       </c>
-      <c r="B2" s="60"/>
-      <c r="C2" s="60"/>
-      <c r="F2" s="60" t="s">
+      <c r="B2" s="61"/>
+      <c r="C2" s="61"/>
+      <c r="F2" s="61" t="s">
         <v>170</v>
       </c>
-      <c r="G2" s="60"/>
-      <c r="H2" s="60"/>
+      <c r="G2" s="61"/>
+      <c r="H2" s="61"/>
     </row>
     <row r="3" spans="1:19">
       <c r="A3" t="s">
-        <v>333</v>
+        <v>346</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>21</v>
       </c>
       <c r="F3" t="s">
-        <v>333</v>
+        <v>346</v>
       </c>
       <c r="G3" s="1" t="s">
         <v>26</v>
@@ -5972,14 +6019,14 @@
     </row>
     <row r="5" spans="1:19">
       <c r="A5" t="s">
-        <v>334</v>
+        <v>347</v>
       </c>
       <c r="B5">
         <f>SUM(C10:C14)</f>
         <v>5000</v>
       </c>
       <c r="F5" t="s">
-        <v>334</v>
+        <v>347</v>
       </c>
       <c r="G5">
         <f>SUM(H10:H14)</f>
@@ -5988,14 +6035,14 @@
     </row>
     <row r="6" spans="1:19">
       <c r="A6" t="s">
-        <v>335</v>
+        <v>348</v>
       </c>
       <c r="B6">
         <f>SUM(C17:C19)</f>
         <v>2000</v>
       </c>
       <c r="F6" t="s">
-        <v>335</v>
+        <v>348</v>
       </c>
       <c r="G6">
         <f>SUM(H17:H19)</f>
@@ -6017,7 +6064,7 @@
         <v>2</v>
       </c>
       <c r="B9" s="17" t="s">
-        <v>336</v>
+        <v>349</v>
       </c>
       <c r="C9" s="17" t="s">
         <v>3</v>
@@ -6026,7 +6073,7 @@
         <v>2</v>
       </c>
       <c r="G9" s="17" t="s">
-        <v>336</v>
+        <v>349</v>
       </c>
       <c r="H9" s="17" t="s">
         <v>3</v>
@@ -6213,19 +6260,19 @@
     </row>
     <row r="16" spans="1:19">
       <c r="A16" s="17" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="B16" s="17" t="s">
-        <v>336</v>
+        <v>349</v>
       </c>
       <c r="C16" t="s">
         <v>3</v>
       </c>
       <c r="F16" s="17" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="G16" s="17" t="s">
-        <v>336</v>
+        <v>349</v>
       </c>
       <c r="H16" t="s">
         <v>3</v>
@@ -6316,8 +6363,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{91273792-62E9-442E-9CC7-E8C6E6BD4008}">
   <dimension ref="B1:V32"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
+    <sheetView topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -7318,13 +7365,13 @@
     <row r="16" spans="2:19">
       <c r="P16">
         <f ca="1">RANDBETWEEN(0,123)</f>
-        <v>90</v>
+        <v>64</v>
       </c>
     </row>
     <row r="17" spans="2:16">
       <c r="P17" s="46">
         <f ca="1">RANDBETWEEN(0,6)</f>
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="18" spans="2:16">
@@ -7420,8 +7467,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F5EC53A5-8F19-4711-93EA-0F4CBD261EC8}">
   <dimension ref="B2:B83"/>
   <sheetViews>
-    <sheetView topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="H25" sqref="H25"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H24" sqref="H24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -7782,10 +7829,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{93013FD4-B940-4A70-A7DA-BF82FD0F616E}">
-  <dimension ref="A2:K81"/>
+  <dimension ref="A2:K82"/>
   <sheetViews>
-    <sheetView topLeftCell="A29" workbookViewId="0">
-      <selection activeCell="H53" sqref="H53"/>
+    <sheetView topLeftCell="A51" workbookViewId="0">
+      <selection activeCell="I83" sqref="I83"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -7887,14 +7934,14 @@
         <v>75</v>
       </c>
       <c r="C23" s="48"/>
-      <c r="D23" s="61" t="s">
+      <c r="D23" s="62" t="s">
         <v>166</v>
       </c>
-      <c r="E23" s="62"/>
-      <c r="F23" s="62"/>
-      <c r="G23" s="62"/>
-      <c r="H23" s="62"/>
-      <c r="I23" s="63"/>
+      <c r="E23" s="63"/>
+      <c r="F23" s="63"/>
+      <c r="G23" s="63"/>
+      <c r="H23" s="63"/>
+      <c r="I23" s="64"/>
       <c r="J23" s="48"/>
       <c r="K23" s="50" t="s">
         <v>167</v>
@@ -7903,24 +7950,24 @@
     <row r="24" spans="1:11">
       <c r="B24" s="48"/>
       <c r="C24" s="48"/>
-      <c r="D24" s="64"/>
-      <c r="E24" s="65"/>
-      <c r="F24" s="65"/>
-      <c r="G24" s="65"/>
-      <c r="H24" s="65"/>
-      <c r="I24" s="66"/>
+      <c r="D24" s="65"/>
+      <c r="E24" s="66"/>
+      <c r="F24" s="66"/>
+      <c r="G24" s="66"/>
+      <c r="H24" s="66"/>
+      <c r="I24" s="67"/>
       <c r="J24" s="48"/>
       <c r="K24" s="48"/>
     </row>
     <row r="25" spans="1:11">
       <c r="B25" s="48"/>
       <c r="C25" s="48"/>
-      <c r="D25" s="64"/>
-      <c r="E25" s="65"/>
-      <c r="F25" s="65"/>
-      <c r="G25" s="65"/>
-      <c r="H25" s="65"/>
-      <c r="I25" s="66"/>
+      <c r="D25" s="65"/>
+      <c r="E25" s="66"/>
+      <c r="F25" s="66"/>
+      <c r="G25" s="66"/>
+      <c r="H25" s="66"/>
+      <c r="I25" s="67"/>
       <c r="J25" s="48"/>
       <c r="K25" s="48"/>
     </row>
@@ -7929,12 +7976,12 @@
         <v>77</v>
       </c>
       <c r="C26" s="48"/>
-      <c r="D26" s="64"/>
-      <c r="E26" s="65"/>
-      <c r="F26" s="65"/>
-      <c r="G26" s="65"/>
-      <c r="H26" s="65"/>
-      <c r="I26" s="66"/>
+      <c r="D26" s="65"/>
+      <c r="E26" s="66"/>
+      <c r="F26" s="66"/>
+      <c r="G26" s="66"/>
+      <c r="H26" s="66"/>
+      <c r="I26" s="67"/>
       <c r="J26" s="48"/>
       <c r="K26" s="50" t="s">
         <v>168</v>
@@ -7943,12 +7990,12 @@
     <row r="27" spans="1:11">
       <c r="B27" s="48"/>
       <c r="C27" s="48"/>
-      <c r="D27" s="64"/>
-      <c r="E27" s="65"/>
-      <c r="F27" s="65"/>
-      <c r="G27" s="65"/>
-      <c r="H27" s="65"/>
-      <c r="I27" s="66"/>
+      <c r="D27" s="65"/>
+      <c r="E27" s="66"/>
+      <c r="F27" s="66"/>
+      <c r="G27" s="66"/>
+      <c r="H27" s="66"/>
+      <c r="I27" s="67"/>
       <c r="J27" s="48"/>
       <c r="K27" s="48"/>
     </row>
@@ -7957,26 +8004,26 @@
         <v>169</v>
       </c>
       <c r="C28" s="49"/>
-      <c r="D28" s="67"/>
-      <c r="E28" s="68"/>
-      <c r="F28" s="68"/>
-      <c r="G28" s="68"/>
-      <c r="H28" s="68"/>
-      <c r="I28" s="69"/>
+      <c r="D28" s="68"/>
+      <c r="E28" s="69"/>
+      <c r="F28" s="69"/>
+      <c r="G28" s="69"/>
+      <c r="H28" s="69"/>
+      <c r="I28" s="70"/>
       <c r="J28" s="49"/>
       <c r="K28" s="48"/>
     </row>
     <row r="29" spans="1:11">
       <c r="B29" s="48"/>
       <c r="C29" s="48"/>
-      <c r="D29" s="61" t="s">
+      <c r="D29" s="62" t="s">
         <v>166</v>
       </c>
-      <c r="E29" s="62"/>
-      <c r="F29" s="62"/>
-      <c r="G29" s="62"/>
-      <c r="H29" s="62"/>
-      <c r="I29" s="63"/>
+      <c r="E29" s="63"/>
+      <c r="F29" s="63"/>
+      <c r="G29" s="63"/>
+      <c r="H29" s="63"/>
+      <c r="I29" s="64"/>
       <c r="J29" s="48"/>
       <c r="K29" s="50" t="s">
         <v>169</v>
@@ -7985,12 +8032,12 @@
     <row r="30" spans="1:11">
       <c r="B30" s="48"/>
       <c r="C30" s="48"/>
-      <c r="D30" s="64"/>
-      <c r="E30" s="65"/>
-      <c r="F30" s="65"/>
-      <c r="G30" s="65"/>
-      <c r="H30" s="65"/>
-      <c r="I30" s="66"/>
+      <c r="D30" s="65"/>
+      <c r="E30" s="66"/>
+      <c r="F30" s="66"/>
+      <c r="G30" s="66"/>
+      <c r="H30" s="66"/>
+      <c r="I30" s="67"/>
       <c r="J30" s="48"/>
       <c r="K30" s="48"/>
     </row>
@@ -7999,12 +8046,12 @@
         <v>168</v>
       </c>
       <c r="C31" s="48"/>
-      <c r="D31" s="64"/>
-      <c r="E31" s="65"/>
-      <c r="F31" s="65"/>
-      <c r="G31" s="65"/>
-      <c r="H31" s="65"/>
-      <c r="I31" s="66"/>
+      <c r="D31" s="65"/>
+      <c r="E31" s="66"/>
+      <c r="F31" s="66"/>
+      <c r="G31" s="66"/>
+      <c r="H31" s="66"/>
+      <c r="I31" s="67"/>
       <c r="J31" s="48"/>
       <c r="K31" s="50" t="s">
         <v>77</v>
@@ -8013,24 +8060,24 @@
     <row r="32" spans="1:11">
       <c r="B32" s="48"/>
       <c r="C32" s="48"/>
-      <c r="D32" s="64"/>
-      <c r="E32" s="65"/>
-      <c r="F32" s="65"/>
-      <c r="G32" s="65"/>
-      <c r="H32" s="65"/>
-      <c r="I32" s="66"/>
+      <c r="D32" s="65"/>
+      <c r="E32" s="66"/>
+      <c r="F32" s="66"/>
+      <c r="G32" s="66"/>
+      <c r="H32" s="66"/>
+      <c r="I32" s="67"/>
       <c r="J32" s="48"/>
       <c r="K32" s="48"/>
     </row>
     <row r="33" spans="1:11">
       <c r="B33" s="48"/>
       <c r="C33" s="48"/>
-      <c r="D33" s="64"/>
-      <c r="E33" s="65"/>
-      <c r="F33" s="65"/>
-      <c r="G33" s="65"/>
-      <c r="H33" s="65"/>
-      <c r="I33" s="66"/>
+      <c r="D33" s="65"/>
+      <c r="E33" s="66"/>
+      <c r="F33" s="66"/>
+      <c r="G33" s="66"/>
+      <c r="H33" s="66"/>
+      <c r="I33" s="67"/>
       <c r="J33" s="48"/>
       <c r="K33" s="48"/>
     </row>
@@ -8042,12 +8089,12 @@
         <v>167</v>
       </c>
       <c r="C34" s="48"/>
-      <c r="D34" s="67"/>
-      <c r="E34" s="68"/>
-      <c r="F34" s="68"/>
-      <c r="G34" s="68"/>
-      <c r="H34" s="68"/>
-      <c r="I34" s="69"/>
+      <c r="D34" s="68"/>
+      <c r="E34" s="69"/>
+      <c r="F34" s="69"/>
+      <c r="G34" s="69"/>
+      <c r="H34" s="69"/>
+      <c r="I34" s="70"/>
       <c r="J34" s="48"/>
       <c r="K34" s="50" t="s">
         <v>75</v>
@@ -8226,6 +8273,11 @@
     <row r="81" spans="2:2">
       <c r="B81" t="s">
         <v>198</v>
+      </c>
+    </row>
+    <row r="82" spans="2:2">
+      <c r="B82" t="s">
+        <v>199</v>
       </c>
     </row>
   </sheetData>
@@ -8249,52 +8301,52 @@
   <sheetData>
     <row r="2" spans="2:2">
       <c r="B2" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
     </row>
     <row r="3" spans="2:2">
       <c r="B3" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
     </row>
     <row r="4" spans="2:2">
       <c r="B4" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
     </row>
     <row r="5" spans="2:2">
       <c r="B5" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
     </row>
     <row r="6" spans="2:2">
       <c r="B6" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
     </row>
     <row r="7" spans="2:2">
       <c r="B7" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
     </row>
     <row r="8" spans="2:2">
       <c r="B8" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
     </row>
     <row r="9" spans="2:2">
       <c r="B9" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
     </row>
     <row r="10" spans="2:2">
       <c r="B10" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
     </row>
     <row r="11" spans="2:2">
       <c r="B11" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
     </row>
   </sheetData>
@@ -8306,8 +8358,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1CADF2F4-A124-44BC-8A72-4CE3F16F5D04}">
   <dimension ref="B2:D39"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+    <sheetView topLeftCell="A23" workbookViewId="0">
+      <selection activeCell="D27" sqref="D27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -8319,311 +8371,311 @@
   <sheetData>
     <row r="2" spans="2:4">
       <c r="B2" s="32" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="C2" s="32" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="D2" s="32" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
     </row>
     <row r="3" spans="2:4" ht="106.5" customHeight="1">
-      <c r="B3" s="72" t="s">
-        <v>212</v>
-      </c>
-      <c r="C3" s="70" t="s">
+      <c r="B3" s="77" t="s">
         <v>213</v>
       </c>
+      <c r="C3" s="71" t="s">
+        <v>214</v>
+      </c>
       <c r="D3" s="28" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
     </row>
     <row r="4" spans="2:4" ht="106.5">
-      <c r="B4" s="73"/>
-      <c r="C4" s="71"/>
+      <c r="B4" s="78"/>
+      <c r="C4" s="72"/>
       <c r="D4" s="29" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
     </row>
     <row r="5" spans="2:4" ht="60.75">
-      <c r="B5" s="73"/>
-      <c r="C5" s="71"/>
+      <c r="B5" s="78"/>
+      <c r="C5" s="72"/>
       <c r="D5" s="30" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
     </row>
     <row r="6" spans="2:4" ht="75">
-      <c r="B6" s="73"/>
-      <c r="C6" s="71"/>
+      <c r="B6" s="78"/>
+      <c r="C6" s="72"/>
       <c r="D6" s="30" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
     </row>
     <row r="7" spans="2:4" ht="106.5">
-      <c r="B7" s="72" t="s">
-        <v>218</v>
-      </c>
-      <c r="C7" s="70" t="s">
+      <c r="B7" s="77" t="s">
         <v>219</v>
       </c>
+      <c r="C7" s="71" t="s">
+        <v>220</v>
+      </c>
       <c r="D7" s="28" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
     </row>
     <row r="8" spans="2:4" ht="90">
-      <c r="B8" s="73"/>
-      <c r="C8" s="71"/>
+      <c r="B8" s="78"/>
+      <c r="C8" s="72"/>
       <c r="D8" s="30" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
     </row>
     <row r="9" spans="2:4" ht="75">
-      <c r="B9" s="72" t="s">
-        <v>222</v>
-      </c>
-      <c r="C9" s="70" t="s">
+      <c r="B9" s="77" t="s">
         <v>223</v>
       </c>
+      <c r="C9" s="71" t="s">
+        <v>224</v>
+      </c>
       <c r="D9" s="28" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
     </row>
     <row r="10" spans="2:4" ht="60.75">
-      <c r="B10" s="75"/>
-      <c r="C10" s="74"/>
+      <c r="B10" s="79"/>
+      <c r="C10" s="73"/>
       <c r="D10" s="31" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
     </row>
     <row r="11" spans="2:4" ht="76.5" customHeight="1">
-      <c r="B11" s="72" t="s">
-        <v>226</v>
-      </c>
-      <c r="C11" s="70" t="s">
+      <c r="B11" s="77" t="s">
         <v>227</v>
       </c>
+      <c r="C11" s="71" t="s">
+        <v>228</v>
+      </c>
       <c r="D11" s="28" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
     </row>
     <row r="12" spans="2:4" ht="30.75">
-      <c r="B12" s="73"/>
-      <c r="C12" s="71"/>
+      <c r="B12" s="78"/>
+      <c r="C12" s="72"/>
       <c r="D12" s="31" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
     </row>
     <row r="13" spans="2:4" ht="45.75">
-      <c r="B13" s="72" t="s">
+      <c r="B13" s="77" t="s">
+        <v>231</v>
+      </c>
+      <c r="C13" s="71" t="s">
+        <v>232</v>
+      </c>
+      <c r="D13" s="28" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="14" spans="2:4" ht="30.75">
+      <c r="B14" s="78"/>
+      <c r="C14" s="72"/>
+      <c r="D14" s="31" t="s">
         <v>230</v>
       </c>
-      <c r="C13" s="70" t="s">
-        <v>231</v>
-      </c>
-      <c r="D13" s="28" t="s">
-        <v>232</v>
-      </c>
-    </row>
-    <row r="14" spans="2:4" ht="30.75">
-      <c r="B14" s="73"/>
-      <c r="C14" s="71"/>
-      <c r="D14" s="31" t="s">
-        <v>229</v>
-      </c>
     </row>
     <row r="15" spans="2:4" ht="45.75">
-      <c r="B15" s="73"/>
-      <c r="C15" s="71"/>
+      <c r="B15" s="78"/>
+      <c r="C15" s="72"/>
       <c r="D15" s="30" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
     </row>
     <row r="16" spans="2:4" ht="60">
-      <c r="B16" s="73"/>
-      <c r="C16" s="71"/>
+      <c r="B16" s="78"/>
+      <c r="C16" s="72"/>
       <c r="D16" s="30" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
     </row>
     <row r="17" spans="2:4" ht="45">
-      <c r="B17" s="72" t="s">
-        <v>235</v>
-      </c>
-      <c r="C17" s="70" t="s">
+      <c r="B17" s="77" t="s">
         <v>236</v>
       </c>
+      <c r="C17" s="71" t="s">
+        <v>237</v>
+      </c>
       <c r="D17" s="28" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
     </row>
     <row r="18" spans="2:4" ht="45">
-      <c r="B18" s="73"/>
-      <c r="C18" s="71"/>
+      <c r="B18" s="78"/>
+      <c r="C18" s="72"/>
       <c r="D18" s="30" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
     </row>
     <row r="19" spans="2:4" ht="60.75" customHeight="1">
-      <c r="B19" s="72" t="s">
-        <v>239</v>
-      </c>
-      <c r="C19" s="70" t="s">
+      <c r="B19" s="77" t="s">
         <v>240</v>
       </c>
+      <c r="C19" s="71" t="s">
+        <v>241</v>
+      </c>
       <c r="D19" s="28" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
     </row>
     <row r="20" spans="2:4" ht="30.75">
-      <c r="B20" s="73"/>
-      <c r="C20" s="71"/>
+      <c r="B20" s="78"/>
+      <c r="C20" s="72"/>
       <c r="D20" s="31" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
     </row>
     <row r="21" spans="2:4" ht="45.75">
-      <c r="B21" s="72" t="s">
-        <v>242</v>
-      </c>
-      <c r="C21" s="70" t="s">
+      <c r="B21" s="77" t="s">
         <v>243</v>
       </c>
+      <c r="C21" s="71" t="s">
+        <v>244</v>
+      </c>
       <c r="D21" s="28" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
     </row>
     <row r="22" spans="2:4" ht="30.75">
-      <c r="B22" s="73"/>
-      <c r="C22" s="71"/>
+      <c r="B22" s="78"/>
+      <c r="C22" s="72"/>
       <c r="D22" s="31" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
     </row>
     <row r="23" spans="2:4" ht="62.25" customHeight="1">
-      <c r="B23" s="72" t="s">
-        <v>245</v>
-      </c>
-      <c r="C23" s="70" t="s">
+      <c r="B23" s="77" t="s">
         <v>246</v>
       </c>
+      <c r="C23" s="71" t="s">
+        <v>247</v>
+      </c>
       <c r="D23" s="28" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
     </row>
     <row r="24" spans="2:4" ht="62.25" customHeight="1">
-      <c r="B24" s="73"/>
-      <c r="C24" s="71"/>
+      <c r="B24" s="78"/>
+      <c r="C24" s="72"/>
       <c r="D24" s="30" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
     </row>
     <row r="25" spans="2:4" ht="30.75">
-      <c r="B25" s="75"/>
-      <c r="C25" s="74"/>
+      <c r="B25" s="79"/>
+      <c r="C25" s="73"/>
       <c r="D25" s="30" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
     </row>
     <row r="26" spans="2:4" ht="45.75">
-      <c r="B26" s="72" t="s">
+      <c r="B26" s="77" t="s">
+        <v>250</v>
+      </c>
+      <c r="C26" s="71" t="s">
+        <v>251</v>
+      </c>
+      <c r="D26" s="28" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="27" spans="2:4" ht="60.75">
+      <c r="B27" s="78"/>
+      <c r="C27" s="72"/>
+      <c r="D27" s="30" t="s">
         <v>249</v>
       </c>
-      <c r="C26" s="70" t="s">
-        <v>250</v>
-      </c>
-      <c r="D26" s="28" t="s">
-        <v>247</v>
-      </c>
-    </row>
-    <row r="27" spans="2:4" ht="60.75">
-      <c r="B27" s="73"/>
-      <c r="C27" s="71"/>
-      <c r="D27" s="30" t="s">
-        <v>248</v>
-      </c>
     </row>
     <row r="28" spans="2:4" ht="30.75">
-      <c r="B28" s="73"/>
-      <c r="C28" s="71"/>
+      <c r="B28" s="78"/>
+      <c r="C28" s="72"/>
       <c r="D28" s="30" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
     </row>
     <row r="29" spans="2:4" ht="45.75">
-      <c r="B29" s="76" t="s">
-        <v>251</v>
-      </c>
-      <c r="C29" s="70" t="s">
-        <v>252</v>
+      <c r="B29" s="74" t="s">
+        <v>253</v>
+      </c>
+      <c r="C29" s="71" t="s">
+        <v>254</v>
       </c>
       <c r="D29" s="28" t="s">
-        <v>247</v>
+        <v>255</v>
       </c>
     </row>
     <row r="30" spans="2:4" ht="60.75">
-      <c r="B30" s="77"/>
-      <c r="C30" s="71"/>
+      <c r="B30" s="75"/>
+      <c r="C30" s="72"/>
       <c r="D30" s="30" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
     </row>
     <row r="31" spans="2:4" ht="30.75">
-      <c r="B31" s="77"/>
-      <c r="C31" s="71"/>
+      <c r="B31" s="75"/>
+      <c r="C31" s="72"/>
       <c r="D31" s="30" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
     </row>
     <row r="32" spans="2:4" ht="60.75">
-      <c r="B32" s="77"/>
-      <c r="C32" s="71"/>
+      <c r="B32" s="75"/>
+      <c r="C32" s="72"/>
       <c r="D32" s="30" t="s">
-        <v>253</v>
+        <v>256</v>
       </c>
     </row>
     <row r="33" spans="2:4" ht="76.5" customHeight="1">
-      <c r="B33" s="76" t="s">
-        <v>254</v>
-      </c>
-      <c r="C33" s="70" t="s">
-        <v>255</v>
+      <c r="B33" s="74" t="s">
+        <v>257</v>
+      </c>
+      <c r="C33" s="71" t="s">
+        <v>258</v>
       </c>
       <c r="D33" s="28" t="s">
-        <v>256</v>
+        <v>259</v>
       </c>
     </row>
     <row r="34" spans="2:4" ht="30.75">
-      <c r="B34" s="77"/>
-      <c r="C34" s="71"/>
+      <c r="B34" s="75"/>
+      <c r="C34" s="72"/>
       <c r="D34" s="30" t="s">
-        <v>257</v>
+        <v>260</v>
       </c>
     </row>
     <row r="35" spans="2:4" ht="30.75">
-      <c r="B35" s="77"/>
-      <c r="C35" s="71"/>
+      <c r="B35" s="75"/>
+      <c r="C35" s="72"/>
       <c r="D35" s="30" t="s">
-        <v>258</v>
+        <v>261</v>
       </c>
     </row>
     <row r="36" spans="2:4" ht="60.75">
-      <c r="B36" s="77"/>
-      <c r="C36" s="71"/>
+      <c r="B36" s="75"/>
+      <c r="C36" s="72"/>
       <c r="D36" s="30" t="s">
-        <v>259</v>
+        <v>262</v>
       </c>
     </row>
     <row r="37" spans="2:4" ht="137.25">
-      <c r="B37" s="77"/>
-      <c r="C37" s="71"/>
+      <c r="B37" s="75"/>
+      <c r="C37" s="72"/>
       <c r="D37" s="30" t="s">
         <v>144</v>
       </c>
     </row>
     <row r="38" spans="2:4" ht="45.75">
-      <c r="B38" s="78"/>
-      <c r="C38" s="74"/>
+      <c r="B38" s="76"/>
+      <c r="C38" s="73"/>
       <c r="D38" s="31" t="s">
         <v>194</v>
       </c>
@@ -8633,14 +8685,6 @@
     </row>
   </sheetData>
   <mergeCells count="24">
-    <mergeCell ref="C33:C38"/>
-    <mergeCell ref="B33:B38"/>
-    <mergeCell ref="C29:C32"/>
-    <mergeCell ref="B29:B32"/>
-    <mergeCell ref="C23:C25"/>
-    <mergeCell ref="B23:B25"/>
-    <mergeCell ref="C26:C28"/>
-    <mergeCell ref="B26:B28"/>
     <mergeCell ref="C21:C22"/>
     <mergeCell ref="B21:B22"/>
     <mergeCell ref="C19:C20"/>
@@ -8657,6 +8701,14 @@
     <mergeCell ref="B13:B16"/>
     <mergeCell ref="C17:C18"/>
     <mergeCell ref="B17:B18"/>
+    <mergeCell ref="C33:C38"/>
+    <mergeCell ref="B33:B38"/>
+    <mergeCell ref="C29:C32"/>
+    <mergeCell ref="B29:B32"/>
+    <mergeCell ref="C23:C25"/>
+    <mergeCell ref="B23:B25"/>
+    <mergeCell ref="C26:C28"/>
+    <mergeCell ref="B26:B28"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -8664,10 +8716,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1914FF74-0E8B-4E92-8BDD-103E839E1854}">
-  <dimension ref="B3:J28"/>
+  <dimension ref="B3:J33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="D28" sqref="D28"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="C37" sqref="C37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -8683,55 +8735,55 @@
         <v>27</v>
       </c>
       <c r="C3" s="47" t="s">
-        <v>260</v>
+        <v>263</v>
       </c>
       <c r="D3" s="51" t="s">
-        <v>261</v>
+        <v>264</v>
       </c>
       <c r="I3" s="51" t="s">
-        <v>262</v>
+        <v>265</v>
       </c>
     </row>
     <row r="4" spans="2:10">
       <c r="B4" s="3" t="s">
-        <v>263</v>
+        <v>266</v>
       </c>
       <c r="C4" t="s">
-        <v>264</v>
+        <v>267</v>
       </c>
       <c r="D4" t="s">
-        <v>265</v>
+        <v>268</v>
       </c>
       <c r="I4" s="56" t="s">
-        <v>266</v>
+        <v>269</v>
       </c>
       <c r="J4" s="57" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
     </row>
     <row r="5" spans="2:10" ht="121.5">
       <c r="B5" s="3" t="s">
-        <v>267</v>
+        <v>270</v>
       </c>
       <c r="C5" t="s">
-        <v>268</v>
+        <v>271</v>
       </c>
       <c r="D5" t="s">
         <v>57</v>
       </c>
       <c r="I5" t="s">
-        <v>265</v>
+        <v>268</v>
       </c>
       <c r="J5" s="53" t="s">
-        <v>269</v>
+        <v>272</v>
       </c>
     </row>
     <row r="6" spans="2:10" ht="91.5">
       <c r="B6" s="3" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="C6" s="53" t="s">
-        <v>271</v>
+        <v>274</v>
       </c>
       <c r="D6" t="s">
         <v>72</v>
@@ -8740,68 +8792,68 @@
         <v>72</v>
       </c>
       <c r="J6" s="53" t="s">
-        <v>272</v>
+        <v>275</v>
       </c>
     </row>
     <row r="7" spans="2:10" ht="137.25">
       <c r="B7" s="3" t="s">
-        <v>273</v>
+        <v>276</v>
       </c>
       <c r="C7" t="s">
-        <v>274</v>
+        <v>277</v>
       </c>
       <c r="D7" t="s">
-        <v>275</v>
+        <v>278</v>
       </c>
       <c r="I7" t="s">
-        <v>275</v>
+        <v>278</v>
       </c>
       <c r="J7" s="53" t="s">
-        <v>276</v>
-      </c>
-    </row>
-    <row r="8" spans="2:10" ht="76.5">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="8" spans="2:10" ht="91.5">
       <c r="B8" s="3" t="s">
-        <v>277</v>
+        <v>280</v>
       </c>
       <c r="C8" s="53" t="s">
-        <v>278</v>
+        <v>281</v>
       </c>
       <c r="I8" t="s">
         <v>57</v>
       </c>
       <c r="J8" s="53" t="s">
-        <v>279</v>
+        <v>282</v>
       </c>
     </row>
     <row r="9" spans="2:10" ht="137.25">
       <c r="B9" s="3" t="s">
-        <v>280</v>
+        <v>283</v>
       </c>
       <c r="C9" t="s">
-        <v>281</v>
+        <v>284</v>
       </c>
       <c r="I9" t="s">
         <v>58</v>
       </c>
       <c r="J9" s="53" t="s">
-        <v>282</v>
+        <v>285</v>
       </c>
     </row>
     <row r="10" spans="2:10">
       <c r="B10" s="3" t="s">
-        <v>283</v>
+        <v>286</v>
       </c>
       <c r="C10" t="s">
-        <v>284</v>
+        <v>287</v>
       </c>
     </row>
     <row r="11" spans="2:10">
       <c r="B11" s="3" t="s">
-        <v>285</v>
+        <v>288</v>
       </c>
       <c r="C11" t="s">
-        <v>286</v>
+        <v>289</v>
       </c>
       <c r="D11" t="s">
         <v>58</v>
@@ -8809,10 +8861,10 @@
     </row>
     <row r="12" spans="2:10">
       <c r="B12" s="3" t="s">
-        <v>287</v>
+        <v>290</v>
       </c>
       <c r="C12" t="s">
-        <v>288</v>
+        <v>291</v>
       </c>
       <c r="D12" t="s">
         <v>58</v>
@@ -8820,21 +8872,21 @@
     </row>
     <row r="13" spans="2:10">
       <c r="B13" s="3" t="s">
-        <v>289</v>
+        <v>292</v>
       </c>
       <c r="C13" t="s">
-        <v>290</v>
+        <v>293</v>
       </c>
       <c r="D13" t="s">
-        <v>265</v>
+        <v>268</v>
       </c>
     </row>
     <row r="14" spans="2:10">
       <c r="B14" s="3" t="s">
-        <v>291</v>
+        <v>294</v>
       </c>
       <c r="C14" t="s">
-        <v>292</v>
+        <v>295</v>
       </c>
       <c r="D14" t="s">
         <v>72</v>
@@ -8842,21 +8894,21 @@
     </row>
     <row r="15" spans="2:10">
       <c r="B15" s="3" t="s">
-        <v>293</v>
+        <v>296</v>
       </c>
       <c r="C15" t="s">
-        <v>294</v>
+        <v>297</v>
       </c>
       <c r="D15" t="s">
-        <v>275</v>
+        <v>278</v>
       </c>
     </row>
     <row r="16" spans="2:10" ht="30.75">
       <c r="B16" s="3" t="s">
-        <v>295</v>
+        <v>298</v>
       </c>
       <c r="C16" s="53" t="s">
-        <v>296</v>
+        <v>299</v>
       </c>
       <c r="D16" t="s">
         <v>57</v>
@@ -8864,21 +8916,21 @@
     </row>
     <row r="17" spans="2:4">
       <c r="B17" s="3" t="s">
-        <v>297</v>
+        <v>300</v>
       </c>
       <c r="C17" t="s">
-        <v>298</v>
+        <v>301</v>
       </c>
       <c r="D17" t="s">
-        <v>275</v>
+        <v>278</v>
       </c>
     </row>
     <row r="18" spans="2:4">
       <c r="B18" s="3" t="s">
-        <v>299</v>
+        <v>302</v>
       </c>
       <c r="C18" t="s">
-        <v>300</v>
+        <v>303</v>
       </c>
       <c r="D18" t="s">
         <v>57</v>
@@ -8886,10 +8938,10 @@
     </row>
     <row r="19" spans="2:4">
       <c r="B19" s="3" t="s">
-        <v>301</v>
+        <v>304</v>
       </c>
       <c r="C19" t="s">
-        <v>302</v>
+        <v>305</v>
       </c>
       <c r="D19" t="s">
         <v>58</v>
@@ -8897,10 +8949,10 @@
     </row>
     <row r="20" spans="2:4" ht="45.75">
       <c r="B20" s="58" t="s">
-        <v>303</v>
+        <v>306</v>
       </c>
       <c r="C20" s="59" t="s">
-        <v>304</v>
+        <v>307</v>
       </c>
       <c r="D20" s="2" t="s">
         <v>72</v>
@@ -8908,64 +8960,64 @@
     </row>
     <row r="21" spans="2:4">
       <c r="B21" s="3" t="s">
-        <v>305</v>
+        <v>308</v>
       </c>
       <c r="C21" t="s">
-        <v>306</v>
+        <v>309</v>
       </c>
       <c r="D21" t="s">
-        <v>265</v>
+        <v>268</v>
       </c>
     </row>
     <row r="22" spans="2:4">
       <c r="B22" s="3" t="s">
-        <v>307</v>
+        <v>310</v>
       </c>
       <c r="C22" t="s">
-        <v>308</v>
+        <v>311</v>
       </c>
     </row>
     <row r="23" spans="2:4">
       <c r="B23" s="3" t="s">
-        <v>309</v>
+        <v>312</v>
       </c>
       <c r="C23" t="s">
-        <v>310</v>
+        <v>313</v>
       </c>
       <c r="D23" t="s">
-        <v>275</v>
+        <v>278</v>
       </c>
     </row>
     <row r="24" spans="2:4" ht="30.75">
       <c r="B24" s="3" t="s">
-        <v>311</v>
+        <v>314</v>
       </c>
       <c r="C24" s="53" t="s">
-        <v>312</v>
+        <v>315</v>
       </c>
     </row>
     <row r="25" spans="2:4">
       <c r="B25" s="3" t="s">
-        <v>313</v>
+        <v>316</v>
       </c>
       <c r="C25" t="s">
-        <v>314</v>
+        <v>317</v>
       </c>
     </row>
     <row r="26" spans="2:4">
       <c r="B26" s="3" t="s">
-        <v>315</v>
+        <v>318</v>
       </c>
       <c r="C26" t="s">
-        <v>316</v>
+        <v>319</v>
       </c>
     </row>
     <row r="27" spans="2:4">
       <c r="B27" s="3" t="s">
-        <v>317</v>
+        <v>320</v>
       </c>
       <c r="C27" t="s">
-        <v>318</v>
+        <v>321</v>
       </c>
       <c r="D27" t="s">
         <v>72</v>
@@ -8973,10 +9025,59 @@
     </row>
     <row r="28" spans="2:4">
       <c r="B28" s="3" t="s">
-        <v>319</v>
+        <v>322</v>
       </c>
       <c r="C28" t="s">
-        <v>320</v>
+        <v>323</v>
+      </c>
+    </row>
+    <row r="29" spans="2:4" ht="45.75">
+      <c r="B29" s="60" t="s">
+        <v>324</v>
+      </c>
+      <c r="C29" s="53" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="30" spans="2:4">
+      <c r="B30" s="3" t="s">
+        <v>326</v>
+      </c>
+      <c r="C30" t="s">
+        <v>327</v>
+      </c>
+      <c r="D30" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="31" spans="2:4">
+      <c r="B31" s="3" t="s">
+        <v>328</v>
+      </c>
+      <c r="C31" t="s">
+        <v>329</v>
+      </c>
+      <c r="D31" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="32" spans="2:4" ht="45.75">
+      <c r="B32" s="3" t="s">
+        <v>330</v>
+      </c>
+      <c r="C32" s="53" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="33" spans="2:4">
+      <c r="B33" s="3" t="s">
+        <v>332</v>
+      </c>
+      <c r="C33" t="s">
+        <v>333</v>
+      </c>
+      <c r="D33" t="s">
+        <v>58</v>
       </c>
     </row>
   </sheetData>
@@ -8992,7 +9093,7 @@
   <dimension ref="B3:D30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+      <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -9007,52 +9108,52 @@
         <v>27</v>
       </c>
       <c r="C3" s="47" t="s">
-        <v>260</v>
+        <v>263</v>
       </c>
       <c r="D3" s="47" t="s">
-        <v>321</v>
+        <v>334</v>
       </c>
     </row>
     <row r="4" spans="2:4" ht="91.5">
       <c r="B4" s="55" t="s">
-        <v>322</v>
+        <v>335</v>
       </c>
       <c r="C4" s="54" t="s">
-        <v>323</v>
+        <v>336</v>
       </c>
       <c r="D4" s="54"/>
     </row>
     <row r="5" spans="2:4" ht="91.5">
       <c r="B5" s="55" t="s">
-        <v>324</v>
+        <v>337</v>
       </c>
       <c r="C5" s="54" t="s">
-        <v>325</v>
+        <v>338</v>
       </c>
       <c r="D5" s="54" t="s">
-        <v>326</v>
+        <v>339</v>
       </c>
     </row>
     <row r="6" spans="2:4" ht="76.5">
       <c r="B6" s="55" t="s">
-        <v>327</v>
+        <v>340</v>
       </c>
       <c r="C6" s="54" t="s">
-        <v>328</v>
+        <v>341</v>
       </c>
       <c r="D6" s="54" t="s">
-        <v>329</v>
+        <v>342</v>
       </c>
     </row>
     <row r="7" spans="2:4" ht="76.5">
       <c r="B7" s="55" t="s">
-        <v>330</v>
+        <v>343</v>
       </c>
       <c r="C7" s="54" t="s">
-        <v>331</v>
+        <v>344</v>
       </c>
       <c r="D7" s="54" t="s">
-        <v>332</v>
+        <v>345</v>
       </c>
     </row>
     <row r="8" spans="2:4">

</xml_diff>

<commit_message>
Added more cards and created Core decks
Added more cards and created Core decks
</commit_message>
<xml_diff>
--- a/ShipCardGameCalcs.xlsx
+++ b/ShipCardGameCalcs.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27321"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27411"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MultiplayerGame\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{4E65C079-02EE-4F6D-9EE7-E529B63EEBE3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{FA957633-AD9D-4FA3-8387-AF6D618A2C17}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="7" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -910,7 +910,7 @@
     <t>Swarm</t>
   </si>
   <si>
-    <t>Create X pod ship/s with 100 hull and can engage to deal 100 damage to enemy ship, they can also be used to block a gun slot</t>
+    <t>Create X pod ship/s with 100 hull and can engage to deal 100 damage to enemy ship, they can also be used to block a gun slot. Ship upgrades cant be attached to pod ships</t>
   </si>
   <si>
     <t>One to keep the enemy under pressure invading their ships during the early game. They will call for help from their swarm and become brutal in the early game, however during the late game they fall off.</t>
@@ -1750,8 +1750,17 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1761,15 +1770,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -7365,13 +7365,13 @@
     <row r="16" spans="2:19">
       <c r="P16">
         <f ca="1">RANDBETWEEN(0,123)</f>
-        <v>64</v>
+        <v>114</v>
       </c>
     </row>
     <row r="17" spans="2:16">
       <c r="P17" s="46">
         <f ca="1">RANDBETWEEN(0,6)</f>
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="18" spans="2:16">
@@ -7831,8 +7831,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{93013FD4-B940-4A70-A7DA-BF82FD0F616E}">
   <dimension ref="A2:K82"/>
   <sheetViews>
-    <sheetView topLeftCell="A51" workbookViewId="0">
-      <selection activeCell="I83" sqref="I83"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -8294,7 +8294,7 @@
   <dimension ref="B2:B11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J14" sqref="J14"/>
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -8381,7 +8381,7 @@
       </c>
     </row>
     <row r="3" spans="2:4" ht="106.5" customHeight="1">
-      <c r="B3" s="77" t="s">
+      <c r="B3" s="73" t="s">
         <v>213</v>
       </c>
       <c r="C3" s="71" t="s">
@@ -8392,28 +8392,28 @@
       </c>
     </row>
     <row r="4" spans="2:4" ht="106.5">
-      <c r="B4" s="78"/>
+      <c r="B4" s="74"/>
       <c r="C4" s="72"/>
       <c r="D4" s="29" t="s">
         <v>216</v>
       </c>
     </row>
     <row r="5" spans="2:4" ht="60.75">
-      <c r="B5" s="78"/>
+      <c r="B5" s="74"/>
       <c r="C5" s="72"/>
       <c r="D5" s="30" t="s">
         <v>217</v>
       </c>
     </row>
     <row r="6" spans="2:4" ht="75">
-      <c r="B6" s="78"/>
+      <c r="B6" s="74"/>
       <c r="C6" s="72"/>
       <c r="D6" s="30" t="s">
         <v>218</v>
       </c>
     </row>
     <row r="7" spans="2:4" ht="106.5">
-      <c r="B7" s="77" t="s">
+      <c r="B7" s="73" t="s">
         <v>219</v>
       </c>
       <c r="C7" s="71" t="s">
@@ -8424,14 +8424,14 @@
       </c>
     </row>
     <row r="8" spans="2:4" ht="90">
-      <c r="B8" s="78"/>
+      <c r="B8" s="74"/>
       <c r="C8" s="72"/>
       <c r="D8" s="30" t="s">
         <v>222</v>
       </c>
     </row>
     <row r="9" spans="2:4" ht="75">
-      <c r="B9" s="77" t="s">
+      <c r="B9" s="73" t="s">
         <v>223</v>
       </c>
       <c r="C9" s="71" t="s">
@@ -8442,14 +8442,14 @@
       </c>
     </row>
     <row r="10" spans="2:4" ht="60.75">
-      <c r="B10" s="79"/>
-      <c r="C10" s="73"/>
+      <c r="B10" s="76"/>
+      <c r="C10" s="75"/>
       <c r="D10" s="31" t="s">
         <v>226</v>
       </c>
     </row>
     <row r="11" spans="2:4" ht="76.5" customHeight="1">
-      <c r="B11" s="77" t="s">
+      <c r="B11" s="73" t="s">
         <v>227</v>
       </c>
       <c r="C11" s="71" t="s">
@@ -8460,14 +8460,14 @@
       </c>
     </row>
     <row r="12" spans="2:4" ht="30.75">
-      <c r="B12" s="78"/>
+      <c r="B12" s="74"/>
       <c r="C12" s="72"/>
       <c r="D12" s="31" t="s">
         <v>230</v>
       </c>
     </row>
     <row r="13" spans="2:4" ht="45.75">
-      <c r="B13" s="77" t="s">
+      <c r="B13" s="73" t="s">
         <v>231</v>
       </c>
       <c r="C13" s="71" t="s">
@@ -8478,28 +8478,28 @@
       </c>
     </row>
     <row r="14" spans="2:4" ht="30.75">
-      <c r="B14" s="78"/>
+      <c r="B14" s="74"/>
       <c r="C14" s="72"/>
       <c r="D14" s="31" t="s">
         <v>230</v>
       </c>
     </row>
     <row r="15" spans="2:4" ht="45.75">
-      <c r="B15" s="78"/>
+      <c r="B15" s="74"/>
       <c r="C15" s="72"/>
       <c r="D15" s="30" t="s">
         <v>234</v>
       </c>
     </row>
     <row r="16" spans="2:4" ht="60">
-      <c r="B16" s="78"/>
+      <c r="B16" s="74"/>
       <c r="C16" s="72"/>
       <c r="D16" s="30" t="s">
         <v>235</v>
       </c>
     </row>
     <row r="17" spans="2:4" ht="45">
-      <c r="B17" s="77" t="s">
+      <c r="B17" s="73" t="s">
         <v>236</v>
       </c>
       <c r="C17" s="71" t="s">
@@ -8510,14 +8510,14 @@
       </c>
     </row>
     <row r="18" spans="2:4" ht="45">
-      <c r="B18" s="78"/>
+      <c r="B18" s="74"/>
       <c r="C18" s="72"/>
       <c r="D18" s="30" t="s">
         <v>239</v>
       </c>
     </row>
     <row r="19" spans="2:4" ht="60.75" customHeight="1">
-      <c r="B19" s="77" t="s">
+      <c r="B19" s="73" t="s">
         <v>240</v>
       </c>
       <c r="C19" s="71" t="s">
@@ -8528,14 +8528,14 @@
       </c>
     </row>
     <row r="20" spans="2:4" ht="30.75">
-      <c r="B20" s="78"/>
+      <c r="B20" s="74"/>
       <c r="C20" s="72"/>
       <c r="D20" s="31" t="s">
         <v>230</v>
       </c>
     </row>
     <row r="21" spans="2:4" ht="45.75">
-      <c r="B21" s="77" t="s">
+      <c r="B21" s="73" t="s">
         <v>243</v>
       </c>
       <c r="C21" s="71" t="s">
@@ -8546,14 +8546,14 @@
       </c>
     </row>
     <row r="22" spans="2:4" ht="30.75">
-      <c r="B22" s="78"/>
+      <c r="B22" s="74"/>
       <c r="C22" s="72"/>
       <c r="D22" s="31" t="s">
         <v>230</v>
       </c>
     </row>
     <row r="23" spans="2:4" ht="62.25" customHeight="1">
-      <c r="B23" s="77" t="s">
+      <c r="B23" s="73" t="s">
         <v>246</v>
       </c>
       <c r="C23" s="71" t="s">
@@ -8564,21 +8564,21 @@
       </c>
     </row>
     <row r="24" spans="2:4" ht="62.25" customHeight="1">
-      <c r="B24" s="78"/>
+      <c r="B24" s="74"/>
       <c r="C24" s="72"/>
       <c r="D24" s="30" t="s">
         <v>249</v>
       </c>
     </row>
     <row r="25" spans="2:4" ht="30.75">
-      <c r="B25" s="79"/>
-      <c r="C25" s="73"/>
+      <c r="B25" s="76"/>
+      <c r="C25" s="75"/>
       <c r="D25" s="30" t="s">
         <v>230</v>
       </c>
     </row>
     <row r="26" spans="2:4" ht="45.75">
-      <c r="B26" s="77" t="s">
+      <c r="B26" s="73" t="s">
         <v>250</v>
       </c>
       <c r="C26" s="71" t="s">
@@ -8589,21 +8589,21 @@
       </c>
     </row>
     <row r="27" spans="2:4" ht="60.75">
-      <c r="B27" s="78"/>
+      <c r="B27" s="74"/>
       <c r="C27" s="72"/>
       <c r="D27" s="30" t="s">
         <v>249</v>
       </c>
     </row>
     <row r="28" spans="2:4" ht="30.75">
-      <c r="B28" s="78"/>
+      <c r="B28" s="74"/>
       <c r="C28" s="72"/>
       <c r="D28" s="30" t="s">
         <v>230</v>
       </c>
     </row>
     <row r="29" spans="2:4" ht="45.75">
-      <c r="B29" s="74" t="s">
+      <c r="B29" s="77" t="s">
         <v>253</v>
       </c>
       <c r="C29" s="71" t="s">
@@ -8614,28 +8614,28 @@
       </c>
     </row>
     <row r="30" spans="2:4" ht="60.75">
-      <c r="B30" s="75"/>
+      <c r="B30" s="78"/>
       <c r="C30" s="72"/>
       <c r="D30" s="30" t="s">
         <v>249</v>
       </c>
     </row>
     <row r="31" spans="2:4" ht="30.75">
-      <c r="B31" s="75"/>
+      <c r="B31" s="78"/>
       <c r="C31" s="72"/>
       <c r="D31" s="30" t="s">
         <v>230</v>
       </c>
     </row>
     <row r="32" spans="2:4" ht="60.75">
-      <c r="B32" s="75"/>
+      <c r="B32" s="78"/>
       <c r="C32" s="72"/>
       <c r="D32" s="30" t="s">
         <v>256</v>
       </c>
     </row>
     <row r="33" spans="2:4" ht="76.5" customHeight="1">
-      <c r="B33" s="74" t="s">
+      <c r="B33" s="77" t="s">
         <v>257</v>
       </c>
       <c r="C33" s="71" t="s">
@@ -8646,36 +8646,36 @@
       </c>
     </row>
     <row r="34" spans="2:4" ht="30.75">
-      <c r="B34" s="75"/>
+      <c r="B34" s="78"/>
       <c r="C34" s="72"/>
       <c r="D34" s="30" t="s">
         <v>260</v>
       </c>
     </row>
     <row r="35" spans="2:4" ht="30.75">
-      <c r="B35" s="75"/>
+      <c r="B35" s="78"/>
       <c r="C35" s="72"/>
       <c r="D35" s="30" t="s">
         <v>261</v>
       </c>
     </row>
     <row r="36" spans="2:4" ht="60.75">
-      <c r="B36" s="75"/>
+      <c r="B36" s="78"/>
       <c r="C36" s="72"/>
       <c r="D36" s="30" t="s">
         <v>262</v>
       </c>
     </row>
     <row r="37" spans="2:4" ht="137.25">
-      <c r="B37" s="75"/>
+      <c r="B37" s="78"/>
       <c r="C37" s="72"/>
       <c r="D37" s="30" t="s">
         <v>144</v>
       </c>
     </row>
     <row r="38" spans="2:4" ht="45.75">
-      <c r="B38" s="76"/>
-      <c r="C38" s="73"/>
+      <c r="B38" s="79"/>
+      <c r="C38" s="75"/>
       <c r="D38" s="31" t="s">
         <v>194</v>
       </c>
@@ -8685,6 +8685,14 @@
     </row>
   </sheetData>
   <mergeCells count="24">
+    <mergeCell ref="C33:C38"/>
+    <mergeCell ref="B33:B38"/>
+    <mergeCell ref="C29:C32"/>
+    <mergeCell ref="B29:B32"/>
+    <mergeCell ref="C23:C25"/>
+    <mergeCell ref="B23:B25"/>
+    <mergeCell ref="C26:C28"/>
+    <mergeCell ref="B26:B28"/>
     <mergeCell ref="C21:C22"/>
     <mergeCell ref="B21:B22"/>
     <mergeCell ref="C19:C20"/>
@@ -8701,14 +8709,6 @@
     <mergeCell ref="B13:B16"/>
     <mergeCell ref="C17:C18"/>
     <mergeCell ref="B17:B18"/>
-    <mergeCell ref="C33:C38"/>
-    <mergeCell ref="B33:B38"/>
-    <mergeCell ref="C29:C32"/>
-    <mergeCell ref="B29:B32"/>
-    <mergeCell ref="C23:C25"/>
-    <mergeCell ref="B23:B25"/>
-    <mergeCell ref="C26:C28"/>
-    <mergeCell ref="B26:B28"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -8718,8 +8718,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1914FF74-0E8B-4E92-8BDD-103E839E1854}">
   <dimension ref="B3:J33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="C37" sqref="C37"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>

</xml_diff>

<commit_message>
Started getting together images for cards
Started creating assets for the cards using midjourney ai
</commit_message>
<xml_diff>
--- a/ShipCardGameCalcs.xlsx
+++ b/ShipCardGameCalcs.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27411"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27421"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MultiplayerGame\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{FA957633-AD9D-4FA3-8387-AF6D618A2C17}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{D157256E-4187-4860-BE7A-BCE16CEA1590}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="7" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -7365,13 +7365,13 @@
     <row r="16" spans="2:19">
       <c r="P16">
         <f ca="1">RANDBETWEEN(0,123)</f>
-        <v>114</v>
+        <v>44</v>
       </c>
     </row>
     <row r="17" spans="2:16">
       <c r="P17" s="46">
         <f ca="1">RANDBETWEEN(0,6)</f>
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="18" spans="2:16">

</xml_diff>